<commit_message>
RDM-1240 - search by metadata - definition store changes to support metadata
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\moj\ccd-definition-store-api\excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{762D8855-9D7A-44BB-B73E-BC2C5764EE6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BEE1A29C-FE1F-4289-9A5F-9476F59E1119}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="16380" windowHeight="8194" tabRatio="757" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="229">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>[STATE]</t>
+  </si>
+  <si>
+    <t>Case Ref</t>
+  </si>
+  <si>
+    <t>[CASE_REFERENCE]</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1162,6 +1168,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2688,7 +2702,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -3035,6 +3049,40 @@
       <c r="Z9" s="35"/>
       <c r="AA9" s="35"/>
     </row>
+    <row r="10" spans="1:27" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="35">
+        <v>10</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="3">
@@ -3046,7 +3094,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3055,7 +3103,7 @@
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{00000000-0002-0000-0900-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
@@ -3074,6 +3122,15 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{95A3FE18-EAD8-4250-AD62-FC435CA29329}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C10:C11</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3082,10 +3139,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -3385,9 +3442,2104 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:1025" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A17" s="77">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="78"/>
+      <c r="C17" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="80">
+        <v>11</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AR17"/>
+      <c r="AS17"/>
+      <c r="AT17"/>
+      <c r="AU17"/>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+      <c r="BA17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BD17"/>
+      <c r="BE17"/>
+      <c r="BF17"/>
+      <c r="BG17"/>
+      <c r="BH17"/>
+      <c r="BI17"/>
+      <c r="BJ17"/>
+      <c r="BK17"/>
+      <c r="BL17"/>
+      <c r="BM17"/>
+      <c r="BN17"/>
+      <c r="BO17"/>
+      <c r="BP17"/>
+      <c r="BQ17"/>
+      <c r="BR17"/>
+      <c r="BS17"/>
+      <c r="BT17"/>
+      <c r="BU17"/>
+      <c r="BV17"/>
+      <c r="BW17"/>
+      <c r="BX17"/>
+      <c r="BY17"/>
+      <c r="BZ17"/>
+      <c r="CA17"/>
+      <c r="CB17"/>
+      <c r="CC17"/>
+      <c r="CD17"/>
+      <c r="CE17"/>
+      <c r="CF17"/>
+      <c r="CG17"/>
+      <c r="CH17"/>
+      <c r="CI17"/>
+      <c r="CJ17"/>
+      <c r="CK17"/>
+      <c r="CL17"/>
+      <c r="CM17"/>
+      <c r="CN17"/>
+      <c r="CO17"/>
+      <c r="CP17"/>
+      <c r="CQ17"/>
+      <c r="CR17"/>
+      <c r="CS17"/>
+      <c r="CT17"/>
+      <c r="CU17"/>
+      <c r="CV17"/>
+      <c r="CW17"/>
+      <c r="CX17"/>
+      <c r="CY17"/>
+      <c r="CZ17"/>
+      <c r="DA17"/>
+      <c r="DB17"/>
+      <c r="DC17"/>
+      <c r="DD17"/>
+      <c r="DE17"/>
+      <c r="DF17"/>
+      <c r="DG17"/>
+      <c r="DH17"/>
+      <c r="DI17"/>
+      <c r="DJ17"/>
+      <c r="DK17"/>
+      <c r="DL17"/>
+      <c r="DM17"/>
+      <c r="DN17"/>
+      <c r="DO17"/>
+      <c r="DP17"/>
+      <c r="DQ17"/>
+      <c r="DR17"/>
+      <c r="DS17"/>
+      <c r="DT17"/>
+      <c r="DU17"/>
+      <c r="DV17"/>
+      <c r="DW17"/>
+      <c r="DX17"/>
+      <c r="DY17"/>
+      <c r="DZ17"/>
+      <c r="EA17"/>
+      <c r="EB17"/>
+      <c r="EC17"/>
+      <c r="ED17"/>
+      <c r="EE17"/>
+      <c r="EF17"/>
+      <c r="EG17"/>
+      <c r="EH17"/>
+      <c r="EI17"/>
+      <c r="EJ17"/>
+      <c r="EK17"/>
+      <c r="EL17"/>
+      <c r="EM17"/>
+      <c r="EN17"/>
+      <c r="EO17"/>
+      <c r="EP17"/>
+      <c r="EQ17"/>
+      <c r="ER17"/>
+      <c r="ES17"/>
+      <c r="ET17"/>
+      <c r="EU17"/>
+      <c r="EV17"/>
+      <c r="EW17"/>
+      <c r="EX17"/>
+      <c r="EY17"/>
+      <c r="EZ17"/>
+      <c r="FA17"/>
+      <c r="FB17"/>
+      <c r="FC17"/>
+      <c r="FD17"/>
+      <c r="FE17"/>
+      <c r="FF17"/>
+      <c r="FG17"/>
+      <c r="FH17"/>
+      <c r="FI17"/>
+      <c r="FJ17"/>
+      <c r="FK17"/>
+      <c r="FL17"/>
+      <c r="FM17"/>
+      <c r="FN17"/>
+      <c r="FO17"/>
+      <c r="FP17"/>
+      <c r="FQ17"/>
+      <c r="FR17"/>
+      <c r="FS17"/>
+      <c r="FT17"/>
+      <c r="FU17"/>
+      <c r="FV17"/>
+      <c r="FW17"/>
+      <c r="FX17"/>
+      <c r="FY17"/>
+      <c r="FZ17"/>
+      <c r="GA17"/>
+      <c r="GB17"/>
+      <c r="GC17"/>
+      <c r="GD17"/>
+      <c r="GE17"/>
+      <c r="GF17"/>
+      <c r="GG17"/>
+      <c r="GH17"/>
+      <c r="GI17"/>
+      <c r="GJ17"/>
+      <c r="GK17"/>
+      <c r="GL17"/>
+      <c r="GM17"/>
+      <c r="GN17"/>
+      <c r="GO17"/>
+      <c r="GP17"/>
+      <c r="GQ17"/>
+      <c r="GR17"/>
+      <c r="GS17"/>
+      <c r="GT17"/>
+      <c r="GU17"/>
+      <c r="GV17"/>
+      <c r="GW17"/>
+      <c r="GX17"/>
+      <c r="GY17"/>
+      <c r="GZ17"/>
+      <c r="HA17"/>
+      <c r="HB17"/>
+      <c r="HC17"/>
+      <c r="HD17"/>
+      <c r="HE17"/>
+      <c r="HF17"/>
+      <c r="HG17"/>
+      <c r="HH17"/>
+      <c r="HI17"/>
+      <c r="HJ17"/>
+      <c r="HK17"/>
+      <c r="HL17"/>
+      <c r="HM17"/>
+      <c r="HN17"/>
+      <c r="HO17"/>
+      <c r="HP17"/>
+      <c r="HQ17"/>
+      <c r="HR17"/>
+      <c r="HS17"/>
+      <c r="HT17"/>
+      <c r="HU17"/>
+      <c r="HV17"/>
+      <c r="HW17"/>
+      <c r="HX17"/>
+      <c r="HY17"/>
+      <c r="HZ17"/>
+      <c r="IA17"/>
+      <c r="IB17"/>
+      <c r="IC17"/>
+      <c r="ID17"/>
+      <c r="IE17"/>
+      <c r="IF17"/>
+      <c r="IG17"/>
+      <c r="IH17"/>
+      <c r="II17"/>
+      <c r="IJ17"/>
+      <c r="IK17"/>
+      <c r="IL17"/>
+      <c r="IM17"/>
+      <c r="IN17"/>
+      <c r="IO17"/>
+      <c r="IP17"/>
+      <c r="IQ17"/>
+      <c r="IR17"/>
+      <c r="IS17"/>
+      <c r="IT17"/>
+      <c r="IU17"/>
+      <c r="IV17"/>
+      <c r="IW17"/>
+      <c r="IX17"/>
+      <c r="IY17"/>
+      <c r="IZ17"/>
+      <c r="JA17"/>
+      <c r="JB17"/>
+      <c r="JC17"/>
+      <c r="JD17"/>
+      <c r="JE17"/>
+      <c r="JF17"/>
+      <c r="JG17"/>
+      <c r="JH17"/>
+      <c r="JI17"/>
+      <c r="JJ17"/>
+      <c r="JK17"/>
+      <c r="JL17"/>
+      <c r="JM17"/>
+      <c r="JN17"/>
+      <c r="JO17"/>
+      <c r="JP17"/>
+      <c r="JQ17"/>
+      <c r="JR17"/>
+      <c r="JS17"/>
+      <c r="JT17"/>
+      <c r="JU17"/>
+      <c r="JV17"/>
+      <c r="JW17"/>
+      <c r="JX17"/>
+      <c r="JY17"/>
+      <c r="JZ17"/>
+      <c r="KA17"/>
+      <c r="KB17"/>
+      <c r="KC17"/>
+      <c r="KD17"/>
+      <c r="KE17"/>
+      <c r="KF17"/>
+      <c r="KG17"/>
+      <c r="KH17"/>
+      <c r="KI17"/>
+      <c r="KJ17"/>
+      <c r="KK17"/>
+      <c r="KL17"/>
+      <c r="KM17"/>
+      <c r="KN17"/>
+      <c r="KO17"/>
+      <c r="KP17"/>
+      <c r="KQ17"/>
+      <c r="KR17"/>
+      <c r="KS17"/>
+      <c r="KT17"/>
+      <c r="KU17"/>
+      <c r="KV17"/>
+      <c r="KW17"/>
+      <c r="KX17"/>
+      <c r="KY17"/>
+      <c r="KZ17"/>
+      <c r="LA17"/>
+      <c r="LB17"/>
+      <c r="LC17"/>
+      <c r="LD17"/>
+      <c r="LE17"/>
+      <c r="LF17"/>
+      <c r="LG17"/>
+      <c r="LH17"/>
+      <c r="LI17"/>
+      <c r="LJ17"/>
+      <c r="LK17"/>
+      <c r="LL17"/>
+      <c r="LM17"/>
+      <c r="LN17"/>
+      <c r="LO17"/>
+      <c r="LP17"/>
+      <c r="LQ17"/>
+      <c r="LR17"/>
+      <c r="LS17"/>
+      <c r="LT17"/>
+      <c r="LU17"/>
+      <c r="LV17"/>
+      <c r="LW17"/>
+      <c r="LX17"/>
+      <c r="LY17"/>
+      <c r="LZ17"/>
+      <c r="MA17"/>
+      <c r="MB17"/>
+      <c r="MC17"/>
+      <c r="MD17"/>
+      <c r="ME17"/>
+      <c r="MF17"/>
+      <c r="MG17"/>
+      <c r="MH17"/>
+      <c r="MI17"/>
+      <c r="MJ17"/>
+      <c r="MK17"/>
+      <c r="ML17"/>
+      <c r="MM17"/>
+      <c r="MN17"/>
+      <c r="MO17"/>
+      <c r="MP17"/>
+      <c r="MQ17"/>
+      <c r="MR17"/>
+      <c r="MS17"/>
+      <c r="MT17"/>
+      <c r="MU17"/>
+      <c r="MV17"/>
+      <c r="MW17"/>
+      <c r="MX17"/>
+      <c r="MY17"/>
+      <c r="MZ17"/>
+      <c r="NA17"/>
+      <c r="NB17"/>
+      <c r="NC17"/>
+      <c r="ND17"/>
+      <c r="NE17"/>
+      <c r="NF17"/>
+      <c r="NG17"/>
+      <c r="NH17"/>
+      <c r="NI17"/>
+      <c r="NJ17"/>
+      <c r="NK17"/>
+      <c r="NL17"/>
+      <c r="NM17"/>
+      <c r="NN17"/>
+      <c r="NO17"/>
+      <c r="NP17"/>
+      <c r="NQ17"/>
+      <c r="NR17"/>
+      <c r="NS17"/>
+      <c r="NT17"/>
+      <c r="NU17"/>
+      <c r="NV17"/>
+      <c r="NW17"/>
+      <c r="NX17"/>
+      <c r="NY17"/>
+      <c r="NZ17"/>
+      <c r="OA17"/>
+      <c r="OB17"/>
+      <c r="OC17"/>
+      <c r="OD17"/>
+      <c r="OE17"/>
+      <c r="OF17"/>
+      <c r="OG17"/>
+      <c r="OH17"/>
+      <c r="OI17"/>
+      <c r="OJ17"/>
+      <c r="OK17"/>
+      <c r="OL17"/>
+      <c r="OM17"/>
+      <c r="ON17"/>
+      <c r="OO17"/>
+      <c r="OP17"/>
+      <c r="OQ17"/>
+      <c r="OR17"/>
+      <c r="OS17"/>
+      <c r="OT17"/>
+      <c r="OU17"/>
+      <c r="OV17"/>
+      <c r="OW17"/>
+      <c r="OX17"/>
+      <c r="OY17"/>
+      <c r="OZ17"/>
+      <c r="PA17"/>
+      <c r="PB17"/>
+      <c r="PC17"/>
+      <c r="PD17"/>
+      <c r="PE17"/>
+      <c r="PF17"/>
+      <c r="PG17"/>
+      <c r="PH17"/>
+      <c r="PI17"/>
+      <c r="PJ17"/>
+      <c r="PK17"/>
+      <c r="PL17"/>
+      <c r="PM17"/>
+      <c r="PN17"/>
+      <c r="PO17"/>
+      <c r="PP17"/>
+      <c r="PQ17"/>
+      <c r="PR17"/>
+      <c r="PS17"/>
+      <c r="PT17"/>
+      <c r="PU17"/>
+      <c r="PV17"/>
+      <c r="PW17"/>
+      <c r="PX17"/>
+      <c r="PY17"/>
+      <c r="PZ17"/>
+      <c r="QA17"/>
+      <c r="QB17"/>
+      <c r="QC17"/>
+      <c r="QD17"/>
+      <c r="QE17"/>
+      <c r="QF17"/>
+      <c r="QG17"/>
+      <c r="QH17"/>
+      <c r="QI17"/>
+      <c r="QJ17"/>
+      <c r="QK17"/>
+      <c r="QL17"/>
+      <c r="QM17"/>
+      <c r="QN17"/>
+      <c r="QO17"/>
+      <c r="QP17"/>
+      <c r="QQ17"/>
+      <c r="QR17"/>
+      <c r="QS17"/>
+      <c r="QT17"/>
+      <c r="QU17"/>
+      <c r="QV17"/>
+      <c r="QW17"/>
+      <c r="QX17"/>
+      <c r="QY17"/>
+      <c r="QZ17"/>
+      <c r="RA17"/>
+      <c r="RB17"/>
+      <c r="RC17"/>
+      <c r="RD17"/>
+      <c r="RE17"/>
+      <c r="RF17"/>
+      <c r="RG17"/>
+      <c r="RH17"/>
+      <c r="RI17"/>
+      <c r="RJ17"/>
+      <c r="RK17"/>
+      <c r="RL17"/>
+      <c r="RM17"/>
+      <c r="RN17"/>
+      <c r="RO17"/>
+      <c r="RP17"/>
+      <c r="RQ17"/>
+      <c r="RR17"/>
+      <c r="RS17"/>
+      <c r="RT17"/>
+      <c r="RU17"/>
+      <c r="RV17"/>
+      <c r="RW17"/>
+      <c r="RX17"/>
+      <c r="RY17"/>
+      <c r="RZ17"/>
+      <c r="SA17"/>
+      <c r="SB17"/>
+      <c r="SC17"/>
+      <c r="SD17"/>
+      <c r="SE17"/>
+      <c r="SF17"/>
+      <c r="SG17"/>
+      <c r="SH17"/>
+      <c r="SI17"/>
+      <c r="SJ17"/>
+      <c r="SK17"/>
+      <c r="SL17"/>
+      <c r="SM17"/>
+      <c r="SN17"/>
+      <c r="SO17"/>
+      <c r="SP17"/>
+      <c r="SQ17"/>
+      <c r="SR17"/>
+      <c r="SS17"/>
+      <c r="ST17"/>
+      <c r="SU17"/>
+      <c r="SV17"/>
+      <c r="SW17"/>
+      <c r="SX17"/>
+      <c r="SY17"/>
+      <c r="SZ17"/>
+      <c r="TA17"/>
+      <c r="TB17"/>
+      <c r="TC17"/>
+      <c r="TD17"/>
+      <c r="TE17"/>
+      <c r="TF17"/>
+      <c r="TG17"/>
+      <c r="TH17"/>
+      <c r="TI17"/>
+      <c r="TJ17"/>
+      <c r="TK17"/>
+      <c r="TL17"/>
+      <c r="TM17"/>
+      <c r="TN17"/>
+      <c r="TO17"/>
+      <c r="TP17"/>
+      <c r="TQ17"/>
+      <c r="TR17"/>
+      <c r="TS17"/>
+      <c r="TT17"/>
+      <c r="TU17"/>
+      <c r="TV17"/>
+      <c r="TW17"/>
+      <c r="TX17"/>
+      <c r="TY17"/>
+      <c r="TZ17"/>
+      <c r="UA17"/>
+      <c r="UB17"/>
+      <c r="UC17"/>
+      <c r="UD17"/>
+      <c r="UE17"/>
+      <c r="UF17"/>
+      <c r="UG17"/>
+      <c r="UH17"/>
+      <c r="UI17"/>
+      <c r="UJ17"/>
+      <c r="UK17"/>
+      <c r="UL17"/>
+      <c r="UM17"/>
+      <c r="UN17"/>
+      <c r="UO17"/>
+      <c r="UP17"/>
+      <c r="UQ17"/>
+      <c r="UR17"/>
+      <c r="US17"/>
+      <c r="UT17"/>
+      <c r="UU17"/>
+      <c r="UV17"/>
+      <c r="UW17"/>
+      <c r="UX17"/>
+      <c r="UY17"/>
+      <c r="UZ17"/>
+      <c r="VA17"/>
+      <c r="VB17"/>
+      <c r="VC17"/>
+      <c r="VD17"/>
+      <c r="VE17"/>
+      <c r="VF17"/>
+      <c r="VG17"/>
+      <c r="VH17"/>
+      <c r="VI17"/>
+      <c r="VJ17"/>
+      <c r="VK17"/>
+      <c r="VL17"/>
+      <c r="VM17"/>
+      <c r="VN17"/>
+      <c r="VO17"/>
+      <c r="VP17"/>
+      <c r="VQ17"/>
+      <c r="VR17"/>
+      <c r="VS17"/>
+      <c r="VT17"/>
+      <c r="VU17"/>
+      <c r="VV17"/>
+      <c r="VW17"/>
+      <c r="VX17"/>
+      <c r="VY17"/>
+      <c r="VZ17"/>
+      <c r="WA17"/>
+      <c r="WB17"/>
+      <c r="WC17"/>
+      <c r="WD17"/>
+      <c r="WE17"/>
+      <c r="WF17"/>
+      <c r="WG17"/>
+      <c r="WH17"/>
+      <c r="WI17"/>
+      <c r="WJ17"/>
+      <c r="WK17"/>
+      <c r="WL17"/>
+      <c r="WM17"/>
+      <c r="WN17"/>
+      <c r="WO17"/>
+      <c r="WP17"/>
+      <c r="WQ17"/>
+      <c r="WR17"/>
+      <c r="WS17"/>
+      <c r="WT17"/>
+      <c r="WU17"/>
+      <c r="WV17"/>
+      <c r="WW17"/>
+      <c r="WX17"/>
+      <c r="WY17"/>
+      <c r="WZ17"/>
+      <c r="XA17"/>
+      <c r="XB17"/>
+      <c r="XC17"/>
+      <c r="XD17"/>
+      <c r="XE17"/>
+      <c r="XF17"/>
+      <c r="XG17"/>
+      <c r="XH17"/>
+      <c r="XI17"/>
+      <c r="XJ17"/>
+      <c r="XK17"/>
+      <c r="XL17"/>
+      <c r="XM17"/>
+      <c r="XN17"/>
+      <c r="XO17"/>
+      <c r="XP17"/>
+      <c r="XQ17"/>
+      <c r="XR17"/>
+      <c r="XS17"/>
+      <c r="XT17"/>
+      <c r="XU17"/>
+      <c r="XV17"/>
+      <c r="XW17"/>
+      <c r="XX17"/>
+      <c r="XY17"/>
+      <c r="XZ17"/>
+      <c r="YA17"/>
+      <c r="YB17"/>
+      <c r="YC17"/>
+      <c r="YD17"/>
+      <c r="YE17"/>
+      <c r="YF17"/>
+      <c r="YG17"/>
+      <c r="YH17"/>
+      <c r="YI17"/>
+      <c r="YJ17"/>
+      <c r="YK17"/>
+      <c r="YL17"/>
+      <c r="YM17"/>
+      <c r="YN17"/>
+      <c r="YO17"/>
+      <c r="YP17"/>
+      <c r="YQ17"/>
+      <c r="YR17"/>
+      <c r="YS17"/>
+      <c r="YT17"/>
+      <c r="YU17"/>
+      <c r="YV17"/>
+      <c r="YW17"/>
+      <c r="YX17"/>
+      <c r="YY17"/>
+      <c r="YZ17"/>
+      <c r="ZA17"/>
+      <c r="ZB17"/>
+      <c r="ZC17"/>
+      <c r="ZD17"/>
+      <c r="ZE17"/>
+      <c r="ZF17"/>
+      <c r="ZG17"/>
+      <c r="ZH17"/>
+      <c r="ZI17"/>
+      <c r="ZJ17"/>
+      <c r="ZK17"/>
+      <c r="ZL17"/>
+      <c r="ZM17"/>
+      <c r="ZN17"/>
+      <c r="ZO17"/>
+      <c r="ZP17"/>
+      <c r="ZQ17"/>
+      <c r="ZR17"/>
+      <c r="ZS17"/>
+      <c r="ZT17"/>
+      <c r="ZU17"/>
+      <c r="ZV17"/>
+      <c r="ZW17"/>
+      <c r="ZX17"/>
+      <c r="ZY17"/>
+      <c r="ZZ17"/>
+      <c r="AAA17"/>
+      <c r="AAB17"/>
+      <c r="AAC17"/>
+      <c r="AAD17"/>
+      <c r="AAE17"/>
+      <c r="AAF17"/>
+      <c r="AAG17"/>
+      <c r="AAH17"/>
+      <c r="AAI17"/>
+      <c r="AAJ17"/>
+      <c r="AAK17"/>
+      <c r="AAL17"/>
+      <c r="AAM17"/>
+      <c r="AAN17"/>
+      <c r="AAO17"/>
+      <c r="AAP17"/>
+      <c r="AAQ17"/>
+      <c r="AAR17"/>
+      <c r="AAS17"/>
+      <c r="AAT17"/>
+      <c r="AAU17"/>
+      <c r="AAV17"/>
+      <c r="AAW17"/>
+      <c r="AAX17"/>
+      <c r="AAY17"/>
+      <c r="AAZ17"/>
+      <c r="ABA17"/>
+      <c r="ABB17"/>
+      <c r="ABC17"/>
+      <c r="ABD17"/>
+      <c r="ABE17"/>
+      <c r="ABF17"/>
+      <c r="ABG17"/>
+      <c r="ABH17"/>
+      <c r="ABI17"/>
+      <c r="ABJ17"/>
+      <c r="ABK17"/>
+      <c r="ABL17"/>
+      <c r="ABM17"/>
+      <c r="ABN17"/>
+      <c r="ABO17"/>
+      <c r="ABP17"/>
+      <c r="ABQ17"/>
+      <c r="ABR17"/>
+      <c r="ABS17"/>
+      <c r="ABT17"/>
+      <c r="ABU17"/>
+      <c r="ABV17"/>
+      <c r="ABW17"/>
+      <c r="ABX17"/>
+      <c r="ABY17"/>
+      <c r="ABZ17"/>
+      <c r="ACA17"/>
+      <c r="ACB17"/>
+      <c r="ACC17"/>
+      <c r="ACD17"/>
+      <c r="ACE17"/>
+      <c r="ACF17"/>
+      <c r="ACG17"/>
+      <c r="ACH17"/>
+      <c r="ACI17"/>
+      <c r="ACJ17"/>
+      <c r="ACK17"/>
+      <c r="ACL17"/>
+      <c r="ACM17"/>
+      <c r="ACN17"/>
+      <c r="ACO17"/>
+      <c r="ACP17"/>
+      <c r="ACQ17"/>
+      <c r="ACR17"/>
+      <c r="ACS17"/>
+      <c r="ACT17"/>
+      <c r="ACU17"/>
+      <c r="ACV17"/>
+      <c r="ACW17"/>
+      <c r="ACX17"/>
+      <c r="ACY17"/>
+      <c r="ACZ17"/>
+      <c r="ADA17"/>
+      <c r="ADB17"/>
+      <c r="ADC17"/>
+      <c r="ADD17"/>
+      <c r="ADE17"/>
+      <c r="ADF17"/>
+      <c r="ADG17"/>
+      <c r="ADH17"/>
+      <c r="ADI17"/>
+      <c r="ADJ17"/>
+      <c r="ADK17"/>
+      <c r="ADL17"/>
+      <c r="ADM17"/>
+      <c r="ADN17"/>
+      <c r="ADO17"/>
+      <c r="ADP17"/>
+      <c r="ADQ17"/>
+      <c r="ADR17"/>
+      <c r="ADS17"/>
+      <c r="ADT17"/>
+      <c r="ADU17"/>
+      <c r="ADV17"/>
+      <c r="ADW17"/>
+      <c r="ADX17"/>
+      <c r="ADY17"/>
+      <c r="ADZ17"/>
+      <c r="AEA17"/>
+      <c r="AEB17"/>
+      <c r="AEC17"/>
+      <c r="AED17"/>
+      <c r="AEE17"/>
+      <c r="AEF17"/>
+      <c r="AEG17"/>
+      <c r="AEH17"/>
+      <c r="AEI17"/>
+      <c r="AEJ17"/>
+      <c r="AEK17"/>
+      <c r="AEL17"/>
+      <c r="AEM17"/>
+      <c r="AEN17"/>
+      <c r="AEO17"/>
+      <c r="AEP17"/>
+      <c r="AEQ17"/>
+      <c r="AER17"/>
+      <c r="AES17"/>
+      <c r="AET17"/>
+      <c r="AEU17"/>
+      <c r="AEV17"/>
+      <c r="AEW17"/>
+      <c r="AEX17"/>
+      <c r="AEY17"/>
+      <c r="AEZ17"/>
+      <c r="AFA17"/>
+      <c r="AFB17"/>
+      <c r="AFC17"/>
+      <c r="AFD17"/>
+      <c r="AFE17"/>
+      <c r="AFF17"/>
+      <c r="AFG17"/>
+      <c r="AFH17"/>
+      <c r="AFI17"/>
+      <c r="AFJ17"/>
+      <c r="AFK17"/>
+      <c r="AFL17"/>
+      <c r="AFM17"/>
+      <c r="AFN17"/>
+      <c r="AFO17"/>
+      <c r="AFP17"/>
+      <c r="AFQ17"/>
+      <c r="AFR17"/>
+      <c r="AFS17"/>
+      <c r="AFT17"/>
+      <c r="AFU17"/>
+      <c r="AFV17"/>
+      <c r="AFW17"/>
+      <c r="AFX17"/>
+      <c r="AFY17"/>
+      <c r="AFZ17"/>
+      <c r="AGA17"/>
+      <c r="AGB17"/>
+      <c r="AGC17"/>
+      <c r="AGD17"/>
+      <c r="AGE17"/>
+      <c r="AGF17"/>
+      <c r="AGG17"/>
+      <c r="AGH17"/>
+      <c r="AGI17"/>
+      <c r="AGJ17"/>
+      <c r="AGK17"/>
+      <c r="AGL17"/>
+      <c r="AGM17"/>
+      <c r="AGN17"/>
+      <c r="AGO17"/>
+      <c r="AGP17"/>
+      <c r="AGQ17"/>
+      <c r="AGR17"/>
+      <c r="AGS17"/>
+      <c r="AGT17"/>
+      <c r="AGU17"/>
+      <c r="AGV17"/>
+      <c r="AGW17"/>
+      <c r="AGX17"/>
+      <c r="AGY17"/>
+      <c r="AGZ17"/>
+      <c r="AHA17"/>
+      <c r="AHB17"/>
+      <c r="AHC17"/>
+      <c r="AHD17"/>
+      <c r="AHE17"/>
+      <c r="AHF17"/>
+      <c r="AHG17"/>
+      <c r="AHH17"/>
+      <c r="AHI17"/>
+      <c r="AHJ17"/>
+      <c r="AHK17"/>
+      <c r="AHL17"/>
+      <c r="AHM17"/>
+      <c r="AHN17"/>
+      <c r="AHO17"/>
+      <c r="AHP17"/>
+      <c r="AHQ17"/>
+      <c r="AHR17"/>
+      <c r="AHS17"/>
+      <c r="AHT17"/>
+      <c r="AHU17"/>
+      <c r="AHV17"/>
+      <c r="AHW17"/>
+      <c r="AHX17"/>
+      <c r="AHY17"/>
+      <c r="AHZ17"/>
+      <c r="AIA17"/>
+      <c r="AIB17"/>
+      <c r="AIC17"/>
+      <c r="AID17"/>
+      <c r="AIE17"/>
+      <c r="AIF17"/>
+      <c r="AIG17"/>
+      <c r="AIH17"/>
+      <c r="AII17"/>
+      <c r="AIJ17"/>
+      <c r="AIK17"/>
+      <c r="AIL17"/>
+      <c r="AIM17"/>
+      <c r="AIN17"/>
+      <c r="AIO17"/>
+      <c r="AIP17"/>
+      <c r="AIQ17"/>
+      <c r="AIR17"/>
+      <c r="AIS17"/>
+      <c r="AIT17"/>
+      <c r="AIU17"/>
+      <c r="AIV17"/>
+      <c r="AIW17"/>
+      <c r="AIX17"/>
+      <c r="AIY17"/>
+      <c r="AIZ17"/>
+      <c r="AJA17"/>
+      <c r="AJB17"/>
+      <c r="AJC17"/>
+      <c r="AJD17"/>
+      <c r="AJE17"/>
+      <c r="AJF17"/>
+      <c r="AJG17"/>
+      <c r="AJH17"/>
+      <c r="AJI17"/>
+      <c r="AJJ17"/>
+      <c r="AJK17"/>
+      <c r="AJL17"/>
+      <c r="AJM17"/>
+      <c r="AJN17"/>
+      <c r="AJO17"/>
+      <c r="AJP17"/>
+      <c r="AJQ17"/>
+      <c r="AJR17"/>
+      <c r="AJS17"/>
+      <c r="AJT17"/>
+      <c r="AJU17"/>
+      <c r="AJV17"/>
+      <c r="AJW17"/>
+      <c r="AJX17"/>
+      <c r="AJY17"/>
+      <c r="AJZ17"/>
+      <c r="AKA17"/>
+      <c r="AKB17"/>
+      <c r="AKC17"/>
+      <c r="AKD17"/>
+      <c r="AKE17"/>
+      <c r="AKF17"/>
+      <c r="AKG17"/>
+      <c r="AKH17"/>
+      <c r="AKI17"/>
+      <c r="AKJ17"/>
+      <c r="AKK17"/>
+      <c r="AKL17"/>
+      <c r="AKM17"/>
+      <c r="AKN17"/>
+      <c r="AKO17"/>
+      <c r="AKP17"/>
+      <c r="AKQ17"/>
+      <c r="AKR17"/>
+      <c r="AKS17"/>
+      <c r="AKT17"/>
+      <c r="AKU17"/>
+      <c r="AKV17"/>
+      <c r="AKW17"/>
+      <c r="AKX17"/>
+      <c r="AKY17"/>
+      <c r="AKZ17"/>
+      <c r="ALA17"/>
+      <c r="ALB17"/>
+      <c r="ALC17"/>
+      <c r="ALD17"/>
+      <c r="ALE17"/>
+      <c r="ALF17"/>
+      <c r="ALG17"/>
+      <c r="ALH17"/>
+      <c r="ALI17"/>
+      <c r="ALJ17"/>
+      <c r="ALK17"/>
+      <c r="ALL17"/>
+      <c r="ALM17"/>
+      <c r="ALN17"/>
+      <c r="ALO17"/>
+      <c r="ALP17"/>
+      <c r="ALQ17"/>
+      <c r="ALR17"/>
+      <c r="ALS17"/>
+      <c r="ALT17"/>
+      <c r="ALU17"/>
+      <c r="ALV17"/>
+      <c r="ALW17"/>
+      <c r="ALX17"/>
+      <c r="ALY17"/>
+      <c r="ALZ17"/>
+      <c r="AMA17"/>
+      <c r="AMB17"/>
+      <c r="AMC17"/>
+      <c r="AMD17"/>
+      <c r="AME17"/>
+      <c r="AMF17"/>
+      <c r="AMG17"/>
+      <c r="AMH17"/>
+      <c r="AMI17"/>
+      <c r="AMJ17"/>
+      <c r="AMK17"/>
+    </row>
+    <row r="18" spans="1:1025" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A18" s="77">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="78"/>
+      <c r="C18" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="79" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="79" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="80">
+        <v>12</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+      <c r="BF18"/>
+      <c r="BG18"/>
+      <c r="BH18"/>
+      <c r="BI18"/>
+      <c r="BJ18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
+      <c r="BM18"/>
+      <c r="BN18"/>
+      <c r="BO18"/>
+      <c r="BP18"/>
+      <c r="BQ18"/>
+      <c r="BR18"/>
+      <c r="BS18"/>
+      <c r="BT18"/>
+      <c r="BU18"/>
+      <c r="BV18"/>
+      <c r="BW18"/>
+      <c r="BX18"/>
+      <c r="BY18"/>
+      <c r="BZ18"/>
+      <c r="CA18"/>
+      <c r="CB18"/>
+      <c r="CC18"/>
+      <c r="CD18"/>
+      <c r="CE18"/>
+      <c r="CF18"/>
+      <c r="CG18"/>
+      <c r="CH18"/>
+      <c r="CI18"/>
+      <c r="CJ18"/>
+      <c r="CK18"/>
+      <c r="CL18"/>
+      <c r="CM18"/>
+      <c r="CN18"/>
+      <c r="CO18"/>
+      <c r="CP18"/>
+      <c r="CQ18"/>
+      <c r="CR18"/>
+      <c r="CS18"/>
+      <c r="CT18"/>
+      <c r="CU18"/>
+      <c r="CV18"/>
+      <c r="CW18"/>
+      <c r="CX18"/>
+      <c r="CY18"/>
+      <c r="CZ18"/>
+      <c r="DA18"/>
+      <c r="DB18"/>
+      <c r="DC18"/>
+      <c r="DD18"/>
+      <c r="DE18"/>
+      <c r="DF18"/>
+      <c r="DG18"/>
+      <c r="DH18"/>
+      <c r="DI18"/>
+      <c r="DJ18"/>
+      <c r="DK18"/>
+      <c r="DL18"/>
+      <c r="DM18"/>
+      <c r="DN18"/>
+      <c r="DO18"/>
+      <c r="DP18"/>
+      <c r="DQ18"/>
+      <c r="DR18"/>
+      <c r="DS18"/>
+      <c r="DT18"/>
+      <c r="DU18"/>
+      <c r="DV18"/>
+      <c r="DW18"/>
+      <c r="DX18"/>
+      <c r="DY18"/>
+      <c r="DZ18"/>
+      <c r="EA18"/>
+      <c r="EB18"/>
+      <c r="EC18"/>
+      <c r="ED18"/>
+      <c r="EE18"/>
+      <c r="EF18"/>
+      <c r="EG18"/>
+      <c r="EH18"/>
+      <c r="EI18"/>
+      <c r="EJ18"/>
+      <c r="EK18"/>
+      <c r="EL18"/>
+      <c r="EM18"/>
+      <c r="EN18"/>
+      <c r="EO18"/>
+      <c r="EP18"/>
+      <c r="EQ18"/>
+      <c r="ER18"/>
+      <c r="ES18"/>
+      <c r="ET18"/>
+      <c r="EU18"/>
+      <c r="EV18"/>
+      <c r="EW18"/>
+      <c r="EX18"/>
+      <c r="EY18"/>
+      <c r="EZ18"/>
+      <c r="FA18"/>
+      <c r="FB18"/>
+      <c r="FC18"/>
+      <c r="FD18"/>
+      <c r="FE18"/>
+      <c r="FF18"/>
+      <c r="FG18"/>
+      <c r="FH18"/>
+      <c r="FI18"/>
+      <c r="FJ18"/>
+      <c r="FK18"/>
+      <c r="FL18"/>
+      <c r="FM18"/>
+      <c r="FN18"/>
+      <c r="FO18"/>
+      <c r="FP18"/>
+      <c r="FQ18"/>
+      <c r="FR18"/>
+      <c r="FS18"/>
+      <c r="FT18"/>
+      <c r="FU18"/>
+      <c r="FV18"/>
+      <c r="FW18"/>
+      <c r="FX18"/>
+      <c r="FY18"/>
+      <c r="FZ18"/>
+      <c r="GA18"/>
+      <c r="GB18"/>
+      <c r="GC18"/>
+      <c r="GD18"/>
+      <c r="GE18"/>
+      <c r="GF18"/>
+      <c r="GG18"/>
+      <c r="GH18"/>
+      <c r="GI18"/>
+      <c r="GJ18"/>
+      <c r="GK18"/>
+      <c r="GL18"/>
+      <c r="GM18"/>
+      <c r="GN18"/>
+      <c r="GO18"/>
+      <c r="GP18"/>
+      <c r="GQ18"/>
+      <c r="GR18"/>
+      <c r="GS18"/>
+      <c r="GT18"/>
+      <c r="GU18"/>
+      <c r="GV18"/>
+      <c r="GW18"/>
+      <c r="GX18"/>
+      <c r="GY18"/>
+      <c r="GZ18"/>
+      <c r="HA18"/>
+      <c r="HB18"/>
+      <c r="HC18"/>
+      <c r="HD18"/>
+      <c r="HE18"/>
+      <c r="HF18"/>
+      <c r="HG18"/>
+      <c r="HH18"/>
+      <c r="HI18"/>
+      <c r="HJ18"/>
+      <c r="HK18"/>
+      <c r="HL18"/>
+      <c r="HM18"/>
+      <c r="HN18"/>
+      <c r="HO18"/>
+      <c r="HP18"/>
+      <c r="HQ18"/>
+      <c r="HR18"/>
+      <c r="HS18"/>
+      <c r="HT18"/>
+      <c r="HU18"/>
+      <c r="HV18"/>
+      <c r="HW18"/>
+      <c r="HX18"/>
+      <c r="HY18"/>
+      <c r="HZ18"/>
+      <c r="IA18"/>
+      <c r="IB18"/>
+      <c r="IC18"/>
+      <c r="ID18"/>
+      <c r="IE18"/>
+      <c r="IF18"/>
+      <c r="IG18"/>
+      <c r="IH18"/>
+      <c r="II18"/>
+      <c r="IJ18"/>
+      <c r="IK18"/>
+      <c r="IL18"/>
+      <c r="IM18"/>
+      <c r="IN18"/>
+      <c r="IO18"/>
+      <c r="IP18"/>
+      <c r="IQ18"/>
+      <c r="IR18"/>
+      <c r="IS18"/>
+      <c r="IT18"/>
+      <c r="IU18"/>
+      <c r="IV18"/>
+      <c r="IW18"/>
+      <c r="IX18"/>
+      <c r="IY18"/>
+      <c r="IZ18"/>
+      <c r="JA18"/>
+      <c r="JB18"/>
+      <c r="JC18"/>
+      <c r="JD18"/>
+      <c r="JE18"/>
+      <c r="JF18"/>
+      <c r="JG18"/>
+      <c r="JH18"/>
+      <c r="JI18"/>
+      <c r="JJ18"/>
+      <c r="JK18"/>
+      <c r="JL18"/>
+      <c r="JM18"/>
+      <c r="JN18"/>
+      <c r="JO18"/>
+      <c r="JP18"/>
+      <c r="JQ18"/>
+      <c r="JR18"/>
+      <c r="JS18"/>
+      <c r="JT18"/>
+      <c r="JU18"/>
+      <c r="JV18"/>
+      <c r="JW18"/>
+      <c r="JX18"/>
+      <c r="JY18"/>
+      <c r="JZ18"/>
+      <c r="KA18"/>
+      <c r="KB18"/>
+      <c r="KC18"/>
+      <c r="KD18"/>
+      <c r="KE18"/>
+      <c r="KF18"/>
+      <c r="KG18"/>
+      <c r="KH18"/>
+      <c r="KI18"/>
+      <c r="KJ18"/>
+      <c r="KK18"/>
+      <c r="KL18"/>
+      <c r="KM18"/>
+      <c r="KN18"/>
+      <c r="KO18"/>
+      <c r="KP18"/>
+      <c r="KQ18"/>
+      <c r="KR18"/>
+      <c r="KS18"/>
+      <c r="KT18"/>
+      <c r="KU18"/>
+      <c r="KV18"/>
+      <c r="KW18"/>
+      <c r="KX18"/>
+      <c r="KY18"/>
+      <c r="KZ18"/>
+      <c r="LA18"/>
+      <c r="LB18"/>
+      <c r="LC18"/>
+      <c r="LD18"/>
+      <c r="LE18"/>
+      <c r="LF18"/>
+      <c r="LG18"/>
+      <c r="LH18"/>
+      <c r="LI18"/>
+      <c r="LJ18"/>
+      <c r="LK18"/>
+      <c r="LL18"/>
+      <c r="LM18"/>
+      <c r="LN18"/>
+      <c r="LO18"/>
+      <c r="LP18"/>
+      <c r="LQ18"/>
+      <c r="LR18"/>
+      <c r="LS18"/>
+      <c r="LT18"/>
+      <c r="LU18"/>
+      <c r="LV18"/>
+      <c r="LW18"/>
+      <c r="LX18"/>
+      <c r="LY18"/>
+      <c r="LZ18"/>
+      <c r="MA18"/>
+      <c r="MB18"/>
+      <c r="MC18"/>
+      <c r="MD18"/>
+      <c r="ME18"/>
+      <c r="MF18"/>
+      <c r="MG18"/>
+      <c r="MH18"/>
+      <c r="MI18"/>
+      <c r="MJ18"/>
+      <c r="MK18"/>
+      <c r="ML18"/>
+      <c r="MM18"/>
+      <c r="MN18"/>
+      <c r="MO18"/>
+      <c r="MP18"/>
+      <c r="MQ18"/>
+      <c r="MR18"/>
+      <c r="MS18"/>
+      <c r="MT18"/>
+      <c r="MU18"/>
+      <c r="MV18"/>
+      <c r="MW18"/>
+      <c r="MX18"/>
+      <c r="MY18"/>
+      <c r="MZ18"/>
+      <c r="NA18"/>
+      <c r="NB18"/>
+      <c r="NC18"/>
+      <c r="ND18"/>
+      <c r="NE18"/>
+      <c r="NF18"/>
+      <c r="NG18"/>
+      <c r="NH18"/>
+      <c r="NI18"/>
+      <c r="NJ18"/>
+      <c r="NK18"/>
+      <c r="NL18"/>
+      <c r="NM18"/>
+      <c r="NN18"/>
+      <c r="NO18"/>
+      <c r="NP18"/>
+      <c r="NQ18"/>
+      <c r="NR18"/>
+      <c r="NS18"/>
+      <c r="NT18"/>
+      <c r="NU18"/>
+      <c r="NV18"/>
+      <c r="NW18"/>
+      <c r="NX18"/>
+      <c r="NY18"/>
+      <c r="NZ18"/>
+      <c r="OA18"/>
+      <c r="OB18"/>
+      <c r="OC18"/>
+      <c r="OD18"/>
+      <c r="OE18"/>
+      <c r="OF18"/>
+      <c r="OG18"/>
+      <c r="OH18"/>
+      <c r="OI18"/>
+      <c r="OJ18"/>
+      <c r="OK18"/>
+      <c r="OL18"/>
+      <c r="OM18"/>
+      <c r="ON18"/>
+      <c r="OO18"/>
+      <c r="OP18"/>
+      <c r="OQ18"/>
+      <c r="OR18"/>
+      <c r="OS18"/>
+      <c r="OT18"/>
+      <c r="OU18"/>
+      <c r="OV18"/>
+      <c r="OW18"/>
+      <c r="OX18"/>
+      <c r="OY18"/>
+      <c r="OZ18"/>
+      <c r="PA18"/>
+      <c r="PB18"/>
+      <c r="PC18"/>
+      <c r="PD18"/>
+      <c r="PE18"/>
+      <c r="PF18"/>
+      <c r="PG18"/>
+      <c r="PH18"/>
+      <c r="PI18"/>
+      <c r="PJ18"/>
+      <c r="PK18"/>
+      <c r="PL18"/>
+      <c r="PM18"/>
+      <c r="PN18"/>
+      <c r="PO18"/>
+      <c r="PP18"/>
+      <c r="PQ18"/>
+      <c r="PR18"/>
+      <c r="PS18"/>
+      <c r="PT18"/>
+      <c r="PU18"/>
+      <c r="PV18"/>
+      <c r="PW18"/>
+      <c r="PX18"/>
+      <c r="PY18"/>
+      <c r="PZ18"/>
+      <c r="QA18"/>
+      <c r="QB18"/>
+      <c r="QC18"/>
+      <c r="QD18"/>
+      <c r="QE18"/>
+      <c r="QF18"/>
+      <c r="QG18"/>
+      <c r="QH18"/>
+      <c r="QI18"/>
+      <c r="QJ18"/>
+      <c r="QK18"/>
+      <c r="QL18"/>
+      <c r="QM18"/>
+      <c r="QN18"/>
+      <c r="QO18"/>
+      <c r="QP18"/>
+      <c r="QQ18"/>
+      <c r="QR18"/>
+      <c r="QS18"/>
+      <c r="QT18"/>
+      <c r="QU18"/>
+      <c r="QV18"/>
+      <c r="QW18"/>
+      <c r="QX18"/>
+      <c r="QY18"/>
+      <c r="QZ18"/>
+      <c r="RA18"/>
+      <c r="RB18"/>
+      <c r="RC18"/>
+      <c r="RD18"/>
+      <c r="RE18"/>
+      <c r="RF18"/>
+      <c r="RG18"/>
+      <c r="RH18"/>
+      <c r="RI18"/>
+      <c r="RJ18"/>
+      <c r="RK18"/>
+      <c r="RL18"/>
+      <c r="RM18"/>
+      <c r="RN18"/>
+      <c r="RO18"/>
+      <c r="RP18"/>
+      <c r="RQ18"/>
+      <c r="RR18"/>
+      <c r="RS18"/>
+      <c r="RT18"/>
+      <c r="RU18"/>
+      <c r="RV18"/>
+      <c r="RW18"/>
+      <c r="RX18"/>
+      <c r="RY18"/>
+      <c r="RZ18"/>
+      <c r="SA18"/>
+      <c r="SB18"/>
+      <c r="SC18"/>
+      <c r="SD18"/>
+      <c r="SE18"/>
+      <c r="SF18"/>
+      <c r="SG18"/>
+      <c r="SH18"/>
+      <c r="SI18"/>
+      <c r="SJ18"/>
+      <c r="SK18"/>
+      <c r="SL18"/>
+      <c r="SM18"/>
+      <c r="SN18"/>
+      <c r="SO18"/>
+      <c r="SP18"/>
+      <c r="SQ18"/>
+      <c r="SR18"/>
+      <c r="SS18"/>
+      <c r="ST18"/>
+      <c r="SU18"/>
+      <c r="SV18"/>
+      <c r="SW18"/>
+      <c r="SX18"/>
+      <c r="SY18"/>
+      <c r="SZ18"/>
+      <c r="TA18"/>
+      <c r="TB18"/>
+      <c r="TC18"/>
+      <c r="TD18"/>
+      <c r="TE18"/>
+      <c r="TF18"/>
+      <c r="TG18"/>
+      <c r="TH18"/>
+      <c r="TI18"/>
+      <c r="TJ18"/>
+      <c r="TK18"/>
+      <c r="TL18"/>
+      <c r="TM18"/>
+      <c r="TN18"/>
+      <c r="TO18"/>
+      <c r="TP18"/>
+      <c r="TQ18"/>
+      <c r="TR18"/>
+      <c r="TS18"/>
+      <c r="TT18"/>
+      <c r="TU18"/>
+      <c r="TV18"/>
+      <c r="TW18"/>
+      <c r="TX18"/>
+      <c r="TY18"/>
+      <c r="TZ18"/>
+      <c r="UA18"/>
+      <c r="UB18"/>
+      <c r="UC18"/>
+      <c r="UD18"/>
+      <c r="UE18"/>
+      <c r="UF18"/>
+      <c r="UG18"/>
+      <c r="UH18"/>
+      <c r="UI18"/>
+      <c r="UJ18"/>
+      <c r="UK18"/>
+      <c r="UL18"/>
+      <c r="UM18"/>
+      <c r="UN18"/>
+      <c r="UO18"/>
+      <c r="UP18"/>
+      <c r="UQ18"/>
+      <c r="UR18"/>
+      <c r="US18"/>
+      <c r="UT18"/>
+      <c r="UU18"/>
+      <c r="UV18"/>
+      <c r="UW18"/>
+      <c r="UX18"/>
+      <c r="UY18"/>
+      <c r="UZ18"/>
+      <c r="VA18"/>
+      <c r="VB18"/>
+      <c r="VC18"/>
+      <c r="VD18"/>
+      <c r="VE18"/>
+      <c r="VF18"/>
+      <c r="VG18"/>
+      <c r="VH18"/>
+      <c r="VI18"/>
+      <c r="VJ18"/>
+      <c r="VK18"/>
+      <c r="VL18"/>
+      <c r="VM18"/>
+      <c r="VN18"/>
+      <c r="VO18"/>
+      <c r="VP18"/>
+      <c r="VQ18"/>
+      <c r="VR18"/>
+      <c r="VS18"/>
+      <c r="VT18"/>
+      <c r="VU18"/>
+      <c r="VV18"/>
+      <c r="VW18"/>
+      <c r="VX18"/>
+      <c r="VY18"/>
+      <c r="VZ18"/>
+      <c r="WA18"/>
+      <c r="WB18"/>
+      <c r="WC18"/>
+      <c r="WD18"/>
+      <c r="WE18"/>
+      <c r="WF18"/>
+      <c r="WG18"/>
+      <c r="WH18"/>
+      <c r="WI18"/>
+      <c r="WJ18"/>
+      <c r="WK18"/>
+      <c r="WL18"/>
+      <c r="WM18"/>
+      <c r="WN18"/>
+      <c r="WO18"/>
+      <c r="WP18"/>
+      <c r="WQ18"/>
+      <c r="WR18"/>
+      <c r="WS18"/>
+      <c r="WT18"/>
+      <c r="WU18"/>
+      <c r="WV18"/>
+      <c r="WW18"/>
+      <c r="WX18"/>
+      <c r="WY18"/>
+      <c r="WZ18"/>
+      <c r="XA18"/>
+      <c r="XB18"/>
+      <c r="XC18"/>
+      <c r="XD18"/>
+      <c r="XE18"/>
+      <c r="XF18"/>
+      <c r="XG18"/>
+      <c r="XH18"/>
+      <c r="XI18"/>
+      <c r="XJ18"/>
+      <c r="XK18"/>
+      <c r="XL18"/>
+      <c r="XM18"/>
+      <c r="XN18"/>
+      <c r="XO18"/>
+      <c r="XP18"/>
+      <c r="XQ18"/>
+      <c r="XR18"/>
+      <c r="XS18"/>
+      <c r="XT18"/>
+      <c r="XU18"/>
+      <c r="XV18"/>
+      <c r="XW18"/>
+      <c r="XX18"/>
+      <c r="XY18"/>
+      <c r="XZ18"/>
+      <c r="YA18"/>
+      <c r="YB18"/>
+      <c r="YC18"/>
+      <c r="YD18"/>
+      <c r="YE18"/>
+      <c r="YF18"/>
+      <c r="YG18"/>
+      <c r="YH18"/>
+      <c r="YI18"/>
+      <c r="YJ18"/>
+      <c r="YK18"/>
+      <c r="YL18"/>
+      <c r="YM18"/>
+      <c r="YN18"/>
+      <c r="YO18"/>
+      <c r="YP18"/>
+      <c r="YQ18"/>
+      <c r="YR18"/>
+      <c r="YS18"/>
+      <c r="YT18"/>
+      <c r="YU18"/>
+      <c r="YV18"/>
+      <c r="YW18"/>
+      <c r="YX18"/>
+      <c r="YY18"/>
+      <c r="YZ18"/>
+      <c r="ZA18"/>
+      <c r="ZB18"/>
+      <c r="ZC18"/>
+      <c r="ZD18"/>
+      <c r="ZE18"/>
+      <c r="ZF18"/>
+      <c r="ZG18"/>
+      <c r="ZH18"/>
+      <c r="ZI18"/>
+      <c r="ZJ18"/>
+      <c r="ZK18"/>
+      <c r="ZL18"/>
+      <c r="ZM18"/>
+      <c r="ZN18"/>
+      <c r="ZO18"/>
+      <c r="ZP18"/>
+      <c r="ZQ18"/>
+      <c r="ZR18"/>
+      <c r="ZS18"/>
+      <c r="ZT18"/>
+      <c r="ZU18"/>
+      <c r="ZV18"/>
+      <c r="ZW18"/>
+      <c r="ZX18"/>
+      <c r="ZY18"/>
+      <c r="ZZ18"/>
+      <c r="AAA18"/>
+      <c r="AAB18"/>
+      <c r="AAC18"/>
+      <c r="AAD18"/>
+      <c r="AAE18"/>
+      <c r="AAF18"/>
+      <c r="AAG18"/>
+      <c r="AAH18"/>
+      <c r="AAI18"/>
+      <c r="AAJ18"/>
+      <c r="AAK18"/>
+      <c r="AAL18"/>
+      <c r="AAM18"/>
+      <c r="AAN18"/>
+      <c r="AAO18"/>
+      <c r="AAP18"/>
+      <c r="AAQ18"/>
+      <c r="AAR18"/>
+      <c r="AAS18"/>
+      <c r="AAT18"/>
+      <c r="AAU18"/>
+      <c r="AAV18"/>
+      <c r="AAW18"/>
+      <c r="AAX18"/>
+      <c r="AAY18"/>
+      <c r="AAZ18"/>
+      <c r="ABA18"/>
+      <c r="ABB18"/>
+      <c r="ABC18"/>
+      <c r="ABD18"/>
+      <c r="ABE18"/>
+      <c r="ABF18"/>
+      <c r="ABG18"/>
+      <c r="ABH18"/>
+      <c r="ABI18"/>
+      <c r="ABJ18"/>
+      <c r="ABK18"/>
+      <c r="ABL18"/>
+      <c r="ABM18"/>
+      <c r="ABN18"/>
+      <c r="ABO18"/>
+      <c r="ABP18"/>
+      <c r="ABQ18"/>
+      <c r="ABR18"/>
+      <c r="ABS18"/>
+      <c r="ABT18"/>
+      <c r="ABU18"/>
+      <c r="ABV18"/>
+      <c r="ABW18"/>
+      <c r="ABX18"/>
+      <c r="ABY18"/>
+      <c r="ABZ18"/>
+      <c r="ACA18"/>
+      <c r="ACB18"/>
+      <c r="ACC18"/>
+      <c r="ACD18"/>
+      <c r="ACE18"/>
+      <c r="ACF18"/>
+      <c r="ACG18"/>
+      <c r="ACH18"/>
+      <c r="ACI18"/>
+      <c r="ACJ18"/>
+      <c r="ACK18"/>
+      <c r="ACL18"/>
+      <c r="ACM18"/>
+      <c r="ACN18"/>
+      <c r="ACO18"/>
+      <c r="ACP18"/>
+      <c r="ACQ18"/>
+      <c r="ACR18"/>
+      <c r="ACS18"/>
+      <c r="ACT18"/>
+      <c r="ACU18"/>
+      <c r="ACV18"/>
+      <c r="ACW18"/>
+      <c r="ACX18"/>
+      <c r="ACY18"/>
+      <c r="ACZ18"/>
+      <c r="ADA18"/>
+      <c r="ADB18"/>
+      <c r="ADC18"/>
+      <c r="ADD18"/>
+      <c r="ADE18"/>
+      <c r="ADF18"/>
+      <c r="ADG18"/>
+      <c r="ADH18"/>
+      <c r="ADI18"/>
+      <c r="ADJ18"/>
+      <c r="ADK18"/>
+      <c r="ADL18"/>
+      <c r="ADM18"/>
+      <c r="ADN18"/>
+      <c r="ADO18"/>
+      <c r="ADP18"/>
+      <c r="ADQ18"/>
+      <c r="ADR18"/>
+      <c r="ADS18"/>
+      <c r="ADT18"/>
+      <c r="ADU18"/>
+      <c r="ADV18"/>
+      <c r="ADW18"/>
+      <c r="ADX18"/>
+      <c r="ADY18"/>
+      <c r="ADZ18"/>
+      <c r="AEA18"/>
+      <c r="AEB18"/>
+      <c r="AEC18"/>
+      <c r="AED18"/>
+      <c r="AEE18"/>
+      <c r="AEF18"/>
+      <c r="AEG18"/>
+      <c r="AEH18"/>
+      <c r="AEI18"/>
+      <c r="AEJ18"/>
+      <c r="AEK18"/>
+      <c r="AEL18"/>
+      <c r="AEM18"/>
+      <c r="AEN18"/>
+      <c r="AEO18"/>
+      <c r="AEP18"/>
+      <c r="AEQ18"/>
+      <c r="AER18"/>
+      <c r="AES18"/>
+      <c r="AET18"/>
+      <c r="AEU18"/>
+      <c r="AEV18"/>
+      <c r="AEW18"/>
+      <c r="AEX18"/>
+      <c r="AEY18"/>
+      <c r="AEZ18"/>
+      <c r="AFA18"/>
+      <c r="AFB18"/>
+      <c r="AFC18"/>
+      <c r="AFD18"/>
+      <c r="AFE18"/>
+      <c r="AFF18"/>
+      <c r="AFG18"/>
+      <c r="AFH18"/>
+      <c r="AFI18"/>
+      <c r="AFJ18"/>
+      <c r="AFK18"/>
+      <c r="AFL18"/>
+      <c r="AFM18"/>
+      <c r="AFN18"/>
+      <c r="AFO18"/>
+      <c r="AFP18"/>
+      <c r="AFQ18"/>
+      <c r="AFR18"/>
+      <c r="AFS18"/>
+      <c r="AFT18"/>
+      <c r="AFU18"/>
+      <c r="AFV18"/>
+      <c r="AFW18"/>
+      <c r="AFX18"/>
+      <c r="AFY18"/>
+      <c r="AFZ18"/>
+      <c r="AGA18"/>
+      <c r="AGB18"/>
+      <c r="AGC18"/>
+      <c r="AGD18"/>
+      <c r="AGE18"/>
+      <c r="AGF18"/>
+      <c r="AGG18"/>
+      <c r="AGH18"/>
+      <c r="AGI18"/>
+      <c r="AGJ18"/>
+      <c r="AGK18"/>
+      <c r="AGL18"/>
+      <c r="AGM18"/>
+      <c r="AGN18"/>
+      <c r="AGO18"/>
+      <c r="AGP18"/>
+      <c r="AGQ18"/>
+      <c r="AGR18"/>
+      <c r="AGS18"/>
+      <c r="AGT18"/>
+      <c r="AGU18"/>
+      <c r="AGV18"/>
+      <c r="AGW18"/>
+      <c r="AGX18"/>
+      <c r="AGY18"/>
+      <c r="AGZ18"/>
+      <c r="AHA18"/>
+      <c r="AHB18"/>
+      <c r="AHC18"/>
+      <c r="AHD18"/>
+      <c r="AHE18"/>
+      <c r="AHF18"/>
+      <c r="AHG18"/>
+      <c r="AHH18"/>
+      <c r="AHI18"/>
+      <c r="AHJ18"/>
+      <c r="AHK18"/>
+      <c r="AHL18"/>
+      <c r="AHM18"/>
+      <c r="AHN18"/>
+      <c r="AHO18"/>
+      <c r="AHP18"/>
+      <c r="AHQ18"/>
+      <c r="AHR18"/>
+      <c r="AHS18"/>
+      <c r="AHT18"/>
+      <c r="AHU18"/>
+      <c r="AHV18"/>
+      <c r="AHW18"/>
+      <c r="AHX18"/>
+      <c r="AHY18"/>
+      <c r="AHZ18"/>
+      <c r="AIA18"/>
+      <c r="AIB18"/>
+      <c r="AIC18"/>
+      <c r="AID18"/>
+      <c r="AIE18"/>
+      <c r="AIF18"/>
+      <c r="AIG18"/>
+      <c r="AIH18"/>
+      <c r="AII18"/>
+      <c r="AIJ18"/>
+      <c r="AIK18"/>
+      <c r="AIL18"/>
+      <c r="AIM18"/>
+      <c r="AIN18"/>
+      <c r="AIO18"/>
+      <c r="AIP18"/>
+      <c r="AIQ18"/>
+      <c r="AIR18"/>
+      <c r="AIS18"/>
+      <c r="AIT18"/>
+      <c r="AIU18"/>
+      <c r="AIV18"/>
+      <c r="AIW18"/>
+      <c r="AIX18"/>
+      <c r="AIY18"/>
+      <c r="AIZ18"/>
+      <c r="AJA18"/>
+      <c r="AJB18"/>
+      <c r="AJC18"/>
+      <c r="AJD18"/>
+      <c r="AJE18"/>
+      <c r="AJF18"/>
+      <c r="AJG18"/>
+      <c r="AJH18"/>
+      <c r="AJI18"/>
+      <c r="AJJ18"/>
+      <c r="AJK18"/>
+      <c r="AJL18"/>
+      <c r="AJM18"/>
+      <c r="AJN18"/>
+      <c r="AJO18"/>
+      <c r="AJP18"/>
+      <c r="AJQ18"/>
+      <c r="AJR18"/>
+      <c r="AJS18"/>
+      <c r="AJT18"/>
+      <c r="AJU18"/>
+      <c r="AJV18"/>
+      <c r="AJW18"/>
+      <c r="AJX18"/>
+      <c r="AJY18"/>
+      <c r="AJZ18"/>
+      <c r="AKA18"/>
+      <c r="AKB18"/>
+      <c r="AKC18"/>
+      <c r="AKD18"/>
+      <c r="AKE18"/>
+      <c r="AKF18"/>
+      <c r="AKG18"/>
+      <c r="AKH18"/>
+      <c r="AKI18"/>
+      <c r="AKJ18"/>
+      <c r="AKK18"/>
+      <c r="AKL18"/>
+      <c r="AKM18"/>
+      <c r="AKN18"/>
+      <c r="AKO18"/>
+      <c r="AKP18"/>
+      <c r="AKQ18"/>
+      <c r="AKR18"/>
+      <c r="AKS18"/>
+      <c r="AKT18"/>
+      <c r="AKU18"/>
+      <c r="AKV18"/>
+      <c r="AKW18"/>
+      <c r="AKX18"/>
+      <c r="AKY18"/>
+      <c r="AKZ18"/>
+      <c r="ALA18"/>
+      <c r="ALB18"/>
+      <c r="ALC18"/>
+      <c r="ALD18"/>
+      <c r="ALE18"/>
+      <c r="ALF18"/>
+      <c r="ALG18"/>
+      <c r="ALH18"/>
+      <c r="ALI18"/>
+      <c r="ALJ18"/>
+      <c r="ALK18"/>
+      <c r="ALL18"/>
+      <c r="ALM18"/>
+      <c r="ALN18"/>
+      <c r="ALO18"/>
+      <c r="ALP18"/>
+      <c r="ALQ18"/>
+      <c r="ALR18"/>
+      <c r="ALS18"/>
+      <c r="ALT18"/>
+      <c r="ALU18"/>
+      <c r="ALV18"/>
+      <c r="ALW18"/>
+      <c r="ALX18"/>
+      <c r="ALY18"/>
+      <c r="ALZ18"/>
+      <c r="AMA18"/>
+      <c r="AMB18"/>
+      <c r="AMC18"/>
+      <c r="AMD18"/>
+      <c r="AME18"/>
+      <c r="AMF18"/>
+      <c r="AMG18"/>
+      <c r="AMH18"/>
+      <c r="AMI18"/>
+      <c r="AMJ18"/>
+      <c r="AMK18"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18" xr:uid="{1F00099F-7F4C-4E99-A7D6-804A330180C3}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{D80B2CA1-288F-4EA2-8328-41CA905C47F5}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C17:C18</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3396,15 +5548,15 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.3046875" customWidth="1"/>
     <col min="2" max="2" width="15.3046875" customWidth="1"/>
-    <col min="3" max="3" width="20.3046875" customWidth="1"/>
-    <col min="4" max="4" width="16.3046875" customWidth="1"/>
+    <col min="3" max="3" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.15234375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.3046875" customWidth="1"/>
     <col min="6" max="6" width="12.61328125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
@@ -3432,7 +5584,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="51.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="38.6" x14ac:dyDescent="0.35">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -3723,9 +5875,45 @@
       <c r="Z9" s="35"/>
       <c r="AA9" s="35"/>
     </row>
+    <row r="10" spans="1:27" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A10" s="81">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="84">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A11" s="81">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="84">
+        <v>12</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
@@ -3734,12 +5922,16 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11" xr:uid="{829E7A99-F642-453E-8ED3-DF1BE1CFAB39}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type" xr:uid="{00000000-0002-0000-0B00-000002000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
@@ -3758,6 +5950,15 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{441327E8-7015-4FEF-B874-4BC3C021DB14}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C10:C11</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3769,7 +5970,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -4247,22 +6448,48 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="18">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I17" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5233,15 +7460,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G16 I4:I16" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5258,7 +7485,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C16</xm:sqref>
+          <xm:sqref>C4:C17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field" xr:uid="{00000000-0002-0000-0C00-000004000000}">
           <x14:formula1>
@@ -5718,7 +7945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -15544,8 +17771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -15837,7 +18064,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:29" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16830,11 +19082,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16851,7 +19103,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C9</xm:sqref>
+          <xm:sqref>C4:C10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -16863,8 +19115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -17501,10 +19753,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A18" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="35">
+        <v>12</v>
+      </c>
+    </row>
     <row r="1048575" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A17" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -17538,7 +19807,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C17</xm:sqref>
+          <xm:sqref>C4:C18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
RDM-1202 - added label and hint for event case fields
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\moj\ccd-definition-store-api\excel-importer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{343F8676-FC21-42C0-974E-02D74C53A164}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C7E476-5637-4E02-AC44-07AD829CA337}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="16380" windowHeight="8194" tabRatio="757" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="16380" windowHeight="8194" tabRatio="757" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="237">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -745,6 +745,24 @@
   </si>
   <si>
     <t># ${PersonLastName} -${[STATE]}</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>Event Case field label override</t>
+  </si>
+  <si>
+    <t>Event Case field hint override</t>
+  </si>
+  <si>
+    <t>Person First Name Label Override</t>
+  </si>
+  <si>
+    <t>Person First Name Hint Override</t>
   </si>
 </sst>
 </file>
@@ -10775,7 +10793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -15165,7 +15183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -17798,10 +17816,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AC1000"/>
+  <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -17815,16 +17833,16 @@
     <col min="8" max="8" width="21.61328125" customWidth="1"/>
     <col min="9" max="9" width="21.61328125" style="17" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
-    <col min="11" max="11" width="12.84375" customWidth="1"/>
-    <col min="12" max="12" width="15.84375" customWidth="1"/>
-    <col min="13" max="13" width="28.61328125" customWidth="1"/>
-    <col min="14" max="14" width="28.61328125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="23.3046875" customWidth="1"/>
-    <col min="16" max="29" width="8.84375" customWidth="1"/>
-    <col min="30" max="1025" width="14.3046875" customWidth="1"/>
+    <col min="11" max="13" width="12.84375" customWidth="1"/>
+    <col min="14" max="14" width="15.84375" customWidth="1"/>
+    <col min="15" max="15" width="28.61328125" customWidth="1"/>
+    <col min="16" max="16" width="28.61328125" style="17" customWidth="1"/>
+    <col min="17" max="17" width="23.3046875" customWidth="1"/>
+    <col min="18" max="31" width="8.84375" customWidth="1"/>
+    <col min="32" max="1027" width="14.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" ht="17.600000000000001" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>161</v>
       </c>
@@ -17844,8 +17862,10 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:29" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27" t="s">
@@ -17876,19 +17896,23 @@
         <v>168</v>
       </c>
       <c r="L2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="N2" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="P2" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="Q2" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
       <c r="R2" s="26"/>
       <c r="S2" s="26"/>
       <c r="T2" s="26"/>
@@ -17901,8 +17925,10 @@
       <c r="AA2" s="26"/>
       <c r="AB2" s="26"/>
       <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
     </row>
-    <row r="3" spans="1:29" ht="17.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="17.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -17937,19 +17963,25 @@
         <v>178</v>
       </c>
       <c r="L3" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="N3" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="M3" s="31" t="s">
+      <c r="O3" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="P3" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="O3" s="31" t="s">
+      <c r="Q3" s="31" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
@@ -17973,7 +18005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
@@ -17997,7 +18029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>42736</v>
       </c>
@@ -18021,7 +18053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
@@ -18044,8 +18076,14 @@
       <c r="J7" s="17">
         <v>1</v>
       </c>
+      <c r="L7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -18069,7 +18107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>42736</v>
       </c>
@@ -18093,7 +18131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>42736</v>
       </c>
@@ -18119,12 +18157,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
RDM-7232 Categories: allow configuration of service-defined categories
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,44 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FAE370-69D6-4B47-9468-D5A5B5B23614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F8FB46-45DE-A142-B26F-7BA31847B6B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55500" yWindow="10040" windowWidth="41860" windowHeight="12480" tabRatio="757" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
     <sheet name="Banner" sheetId="22" r:id="rId2"/>
     <sheet name="CaseType" sheetId="2" r:id="rId3"/>
     <sheet name="CaseField" sheetId="3" r:id="rId4"/>
-    <sheet name="FixedLists" sheetId="4" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="5" r:id="rId6"/>
-    <sheet name="State" sheetId="6" r:id="rId7"/>
-    <sheet name="CaseEvent" sheetId="7" r:id="rId8"/>
-    <sheet name="CaseEventToFields" sheetId="8" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="9" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="10" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="CaseTypeTab" sheetId="13" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId20"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId21"/>
+    <sheet name="Categories" sheetId="23" r:id="rId5"/>
+    <sheet name="FixedLists" sheetId="4" r:id="rId6"/>
+    <sheet name="ComplexTypes" sheetId="5" r:id="rId7"/>
+    <sheet name="State" sheetId="6" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="7" r:id="rId9"/>
+    <sheet name="CaseEventToFields" sheetId="8" r:id="rId10"/>
+    <sheet name="SearchInputFields" sheetId="9" r:id="rId11"/>
+    <sheet name="SearchResultFields" sheetId="10" r:id="rId12"/>
+    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId13"/>
+    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="CaseTypeTab" sheetId="13" r:id="rId15"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId16"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId21"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId22"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
   </externalReferences>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="302">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -933,6 +934,48 @@
   </si>
   <si>
     <t>http://localhost:3451/test</t>
+  </si>
+  <si>
+    <t>BirthCertificate</t>
+  </si>
+  <si>
+    <t>Birth Certificate</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>Certificates</t>
+  </si>
+  <si>
+    <t>certificates</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CategoryGroupID</t>
+  </si>
+  <si>
+    <t>CategoryGroupName</t>
+  </si>
+  <si>
+    <t>ParentCategoryID</t>
+  </si>
+  <si>
+    <t>CategoryLabel</t>
+  </si>
+  <si>
+    <t>CategoryDisplayOrder</t>
+  </si>
+  <si>
+    <t>mainAddressBookDocs</t>
+  </si>
+  <si>
+    <t>Main address docs</t>
   </si>
 </sst>
 </file>
@@ -3023,6 +3066,1473 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AF1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="32" width="8.83203125" customWidth="1"/>
+    <col min="33" max="1028" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+    </row>
+    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="R3" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="17">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="H14" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+          <x14:formula1>
+            <xm:f>CaseType!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
@@ -3726,7 +5236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -4166,7 +5676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
@@ -6572,7 +8082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -6994,7 +8504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -8608,7 +10118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -8692,7 +10202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -8778,7 +10288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
@@ -8961,7 +10471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -9045,7 +10555,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="108"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="109" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="112" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -9173,85 +10761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>276</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
-        <v>277</v>
-      </c>
-      <c r="B2" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="109" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="109" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="110" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="110" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="110" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="111" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="113" t="s">
-        <v>287</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU6"/>
   <sheetViews>
@@ -10875,7 +12385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -10994,7 +12504,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12191,10 +13701,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12205,15 +13715,15 @@
     <col min="4" max="4" width="41.5" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="8" width="37" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="27" width="8.83203125" customWidth="1"/>
-    <col min="28" max="1025" width="14.5" customWidth="1"/>
+    <col min="7" max="9" width="37" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="28" width="8.83203125" customWidth="1"/>
+    <col min="29" max="1026" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -12232,8 +13742,9 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:28" s="14" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -12251,19 +13762,19 @@
       <c r="G2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -12279,8 +13790,9 @@
       <c r="Y2" s="13"/>
       <c r="Z2" s="13"/>
       <c r="AA2" s="13"/>
-    </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AB2" s="13"/>
+    </row>
+    <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -12302,25 +13814,27 @@
       <c r="G3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -12334,8 +13848,9 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
@@ -12354,15 +13869,16 @@
         <v>48</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
@@ -12381,15 +13897,16 @@
         <v>48</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42736</v>
       </c>
@@ -12410,11 +13927,12 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
@@ -12433,15 +13951,16 @@
         <v>48</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -12460,15 +13979,16 @@
         <v>48</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42736</v>
       </c>
@@ -12489,11 +14009,12 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>42736</v>
       </c>
@@ -12514,11 +14035,12 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>42736</v>
       </c>
@@ -12536,14 +14058,15 @@
       <c r="G11" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>42736</v>
       </c>
@@ -12564,11 +14087,12 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>42736</v>
       </c>
@@ -12586,14 +14110,15 @@
       <c r="G13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>42736</v>
       </c>
@@ -12614,11 +14139,12 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>42736</v>
       </c>
@@ -12639,11 +14165,12 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>42736</v>
       </c>
@@ -12661,16 +14188,17 @@
       <c r="G16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>42736</v>
       </c>
@@ -12688,16 +14216,17 @@
       <c r="G17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>42736</v>
       </c>
@@ -12715,16 +14244,17 @@
       <c r="G18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>42736</v>
       </c>
@@ -12742,16 +14272,17 @@
       <c r="G19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>42736</v>
       </c>
@@ -12772,11 +14303,12 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>42736</v>
       </c>
@@ -12797,11 +14329,12 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
         <v>42736</v>
       </c>
@@ -12817,14 +14350,15 @@
       <c r="G22" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="86" t="s">
+      <c r="H22" s="86"/>
+      <c r="I22" s="86" t="s">
         <v>261</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
@@ -12840,14 +14374,15 @@
       <c r="G23" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="86"/>
+      <c r="I23" s="86" t="s">
         <v>262</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
@@ -12863,21 +14398,45 @@
       <c r="G24" s="86" t="s">
         <v>260</v>
       </c>
-      <c r="H24" s="86" t="s">
+      <c r="H24" s="86"/>
+      <c r="I24" s="86" t="s">
         <v>263</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="86" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" s="86" t="s">
+        <v>289</v>
+      </c>
+      <c r="G25" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="H25" s="86" t="s">
+        <v>293</v>
+      </c>
+      <c r="I25" s="86"/>
+      <c r="L25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13848,7 +15407,7 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A24" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13869,7 +15428,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C24</xm:sqref>
+          <xm:sqref>C4:C25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13878,6 +15437,79 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B0041-E0F3-AE49-A1C6-5EE0A6B84A11}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -15178,11 +16810,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -16771,7 +18403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -18031,7 +19663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC992"/>
   <sheetViews>
@@ -19403,1471 +21035,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AF1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="28.5" customWidth="1"/>
-    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="32" width="8.83203125" customWidth="1"/>
-    <col min="33" max="1028" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-    </row>
-    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="R3" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="86" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="17">
-        <v>1</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="85" t="s">
-        <v>239</v>
-      </c>
-      <c r="K11" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K12" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
-          <x14:formula1>
-            <xm:f>CaseType!$C$4:$C$1000</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C4:C14</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-8509 Added validation for useCase and unit tests
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,44 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FAE370-69D6-4B47-9468-D5A5B5B23614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EDE679-CBA4-0C48-A12F-CBEA548094B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
-    <sheet name="Banner" sheetId="22" r:id="rId2"/>
-    <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId4"/>
-    <sheet name="FixedLists" sheetId="4" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="5" r:id="rId6"/>
-    <sheet name="State" sheetId="6" r:id="rId7"/>
-    <sheet name="CaseEvent" sheetId="7" r:id="rId8"/>
-    <sheet name="CaseEventToFields" sheetId="8" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="9" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="10" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="CaseTypeTab" sheetId="13" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId20"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId21"/>
+    <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId2"/>
+    <sheet name="Banner" sheetId="22" r:id="rId3"/>
+    <sheet name="CaseType" sheetId="2" r:id="rId4"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId5"/>
+    <sheet name="FixedLists" sheetId="4" r:id="rId6"/>
+    <sheet name="ComplexTypes" sheetId="5" r:id="rId7"/>
+    <sheet name="State" sheetId="6" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="7" r:id="rId9"/>
+    <sheet name="CaseEventToFields" sheetId="8" r:id="rId10"/>
+    <sheet name="SearchInputFields" sheetId="9" r:id="rId11"/>
+    <sheet name="SearchResultFields" sheetId="10" r:id="rId12"/>
+    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId13"/>
+    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="CaseTypeTab" sheetId="13" r:id="rId15"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId16"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId21"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId22"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
   </externalReferences>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="292">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -933,6 +935,18 @@
   </si>
   <si>
     <t>http://localhost:3451/test</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>ORGCASES</t>
   </si>
 </sst>
 </file>
@@ -944,7 +958,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1128,7 +1142,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1142,21 +1156,21 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1203,7 +1217,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1223,12 +1237,44 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF6A8759"/>
       <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1327,7 +1373,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1484,6 +1530,22 @@
     <xf numFmtId="49" fontId="34" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1582,6 +1644,59 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Jurisdiction"/>
+      <sheetName val="CaseType"/>
+      <sheetName val="CaseField"/>
+      <sheetName val="FixedLists"/>
+      <sheetName val="ComplexTypes"/>
+      <sheetName val="State"/>
+      <sheetName val="CaseEvent"/>
+      <sheetName val="CaseEventToFields"/>
+      <sheetName val="SearchInputFields"/>
+      <sheetName val="SearchResultFields"/>
+      <sheetName val="WorkBasketInputFields"/>
+      <sheetName val="SearchCasesResultFields"/>
+      <sheetName val="WorkBasketResultFields"/>
+      <sheetName val="CaseEventToComplexTypes"/>
+      <sheetName val="CaseTypeTab"/>
+      <sheetName val="UserProfile"/>
+      <sheetName val="AuthorisationCaseType"/>
+      <sheetName val="AuthorisationCaseState"/>
+      <sheetName val="AuthorisationCaseEvent"/>
+      <sheetName val="AuthorisationCaseField"/>
+      <sheetName val="AuthorisationComplexType"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1883,27 +1998,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
+  <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" customWidth="1"/>
-    <col min="6" max="27" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="27" width="8.83203125" customWidth="1"/>
     <col min="28" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="114" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="121" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="122" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" s="123" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="122" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="35">
+        <v>2</v>
+      </c>
+      <c r="G5" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+    </row>
+    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="35">
+        <v>3</v>
+      </c>
+      <c r="G6" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
+    </row>
+    <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="35">
+        <v>2</v>
+      </c>
+      <c r="G7" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+    </row>
+    <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="35">
+        <v>3</v>
+      </c>
+      <c r="G8" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+    </row>
+    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+    </row>
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="35">
+        <v>9</v>
+      </c>
+      <c r="G10" s="125" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="35">
+        <v>10</v>
+      </c>
+      <c r="G11" s="125" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B21" s="114"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="122"/>
+      <c r="I23" s="123"/>
+      <c r="J23" s="122"/>
+    </row>
+    <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="39"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="125"/>
+      <c r="I24" s="125"/>
+      <c r="J24" s="125"/>
+    </row>
+    <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="39"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="125"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="39"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="39"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="39"/>
+      <c r="C28" s="124"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="39"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{196F8254-3891-7C48-9C94-B0438E76405D}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{21A19DA0-6946-0A4B-A347-CB10057DF014}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{FE466DE1-FC19-8246-9866-577AA4A3437C}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11" xr:uid="{286F1893-DAA9-BF46-8DD2-2F855FE269CE}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29" xr:uid="{EEEE544D-B05A-674D-B1BA-5DF93F387B24}">
+      <formula1>42736</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29" xr:uid="{D59EF0B7-2533-BF41-BC09-F633E82C7490}">
+      <formula1>IF((DATEDIF(B24,C24,"d")&gt;0),C24)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{131819C2-A65A-DD42-B849-D2D760F10819}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C10:C11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{73198D0A-5E38-8948-B00C-1D567B6A4CD2}">
+          <x14:formula1>
+            <xm:f>CaseField!$D$4:$D$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>D4:D9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{4366089E-018C-8E4A-B286-D89B84F0C64D}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{67DD8A62-65C2-414E-89EC-65950C8FBA95}">
+          <x14:formula1>
+            <xm:f>'/Users/rebeccabaker/HMCTS/Reform/ccd-docker/[CCD_CNP_27_safe.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E24:E29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AF1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="32" width="8.83203125" customWidth="1"/>
+    <col min="33" max="1028" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1920,43 +2630,76 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-    </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+    </row>
+    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1964,64 +2707,334 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="R3" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>46</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="17">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="H14" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3008,21 +4021,36 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+          <x14:formula1>
+            <xm:f>CaseType!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
@@ -3726,7 +4754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -4166,7 +5194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
@@ -6572,7 +7600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -6994,7 +8022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -8608,7 +9636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -8692,7 +9720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -8778,7 +9806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
@@ -8961,7 +9989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -9045,7 +10073,1147 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+    <col min="6" max="27" width="8.83203125" customWidth="1"/>
+    <col min="28" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+    </row>
+    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+    </row>
+    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -9173,85 +11341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>276</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
-        <v>277</v>
-      </c>
-      <c r="B2" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="109" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="109" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="110" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="110" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="110" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="111" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="113" t="s">
-        <v>287</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU6"/>
   <sheetViews>
@@ -10875,7 +12965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -10990,6 +13080,84 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="108"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="109" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="112" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -12189,7 +14357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -13877,7 +16045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -15178,7 +17346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -16771,7 +18939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -18031,7 +20199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC992"/>
   <sheetViews>
@@ -19403,1471 +21571,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AF1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="28.5" customWidth="1"/>
-    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="32" width="8.83203125" customWidth="1"/>
-    <col min="33" max="1028" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-    </row>
-    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="R3" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="86" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="17">
-        <v>1</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="85" t="s">
-        <v>239</v>
-      </c>
-      <c r="K11" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K12" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
-          <x14:formula1>
-            <xm:f>CaseType!$C$4:$C$1000</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C4:C14</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-8509 search case results field tab (#618)
* RDM-8509 WIP initial commit of the new tab SearchCasesResultFields

* RDM-8509 Added validation for useCase and unit tests

* RDM-8509 removed deprecated method

* RDM-8509 added temp suppressions

* RDM-8509 corrected query

* RDM-8509 fixed checkstyle

* RDM-8509 tidy up and added a few more tests

* RDM-8509 updated request variable

* RDM-8509 tidy up of files

* RDM-8509 tidy up of files

* RDM-8509 updated files to remove validation on useCase

* RDM-8509 fixed scenario where searchCaseResultsFields would complain if not all caseTypes were defined in the tab

* RDM-8509 fixed unit test
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,44 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FAE370-69D6-4B47-9468-D5A5B5B23614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EDE679-CBA4-0C48-A12F-CBEA548094B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
-    <sheet name="Banner" sheetId="22" r:id="rId2"/>
-    <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId4"/>
-    <sheet name="FixedLists" sheetId="4" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="5" r:id="rId6"/>
-    <sheet name="State" sheetId="6" r:id="rId7"/>
-    <sheet name="CaseEvent" sheetId="7" r:id="rId8"/>
-    <sheet name="CaseEventToFields" sheetId="8" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="9" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="10" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="CaseTypeTab" sheetId="13" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId20"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId21"/>
+    <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId2"/>
+    <sheet name="Banner" sheetId="22" r:id="rId3"/>
+    <sheet name="CaseType" sheetId="2" r:id="rId4"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId5"/>
+    <sheet name="FixedLists" sheetId="4" r:id="rId6"/>
+    <sheet name="ComplexTypes" sheetId="5" r:id="rId7"/>
+    <sheet name="State" sheetId="6" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="7" r:id="rId9"/>
+    <sheet name="CaseEventToFields" sheetId="8" r:id="rId10"/>
+    <sheet name="SearchInputFields" sheetId="9" r:id="rId11"/>
+    <sheet name="SearchResultFields" sheetId="10" r:id="rId12"/>
+    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId13"/>
+    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="CaseTypeTab" sheetId="13" r:id="rId15"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId16"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId21"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId22"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
   </externalReferences>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="292">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -933,6 +935,18 @@
   </si>
   <si>
     <t>http://localhost:3451/test</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>ORGCASES</t>
   </si>
 </sst>
 </file>
@@ -944,7 +958,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1128,7 +1142,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1142,21 +1156,21 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1203,7 +1217,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1223,12 +1237,44 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF6A8759"/>
       <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1327,7 +1373,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1484,6 +1530,22 @@
     <xf numFmtId="49" fontId="34" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1582,6 +1644,59 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Jurisdiction"/>
+      <sheetName val="CaseType"/>
+      <sheetName val="CaseField"/>
+      <sheetName val="FixedLists"/>
+      <sheetName val="ComplexTypes"/>
+      <sheetName val="State"/>
+      <sheetName val="CaseEvent"/>
+      <sheetName val="CaseEventToFields"/>
+      <sheetName val="SearchInputFields"/>
+      <sheetName val="SearchResultFields"/>
+      <sheetName val="WorkBasketInputFields"/>
+      <sheetName val="SearchCasesResultFields"/>
+      <sheetName val="WorkBasketResultFields"/>
+      <sheetName val="CaseEventToComplexTypes"/>
+      <sheetName val="CaseTypeTab"/>
+      <sheetName val="UserProfile"/>
+      <sheetName val="AuthorisationCaseType"/>
+      <sheetName val="AuthorisationCaseState"/>
+      <sheetName val="AuthorisationCaseEvent"/>
+      <sheetName val="AuthorisationCaseField"/>
+      <sheetName val="AuthorisationComplexType"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1883,27 +1998,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
+  <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" customWidth="1"/>
-    <col min="6" max="27" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="27" width="8.83203125" customWidth="1"/>
     <col min="28" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="114" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="119" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="121" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="122" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" s="123" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="122" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="35">
+        <v>2</v>
+      </c>
+      <c r="G5" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+    </row>
+    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="35">
+        <v>3</v>
+      </c>
+      <c r="G6" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
+    </row>
+    <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="35">
+        <v>2</v>
+      </c>
+      <c r="G7" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+    </row>
+    <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="35">
+        <v>3</v>
+      </c>
+      <c r="G8" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+    </row>
+    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="39">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="125" t="s">
+        <v>291</v>
+      </c>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+    </row>
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="35">
+        <v>9</v>
+      </c>
+      <c r="G10" s="125" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="35">
+        <v>10</v>
+      </c>
+      <c r="G11" s="125" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B21" s="114"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="122"/>
+      <c r="I23" s="123"/>
+      <c r="J23" s="122"/>
+    </row>
+    <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="39"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="125"/>
+      <c r="I24" s="125"/>
+      <c r="J24" s="125"/>
+    </row>
+    <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="39"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="125"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="39"/>
+      <c r="C26" s="124"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="39"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="39"/>
+      <c r="C28" s="124"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="125"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="39"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="125"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{196F8254-3891-7C48-9C94-B0438E76405D}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{21A19DA0-6946-0A4B-A347-CB10057DF014}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{FE466DE1-FC19-8246-9866-577AA4A3437C}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11" xr:uid="{286F1893-DAA9-BF46-8DD2-2F855FE269CE}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29" xr:uid="{EEEE544D-B05A-674D-B1BA-5DF93F387B24}">
+      <formula1>42736</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29" xr:uid="{D59EF0B7-2533-BF41-BC09-F633E82C7490}">
+      <formula1>IF((DATEDIF(B24,C24,"d")&gt;0),C24)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{131819C2-A65A-DD42-B849-D2D760F10819}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C10:C11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{73198D0A-5E38-8948-B00C-1D567B6A4CD2}">
+          <x14:formula1>
+            <xm:f>CaseField!$D$4:$D$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>D4:D9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{4366089E-018C-8E4A-B286-D89B84F0C64D}">
+          <x14:formula1>
+            <xm:f>CaseField!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{67DD8A62-65C2-414E-89EC-65950C8FBA95}">
+          <x14:formula1>
+            <xm:f>'/Users/rebeccabaker/HMCTS/Reform/ccd-docker/[CCD_CNP_27_safe.xlsx]CaseField'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E24:E29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AF1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="14" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="32" width="8.83203125" customWidth="1"/>
+    <col min="33" max="1028" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1920,43 +2630,76 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-    </row>
-    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+    </row>
+    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -1964,64 +2707,334 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="R3" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>46</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="17">
+        <v>1</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="H14" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="K14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3008,21 +4021,36 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+          <x14:formula1>
+            <xm:f>CaseType!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
@@ -3726,7 +4754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -4166,7 +5194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
@@ -6572,7 +7600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -6994,7 +8022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -8608,7 +9636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -8692,7 +9720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -8778,7 +9806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
@@ -8961,7 +9989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -9045,7 +10073,1147 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+    <col min="6" max="27" width="8.83203125" customWidth="1"/>
+    <col min="28" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+    </row>
+    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+    </row>
+    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -9173,85 +11341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>276</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
-        <v>277</v>
-      </c>
-      <c r="B2" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="109" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="109" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="110" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="110" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="110" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="111" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="113" t="s">
-        <v>287</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU6"/>
   <sheetViews>
@@ -10875,7 +12965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -10990,6 +13080,84 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="108"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="109" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="112" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -12189,7 +14357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -13877,7 +16045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -15178,7 +17346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -16771,7 +18939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -18031,7 +20199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC992"/>
   <sheetViews>
@@ -19403,1471 +21571,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AF1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="37.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="7" width="20.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="10" width="21.5" style="17" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="28.5" customWidth="1"/>
-    <col min="17" max="17" width="28.5" style="17" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="32" width="8.83203125" customWidth="1"/>
-    <col min="33" max="1028" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:32" s="29" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="N2" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-    </row>
-    <row r="3" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="R3" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="86" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="17">
-        <v>1</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="85" t="s">
-        <v>239</v>
-      </c>
-      <c r="K11" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K12" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10">
-        <v>42736</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="87" t="s">
-        <v>267</v>
-      </c>
-      <c r="K14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
-      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
-          <x14:formula1>
-            <xm:f>CaseType!$C$4:$C$1000</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C4:C14</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-9338: addressed code review comments
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,44 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EDE679-CBA4-0C48-A12F-CBEA548094B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918E1F94-4F43-024A-84D7-5CE74AA3A29B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId2"/>
     <sheet name="Banner" sheetId="22" r:id="rId3"/>
     <sheet name="CaseType" sheetId="2" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId5"/>
-    <sheet name="FixedLists" sheetId="4" r:id="rId6"/>
-    <sheet name="ComplexTypes" sheetId="5" r:id="rId7"/>
-    <sheet name="State" sheetId="6" r:id="rId8"/>
-    <sheet name="CaseEvent" sheetId="7" r:id="rId9"/>
-    <sheet name="CaseEventToFields" sheetId="8" r:id="rId10"/>
-    <sheet name="SearchInputFields" sheetId="9" r:id="rId11"/>
-    <sheet name="SearchResultFields" sheetId="10" r:id="rId12"/>
-    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId13"/>
-    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId14"/>
-    <sheet name="CaseTypeTab" sheetId="13" r:id="rId15"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId16"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId19"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId21"/>
-    <sheet name="SearchAlias" sheetId="20" r:id="rId22"/>
+    <sheet name="NoCConfig" sheetId="24" r:id="rId5"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId6"/>
+    <sheet name="FixedLists" sheetId="4" r:id="rId7"/>
+    <sheet name="ComplexTypes" sheetId="5" r:id="rId8"/>
+    <sheet name="State" sheetId="6" r:id="rId9"/>
+    <sheet name="CaseEvent" sheetId="7" r:id="rId10"/>
+    <sheet name="CaseEventToFields" sheetId="8" r:id="rId11"/>
+    <sheet name="SearchInputFields" sheetId="9" r:id="rId12"/>
+    <sheet name="SearchResultFields" sheetId="10" r:id="rId13"/>
+    <sheet name="WorkBasketInputFields" sheetId="11" r:id="rId14"/>
+    <sheet name="WorkBasketResultFields" sheetId="12" r:id="rId15"/>
+    <sheet name="CaseTypeTab" sheetId="13" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId20"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId21"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId22"/>
+    <sheet name="SearchAlias" sheetId="20" r:id="rId23"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId23"/>
     <externalReference r:id="rId24"/>
+    <externalReference r:id="rId25"/>
   </externalReferences>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="300">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -947,6 +948,30 @@
   </si>
   <si>
     <t>ORGCASES</t>
+  </si>
+  <si>
+    <t>NoCConfig</t>
+  </si>
+  <si>
+    <t>CaseTypeId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes or No, to enable or disable the reason field.                     </t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the noc action interpretaion</t>
+  </si>
+  <si>
+    <t>ReasonRequired</t>
+  </si>
+  <si>
+    <t>NoCActionInterpretationRequired</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -958,7 +983,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1277,8 +1302,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1291,8 +1334,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1364,6 +1413,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1373,7 +1470,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1546,6 +1643,27 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="48" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="48" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1555,7 +1673,222 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1640,19 +1973,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="CaseType"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Jurisdiction"/>
       <sheetName val="CaseType"/>
       <sheetName val="CaseField"/>
@@ -1700,6 +2020,30 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CaseType"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="0" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2001,7 +2345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2584,6 +2928,1380 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AC992"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="34.5" customWidth="1"/>
+    <col min="6" max="6" width="45.5" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="45.5" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="29.5" style="14" customWidth="1"/>
+    <col min="11" max="11" width="32" style="14" customWidth="1"/>
+    <col min="12" max="12" width="31.5" style="14" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="14" customWidth="1"/>
+    <col min="14" max="14" width="26.5" style="14" customWidth="1"/>
+    <col min="15" max="15" width="29.5" style="14" customWidth="1"/>
+    <col min="16" max="16" width="23.5" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="18" max="29" width="8.83203125" customWidth="1"/>
+    <col min="30" max="1025" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+    </row>
+    <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0600-000000000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
+      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9" xr:uid="{00000000-0002-0000-0600-000002000000}">
+      <formula1>42736</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0600-000003000000}">
+          <x14:formula1>
+            <xm:f>CaseType!$C$4:$C$1000</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C4:C9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
@@ -4050,7 +5768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
@@ -4754,7 +6472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -5194,7 +6912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
@@ -7600,7 +9318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
@@ -8022,7 +9740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -9636,7 +11354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -9720,7 +11438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -9806,7 +11524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
@@ -9986,90 +11704,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="100" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="100"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="95" t="s">
-        <v>270</v>
-      </c>
-      <c r="B1" s="96" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="97" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" s="102" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" s="102" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="103" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="104" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="104" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" s="105" t="s">
-        <v>216</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11214,6 +12848,90 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="100" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="100" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="100" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="100" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="100" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="100" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="100" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="100"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="95" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="102" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="102" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="102" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="102" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="102" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="104" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="104" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="105" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
@@ -11341,7 +13059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU6"/>
   <sheetViews>
@@ -12965,7 +14683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -14358,6 +16076,84 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+    </row>
+    <row r="2" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A3" s="126" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" s="127" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" s="128" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="129" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A5" s="129"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A6" s="129"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="132"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A7" s="129"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="130"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -16045,7 +17841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
@@ -17346,7 +19142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -18939,7 +20735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
@@ -20197,1378 +21993,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AC992"/>
-  <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="45.5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="45.5" customWidth="1"/>
-    <col min="9" max="9" width="25.5" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="14" customWidth="1"/>
-    <col min="11" max="11" width="32" style="14" customWidth="1"/>
-    <col min="12" max="12" width="31.5" style="14" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="26.5" style="14" customWidth="1"/>
-    <col min="15" max="15" width="29.5" style="14" customWidth="1"/>
-    <col min="16" max="16" width="23.5" customWidth="1"/>
-    <col min="17" max="17" width="31.1640625" customWidth="1"/>
-    <col min="18" max="29" width="8.83203125" customWidth="1"/>
-    <col min="30" max="1025" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:29" ht="84" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-    </row>
-    <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G6" s="5">
-        <v>3</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G8" s="5">
-        <v>2</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G9" s="5">
-        <v>3</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0600-000000000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
-      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9" xr:uid="{00000000-0002-0000-0600-000002000000}">
-      <formula1>42736</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0600-000003000000}">
-          <x14:formula1>
-            <xm:f>CaseType!$C$4:$C$1000</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C4:C9</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-10429: Event Enabling Condition - Definition Store Changes
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B66A3D-8B24-B546-984A-F129D5384C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342DC49-794D-C249-A697-9D59E65367A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="303">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -972,6 +972,16 @@
   </si>
   <si>
     <t>NoticeOfChangeConfig</t>
+  </si>
+  <si>
+    <t>Event enabling condition
+ MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
+  </si>
+  <si>
+    <t>PersonFirstName="Test" AND PersonLastName="Test"</t>
   </si>
 </sst>
 </file>
@@ -2929,10 +2939,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AC992"/>
+  <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2945,19 +2955,20 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="45.5" customWidth="1"/>
     <col min="9" max="9" width="25.5" customWidth="1"/>
-    <col min="10" max="10" width="29.5" style="14" customWidth="1"/>
-    <col min="11" max="11" width="32" style="14" customWidth="1"/>
-    <col min="12" max="12" width="31.5" style="14" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="26.5" style="14" customWidth="1"/>
-    <col min="15" max="15" width="29.5" style="14" customWidth="1"/>
-    <col min="16" max="16" width="23.5" customWidth="1"/>
-    <col min="17" max="17" width="31.1640625" customWidth="1"/>
-    <col min="18" max="29" width="8.83203125" customWidth="1"/>
-    <col min="30" max="1025" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="45.5" customWidth="1"/>
+    <col min="11" max="11" width="29.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="32" style="14" customWidth="1"/>
+    <col min="13" max="13" width="31.5" style="14" customWidth="1"/>
+    <col min="14" max="14" width="29.83203125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="26.5" style="14" customWidth="1"/>
+    <col min="16" max="16" width="29.5" style="14" customWidth="1"/>
+    <col min="17" max="17" width="23.5" customWidth="1"/>
+    <col min="18" max="18" width="31.1640625" customWidth="1"/>
+    <col min="19" max="30" width="8.83203125" customWidth="1"/>
+    <col min="31" max="1026" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -2976,7 +2987,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:29" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -3000,31 +3011,33 @@
       <c r="I2" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
@@ -3036,8 +3049,9 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
-    </row>
-    <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AD2" s="7"/>
+    </row>
+    <row r="3" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -3065,31 +3079,33 @@
       <c r="I3" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -3101,8 +3117,9 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AD3" s="8"/>
+    </row>
+    <row r="4" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
@@ -3126,16 +3143,16 @@
       <c r="I4" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>27</v>
       </c>
-      <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AD4" s="8"/>
+    </row>
+    <row r="5" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
@@ -3161,11 +3178,11 @@
       <c r="I5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="Q5" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42736</v>
       </c>
@@ -3191,11 +3208,11 @@
       <c r="I6" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="Q6" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
@@ -3219,11 +3236,14 @@
       <c r="I7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="J7" s="107" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q7" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -3249,11 +3269,11 @@
       <c r="I8" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="Q8" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42736</v>
       </c>
@@ -3279,17 +3299,17 @@
       <c r="I9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="Q9" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16079,7 +16099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "RDM-10429: Event Enabling Condition - Definition Store Changes"
This reverts commit 9d2fab90
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342DC49-794D-C249-A697-9D59E65367A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B66A3D-8B24-B546-984A-F129D5384C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="300">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -972,16 +972,6 @@
   </si>
   <si>
     <t>NoticeOfChangeConfig</t>
-  </si>
-  <si>
-    <t>Event enabling condition
- MaxLength: 1000</t>
-  </si>
-  <si>
-    <t>EventEnablingCondition</t>
-  </si>
-  <si>
-    <t>PersonFirstName="Test" AND PersonLastName="Test"</t>
   </si>
 </sst>
 </file>
@@ -2939,10 +2929,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AD992"/>
+  <dimension ref="A1:AC992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2955,20 +2945,19 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="45.5" customWidth="1"/>
     <col min="9" max="9" width="25.5" customWidth="1"/>
-    <col min="10" max="10" width="45.5" customWidth="1"/>
-    <col min="11" max="11" width="29.5" style="14" customWidth="1"/>
-    <col min="12" max="12" width="32" style="14" customWidth="1"/>
-    <col min="13" max="13" width="31.5" style="14" customWidth="1"/>
-    <col min="14" max="14" width="29.83203125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="26.5" style="14" customWidth="1"/>
-    <col min="16" max="16" width="29.5" style="14" customWidth="1"/>
-    <col min="17" max="17" width="23.5" customWidth="1"/>
-    <col min="18" max="18" width="31.1640625" customWidth="1"/>
-    <col min="19" max="30" width="8.83203125" customWidth="1"/>
-    <col min="31" max="1026" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="29.5" style="14" customWidth="1"/>
+    <col min="11" max="11" width="32" style="14" customWidth="1"/>
+    <col min="12" max="12" width="31.5" style="14" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="14" customWidth="1"/>
+    <col min="14" max="14" width="26.5" style="14" customWidth="1"/>
+    <col min="15" max="15" width="29.5" style="14" customWidth="1"/>
+    <col min="16" max="16" width="23.5" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="18" max="29" width="8.83203125" customWidth="1"/>
+    <col min="30" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -2987,7 +2976,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:30" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -3011,33 +3000,31 @@
       <c r="I2" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>300</v>
+      <c r="J2" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="K2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="Q2" s="13" t="s">
         <v>144</v>
       </c>
+      <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
@@ -3049,9 +3036,8 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-    </row>
-    <row r="3" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -3079,33 +3065,31 @@
       <c r="I3" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>301</v>
+      <c r="J3" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="P3" s="16" t="s">
         <v>152</v>
       </c>
+      <c r="P3" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="Q3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="8" t="s">
         <v>153</v>
       </c>
+      <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -3117,9 +3101,8 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-    </row>
-    <row r="4" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>42736</v>
       </c>
@@ -3143,16 +3126,16 @@
       <c r="I4" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
+      <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-    </row>
-    <row r="5" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>42736</v>
       </c>
@@ -3178,11 +3161,11 @@
       <c r="I5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="P5" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>42736</v>
       </c>
@@ -3208,11 +3191,11 @@
       <c r="I6" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="P6" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>42736</v>
       </c>
@@ -3236,14 +3219,11 @@
       <c r="I7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="107" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q7" s="17" t="s">
+      <c r="P7" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>42736</v>
       </c>
@@ -3269,11 +3249,11 @@
       <c r="I8" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="Q8" s="17" t="s">
+      <c r="P8" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>42736</v>
       </c>
@@ -3299,17 +3279,17 @@
       <c r="I9" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="P9" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16099,7 +16079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-10539 accept AccessProfile and UserRole column
   [RDM-10539](https://tools.hmcts.net/jira/browse/RDM-10539)

Accept both AccessProfile and legacy UserRole column name.
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342DC49-794D-C249-A697-9D59E65367A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EF084C-AC8B-7E43-AA80-5D0BCEE64E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="757" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="301">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -708,15 +708,9 @@
     <t>AuthorisationCaseType</t>
   </si>
   <si>
-    <t>MaxLength: 100. no entry for role means ReadOnly</t>
-  </si>
-  <si>
     <t>Case Events can have Create,Read,Update and Delete. MaxLength: 5</t>
   </si>
   <si>
-    <t>UserRole</t>
-  </si>
-  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -730,9 +724,6 @@
   </si>
   <si>
     <t>AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t>MaxLength: 40 no entry for role means ReadOnly</t>
   </si>
   <si>
     <t>AuthorisationCaseState</t>
@@ -894,10 +885,6 @@
 MaxLength: 70</t>
   </si>
   <si>
-    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
-MaxLength: 100.</t>
-  </si>
-  <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
@@ -982,18 +969,25 @@
   </si>
   <si>
     <t>PersonFirstName="Test" AND PersonLastName="Test"</t>
+  </si>
+  <si>
+    <t>AccessProfile</t>
+  </si>
+  <si>
+    <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
+MaxLength: 100.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1261,13 +1255,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -1478,9 +1465,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1585,13 +1572,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="28" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1624,9 +1604,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="49" fontId="31" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1635,12 +1612,12 @@
     </xf>
     <xf numFmtId="49" fontId="37" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="34" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1648,32 +1625,43 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1683,7 +1671,381 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF984807"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF984807"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1898,8 +2260,94 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="totalRow" dxfId="34"/>
+      <tableStyleElement type="firstColumn" dxfId="33"/>
+      <tableStyleElement type="lastColumn" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="30"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1967,6 +2415,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0432FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2046,13 +2497,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
+    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
+    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
+    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2372,16 +2926,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
-        <v>288</v>
-      </c>
-      <c r="B1" s="115" t="s">
+      <c r="A1" s="106" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="109" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5"/>
@@ -2392,15 +2946,15 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="119" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="111" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="111" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2426,32 +2980,32 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="121" t="s">
+      <c r="D3" s="113" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="122" t="s">
-        <v>289</v>
-      </c>
-      <c r="H3" s="123" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" s="122" t="s">
-        <v>290</v>
+      <c r="G3" s="114" t="s">
+        <v>285</v>
+      </c>
+      <c r="H3" s="115" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="114" t="s">
+        <v>286</v>
       </c>
       <c r="J3" s="38"/>
       <c r="K3" s="38"/>
@@ -2489,8 +3043,8 @@
       <c r="F4" s="35">
         <v>1</v>
       </c>
-      <c r="G4" s="125" t="s">
-        <v>291</v>
+      <c r="G4" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -2530,8 +3084,8 @@
       <c r="F5" s="35">
         <v>2</v>
       </c>
-      <c r="G5" s="125" t="s">
-        <v>291</v>
+      <c r="G5" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
@@ -2571,8 +3125,8 @@
       <c r="F6" s="35">
         <v>3</v>
       </c>
-      <c r="G6" s="125" t="s">
-        <v>291</v>
+      <c r="G6" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -2612,8 +3166,8 @@
       <c r="F7" s="35">
         <v>2</v>
       </c>
-      <c r="G7" s="125" t="s">
-        <v>291</v>
+      <c r="G7" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -2653,8 +3207,8 @@
       <c r="F8" s="35">
         <v>3</v>
       </c>
-      <c r="G8" s="125" t="s">
-        <v>291</v>
+      <c r="G8" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -2694,8 +3248,8 @@
       <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="125" t="s">
-        <v>291</v>
+      <c r="G9" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -2726,7 +3280,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -2734,8 +3288,8 @@
       <c r="F10" s="35">
         <v>9</v>
       </c>
-      <c r="G10" s="125" t="s">
-        <v>291</v>
+      <c r="G10" s="117" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -2746,23 +3300,23 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
       </c>
-      <c r="G11" s="125" t="s">
-        <v>291</v>
+      <c r="G11" s="117" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B21" s="114"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="117"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="17"/>
@@ -2770,90 +3324,90 @@
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="122"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="122"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="114"/>
     </row>
     <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="39"/>
-      <c r="C24" s="124"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="125"/>
-      <c r="J24" s="125"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
     </row>
     <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="39"/>
-      <c r="C25" s="124"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="125"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="117"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="39"/>
-      <c r="C26" s="124"/>
+      <c r="C26" s="116"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="125"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="117"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="39"/>
-      <c r="C27" s="124"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="124"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="117"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="39"/>
-      <c r="C28" s="124"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="125"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="117"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="39"/>
-      <c r="C29" s="124"/>
+      <c r="C29" s="116"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="124"/>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="117"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
     </row>
@@ -2941,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3012,7 +3566,7 @@
         <v>142</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>143</v>
@@ -3080,7 +3634,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>147</v>
@@ -3236,8 +3790,8 @@
       <c r="I7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="107" t="s">
-        <v>302</v>
+      <c r="J7" s="99" t="s">
+        <v>298</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>27</v>
@@ -4405,10 +4959,10 @@
         <v>168</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>164</v>
@@ -4466,7 +5020,7 @@
         <v>176</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K3" s="30" t="s">
         <v>177</v>
@@ -4475,10 +5029,10 @@
         <v>178</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>179</v>
@@ -4529,7 +5083,7 @@
       <c r="D5" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="81" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="5"/>
@@ -4593,10 +5147,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4661,7 +5215,7 @@
         <v>154</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -4689,14 +5243,14 @@
       <c r="E11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="86" t="s">
+      <c r="H11" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="85" t="s">
-        <v>239</v>
+      <c r="I11" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="J11" s="80" t="s">
+        <v>236</v>
       </c>
       <c r="K11" s="17">
         <v>1</v>
@@ -4712,14 +5266,14 @@
       <c r="D12" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="86" t="s">
+      <c r="E12" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="H12" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="87" t="s">
-        <v>267</v>
+      <c r="I12" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K12" s="17">
         <v>1</v>
@@ -4735,14 +5289,14 @@
       <c r="D13" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="86" t="s">
+      <c r="E13" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="87" t="s">
-        <v>267</v>
+      <c r="I13" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K13" s="17">
         <v>1</v>
@@ -4758,14 +5312,14 @@
       <c r="D14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" s="86" t="s">
+      <c r="E14" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="H14" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="87" t="s">
-        <v>267</v>
+      <c r="I14" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K14" s="17">
         <v>1</v>
@@ -6421,7 +6975,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>126</v>
@@ -6438,10 +6992,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F18" s="35">
         <v>12</v>
@@ -6852,7 +7406,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -6869,10 +7423,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
@@ -7238,20 +7792,20 @@
       </c>
     </row>
     <row r="17" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="77">
+      <c r="A17" s="72">
         <v>42736</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="79" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="79" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="79" t="s">
+      <c r="D17" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="80">
+      <c r="F17" s="75">
         <v>11</v>
       </c>
       <c r="G17"/>
@@ -8275,20 +8829,20 @@
       <c r="AMK17"/>
     </row>
     <row r="18" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="77">
+      <c r="A18" s="72">
         <v>42736</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79" t="s">
+      <c r="B18" s="73"/>
+      <c r="C18" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="79" t="s">
-        <v>228</v>
-      </c>
-      <c r="E18" s="79" t="s">
-        <v>227</v>
-      </c>
-      <c r="F18" s="80">
+      <c r="D18" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="F18" s="75">
         <v>12</v>
       </c>
       <c r="G18"/>
@@ -9671,38 +10225,38 @@
       <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="81">
+      <c r="A10" s="76">
         <v>42736</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="83" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="83" t="s">
+      <c r="D10" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="84">
+      <c r="F10" s="79">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="81">
+      <c r="A11" s="76">
         <v>42736</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="83" t="s">
-        <v>228</v>
-      </c>
-      <c r="E11" s="83" t="s">
-        <v>227</v>
-      </c>
-      <c r="F11" s="84">
+      <c r="D11" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="79">
         <v>12</v>
       </c>
     </row>
@@ -9856,7 +10410,7 @@
         <v>200</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -10266,7 +10820,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I17" s="5">
         <v>7</v>
@@ -10282,17 +10836,17 @@
       <c r="D18" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E18" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F18" s="86" t="s">
-        <v>269</v>
+      <c r="E18" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G18" s="5">
         <v>5</v>
       </c>
-      <c r="H18" s="86" t="s">
-        <v>254</v>
+      <c r="H18" s="81" t="s">
+        <v>251</v>
       </c>
       <c r="I18" s="5">
         <v>1</v>
@@ -10308,17 +10862,17 @@
       <c r="D19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F19" s="86" t="s">
-        <v>269</v>
+      <c r="E19" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G19" s="5">
         <v>5</v>
       </c>
-      <c r="H19" s="86" t="s">
-        <v>255</v>
+      <c r="H19" s="81" t="s">
+        <v>252</v>
       </c>
       <c r="I19" s="5">
         <v>2</v>
@@ -10334,17 +10888,17 @@
       <c r="D20" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F20" s="86" t="s">
-        <v>269</v>
+      <c r="E20" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G20" s="5">
         <v>5</v>
       </c>
-      <c r="H20" s="86" t="s">
-        <v>256</v>
+      <c r="H20" s="81" t="s">
+        <v>253</v>
       </c>
       <c r="I20" s="5">
         <v>3</v>
@@ -11462,8 +12016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11495,17 +12049,17 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -11519,10 +12073,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -11532,15 +12086,18 @@
         <v>25</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11549,7 +12106,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11563,7 +12120,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -11580,7 +12137,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -11589,11 +12146,11 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>4</v>
+      <c r="E2" s="12" t="s">
+        <v>300</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -11631,10 +12188,10 @@
         <v>172</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11645,10 +12202,10 @@
         <v>46</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11659,10 +12216,10 @@
         <v>50</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11673,57 +12230,60 @@
         <v>52</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" s="86" t="s">
-        <v>216</v>
+      <c r="D7" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="E8" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F8" s="86" t="s">
-        <v>216</v>
+      <c r="D8" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="86" t="s">
-        <v>216</v>
+      <c r="D9" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12869,85 +13429,169 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="100" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="100"/>
+    <col min="1" max="1" width="33.1640625" style="95" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="95" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="95" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="95" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="95" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="95" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="95"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="90" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+    </row>
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="97" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="97" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="96" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="97" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102" t="s">
+      <c r="F2" s="97" t="s">
+        <v>300</v>
+      </c>
+      <c r="G2" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="102" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" s="102" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" s="105" t="s">
-        <v>216</v>
-      </c>
+      <c r="F3" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="126"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="126"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="126"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="126"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="126"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="126"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="126"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="126"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12955,8 +13599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12970,7 +13614,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -12988,7 +13632,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -12998,10 +13642,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>221</v>
+        <v>300</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -13039,10 +13683,10 @@
         <v>171</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13053,10 +13697,10 @@
         <v>154</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13067,24 +13711,27 @@
         <v>156</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:IU6"/>
+  <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13093,13 +13740,13 @@
     <col min="2" max="2" width="15.5" style="58" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="58" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="58" customWidth="1"/>
-    <col min="5" max="255" width="14.5" style="58" customWidth="1"/>
-    <col min="256" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="5" max="250" width="14.5" style="58" customWidth="1"/>
+    <col min="251" max="1020" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:250" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -13112,12 +13759,12 @@
       </c>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
       <c r="M1" s="65"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
@@ -13355,14 +14002,9 @@
       <c r="IM1" s="65"/>
       <c r="IN1" s="65"/>
       <c r="IO1" s="65"/>
-      <c r="IP1" s="65"/>
-      <c r="IQ1" s="65"/>
-      <c r="IR1" s="65"/>
-      <c r="IS1" s="65"/>
-      <c r="IT1" s="65"/>
-      <c r="IU1" s="66"/>
-    </row>
-    <row r="2" spans="1:255" ht="70" x14ac:dyDescent="0.15">
+      <c r="IP1" s="66"/>
+    </row>
+    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -13372,17 +14014,17 @@
         <v>4</v>
       </c>
       <c r="E2" s="68" t="s">
-        <v>221</v>
+        <v>300</v>
       </c>
       <c r="F2" s="68" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="69"/>
+        <v>213</v>
+      </c>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
       <c r="O2" s="70"/>
@@ -13620,38 +14262,33 @@
       <c r="IM2" s="70"/>
       <c r="IN2" s="70"/>
       <c r="IO2" s="70"/>
-      <c r="IP2" s="70"/>
-      <c r="IQ2" s="70"/>
-      <c r="IR2" s="70"/>
-      <c r="IS2" s="70"/>
-      <c r="IT2" s="70"/>
-      <c r="IU2" s="71"/>
-    </row>
-    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="72" t="s">
+      <c r="IP2" s="71"/>
+    </row>
+    <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="73" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="69"/>
+      <c r="D3" s="128" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="128" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" s="69"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
       <c r="O3" s="70"/>
@@ -13889,36 +14526,31 @@
       <c r="IM3" s="70"/>
       <c r="IN3" s="70"/>
       <c r="IO3" s="70"/>
-      <c r="IP3" s="70"/>
-      <c r="IQ3" s="70"/>
-      <c r="IR3" s="70"/>
-      <c r="IS3" s="70"/>
-      <c r="IT3" s="70"/>
-      <c r="IU3" s="71"/>
-    </row>
-    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="74">
+      <c r="IP3" s="71"/>
+    </row>
+    <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="129">
         <v>42736</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="130"/>
+      <c r="C4" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="69"/>
+      <c r="E4" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="131" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
       <c r="M4" s="70"/>
       <c r="N4" s="70"/>
       <c r="O4" s="70"/>
@@ -14156,36 +14788,31 @@
       <c r="IM4" s="70"/>
       <c r="IN4" s="70"/>
       <c r="IO4" s="70"/>
-      <c r="IP4" s="70"/>
-      <c r="IQ4" s="70"/>
-      <c r="IR4" s="70"/>
-      <c r="IS4" s="70"/>
-      <c r="IT4" s="70"/>
-      <c r="IU4" s="71"/>
-    </row>
-    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74">
+      <c r="IP4" s="71"/>
+    </row>
+    <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="129">
         <v>42736</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="130"/>
+      <c r="C5" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="131" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F5" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="69"/>
+      <c r="E5" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="131" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="69"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
       <c r="M5" s="70"/>
       <c r="N5" s="70"/>
       <c r="O5" s="70"/>
@@ -14423,36 +15050,31 @@
       <c r="IM5" s="70"/>
       <c r="IN5" s="70"/>
       <c r="IO5" s="70"/>
-      <c r="IP5" s="70"/>
-      <c r="IQ5" s="70"/>
-      <c r="IR5" s="70"/>
-      <c r="IS5" s="70"/>
-      <c r="IT5" s="70"/>
-      <c r="IU5" s="71"/>
-    </row>
-    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="74">
+      <c r="IP5" s="71"/>
+    </row>
+    <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="129">
         <v>42736</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="75" t="s">
+      <c r="B6" s="130"/>
+      <c r="C6" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="131" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F6" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="69"/>
+      <c r="E6" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="131" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
       <c r="O6" s="70"/>
@@ -14690,16 +15312,62 @@
       <c r="IM6" s="70"/>
       <c r="IN6" s="70"/>
       <c r="IO6" s="70"/>
-      <c r="IP6" s="70"/>
-      <c r="IQ6" s="70"/>
-      <c r="IR6" s="70"/>
-      <c r="IS6" s="70"/>
-      <c r="IT6" s="70"/>
-      <c r="IU6" s="71"/>
+      <c r="IP6" s="71"/>
+    </row>
+    <row r="7" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A7" s="133"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+    </row>
+    <row r="8" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A8" s="133"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+    </row>
+    <row r="9" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A9" s="133"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+    </row>
+    <row r="10" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A10" s="133"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+    </row>
+    <row r="11" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A11" s="133"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+    </row>
+    <row r="12" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A12" s="133"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -14720,82 +15388,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+      <c r="A2" s="87"/>
+      <c r="B2" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="87"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="88" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="92" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="92"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="93" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="93"/>
+      <c r="D3" s="88"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="94" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="D4" s="73"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="94" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="94" t="s">
+      <c r="B5" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="78"/>
+      <c r="D5" s="73"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="78" t="s">
-        <v>245</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="78"/>
+      <c r="B6" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="73"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14828,63 +15496,63 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="100"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="101" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="101" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="101" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
+      <c r="C3" s="102" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="109" t="s">
+      <c r="D3" s="102" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="109" t="s">
+      <c r="E3" s="102" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="110" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="103" t="s">
         <v>280</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C4" s="104" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D4" s="104" t="s">
         <v>282</v>
       </c>
-      <c r="E3" s="110" t="s">
+      <c r="E4" s="105" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="111" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="113" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -16111,59 +16779,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>299</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
+      <c r="A1" s="98" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
     </row>
     <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="101" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A3" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="119" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="120" t="s">
         <v>292</v>
       </c>
-      <c r="B2" s="109" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="121" t="s">
         <v>293</v>
       </c>
-      <c r="C2" s="109" t="s">
+      <c r="C4" s="122" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A3" s="126" t="s">
-        <v>292</v>
-      </c>
-      <c r="B3" s="127" t="s">
-        <v>295</v>
-      </c>
-      <c r="C3" s="128" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A4" s="129" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="129" t="s">
-        <v>297</v>
-      </c>
-      <c r="C4" s="130" t="s">
-        <v>298</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A5" s="129"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122"/>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A6" s="129"/>
-      <c r="B6" s="131"/>
-      <c r="C6" s="132"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="124"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A7" s="129"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="122"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16744,14 +17412,14 @@
         <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -16769,14 +17437,14 @@
         <v>28</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -16792,17 +17460,17 @@
       <c r="C22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="E22" s="86" t="s">
-        <v>257</v>
-      </c>
-      <c r="G22" s="86" t="s">
+      <c r="G22" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="86" t="s">
-        <v>261</v>
+      <c r="H22" s="81" t="s">
+        <v>258</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>27</v>
@@ -16815,17 +17483,17 @@
       <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="81" t="s">
         <v>255</v>
       </c>
-      <c r="E23" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="G23" s="86" t="s">
+      <c r="G23" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="H23" s="86" t="s">
-        <v>262</v>
+      <c r="H23" s="81" t="s">
+        <v>259</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>27</v>
@@ -16838,17 +17506,17 @@
       <c r="C24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="D24" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="81" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="86" t="s">
-        <v>259</v>
-      </c>
-      <c r="G24" s="86" t="s">
+      <c r="G24" s="81" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="81" t="s">
         <v>260</v>
-      </c>
-      <c r="H24" s="86" t="s">
-        <v>263</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>27</v>
@@ -18082,84 +18750,84 @@
       <c r="A11" s="23">
         <v>42736</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="81" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="86" t="s">
-        <v>266</v>
+      <c r="E11" s="81" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>42736</v>
       </c>
-      <c r="C12" s="86" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="86" t="s">
-        <v>265</v>
+      <c r="C12" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>262</v>
       </c>
       <c r="E12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>42736</v>
       </c>
-      <c r="C13" s="86" t="s">
-        <v>262</v>
-      </c>
-      <c r="D13" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>266</v>
+      <c r="C13" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="E13" s="81" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>42736</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="81" t="s">
         <v>262</v>
       </c>
-      <c r="D14" s="86" t="s">
-        <v>265</v>
-      </c>
       <c r="E14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>42736</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="E15" s="81" t="s">
         <v>263</v>
-      </c>
-      <c r="D15" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E15" s="86" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>42736</v>
       </c>
-      <c r="C16" s="86" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" s="86" t="s">
-        <v>265</v>
+      <c r="C16" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="D16" s="81" t="s">
+        <v>262</v>
       </c>
       <c r="E16" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20851,7 +21519,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>128</v>
@@ -20873,7 +21541,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -20895,7 +21563,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
@@ -20917,7 +21585,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H6" s="5">
         <v>3</v>
@@ -20939,7 +21607,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -20961,7 +21629,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H8" s="5">
         <v>2</v>
@@ -20983,7 +21651,7 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H9" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
Revert "RDM-10539 Update User Role Column and codebase rename of UserRole to AccessProfile (#961)"
This reverts commit 80a45c59c434ad690285a90cf78130b6f1aa3d8b.
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EF084C-AC8B-7E43-AA80-5D0BCEE64E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342DC49-794D-C249-A697-9D59E65367A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="757" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="303">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -708,9 +708,15 @@
     <t>AuthorisationCaseType</t>
   </si>
   <si>
+    <t>MaxLength: 100. no entry for role means ReadOnly</t>
+  </si>
+  <si>
     <t>Case Events can have Create,Read,Update and Delete. MaxLength: 5</t>
   </si>
   <si>
+    <t>UserRole</t>
+  </si>
+  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -724,6 +730,9 @@
   </si>
   <si>
     <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>MaxLength: 40 no entry for role means ReadOnly</t>
   </si>
   <si>
     <t>AuthorisationCaseState</t>
@@ -885,6 +894,10 @@
 MaxLength: 70</t>
   </si>
   <si>
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+MaxLength: 100.</t>
+  </si>
+  <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
@@ -969,25 +982,18 @@
   </si>
   <si>
     <t>PersonFirstName="Test" AND PersonLastName="Test"</t>
-  </si>
-  <si>
-    <t>AccessProfile</t>
-  </si>
-  <si>
-    <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
-MaxLength: 100.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1255,6 +1261,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -1465,9 +1478,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1572,6 +1585,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="28" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1604,6 +1624,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="49" fontId="31" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1612,12 +1635,12 @@
     </xf>
     <xf numFmtId="49" fontId="37" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="34" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1625,43 +1648,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="48" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="48" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1671,381 +1683,7 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFFFC000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF984807"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFFFC000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF984807"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -2260,94 +1898,8 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstColumn" dxfId="33"/>
-      <tableStyleElement type="lastColumn" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="30"/>
-    </tableStyle>
-  </tableStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2415,9 +1967,6 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
-    <mruColors>
-      <color rgb="FF0432FF"/>
-    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2497,116 +2046,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
-    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
-    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
-  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
-    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
-  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2926,16 +2372,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>284</v>
-      </c>
-      <c r="B1" s="107" t="s">
+      <c r="A1" s="114" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="117" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5"/>
@@ -2946,15 +2392,15 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
-      <c r="A2" s="110"/>
-      <c r="B2" s="110"/>
-      <c r="C2" s="111" t="s">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="119" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="119" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2980,32 +2426,32 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="112" t="s">
+      <c r="E3" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="112" t="s">
+      <c r="F3" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="114" t="s">
-        <v>285</v>
-      </c>
-      <c r="H3" s="115" t="s">
-        <v>234</v>
-      </c>
-      <c r="I3" s="114" t="s">
-        <v>286</v>
+      <c r="G3" s="122" t="s">
+        <v>289</v>
+      </c>
+      <c r="H3" s="123" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="122" t="s">
+        <v>290</v>
       </c>
       <c r="J3" s="38"/>
       <c r="K3" s="38"/>
@@ -3043,8 +2489,8 @@
       <c r="F4" s="35">
         <v>1</v>
       </c>
-      <c r="G4" s="117" t="s">
-        <v>287</v>
+      <c r="G4" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -3084,8 +2530,8 @@
       <c r="F5" s="35">
         <v>2</v>
       </c>
-      <c r="G5" s="117" t="s">
-        <v>287</v>
+      <c r="G5" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
@@ -3125,8 +2571,8 @@
       <c r="F6" s="35">
         <v>3</v>
       </c>
-      <c r="G6" s="117" t="s">
-        <v>287</v>
+      <c r="G6" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -3166,8 +2612,8 @@
       <c r="F7" s="35">
         <v>2</v>
       </c>
-      <c r="G7" s="117" t="s">
-        <v>287</v>
+      <c r="G7" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -3207,8 +2653,8 @@
       <c r="F8" s="35">
         <v>3</v>
       </c>
-      <c r="G8" s="117" t="s">
-        <v>287</v>
+      <c r="G8" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -3248,8 +2694,8 @@
       <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="117" t="s">
-        <v>287</v>
+      <c r="G9" s="125" t="s">
+        <v>291</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -3280,7 +2726,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -3288,8 +2734,8 @@
       <c r="F10" s="35">
         <v>9</v>
       </c>
-      <c r="G10" s="117" t="s">
-        <v>287</v>
+      <c r="G10" s="125" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -3300,23 +2746,23 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
       </c>
-      <c r="G11" s="117" t="s">
-        <v>287</v>
+      <c r="G11" s="125" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B21" s="106"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="109"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="17"/>
@@ -3324,90 +2770,90 @@
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="111"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="112"/>
-      <c r="C23" s="112"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="114"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="114"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="122"/>
+      <c r="I23" s="123"/>
+      <c r="J23" s="122"/>
     </row>
     <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="39"/>
-      <c r="C24" s="116"/>
+      <c r="C24" s="124"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="125"/>
+      <c r="I24" s="125"/>
+      <c r="J24" s="125"/>
     </row>
     <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="39"/>
-      <c r="C25" s="116"/>
+      <c r="C25" s="124"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="117"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="125"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="39"/>
-      <c r="C26" s="116"/>
+      <c r="C26" s="124"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="117"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="124"/>
+      <c r="H26" s="125"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="39"/>
-      <c r="C27" s="116"/>
+      <c r="C27" s="124"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="117"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="124"/>
+      <c r="H27" s="125"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="39"/>
-      <c r="C28" s="116"/>
+      <c r="C28" s="124"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="116"/>
-      <c r="H28" s="117"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
+      <c r="H28" s="125"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="39"/>
-      <c r="C29" s="116"/>
+      <c r="C29" s="124"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="117"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="125"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
     </row>
@@ -3495,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3566,7 +3012,7 @@
         <v>142</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>143</v>
@@ -3634,7 +3080,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>147</v>
@@ -3790,8 +3236,8 @@
       <c r="I7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="99" t="s">
-        <v>298</v>
+      <c r="J7" s="107" t="s">
+        <v>302</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>27</v>
@@ -4959,10 +4405,10 @@
         <v>168</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>164</v>
@@ -5020,7 +4466,7 @@
         <v>176</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="K3" s="30" t="s">
         <v>177</v>
@@ -5029,10 +4475,10 @@
         <v>178</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>179</v>
@@ -5083,7 +4529,7 @@
       <c r="D5" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="86" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="5"/>
@@ -5147,10 +4593,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5215,7 +4661,7 @@
         <v>154</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -5243,14 +4689,14 @@
       <c r="E11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="81" t="s">
+      <c r="H11" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="82" t="s">
-        <v>235</v>
-      </c>
-      <c r="J11" s="80" t="s">
-        <v>236</v>
+      <c r="I11" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="85" t="s">
+        <v>239</v>
       </c>
       <c r="K11" s="17">
         <v>1</v>
@@ -5266,14 +4712,14 @@
       <c r="D12" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="81" t="s">
-        <v>251</v>
-      </c>
-      <c r="H12" s="81" t="s">
+      <c r="E12" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="82" t="s">
-        <v>264</v>
+      <c r="I12" s="87" t="s">
+        <v>267</v>
       </c>
       <c r="K12" s="17">
         <v>1</v>
@@ -5289,14 +4735,14 @@
       <c r="D13" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="81" t="s">
-        <v>252</v>
-      </c>
-      <c r="H13" s="81" t="s">
+      <c r="E13" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="82" t="s">
-        <v>264</v>
+      <c r="I13" s="87" t="s">
+        <v>267</v>
       </c>
       <c r="K13" s="17">
         <v>1</v>
@@ -5312,14 +4758,14 @@
       <c r="D14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="81" t="s">
-        <v>253</v>
-      </c>
-      <c r="H14" s="81" t="s">
+      <c r="E14" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="H14" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="82" t="s">
-        <v>264</v>
+      <c r="I14" s="87" t="s">
+        <v>267</v>
       </c>
       <c r="K14" s="17">
         <v>1</v>
@@ -6975,7 +6421,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>126</v>
@@ -6992,10 +6438,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F18" s="35">
         <v>12</v>
@@ -7406,7 +6852,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -7423,10 +6869,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
@@ -7792,20 +7238,20 @@
       </c>
     </row>
     <row r="17" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="72">
+      <c r="A17" s="77">
         <v>42736</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="74" t="s">
+      <c r="B17" s="78"/>
+      <c r="C17" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="74" t="s">
-        <v>223</v>
-      </c>
-      <c r="E17" s="74" t="s">
+      <c r="D17" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="80">
         <v>11</v>
       </c>
       <c r="G17"/>
@@ -8829,20 +8275,20 @@
       <c r="AMK17"/>
     </row>
     <row r="18" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="72">
+      <c r="A18" s="77">
         <v>42736</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="74" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="F18" s="75">
+      <c r="D18" s="79" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="79" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="80">
         <v>12</v>
       </c>
       <c r="G18"/>
@@ -10225,38 +9671,38 @@
       <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="76">
+      <c r="A10" s="81">
         <v>42736</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="78" t="s">
+      <c r="B10" s="82"/>
+      <c r="C10" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="78" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10" s="78" t="s">
+      <c r="D10" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="79">
+      <c r="F10" s="84">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="76">
+      <c r="A11" s="81">
         <v>42736</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78" t="s">
+      <c r="B11" s="82"/>
+      <c r="C11" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="78" t="s">
-        <v>225</v>
-      </c>
-      <c r="E11" s="78" t="s">
-        <v>224</v>
-      </c>
-      <c r="F11" s="79">
+      <c r="D11" s="83" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="84">
         <v>12</v>
       </c>
     </row>
@@ -10410,7 +9856,7 @@
         <v>200</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -10820,7 +10266,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I17" s="5">
         <v>7</v>
@@ -10836,17 +10282,17 @@
       <c r="D18" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E18" s="81" t="s">
-        <v>265</v>
-      </c>
-      <c r="F18" s="81" t="s">
-        <v>266</v>
+      <c r="E18" s="86" t="s">
+        <v>268</v>
+      </c>
+      <c r="F18" s="86" t="s">
+        <v>269</v>
       </c>
       <c r="G18" s="5">
         <v>5</v>
       </c>
-      <c r="H18" s="81" t="s">
-        <v>251</v>
+      <c r="H18" s="86" t="s">
+        <v>254</v>
       </c>
       <c r="I18" s="5">
         <v>1</v>
@@ -10862,17 +10308,17 @@
       <c r="D19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="81" t="s">
-        <v>265</v>
-      </c>
-      <c r="F19" s="81" t="s">
-        <v>266</v>
+      <c r="E19" s="86" t="s">
+        <v>268</v>
+      </c>
+      <c r="F19" s="86" t="s">
+        <v>269</v>
       </c>
       <c r="G19" s="5">
         <v>5</v>
       </c>
-      <c r="H19" s="81" t="s">
-        <v>252</v>
+      <c r="H19" s="86" t="s">
+        <v>255</v>
       </c>
       <c r="I19" s="5">
         <v>2</v>
@@ -10888,17 +10334,17 @@
       <c r="D20" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="81" t="s">
-        <v>265</v>
-      </c>
-      <c r="F20" s="81" t="s">
-        <v>266</v>
+      <c r="E20" s="86" t="s">
+        <v>268</v>
+      </c>
+      <c r="F20" s="86" t="s">
+        <v>269</v>
       </c>
       <c r="G20" s="5">
         <v>5</v>
       </c>
-      <c r="H20" s="81" t="s">
-        <v>253</v>
+      <c r="H20" s="86" t="s">
+        <v>256</v>
       </c>
       <c r="I20" s="5">
         <v>3</v>
@@ -12016,8 +11462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12049,17 +11495,17 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>300</v>
+        <v>213</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -12073,10 +11519,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>299</v>
+        <v>215</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -12086,18 +11532,15 @@
         <v>25</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -12106,7 +11549,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12120,7 +11563,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -12137,7 +11580,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -12146,11 +11589,11 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>300</v>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -12188,10 +11631,10 @@
         <v>172</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>299</v>
+        <v>215</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12202,10 +11645,10 @@
         <v>46</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12216,10 +11659,10 @@
         <v>50</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -12230,60 +11673,57 @@
         <v>52</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="81" t="s">
-        <v>251</v>
-      </c>
-      <c r="E7" s="81" t="s">
-        <v>215</v>
-      </c>
-      <c r="F7" s="81" t="s">
-        <v>214</v>
+      <c r="D7" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="81" t="s">
-        <v>252</v>
-      </c>
-      <c r="E8" s="81" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="81" t="s">
-        <v>214</v>
+      <c r="D8" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="81" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="81" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="81" t="s">
-        <v>214</v>
+      <c r="D9" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="86" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -13429,169 +12869,85 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="95" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="95" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="95" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="95" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="95" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="95" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="95"/>
+    <col min="1" max="1" width="33.1640625" style="100" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="100" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="100" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="100" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="100" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="100" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="100" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="100"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="90" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="91" t="s">
+      <c r="A1" s="95" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-    </row>
-    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
-      <c r="A2" s="96"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="97" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="97" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="97" t="s">
-        <v>270</v>
-      </c>
-      <c r="F2" s="97" t="s">
-        <v>300</v>
-      </c>
-      <c r="G2" s="97" t="s">
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="102" t="s">
         <v>271</v>
       </c>
+      <c r="D2" s="102" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="102" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="102" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="102" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="125" t="s">
+      <c r="D3" s="104" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>299</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="126"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="126"/>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="126"/>
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="126"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="126"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="126"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="126"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="126"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="126"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="126"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="126"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
+      <c r="F3" s="105" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="105" t="s">
+        <v>216</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -13599,8 +12955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13614,7 +12970,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -13632,7 +12988,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -13642,10 +12998,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>300</v>
+        <v>221</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -13683,10 +13039,10 @@
         <v>171</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>299</v>
+        <v>215</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13697,10 +13053,10 @@
         <v>154</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13711,27 +13067,24 @@
         <v>156</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:IP12"/>
+  <dimension ref="A1:IU6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13740,13 +13093,13 @@
     <col min="2" max="2" width="15.5" style="58" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="58" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="58" customWidth="1"/>
-    <col min="5" max="250" width="14.5" style="58" customWidth="1"/>
-    <col min="251" max="1020" width="8.83203125" customWidth="1"/>
+    <col min="5" max="255" width="14.5" style="58" customWidth="1"/>
+    <col min="256" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -13759,12 +13112,12 @@
       </c>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64"/>
       <c r="M1" s="65"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
@@ -14002,9 +13355,14 @@
       <c r="IM1" s="65"/>
       <c r="IN1" s="65"/>
       <c r="IO1" s="65"/>
-      <c r="IP1" s="66"/>
-    </row>
-    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
+      <c r="IP1" s="65"/>
+      <c r="IQ1" s="65"/>
+      <c r="IR1" s="65"/>
+      <c r="IS1" s="65"/>
+      <c r="IT1" s="65"/>
+      <c r="IU1" s="66"/>
+    </row>
+    <row r="2" spans="1:255" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -14014,17 +13372,17 @@
         <v>4</v>
       </c>
       <c r="E2" s="68" t="s">
-        <v>300</v>
+        <v>221</v>
       </c>
       <c r="F2" s="68" t="s">
-        <v>213</v>
-      </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
+        <v>214</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
       <c r="O2" s="70"/>
@@ -14262,33 +13620,38 @@
       <c r="IM2" s="70"/>
       <c r="IN2" s="70"/>
       <c r="IO2" s="70"/>
-      <c r="IP2" s="71"/>
-    </row>
-    <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="127" t="s">
+      <c r="IP2" s="70"/>
+      <c r="IQ2" s="70"/>
+      <c r="IR2" s="70"/>
+      <c r="IS2" s="70"/>
+      <c r="IT2" s="70"/>
+      <c r="IU2" s="71"/>
+    </row>
+    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="128" t="s">
-        <v>220</v>
-      </c>
-      <c r="E3" s="128" t="s">
-        <v>299</v>
-      </c>
-      <c r="F3" s="127" t="s">
-        <v>214</v>
-      </c>
-      <c r="G3" s="69"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="D3" s="73" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
       <c r="O3" s="70"/>
@@ -14526,31 +13889,36 @@
       <c r="IM3" s="70"/>
       <c r="IN3" s="70"/>
       <c r="IO3" s="70"/>
-      <c r="IP3" s="71"/>
-    </row>
-    <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="129">
+      <c r="IP3" s="70"/>
+      <c r="IQ3" s="70"/>
+      <c r="IR3" s="70"/>
+      <c r="IS3" s="70"/>
+      <c r="IT3" s="70"/>
+      <c r="IU3" s="71"/>
+    </row>
+    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="74">
         <v>42736</v>
       </c>
-      <c r="B4" s="130"/>
-      <c r="C4" s="131" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="131" t="s">
+      <c r="D4" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="132" t="s">
-        <v>215</v>
-      </c>
-      <c r="F4" s="131" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
+      <c r="E4" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="69"/>
       <c r="M4" s="70"/>
       <c r="N4" s="70"/>
       <c r="O4" s="70"/>
@@ -14788,31 +14156,36 @@
       <c r="IM4" s="70"/>
       <c r="IN4" s="70"/>
       <c r="IO4" s="70"/>
-      <c r="IP4" s="71"/>
-    </row>
-    <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="129">
+      <c r="IP4" s="70"/>
+      <c r="IQ4" s="70"/>
+      <c r="IR4" s="70"/>
+      <c r="IS4" s="70"/>
+      <c r="IT4" s="70"/>
+      <c r="IU4" s="71"/>
+    </row>
+    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="74">
         <v>42736</v>
       </c>
-      <c r="B5" s="130"/>
-      <c r="C5" s="131" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="131" t="s">
+      <c r="D5" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="132" t="s">
-        <v>215</v>
-      </c>
-      <c r="F5" s="131" t="s">
-        <v>222</v>
-      </c>
-      <c r="G5" s="69"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
+      <c r="E5" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="69"/>
       <c r="M5" s="70"/>
       <c r="N5" s="70"/>
       <c r="O5" s="70"/>
@@ -15050,31 +14423,36 @@
       <c r="IM5" s="70"/>
       <c r="IN5" s="70"/>
       <c r="IO5" s="70"/>
-      <c r="IP5" s="71"/>
-    </row>
-    <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="129">
+      <c r="IP5" s="70"/>
+      <c r="IQ5" s="70"/>
+      <c r="IR5" s="70"/>
+      <c r="IS5" s="70"/>
+      <c r="IT5" s="70"/>
+      <c r="IU5" s="71"/>
+    </row>
+    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="74">
         <v>42736</v>
       </c>
-      <c r="B6" s="130"/>
-      <c r="C6" s="131" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="D6" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="132" t="s">
-        <v>215</v>
-      </c>
-      <c r="F6" s="131" t="s">
-        <v>222</v>
-      </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
+      <c r="E6" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="69"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
       <c r="O6" s="70"/>
@@ -15312,62 +14690,16 @@
       <c r="IM6" s="70"/>
       <c r="IN6" s="70"/>
       <c r="IO6" s="70"/>
-      <c r="IP6" s="71"/>
-    </row>
-    <row r="7" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A7" s="133"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-    </row>
-    <row r="8" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A8" s="133"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-    </row>
-    <row r="9" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A9" s="133"/>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-    </row>
-    <row r="10" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A10" s="133"/>
-      <c r="B10" s="133"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-    </row>
-    <row r="11" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A11" s="133"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="133"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-    </row>
-    <row r="12" spans="1:250" x14ac:dyDescent="0.15">
-      <c r="A12" s="133"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
+      <c r="IP6" s="70"/>
+      <c r="IQ6" s="70"/>
+      <c r="IR6" s="70"/>
+      <c r="IS6" s="70"/>
+      <c r="IT6" s="70"/>
+      <c r="IU6" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -15388,82 +14720,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
-        <v>237</v>
-      </c>
-      <c r="B1" s="84" t="s">
+      <c r="A1" s="88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="91" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="C2" s="87" t="s">
-        <v>239</v>
-      </c>
-      <c r="D2" s="87"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="92" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="92"/>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="88" t="s">
+      <c r="B3" s="93" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="88"/>
+      <c r="D3" s="93"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="89" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="89" t="s">
+      <c r="B4" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="73"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="89" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5" s="89" t="s">
+      <c r="B5" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="73"/>
+      <c r="D5" s="78"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" s="73"/>
+      <c r="B6" s="78" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="78"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15496,63 +14828,63 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
-        <v>272</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="100"/>
+      <c r="A1" s="106" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="108"/>
     </row>
     <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="101" t="s">
-        <v>273</v>
-      </c>
-      <c r="B2" s="101" t="s">
+      <c r="A2" s="109" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="101" t="s">
-        <v>274</v>
-      </c>
-      <c r="E2" s="101" t="s">
-        <v>275</v>
+      <c r="D2" s="109" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="109" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="102" t="s">
-        <v>276</v>
-      </c>
-      <c r="C3" s="102" t="s">
-        <v>277</v>
-      </c>
-      <c r="D3" s="102" t="s">
-        <v>278</v>
-      </c>
-      <c r="E3" s="102" t="s">
-        <v>279</v>
+      <c r="B3" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="103" t="s">
-        <v>280</v>
-      </c>
-      <c r="C4" s="104" t="s">
-        <v>281</v>
-      </c>
-      <c r="D4" s="104" t="s">
-        <v>282</v>
-      </c>
-      <c r="E4" s="105" t="s">
-        <v>283</v>
+      <c r="B4" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="112" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="113" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -16779,59 +16111,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="106" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+    </row>
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="109" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A3" s="126" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="127" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-    </row>
-    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="101" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="101" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" s="101" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A3" s="118" t="s">
-        <v>288</v>
-      </c>
-      <c r="B3" s="119" t="s">
-        <v>291</v>
-      </c>
-      <c r="C3" s="120" t="s">
-        <v>292</v>
+      <c r="C3" s="128" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="121" t="s">
-        <v>293</v>
-      </c>
-      <c r="C4" s="122" t="s">
-        <v>294</v>
+      <c r="B4" s="129" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
+      <c r="A5" s="129"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A6" s="121"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="124"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="132"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A7" s="121"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="122"/>
+      <c r="A7" s="129"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="130"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17412,14 +16744,14 @@
         <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -17437,14 +16769,14 @@
         <v>28</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -17460,17 +16792,17 @@
       <c r="C22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="81" t="s">
-        <v>251</v>
-      </c>
-      <c r="E22" s="81" t="s">
+      <c r="D22" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="G22" s="81" t="s">
+      <c r="E22" s="86" t="s">
+        <v>257</v>
+      </c>
+      <c r="G22" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="81" t="s">
-        <v>258</v>
+      <c r="H22" s="86" t="s">
+        <v>261</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>27</v>
@@ -17483,17 +16815,17 @@
       <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="81" t="s">
-        <v>252</v>
-      </c>
-      <c r="E23" s="81" t="s">
+      <c r="D23" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="G23" s="81" t="s">
+      <c r="E23" s="86" t="s">
+        <v>258</v>
+      </c>
+      <c r="G23" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="H23" s="81" t="s">
-        <v>259</v>
+      <c r="H23" s="86" t="s">
+        <v>262</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>27</v>
@@ -17506,17 +16838,17 @@
       <c r="C24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="81" t="s">
-        <v>253</v>
-      </c>
-      <c r="E24" s="81" t="s">
+      <c r="D24" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="G24" s="81" t="s">
-        <v>257</v>
-      </c>
-      <c r="H24" s="81" t="s">
+      <c r="E24" s="86" t="s">
+        <v>259</v>
+      </c>
+      <c r="G24" s="86" t="s">
         <v>260</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>263</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>27</v>
@@ -18750,84 +18082,84 @@
       <c r="A11" s="23">
         <v>42736</v>
       </c>
-      <c r="C11" s="81" t="s">
-        <v>258</v>
-      </c>
-      <c r="D11" s="81" t="s">
+      <c r="C11" s="86" t="s">
         <v>261</v>
       </c>
-      <c r="E11" s="81" t="s">
-        <v>263</v>
+      <c r="D11" s="86" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="86" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>42736</v>
       </c>
-      <c r="C12" s="81" t="s">
-        <v>258</v>
-      </c>
-      <c r="D12" s="81" t="s">
-        <v>262</v>
+      <c r="C12" s="86" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>265</v>
       </c>
       <c r="E12" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>42736</v>
       </c>
-      <c r="C13" s="81" t="s">
-        <v>259</v>
-      </c>
-      <c r="D13" s="81" t="s">
-        <v>261</v>
-      </c>
-      <c r="E13" s="81" t="s">
-        <v>263</v>
+      <c r="C13" s="86" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="86" t="s">
+        <v>264</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>42736</v>
       </c>
-      <c r="C14" s="81" t="s">
-        <v>259</v>
-      </c>
-      <c r="D14" s="81" t="s">
+      <c r="C14" s="86" t="s">
         <v>262</v>
       </c>
+      <c r="D14" s="86" t="s">
+        <v>265</v>
+      </c>
       <c r="E14" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>42736</v>
       </c>
-      <c r="C15" s="81" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" s="81" t="s">
-        <v>261</v>
-      </c>
-      <c r="E15" s="81" t="s">
+      <c r="C15" s="86" t="s">
         <v>263</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>264</v>
+      </c>
+      <c r="E15" s="86" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>42736</v>
       </c>
-      <c r="C16" s="81" t="s">
-        <v>260</v>
-      </c>
-      <c r="D16" s="81" t="s">
-        <v>262</v>
+      <c r="C16" s="86" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>265</v>
       </c>
       <c r="E16" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21519,7 +20851,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>128</v>
@@ -21541,7 +20873,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -21563,7 +20895,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
@@ -21585,7 +20917,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H6" s="5">
         <v>3</v>
@@ -21607,7 +20939,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -21629,7 +20961,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H8" s="5">
         <v>2</v>
@@ -21651,7 +20983,7 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H9" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
CCD-1223: separate beta-fw & ccd-test-definitions
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6342DC49-794D-C249-A697-9D59E65367A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EF084C-AC8B-7E43-AA80-5D0BCEE64E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16560" tabRatio="757" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="757" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="301">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -708,15 +708,9 @@
     <t>AuthorisationCaseType</t>
   </si>
   <si>
-    <t>MaxLength: 100. no entry for role means ReadOnly</t>
-  </si>
-  <si>
     <t>Case Events can have Create,Read,Update and Delete. MaxLength: 5</t>
   </si>
   <si>
-    <t>UserRole</t>
-  </si>
-  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -730,9 +724,6 @@
   </si>
   <si>
     <t>AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t>MaxLength: 40 no entry for role means ReadOnly</t>
   </si>
   <si>
     <t>AuthorisationCaseState</t>
@@ -894,10 +885,6 @@
 MaxLength: 70</t>
   </si>
   <si>
-    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
-MaxLength: 100.</t>
-  </si>
-  <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
@@ -982,18 +969,25 @@
   </si>
   <si>
     <t>PersonFirstName="Test" AND PersonLastName="Test"</t>
+  </si>
+  <si>
+    <t>AccessProfile</t>
+  </si>
+  <si>
+    <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
+MaxLength: 100.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1261,13 +1255,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -1478,9 +1465,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1585,13 +1572,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="28" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1624,9 +1604,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="49" fontId="31" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1635,12 +1612,12 @@
     </xf>
     <xf numFmtId="49" fontId="37" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="34" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1648,32 +1625,43 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="46" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="47" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1683,7 +1671,381 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF984807"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF984807"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1898,8 +2260,94 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="totalRow" dxfId="34"/>
+      <tableStyleElement type="firstColumn" dxfId="33"/>
+      <tableStyleElement type="lastColumn" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="30"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1967,6 +2415,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0432FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2046,13 +2497,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
+    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
+    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
+    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2372,16 +2926,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
-        <v>288</v>
-      </c>
-      <c r="B1" s="115" t="s">
+      <c r="A1" s="106" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="109" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5"/>
@@ -2392,15 +2946,15 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="119" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="111" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="111" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2426,32 +2980,32 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="121" t="s">
+      <c r="D3" s="113" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="122" t="s">
-        <v>289</v>
-      </c>
-      <c r="H3" s="123" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" s="122" t="s">
-        <v>290</v>
+      <c r="G3" s="114" t="s">
+        <v>285</v>
+      </c>
+      <c r="H3" s="115" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="114" t="s">
+        <v>286</v>
       </c>
       <c r="J3" s="38"/>
       <c r="K3" s="38"/>
@@ -2489,8 +3043,8 @@
       <c r="F4" s="35">
         <v>1</v>
       </c>
-      <c r="G4" s="125" t="s">
-        <v>291</v>
+      <c r="G4" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
@@ -2530,8 +3084,8 @@
       <c r="F5" s="35">
         <v>2</v>
       </c>
-      <c r="G5" s="125" t="s">
-        <v>291</v>
+      <c r="G5" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
@@ -2571,8 +3125,8 @@
       <c r="F6" s="35">
         <v>3</v>
       </c>
-      <c r="G6" s="125" t="s">
-        <v>291</v>
+      <c r="G6" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
@@ -2612,8 +3166,8 @@
       <c r="F7" s="35">
         <v>2</v>
       </c>
-      <c r="G7" s="125" t="s">
-        <v>291</v>
+      <c r="G7" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
@@ -2653,8 +3207,8 @@
       <c r="F8" s="35">
         <v>3</v>
       </c>
-      <c r="G8" s="125" t="s">
-        <v>291</v>
+      <c r="G8" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
@@ -2694,8 +3248,8 @@
       <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="125" t="s">
-        <v>291</v>
+      <c r="G9" s="117" t="s">
+        <v>287</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
@@ -2726,7 +3280,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -2734,8 +3288,8 @@
       <c r="F10" s="35">
         <v>9</v>
       </c>
-      <c r="G10" s="125" t="s">
-        <v>291</v>
+      <c r="G10" s="117" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
@@ -2746,23 +3300,23 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
       </c>
-      <c r="G11" s="125" t="s">
-        <v>291</v>
+      <c r="G11" s="117" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B21" s="114"/>
-      <c r="C21" s="115"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="117"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="17"/>
@@ -2770,90 +3324,90 @@
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="122"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="122"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="114"/>
     </row>
     <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="39"/>
-      <c r="C24" s="124"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="17"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="124"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="125"/>
-      <c r="J24" s="125"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="117"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="117"/>
     </row>
     <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="39"/>
-      <c r="C25" s="124"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="125"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="117"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="39"/>
-      <c r="C26" s="124"/>
+      <c r="C26" s="116"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="125"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="116"/>
+      <c r="H26" s="117"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="39"/>
-      <c r="C27" s="124"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="124"/>
-      <c r="G27" s="124"/>
-      <c r="H27" s="125"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="117"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B28" s="39"/>
-      <c r="C28" s="124"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="124"/>
-      <c r="H28" s="125"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="116"/>
+      <c r="G28" s="116"/>
+      <c r="H28" s="117"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="39"/>
-      <c r="C29" s="124"/>
+      <c r="C29" s="116"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="124"/>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="117"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
     </row>
@@ -2941,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3012,7 +3566,7 @@
         <v>142</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>143</v>
@@ -3080,7 +3634,7 @@
         <v>146</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>147</v>
@@ -3236,8 +3790,8 @@
       <c r="I7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="107" t="s">
-        <v>302</v>
+      <c r="J7" s="99" t="s">
+        <v>298</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>27</v>
@@ -4405,10 +4959,10 @@
         <v>168</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>164</v>
@@ -4466,7 +5020,7 @@
         <v>176</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K3" s="30" t="s">
         <v>177</v>
@@ -4475,10 +5029,10 @@
         <v>178</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>179</v>
@@ -4529,7 +5083,7 @@
       <c r="D5" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="81" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="5"/>
@@ -4593,10 +5147,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:32" s="17" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4661,7 +5215,7 @@
         <v>154</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -4689,14 +5243,14 @@
       <c r="E11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="86" t="s">
+      <c r="H11" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="87" t="s">
-        <v>238</v>
-      </c>
-      <c r="J11" s="85" t="s">
-        <v>239</v>
+      <c r="I11" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="J11" s="80" t="s">
+        <v>236</v>
       </c>
       <c r="K11" s="17">
         <v>1</v>
@@ -4712,14 +5266,14 @@
       <c r="D12" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="86" t="s">
+      <c r="E12" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="H12" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="87" t="s">
-        <v>267</v>
+      <c r="I12" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K12" s="17">
         <v>1</v>
@@ -4735,14 +5289,14 @@
       <c r="D13" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="86" t="s">
+      <c r="E13" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="87" t="s">
-        <v>267</v>
+      <c r="I13" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K13" s="17">
         <v>1</v>
@@ -4758,14 +5312,14 @@
       <c r="D14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" s="86" t="s">
+      <c r="E14" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="H14" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="87" t="s">
-        <v>267</v>
+      <c r="I14" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="K14" s="17">
         <v>1</v>
@@ -6421,7 +6975,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>126</v>
@@ -6438,10 +6992,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F18" s="35">
         <v>12</v>
@@ -6852,7 +7406,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>126</v>
@@ -6869,10 +7423,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F11" s="35">
         <v>10</v>
@@ -7238,20 +7792,20 @@
       </c>
     </row>
     <row r="17" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="77">
+      <c r="A17" s="72">
         <v>42736</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="79" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="79" t="s">
-        <v>226</v>
-      </c>
-      <c r="E17" s="79" t="s">
+      <c r="D17" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="80">
+      <c r="F17" s="75">
         <v>11</v>
       </c>
       <c r="G17"/>
@@ -8275,20 +8829,20 @@
       <c r="AMK17"/>
     </row>
     <row r="18" spans="1:1025" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="77">
+      <c r="A18" s="72">
         <v>42736</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79" t="s">
+      <c r="B18" s="73"/>
+      <c r="C18" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="79" t="s">
-        <v>228</v>
-      </c>
-      <c r="E18" s="79" t="s">
-        <v>227</v>
-      </c>
-      <c r="F18" s="80">
+      <c r="D18" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="F18" s="75">
         <v>12</v>
       </c>
       <c r="G18"/>
@@ -9671,38 +10225,38 @@
       <c r="AA9" s="35"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="81">
+      <c r="A10" s="76">
         <v>42736</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="83" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="83" t="s">
+      <c r="D10" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="84">
+      <c r="F10" s="79">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="81">
+      <c r="A11" s="76">
         <v>42736</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="83" t="s">
-        <v>228</v>
-      </c>
-      <c r="E11" s="83" t="s">
-        <v>227</v>
-      </c>
-      <c r="F11" s="84">
+      <c r="D11" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="79">
         <v>12</v>
       </c>
     </row>
@@ -9856,7 +10410,7 @@
         <v>200</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
@@ -10266,7 +10820,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I17" s="5">
         <v>7</v>
@@ -10282,17 +10836,17 @@
       <c r="D18" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E18" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F18" s="86" t="s">
-        <v>269</v>
+      <c r="E18" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G18" s="5">
         <v>5</v>
       </c>
-      <c r="H18" s="86" t="s">
-        <v>254</v>
+      <c r="H18" s="81" t="s">
+        <v>251</v>
       </c>
       <c r="I18" s="5">
         <v>1</v>
@@ -10308,17 +10862,17 @@
       <c r="D19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F19" s="86" t="s">
-        <v>269</v>
+      <c r="E19" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G19" s="5">
         <v>5</v>
       </c>
-      <c r="H19" s="86" t="s">
-        <v>255</v>
+      <c r="H19" s="81" t="s">
+        <v>252</v>
       </c>
       <c r="I19" s="5">
         <v>2</v>
@@ -10334,17 +10888,17 @@
       <c r="D20" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="86" t="s">
-        <v>268</v>
-      </c>
-      <c r="F20" s="86" t="s">
-        <v>269</v>
+      <c r="E20" s="81" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="G20" s="5">
         <v>5</v>
       </c>
-      <c r="H20" s="86" t="s">
-        <v>256</v>
+      <c r="H20" s="81" t="s">
+        <v>253</v>
       </c>
       <c r="I20" s="5">
         <v>3</v>
@@ -11462,8 +12016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11495,17 +12049,17 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -11519,10 +12073,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -11532,15 +12086,18 @@
         <v>25</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11549,7 +12106,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11563,7 +12120,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -11580,7 +12137,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -11589,11 +12146,11 @@
       <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>4</v>
+      <c r="E2" s="12" t="s">
+        <v>300</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -11631,10 +12188,10 @@
         <v>172</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11645,10 +12202,10 @@
         <v>46</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11659,10 +12216,10 @@
         <v>50</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -11673,57 +12230,60 @@
         <v>52</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" s="86" t="s">
-        <v>216</v>
+      <c r="D7" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="E8" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F8" s="86" t="s">
-        <v>216</v>
+      <c r="D8" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="86" t="s">
-        <v>256</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="86" t="s">
-        <v>216</v>
+      <c r="D9" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="81" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12869,85 +13429,169 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="100" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="100" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="100" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="100" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="100"/>
+    <col min="1" max="1" width="33.1640625" style="95" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="95" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="95" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="95" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="95" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="95" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="95"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="90" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+    </row>
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="97" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="97" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="96" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="97" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="101"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102" t="s">
+      <c r="F2" s="97" t="s">
+        <v>300</v>
+      </c>
+      <c r="G2" s="97" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="102" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" s="102" t="s">
-        <v>273</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" s="105" t="s">
-        <v>216</v>
-      </c>
+      <c r="F3" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="126"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="126"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="126"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="126"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="126"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="126"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="126"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="126"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12955,8 +13599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12970,7 +13614,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -12988,7 +13632,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -12998,10 +13642,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>221</v>
+        <v>300</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -13039,10 +13683,10 @@
         <v>171</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13053,10 +13697,10 @@
         <v>154</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:27" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -13067,24 +13711,27 @@
         <v>156</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:IU6"/>
+  <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13093,13 +13740,13 @@
     <col min="2" max="2" width="15.5" style="58" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="58" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="58" customWidth="1"/>
-    <col min="5" max="255" width="14.5" style="58" customWidth="1"/>
-    <col min="256" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="5" max="250" width="14.5" style="58" customWidth="1"/>
+    <col min="251" max="1020" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:250" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -13112,12 +13759,12 @@
       </c>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
       <c r="M1" s="65"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
@@ -13355,14 +14002,9 @@
       <c r="IM1" s="65"/>
       <c r="IN1" s="65"/>
       <c r="IO1" s="65"/>
-      <c r="IP1" s="65"/>
-      <c r="IQ1" s="65"/>
-      <c r="IR1" s="65"/>
-      <c r="IS1" s="65"/>
-      <c r="IT1" s="65"/>
-      <c r="IU1" s="66"/>
-    </row>
-    <row r="2" spans="1:255" ht="70" x14ac:dyDescent="0.15">
+      <c r="IP1" s="66"/>
+    </row>
+    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -13372,17 +14014,17 @@
         <v>4</v>
       </c>
       <c r="E2" s="68" t="s">
-        <v>221</v>
+        <v>300</v>
       </c>
       <c r="F2" s="68" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="69"/>
+        <v>213</v>
+      </c>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="70"/>
       <c r="N2" s="70"/>
       <c r="O2" s="70"/>
@@ -13620,38 +14262,33 @@
       <c r="IM2" s="70"/>
       <c r="IN2" s="70"/>
       <c r="IO2" s="70"/>
-      <c r="IP2" s="70"/>
-      <c r="IQ2" s="70"/>
-      <c r="IR2" s="70"/>
-      <c r="IS2" s="70"/>
-      <c r="IT2" s="70"/>
-      <c r="IU2" s="71"/>
-    </row>
-    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="72" t="s">
+      <c r="IP2" s="71"/>
+    </row>
+    <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="73" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="69"/>
+      <c r="D3" s="128" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="128" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="127" t="s">
+        <v>214</v>
+      </c>
+      <c r="G3" s="69"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
       <c r="M3" s="70"/>
       <c r="N3" s="70"/>
       <c r="O3" s="70"/>
@@ -13889,36 +14526,31 @@
       <c r="IM3" s="70"/>
       <c r="IN3" s="70"/>
       <c r="IO3" s="70"/>
-      <c r="IP3" s="70"/>
-      <c r="IQ3" s="70"/>
-      <c r="IR3" s="70"/>
-      <c r="IS3" s="70"/>
-      <c r="IT3" s="70"/>
-      <c r="IU3" s="71"/>
-    </row>
-    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="74">
+      <c r="IP3" s="71"/>
+    </row>
+    <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="129">
         <v>42736</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="130"/>
+      <c r="C4" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="69"/>
+      <c r="E4" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="131" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
       <c r="M4" s="70"/>
       <c r="N4" s="70"/>
       <c r="O4" s="70"/>
@@ -14156,36 +14788,31 @@
       <c r="IM4" s="70"/>
       <c r="IN4" s="70"/>
       <c r="IO4" s="70"/>
-      <c r="IP4" s="70"/>
-      <c r="IQ4" s="70"/>
-      <c r="IR4" s="70"/>
-      <c r="IS4" s="70"/>
-      <c r="IT4" s="70"/>
-      <c r="IU4" s="71"/>
-    </row>
-    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74">
+      <c r="IP4" s="71"/>
+    </row>
+    <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="129">
         <v>42736</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="130"/>
+      <c r="C5" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="131" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F5" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="69"/>
+      <c r="E5" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="131" t="s">
+        <v>222</v>
+      </c>
+      <c r="G5" s="69"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
       <c r="M5" s="70"/>
       <c r="N5" s="70"/>
       <c r="O5" s="70"/>
@@ -14423,36 +15050,31 @@
       <c r="IM5" s="70"/>
       <c r="IN5" s="70"/>
       <c r="IO5" s="70"/>
-      <c r="IP5" s="70"/>
-      <c r="IQ5" s="70"/>
-      <c r="IR5" s="70"/>
-      <c r="IS5" s="70"/>
-      <c r="IT5" s="70"/>
-      <c r="IU5" s="71"/>
-    </row>
-    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="74">
+      <c r="IP5" s="71"/>
+    </row>
+    <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="129">
         <v>42736</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="75" t="s">
+      <c r="B6" s="130"/>
+      <c r="C6" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="131" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="F6" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="69"/>
+      <c r="E6" s="132" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="131" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
       <c r="M6" s="70"/>
       <c r="N6" s="70"/>
       <c r="O6" s="70"/>
@@ -14690,16 +15312,62 @@
       <c r="IM6" s="70"/>
       <c r="IN6" s="70"/>
       <c r="IO6" s="70"/>
-      <c r="IP6" s="70"/>
-      <c r="IQ6" s="70"/>
-      <c r="IR6" s="70"/>
-      <c r="IS6" s="70"/>
-      <c r="IT6" s="70"/>
-      <c r="IU6" s="71"/>
+      <c r="IP6" s="71"/>
+    </row>
+    <row r="7" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A7" s="133"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+    </row>
+    <row r="8" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A8" s="133"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+    </row>
+    <row r="9" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A9" s="133"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+    </row>
+    <row r="10" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A10" s="133"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+    </row>
+    <row r="11" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A11" s="133"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+    </row>
+    <row r="12" spans="1:250" x14ac:dyDescent="0.15">
+      <c r="A12" s="133"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -14720,82 +15388,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+      <c r="A2" s="87"/>
+      <c r="B2" s="87" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="87"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="88" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="91" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="92" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="92"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="93" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="93"/>
+      <c r="D3" s="88"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="94" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="D4" s="73"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="94" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="94" t="s">
+      <c r="B5" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="78"/>
+      <c r="D5" s="73"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="78" t="s">
-        <v>245</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="78"/>
+      <c r="B6" s="73" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="73"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="78"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14828,63 +15496,63 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="98" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="100"/>
+    </row>
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A2" s="101" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="101" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="101" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="108"/>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
+      <c r="C3" s="102" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="109" t="s">
+      <c r="D3" s="102" t="s">
         <v>278</v>
       </c>
-      <c r="E2" s="109" t="s">
+      <c r="E3" s="102" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="110" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="103" t="s">
         <v>280</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C4" s="104" t="s">
         <v>281</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D4" s="104" t="s">
         <v>282</v>
       </c>
-      <c r="E3" s="110" t="s">
+      <c r="E4" s="105" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="111" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="D4" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="113" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -16111,59 +16779,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
-        <v>299</v>
-      </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
+      <c r="A1" s="98" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
     </row>
     <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="101" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A3" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="119" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="120" t="s">
         <v>292</v>
       </c>
-      <c r="B2" s="109" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
+      <c r="A4" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="121" t="s">
         <v>293</v>
       </c>
-      <c r="C2" s="109" t="s">
+      <c r="C4" s="122" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A3" s="126" t="s">
-        <v>292</v>
-      </c>
-      <c r="B3" s="127" t="s">
-        <v>295</v>
-      </c>
-      <c r="C3" s="128" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A4" s="129" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="129" t="s">
-        <v>297</v>
-      </c>
-      <c r="C4" s="130" t="s">
-        <v>298</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A5" s="129"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122"/>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A6" s="129"/>
-      <c r="B6" s="131"/>
-      <c r="C6" s="132"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="124"/>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A7" s="129"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="122"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16744,14 +17412,14 @@
         <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -16769,14 +17437,14 @@
         <v>28</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -16792,17 +17460,17 @@
       <c r="C22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="81" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="E22" s="86" t="s">
-        <v>257</v>
-      </c>
-      <c r="G22" s="86" t="s">
+      <c r="G22" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="86" t="s">
-        <v>261</v>
+      <c r="H22" s="81" t="s">
+        <v>258</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>27</v>
@@ -16815,17 +17483,17 @@
       <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="81" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" s="81" t="s">
         <v>255</v>
       </c>
-      <c r="E23" s="86" t="s">
-        <v>258</v>
-      </c>
-      <c r="G23" s="86" t="s">
+      <c r="G23" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="H23" s="86" t="s">
-        <v>262</v>
+      <c r="H23" s="81" t="s">
+        <v>259</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>27</v>
@@ -16838,17 +17506,17 @@
       <c r="C24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="D24" s="81" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="81" t="s">
         <v>256</v>
       </c>
-      <c r="E24" s="86" t="s">
-        <v>259</v>
-      </c>
-      <c r="G24" s="86" t="s">
+      <c r="G24" s="81" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="81" t="s">
         <v>260</v>
-      </c>
-      <c r="H24" s="86" t="s">
-        <v>263</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>27</v>
@@ -18082,84 +18750,84 @@
       <c r="A11" s="23">
         <v>42736</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="81" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="86" t="s">
-        <v>266</v>
+      <c r="E11" s="81" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="23">
         <v>42736</v>
       </c>
-      <c r="C12" s="86" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="86" t="s">
-        <v>265</v>
+      <c r="C12" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>262</v>
       </c>
       <c r="E12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23">
         <v>42736</v>
       </c>
-      <c r="C13" s="86" t="s">
-        <v>262</v>
-      </c>
-      <c r="D13" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>266</v>
+      <c r="C13" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="E13" s="81" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="23">
         <v>42736</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="81" t="s">
         <v>262</v>
       </c>
-      <c r="D14" s="86" t="s">
-        <v>265</v>
-      </c>
       <c r="E14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="23">
         <v>42736</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="E15" s="81" t="s">
         <v>263</v>
-      </c>
-      <c r="D15" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="E15" s="86" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="23">
         <v>42736</v>
       </c>
-      <c r="C16" s="86" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" s="86" t="s">
-        <v>265</v>
+      <c r="C16" s="81" t="s">
+        <v>260</v>
+      </c>
+      <c r="D16" s="81" t="s">
+        <v>262</v>
       </c>
       <c r="E16" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20851,7 +21519,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>128</v>
@@ -20873,7 +21541,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -20895,7 +21563,7 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H5" s="5">
         <v>2</v>
@@ -20917,7 +21585,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H6" s="5">
         <v>3</v>
@@ -20939,7 +21607,7 @@
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -20961,7 +21629,7 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H8" s="5">
         <v>2</v>
@@ -20983,7 +21651,7 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H9" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
RDM-13136 - refactor ImportServiceImplTest to separate base types and predefined base types
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EF084C-AC8B-7E43-AA80-5D0BCEE64E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728A544-2ED8-D04F-A5C0-8EC198FF3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="757" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" tabRatio="757" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="304">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -976,6 +976,15 @@
   <si>
     <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
 MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>CaseLinkField</t>
+  </si>
+  <si>
+    <t>Case Link Field</t>
+  </si>
+  <si>
+    <t>CaseLink</t>
   </si>
 </sst>
 </file>
@@ -12016,7 +12025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -12105,7 +12114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -16845,8 +16854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17522,7 +17531,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" t="s">
+        <v>302</v>
+      </c>
+      <c r="G25" t="s">
+        <v>303</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18500,7 +18528,7 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A24" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18521,7 +18549,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C24</xm:sqref>
+          <xm:sqref>C4:C25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Case retention and disposal (#1220)
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/hmcts/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EF084C-AC8B-7E43-AA80-5D0BCEE64E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728A544-2ED8-D04F-A5C0-8EC198FF3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="757" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" tabRatio="757" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="304">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -976,6 +976,15 @@
   <si>
     <t>Must match ID of AccessProfile or CaseRole.  If it doesn’t have a Row below that means no access to.
 MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>CaseLinkField</t>
+  </si>
+  <si>
+    <t>Case Link Field</t>
+  </si>
+  <si>
+    <t>CaseLink</t>
   </si>
 </sst>
 </file>
@@ -12016,7 +12025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -12105,7 +12114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -16845,8 +16854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17522,7 +17531,26 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A25" s="10">
+        <v>42736</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" t="s">
+        <v>302</v>
+      </c>
+      <c r="G25" t="s">
+        <v>303</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18500,7 +18528,7 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A24" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18521,7 +18549,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C4:C24</xm:sqref>
+          <xm:sqref>C4:C25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
CCD-3686 Add JudicialUser complex type
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdathorne/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728A544-2ED8-D04F-A5C0-8EC198FF3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" tabRatio="757" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38560" yWindow="4520" windowWidth="35840" windowHeight="19780" tabRatio="757" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +40,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="309">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -986,11 +985,26 @@
   <si>
     <t>CaseLink</t>
   </si>
+  <si>
+    <t>JudicialUser</t>
+  </si>
+  <si>
+    <t>idamId</t>
+  </si>
+  <si>
+    <t>personalCode</t>
+  </si>
+  <si>
+    <t>IdamId</t>
+  </si>
+  <si>
+    <t>PersonalCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -1422,47 +1436,47 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1676,9 +1690,9 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{7C45A778-CE75-2E43-8120-E0324D4036B7}"/>
-    <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="4"/>
   </cellStyles>
   <dxfs count="37">
     <dxf>
@@ -1695,7 +1709,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1720,7 +1733,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1745,7 +1757,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1770,7 +1781,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1795,7 +1805,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1820,7 +1829,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1852,7 +1860,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1885,8 +1892,6 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1922,8 +1927,6 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2005,8 +2008,6 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -2030,8 +2031,6 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2049,8 +2048,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2069,7 +2066,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2112,7 +2108,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2154,7 +2149,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2214,7 +2208,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2247,7 +2240,6 @@
         <sz val="14"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2347,7 +2339,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
+    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="36"/>
       <tableStyleElement type="headerRow" dxfId="35"/>
       <tableStyleElement type="totalRow" dxfId="34"/>
@@ -2506,19 +2498,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="CaseTypeId" dataDxfId="24"/>
+    <tableColumn id="2" name="ReasonRequired" dataDxfId="23"/>
+    <tableColumn id="4" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:E8">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2526,19 +2518,19 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
-    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="AccessProfile"/>
+    <tableColumn id="5" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:F14">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2547,20 +2539,20 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
-    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="CaseFieldID"/>
+    <tableColumn id="5" name="AccessProfile"/>
+    <tableColumn id="6" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
-  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+  <autoFilter ref="A3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2570,21 +2562,21 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:F10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2593,27 +2585,27 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
-    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="CaseEventID"/>
+    <tableColumn id="5" name="AccessProfile"/>
+    <tableColumn id="6" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
-  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+  <autoFilter ref="A3:F12"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2915,7 +2907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2954,7 +2946,7 @@
       <c r="I1" s="17"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="110"/>
       <c r="B2" s="110"/>
       <c r="C2" s="111" t="s">
@@ -3434,25 +3426,25 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{196F8254-3891-7C48-9C94-B0438E76405D}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{21A19DA0-6946-0A4B-A347-CB10057DF014}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{FE466DE1-FC19-8246-9866-577AA4A3437C}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11" xr:uid="{286F1893-DAA9-BF46-8DD2-2F855FE269CE}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29" xr:uid="{EEEE544D-B05A-674D-B1BA-5DF93F387B24}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29" xr:uid="{D59EF0B7-2533-BF41-BC09-F633E82C7490}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29">
       <formula1>IF((DATEDIF(B24,C24,"d")&gt;0),C24)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3461,7 +3453,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{131819C2-A65A-DD42-B849-D2D760F10819}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3470,7 +3462,7 @@
           </x14:formula2>
           <xm:sqref>C10:C11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{73198D0A-5E38-8948-B00C-1D567B6A4CD2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -3479,7 +3471,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{4366089E-018C-8E4A-B286-D89B84F0C64D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3488,9 +3480,9 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{67DD8A62-65C2-414E-89EC-65950C8FBA95}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
-            <xm:f>'/Users/rebeccabaker/HMCTS/Reform/ccd-docker/[CCD_CNP_27_safe.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>[1]CaseField!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E24:E29</xm:sqref>
         </x14:dataValidation>
@@ -3501,10 +3493,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3550,7 +3542,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:30" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -4851,15 +4843,15 @@
     <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4869,7 +4861,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0600-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -4885,7 +4877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6322,11 +6314,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6336,7 +6328,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -6352,7 +6344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6391,7 +6383,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7013,15 +7005,15 @@
     <row r="1048575" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7031,7 +7023,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7040,7 +7032,7 @@
           </x14:formula2>
           <xm:sqref>D4:D16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0800-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7056,7 +7048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7095,7 +7087,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7444,15 +7436,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7462,7 +7454,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{00000000-0002-0000-0900-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7471,7 +7463,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7480,7 +7472,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0900-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7496,7 +7488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7530,7 +7522,7 @@
       <c r="E1" s="45"/>
       <c r="F1" s="45"/>
     </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
@@ -9876,7 +9868,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9886,7 +9878,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -9902,7 +9894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9942,7 +9934,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -10272,15 +10264,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10290,7 +10282,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type" xr:uid="{00000000-0002-0000-0B00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10299,7 +10291,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -10308,7 +10300,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0B00-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10324,7 +10316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11895,15 +11887,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11913,7 +11905,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0C00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -11922,7 +11914,7 @@
           </x14:formula2>
           <xm:sqref>C4:C20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field" xr:uid="{00000000-0002-0000-0C00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -11938,7 +11930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12014,7 +12006,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12022,7 +12014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12058,7 +12050,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -12111,10 +12103,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -12146,7 +12138,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -12297,7 +12289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13422,11 +13414,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13437,10 +13429,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -13473,7 +13465,7 @@
       <c r="F1" s="94"/>
       <c r="G1" s="94"/>
     </row>
-    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A2" s="96"/>
       <c r="B2" s="96"/>
       <c r="C2" s="97" t="s">
@@ -13605,7 +13597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13641,7 +13633,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -13736,7 +13728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14013,7 +14005,7 @@
       <c r="IO1" s="65"/>
       <c r="IP1" s="66"/>
     </row>
-    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -15381,7 +15373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15410,7 +15402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="52" x14ac:dyDescent="0.15">
       <c r="A2" s="87"/>
       <c r="B2" s="87" t="s">
         <v>238</v>
@@ -15479,9 +15471,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-1200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
-            <xm:f>[CCD_TestDefinition11.xlsx]CaseType!#REF!</xm:f>
+            <xm:f>[2]CaseType!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -15495,7 +15487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15513,7 +15505,7 @@
       <c r="D1" s="99"/>
       <c r="E1" s="100"/>
     </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>273</v>
       </c>
@@ -15566,14 +15558,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -16758,11 +16750,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16773,7 +16765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16794,7 +16786,7 @@
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
     </row>
-    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>288</v>
       </c>
@@ -16851,10 +16843,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -18528,11 +18520,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18542,7 +18534,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -18558,7 +18550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19844,11 +19836,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -19859,11 +19851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20455,8 +20447,46 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10">
+        <v>44827</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10">
+        <v>44827</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21437,11 +21467,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A22">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21452,7 +21482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22678,15 +22708,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22696,7 +22726,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0500-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
CCD-3686 Rollback Test definition file and remove other BEFTA Master def files
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdathorne/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728A544-2ED8-D04F-A5C0-8EC198FF3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38560" yWindow="4520" windowWidth="35840" windowHeight="19780" tabRatio="757" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" tabRatio="757" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -40,7 +41,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="304">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -985,26 +986,11 @@
   <si>
     <t>CaseLink</t>
   </si>
-  <si>
-    <t>JudicialUser</t>
-  </si>
-  <si>
-    <t>idamId</t>
-  </si>
-  <si>
-    <t>personalCode</t>
-  </si>
-  <si>
-    <t>IdamId</t>
-  </si>
-  <si>
-    <t>PersonalCode</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -1436,47 +1422,47 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1690,9 +1676,9 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 2 3" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{7C45A778-CE75-2E43-8120-E0324D4036B7}"/>
+    <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
   <dxfs count="37">
     <dxf>
@@ -1709,6 +1695,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1733,6 +1720,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1757,6 +1745,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1781,6 +1770,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1805,6 +1795,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1829,6 +1820,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1860,6 +1852,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1892,6 +1885,8 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1927,6 +1922,8 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2008,6 +2005,8 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -2031,6 +2030,8 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2048,6 +2049,8 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2066,6 +2069,7 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2108,6 +2112,7 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2149,6 +2154,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2208,6 +2214,7 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2240,6 +2247,7 @@
         <sz val="14"/>
         <color theme="0"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2339,7 +2347,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7">
+    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
       <tableStyleElement type="wholeTable" dxfId="36"/>
       <tableStyleElement type="headerRow" dxfId="35"/>
       <tableStyleElement type="totalRow" dxfId="34"/>
@@ -2498,19 +2506,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="3">
-    <tableColumn id="1" name="CaseTypeId" dataDxfId="24"/>
-    <tableColumn id="2" name="ReasonRequired" dataDxfId="23"/>
-    <tableColumn id="4" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:E8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2518,19 +2526,19 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="LiveFrom"/>
-    <tableColumn id="2" name="LiveTo"/>
-    <tableColumn id="3" name="CaseTypeID"/>
-    <tableColumn id="4" name="AccessProfile"/>
-    <tableColumn id="5" name="CRUD"/>
+    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
+    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A3:F14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2539,20 +2547,20 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="LiveFrom"/>
-    <tableColumn id="2" name="LiveTo"/>
-    <tableColumn id="3" name="CaseTypeID"/>
-    <tableColumn id="4" name="CaseFieldID"/>
-    <tableColumn id="5" name="AccessProfile"/>
-    <tableColumn id="6" name="CRUD"/>
+    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
+    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
-  <autoFilter ref="A3:G12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2562,21 +2570,21 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:F10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2585,27 +2593,27 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="LiveFrom"/>
-    <tableColumn id="2" name="LiveTo"/>
-    <tableColumn id="3" name="CaseTypeID"/>
-    <tableColumn id="4" name="CaseEventID"/>
-    <tableColumn id="5" name="AccessProfile"/>
-    <tableColumn id="6" name="CRUD"/>
+    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
+    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
+    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
+    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
+    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
+    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
-  <autoFilter ref="A3:F12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2907,7 +2915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2946,7 +2954,7 @@
       <c r="I1" s="17"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="110"/>
       <c r="B2" s="110"/>
       <c r="C2" s="111" t="s">
@@ -3426,25 +3434,25 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{196F8254-3891-7C48-9C94-B0438E76405D}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{21A19DA0-6946-0A4B-A347-CB10057DF014}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{FE466DE1-FC19-8246-9866-577AA4A3437C}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11" xr:uid="{286F1893-DAA9-BF46-8DD2-2F855FE269CE}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29" xr:uid="{EEEE544D-B05A-674D-B1BA-5DF93F387B24}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29" xr:uid="{D59EF0B7-2533-BF41-BC09-F633E82C7490}">
       <formula1>IF((DATEDIF(B24,C24,"d")&gt;0),C24)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3453,7 +3461,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{131819C2-A65A-DD42-B849-D2D760F10819}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3462,7 +3470,7 @@
           </x14:formula2>
           <xm:sqref>C10:C11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{73198D0A-5E38-8948-B00C-1D567B6A4CD2}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -3471,7 +3479,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{4366089E-018C-8E4A-B286-D89B84F0C64D}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3480,9 +3488,9 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{67DD8A62-65C2-414E-89EC-65950C8FBA95}">
           <x14:formula1>
-            <xm:f>[1]CaseField!#REF!</xm:f>
+            <xm:f>'/Users/rebeccabaker/HMCTS/Reform/ccd-docker/[CCD_CNP_27_safe.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E24:E29</xm:sqref>
         </x14:dataValidation>
@@ -3493,10 +3501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3542,7 +3550,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:30" ht="65" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -4843,15 +4851,15 @@
     <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4861,7 +4869,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -4877,7 +4885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6314,11 +6322,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6328,7 +6336,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -6344,7 +6352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6383,7 +6391,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7005,15 +7013,15 @@
     <row r="1048575" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7023,7 +7031,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7032,7 +7040,7 @@
           </x14:formula2>
           <xm:sqref>D4:D16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0800-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7048,7 +7056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7087,7 +7095,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7436,15 +7444,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7454,7 +7462,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{00000000-0002-0000-0900-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7463,7 +7471,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7472,7 +7480,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0900-000005000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7488,7 +7496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7522,7 +7530,7 @@
       <c r="E1" s="45"/>
       <c r="F1" s="45"/>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
@@ -9868,7 +9876,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9878,7 +9886,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0A00-000001000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -9894,7 +9902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9934,7 +9942,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -10264,15 +10272,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10282,7 +10290,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type" xr:uid="{00000000-0002-0000-0B00-000003000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10291,7 +10299,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -10300,7 +10308,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0B00-000005000000}">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10316,7 +10324,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11887,15 +11895,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11905,7 +11913,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0C00-000003000000}">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -11914,7 +11922,7 @@
           </x14:formula2>
           <xm:sqref>C4:C20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field" xr:uid="{00000000-0002-0000-0C00-000004000000}">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -11930,7 +11938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12006,7 +12014,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts"/>
+    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12014,7 +12022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12050,7 +12058,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="91" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -12103,10 +12111,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -12138,7 +12146,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="104" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -12289,7 +12297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13414,11 +13422,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13429,10 +13437,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -13465,7 +13473,7 @@
       <c r="F1" s="94"/>
       <c r="G1" s="94"/>
     </row>
-    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="96"/>
       <c r="B2" s="96"/>
       <c r="C2" s="97" t="s">
@@ -13597,7 +13605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13633,7 +13641,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="104" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -13728,7 +13736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14005,7 +14013,7 @@
       <c r="IO1" s="65"/>
       <c r="IP1" s="66"/>
     </row>
-    <row r="2" spans="1:250" ht="104" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -15373,7 +15381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15402,7 +15410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="87"/>
       <c r="B2" s="87" t="s">
         <v>238</v>
@@ -15471,9 +15479,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-1200-000000000000}">
           <x14:formula1>
-            <xm:f>[2]CaseType!#REF!</xm:f>
+            <xm:f>[CCD_TestDefinition11.xlsx]CaseType!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -15487,7 +15495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15505,7 +15513,7 @@
       <c r="D1" s="99"/>
       <c r="E1" s="100"/>
     </row>
-    <row r="2" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>273</v>
       </c>
@@ -15558,14 +15566,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -16750,11 +16758,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16765,7 +16773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16786,7 +16794,7 @@
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
     </row>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>288</v>
       </c>
@@ -16843,10 +16851,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -18520,11 +18528,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18534,7 +18542,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -18550,7 +18558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19836,11 +19844,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -19851,11 +19859,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20447,46 +20455,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="10">
-        <v>44827</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="10">
-        <v>44827</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21467,11 +21437,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A22">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21482,7 +21452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22708,15 +22678,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22726,7 +22696,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0500-000003000000}">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Revert "CCD-3686 Rollback Test definition file and remove other BEFTA Master def files"
This reverts commit 8057dca9a47dd0b60fe7a60b38d7a87e8d69c05f.
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27809"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markdathorne/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6728A544-2ED8-D04F-A5C0-8EC198FF3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" tabRatio="757" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38560" yWindow="4520" windowWidth="35840" windowHeight="19780" tabRatio="757" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -41,7 +40,7 @@
     <externalReference r:id="rId24"/>
     <externalReference r:id="rId25"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="309">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -986,11 +985,26 @@
   <si>
     <t>CaseLink</t>
   </si>
+  <si>
+    <t>JudicialUser</t>
+  </si>
+  <si>
+    <t>idamId</t>
+  </si>
+  <si>
+    <t>personalCode</t>
+  </si>
+  <si>
+    <t>IdamId</t>
+  </si>
+  <si>
+    <t>PersonalCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -1422,47 +1436,47 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1676,9 +1690,9 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{7C45A778-CE75-2E43-8120-E0324D4036B7}"/>
-    <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="4"/>
   </cellStyles>
   <dxfs count="37">
     <dxf>
@@ -1695,7 +1709,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1720,7 +1733,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1745,7 +1757,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1770,7 +1781,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1795,7 +1805,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1820,7 +1829,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1852,7 +1860,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1885,8 +1892,6 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1922,8 +1927,6 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2005,8 +2008,6 @@
         <sz val="10"/>
         <color rgb="FFFFC000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -2030,8 +2031,6 @@
         <sz val="10"/>
         <color rgb="FF984807"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -2049,8 +2048,6 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2069,7 +2066,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2112,7 +2108,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2154,7 +2149,6 @@
         <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2214,7 +2208,6 @@
         <sz val="14"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2247,7 +2240,6 @@
         <sz val="14"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2347,7 +2339,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
+    <tableStyle name="TableStyleMedium2 2" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="36"/>
       <tableStyleElement type="headerRow" dxfId="35"/>
       <tableStyleElement type="totalRow" dxfId="34"/>
@@ -2506,19 +2498,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="CaseTypeId" dataDxfId="24"/>
+    <tableColumn id="2" name="ReasonRequired" dataDxfId="23"/>
+    <tableColumn id="4" name="NoCActionInterpretationRequired" dataDxfId="22" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A3:E8">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2526,19 +2518,19 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF7173A2-D8A2-FF4D-8E03-DEC08E54E617}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{6E5C3711-944B-B04F-9EDB-7837F57B014C}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{9F6A53E8-0AAE-E94D-AF63-B78FA41263EA}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{4B772456-DFD3-3A44-B324-E8B7685774B7}" name="AccessProfile"/>
-    <tableColumn id="5" xr3:uid="{436850B0-045F-3740-A457-A64C67740B4B}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="AccessProfile"/>
+    <tableColumn id="5" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A3:F14">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2547,20 +2539,20 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36B9DD6B-A914-3F40-B9D3-0AAB614B81F8}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{1AB780D5-E4FA-CB45-89D5-692A85EC22D5}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{2535DE7E-787D-5843-B6B8-AE672C622282}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{FCF263F2-B2CC-FE43-B691-A6C1753C6461}" name="CaseFieldID"/>
-    <tableColumn id="5" xr3:uid="{D2E07587-0A5A-2D4F-85C4-4E4CB788A832}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{EFDBE89F-7B5F-374C-8C53-7E7817BC8F29}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="CaseFieldID"/>
+    <tableColumn id="5" name="AccessProfile"/>
+    <tableColumn id="6" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
-  <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+  <autoFilter ref="A3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2570,21 +2562,21 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" name="LiveFrom" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" name="LiveTo" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" name="CaseTypeID" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" name="CaseFieldID" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" name="ListElementCode" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" name="AccessProfile" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" name="CRUD" dataDxfId="11" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:F10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2593,27 +2585,27 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{ADCC110E-1702-8448-A1B4-78E05E64F156}" name="LiveFrom"/>
-    <tableColumn id="2" xr3:uid="{AE305D3E-D969-6749-9A76-430CABD7D502}" name="LiveTo"/>
-    <tableColumn id="3" xr3:uid="{E4F2602F-5EA6-E041-B0A2-774CE0EA60CE}" name="CaseTypeID"/>
-    <tableColumn id="4" xr3:uid="{754AE0AB-4F94-624D-A34D-E95D40897FD3}" name="CaseEventID"/>
-    <tableColumn id="5" xr3:uid="{1EE05B86-49EC-F148-8D48-563E5CEE442B}" name="AccessProfile"/>
-    <tableColumn id="6" xr3:uid="{9352A5DF-7772-274C-A8F8-B484BFA96F8F}" name="CRUD"/>
+    <tableColumn id="1" name="LiveFrom"/>
+    <tableColumn id="2" name="LiveTo"/>
+    <tableColumn id="3" name="CaseTypeID"/>
+    <tableColumn id="4" name="CaseEventID"/>
+    <tableColumn id="5" name="AccessProfile"/>
+    <tableColumn id="6" name="CRUD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
-  <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+  <autoFilter ref="A3:F12"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" name="LiveFrom" dataDxfId="5" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" name="LiveTo" dataDxfId="4" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" name="CaseTypeID" dataDxfId="3" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" name="CaseStateID" dataDxfId="2" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" name="AccessProfile" dataDxfId="1" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" name="CRUD" dataDxfId="0" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2915,7 +2907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8686C2A1-9CB4-7545-A86A-C2D235EA8904}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2954,7 +2946,7 @@
       <c r="I1" s="17"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="110"/>
       <c r="B2" s="110"/>
       <c r="C2" s="111" t="s">
@@ -3434,25 +3426,25 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{196F8254-3891-7C48-9C94-B0438E76405D}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{21A19DA0-6946-0A4B-A347-CB10057DF014}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{FE466DE1-FC19-8246-9866-577AA4A3437C}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11" xr:uid="{286F1893-DAA9-BF46-8DD2-2F855FE269CE}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G24:H29 G4:G11">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29" xr:uid="{EEEE544D-B05A-674D-B1BA-5DF93F387B24}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="B24:B29">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29" xr:uid="{D59EF0B7-2533-BF41-BC09-F633E82C7490}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="C24:C29">
       <formula1>IF((DATEDIF(B24,C24,"d")&gt;0),C24)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3461,7 +3453,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{131819C2-A65A-DD42-B849-D2D760F10819}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3470,7 +3462,7 @@
           </x14:formula2>
           <xm:sqref>C10:C11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{73198D0A-5E38-8948-B00C-1D567B6A4CD2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -3479,7 +3471,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{4366089E-018C-8E4A-B286-D89B84F0C64D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -3488,9 +3480,9 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{67DD8A62-65C2-414E-89EC-65950C8FBA95}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
-            <xm:f>'/Users/rebeccabaker/HMCTS/Reform/ccd-docker/[CCD_CNP_27_safe.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>[1]CaseField!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E24:E29</xm:sqref>
         </x14:dataValidation>
@@ -3501,10 +3493,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="113" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3550,7 +3542,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:30" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="65" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -4851,15 +4843,15 @@
     <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A9">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4869,7 +4861,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0600-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -4885,7 +4877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6322,11 +6314,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A14">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B10">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6336,7 +6328,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0700-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -6352,7 +6344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6391,7 +6383,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7013,15 +7005,15 @@
     <row r="1048575" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F16">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B16">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7031,7 +7023,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7040,7 +7032,7 @@
           </x14:formula2>
           <xm:sqref>D4:D16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0800-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7056,7 +7048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7095,7 +7087,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -7444,15 +7436,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7462,7 +7454,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type" xr:uid="{00000000-0002-0000-0900-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7471,7 +7463,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -7480,7 +7472,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0900-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -7496,7 +7488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7530,7 +7522,7 @@
       <c r="E1" s="45"/>
       <c r="F1" s="45"/>
     </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
@@ -9876,7 +9868,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9886,7 +9878,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -9902,7 +9894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9942,7 +9934,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -10272,15 +10264,15 @@
     <row r="1048576" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A10:A11">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10290,7 +10282,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type" xr:uid="{00000000-0002-0000-0B00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No Fields defined for the case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10299,7 +10291,7 @@
           </x14:formula2>
           <xm:sqref>C4:C9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -10308,7 +10300,7 @@
           </x14:formula2>
           <xm:sqref>D4:D9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type" xr:uid="{00000000-0002-0000-0B00-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="No fields defined for this case type">
           <x14:formula1>
             <xm:f>CaseField!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -10324,7 +10316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11895,15 +11887,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B17">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G17 I4:I17">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11913,7 +11905,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0C00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -11922,7 +11914,7 @@
           </x14:formula2>
           <xm:sqref>C4:C20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field" xr:uid="{00000000-0002-0000-0C00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field">
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$1000</xm:f>
           </x14:formula1>
@@ -11938,7 +11930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12014,7 +12006,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId1" display="CaseWorkerProbate@hmcts"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12022,7 +12014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12058,7 +12050,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="14" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="12" t="s">
@@ -12111,10 +12103,10 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -12146,7 +12138,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -12297,7 +12289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13422,11 +13414,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after LiveFrom" sqref="B4">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13437,10 +13429,10 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -13473,7 +13465,7 @@
       <c r="F1" s="94"/>
       <c r="G1" s="94"/>
     </row>
-    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A2" s="96"/>
       <c r="B2" s="96"/>
       <c r="C2" s="97" t="s">
@@ -13605,7 +13597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13641,7 +13633,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" s="14" customFormat="1" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
@@ -13736,7 +13728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IP12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14013,7 +14005,7 @@
       <c r="IO1" s="65"/>
       <c r="IP1" s="66"/>
     </row>
-    <row r="2" spans="1:250" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -15381,7 +15373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15410,7 +15402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="52" x14ac:dyDescent="0.15">
       <c r="A2" s="87"/>
       <c r="B2" s="87" t="s">
         <v>238</v>
@@ -15479,9 +15471,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-1200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
-            <xm:f>[CCD_TestDefinition11.xlsx]CaseType!#REF!</xm:f>
+            <xm:f>[2]CaseType!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -15495,7 +15487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D411D1-BCCC-A84F-9B54-A0833B494932}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15513,7 +15505,7 @@
       <c r="D1" s="99"/>
       <c r="E1" s="100"/>
     </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>273</v>
       </c>
@@ -15566,14 +15558,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -16758,11 +16750,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16773,7 +16765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C09F299-AE30-C349-B30B-F04210A51D7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16794,7 +16786,7 @@
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
     </row>
-    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="101" t="s">
         <v>288</v>
       </c>
@@ -16851,10 +16843,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -18528,11 +18520,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A25">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B21">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18542,7 +18534,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>
@@ -18558,7 +18550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19844,11 +19836,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A16">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -19859,11 +19851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20455,8 +20447,46 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10">
+        <v>44827</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10">
+        <v>44827</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21437,11 +21467,11 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A20" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A22">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B20">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21452,7 +21482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22678,15 +22708,15 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="H4:H9">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22696,7 +22726,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type" xr:uid="{00000000-0002-0000-0500-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid case type">
           <x14:formula1>
             <xm:f>CaseType!$C$4:$C$1000</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
GA-3: Increase code coverage
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenbird/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1C8F22-06D0-CA4A-969F-1B2B6124F848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0942AC-1B5F-2E41-8EAB-850DD3548EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -36,11 +36,12 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId21"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId22"/>
     <sheet name="SearchAlias" sheetId="20" r:id="rId23"/>
-    <sheet name="AccessTypeRoles" sheetId="25" r:id="rId24"/>
+    <sheet name="RoleToAccessProfiles" sheetId="26" r:id="rId24"/>
+    <sheet name="AccessTypeRoles" sheetId="25" r:id="rId25"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId25"/>
     <externalReference r:id="rId26"/>
+    <externalReference r:id="rId27"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="351">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1082,9 +1083,6 @@
     <t>CaseAccessGroupIDTemplate</t>
   </si>
   <si>
-    <t>FT_MasterCaseType</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -1101,6 +1099,48 @@
   </si>
   <si>
     <t>respondents</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Case Type Id</t>
+  </si>
+  <si>
+    <t>Access Profiles</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>CaseAccessCategories</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>auth1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>AccessProfile1</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1694,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1877,6 +1917,10 @@
     <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1886,7 +1930,7 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="86">
     <dxf>
       <font>
         <b val="0"/>
@@ -2246,13 +2290,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2288,6 +2325,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2326,79 +2370,282 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0432FF"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <border>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color theme="1"/>
+          <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3065,25 +3312,186 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0432FF"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0432FF"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleDefinitionsTab" pivot="0" count="7" xr9:uid="{5DF7EA3F-64CE-4247-925E-FA6B786D4D35}">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="totalRow" dxfId="25"/>
-      <tableStyleElement type="firstColumn" dxfId="24"/>
-      <tableStyleElement type="lastColumn" dxfId="23"/>
-      <tableStyleElement type="firstRowStripe" dxfId="22"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="21"/>
+      <tableStyleElement type="wholeTable" dxfId="85"/>
+      <tableStyleElement type="headerRow" dxfId="84"/>
+      <tableStyleElement type="totalRow" dxfId="83"/>
+      <tableStyleElement type="firstColumn" dxfId="82"/>
+      <tableStyleElement type="lastColumn" dxfId="81"/>
+      <tableStyleElement type="firstRowStripe" dxfId="80"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="79"/>
+    </tableStyle>
+    <tableStyle name="TableStyleDefinitionsTab 2" pivot="0" count="7" xr9:uid="{07DBC3E2-672D-304E-8827-44CA02ACC044}">
+      <tableStyleElement type="wholeTable" dxfId="78"/>
+      <tableStyleElement type="headerRow" dxfId="77"/>
+      <tableStyleElement type="totalRow" dxfId="76"/>
+      <tableStyleElement type="firstColumn" dxfId="75"/>
+      <tableStyleElement type="lastColumn" dxfId="74"/>
+      <tableStyleElement type="firstRowStripe" dxfId="73"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="72"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
-      <tableStyleElement type="wholeTable" dxfId="64"/>
-      <tableStyleElement type="headerRow" dxfId="63"/>
-      <tableStyleElement type="totalRow" dxfId="62"/>
-      <tableStyleElement type="firstColumn" dxfId="61"/>
-      <tableStyleElement type="lastColumn" dxfId="60"/>
-      <tableStyleElement type="firstRowStripe" dxfId="59"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="58"/>
+      <tableStyleElement type="wholeTable" dxfId="71"/>
+      <tableStyleElement type="headerRow" dxfId="70"/>
+      <tableStyleElement type="totalRow" dxfId="69"/>
+      <tableStyleElement type="firstColumn" dxfId="68"/>
+      <tableStyleElement type="lastColumn" dxfId="67"/>
+      <tableStyleElement type="firstRowStripe" dxfId="66"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="65"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3235,18 +3643,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="50" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="57" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="56">
   <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3266,7 +3674,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="55">
   <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3288,7 +3696,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
   <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3299,20 +3707,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="45" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="44" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="43" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="42" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="41" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="40" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="39" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="52" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="51" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="50" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="49" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="48" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="47" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="46" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3334,22 +3742,40 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
   <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="33" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="32" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="31" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="30" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="29" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="28" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="40" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="39" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="38" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="37" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="36" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="35" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}" name="Table230" displayName="Table230" ref="A3:P128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}" name="Table2214" displayName="Table2214" ref="A3:I57" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+  <autoFilter ref="A3:I57" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{33AF10A0-FD17-A947-9CAA-77E9D3542027}" name="LiveFrom" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{E7E5D7A6-3126-B949-A296-371E77432DF6}" name="LiveTo" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{1FFE52D3-59DC-5F48-8695-25CA9FA2F50C}" name="RoleName" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{EF4600F5-0195-3240-930C-17499C4A0874}" name="Authorisation" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{48CA193A-9E00-BD47-A75E-FF4789D4202D}" name="CaseTypeID" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{45A53A60-CAD6-4F42-A6E3-8EF7193F4F4E}" name="AccessProfiles" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{B51B665F-933C-0B41-9EB0-3A10D78D250E}" name="ReadOnly" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{C959F86F-34F5-3540-91F1-44591632390E}" name="Disabled" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{F4A1B44D-5922-8542-A473-3D3610C6383D}" name="CaseAccessCategories" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}" name="Table230" displayName="Table230" ref="A3:P128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A3:P128" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{8C3C6264-6488-4B46-844F-78CC8AF0EDBF}" name="LiveFrom" dataDxfId="15"/>
@@ -4174,6 +4600,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -5575,6 +6004,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -7002,6 +7434,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -7691,6 +8126,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -8116,6 +8554,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -8502,6 +8943,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -8525,7 +8969,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8898,6 +9342,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -8939,7 +9386,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9050,7 +9497,7 @@
         <v>42736</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" t="s">
+      <c r="C4" s="66" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
@@ -10516,6 +10963,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -10618,6 +11068,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -10626,7 +11079,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10688,7 +11141,7 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>215</v>
       </c>
       <c r="E4" t="s">
@@ -10698,6 +11151,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -10709,7 +11165,7 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10796,7 +11252,7 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>46</v>
       </c>
       <c r="E4" t="s">
@@ -10879,6 +11335,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -12016,15 +12475,18 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12098,8 +12560,20 @@
         <v>214</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="133"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="123"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -12225,6 +12699,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -12612,6 +13089,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -12714,6 +13194,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -12733,11 +13216,475 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01A3093-2002-4A4A-8D4C-7A6AF114CAB2}">
+  <dimension ref="A1:I57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="75.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="111" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="114" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="114"/>
+    </row>
+    <row r="2" spans="1:9" s="132" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="117" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="117" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117" t="s">
+        <v>339</v>
+      </c>
+      <c r="F2" s="117" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="117" t="s">
+        <v>341</v>
+      </c>
+      <c r="H2" s="117" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2" s="132" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="121" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="119" t="s">
+        <v>344</v>
+      </c>
+      <c r="D3" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="E3" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="119" t="s">
+        <v>346</v>
+      </c>
+      <c r="G3" s="119" t="s">
+        <v>347</v>
+      </c>
+      <c r="H3" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="I3" s="119" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="122">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="122"/>
+      <c r="C4" s="124" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" s="124" t="s">
+        <v>348</v>
+      </c>
+      <c r="E4" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="124" t="s">
+        <v>350</v>
+      </c>
+      <c r="G4" s="124" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" s="123" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="122"/>
+      <c r="B5" s="122"/>
+      <c r="E5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+    </row>
+    <row r="6" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="122"/>
+      <c r="B6" s="122"/>
+      <c r="E6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+    </row>
+    <row r="7" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="122"/>
+      <c r="B7" s="122"/>
+      <c r="E7" s="123"/>
+      <c r="H7" s="123"/>
+    </row>
+    <row r="8" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="122"/>
+      <c r="B8" s="122"/>
+      <c r="E8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+    </row>
+    <row r="9" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="122"/>
+      <c r="B9" s="122"/>
+      <c r="E9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+    </row>
+    <row r="10" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="122"/>
+      <c r="B10" s="122"/>
+      <c r="E10" s="123"/>
+      <c r="H10" s="123"/>
+    </row>
+    <row r="11" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A11" s="122"/>
+      <c r="B11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+    </row>
+    <row r="12" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="122"/>
+      <c r="B12" s="122"/>
+      <c r="E12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+    </row>
+    <row r="13" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="122"/>
+      <c r="B13" s="122"/>
+      <c r="E13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+    </row>
+    <row r="14" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="122"/>
+      <c r="B14" s="122"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+    </row>
+    <row r="15" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="122"/>
+      <c r="B15" s="122"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+    </row>
+    <row r="16" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="122"/>
+      <c r="B16" s="122"/>
+      <c r="E16" s="123"/>
+      <c r="H16" s="123"/>
+    </row>
+    <row r="17" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="122"/>
+      <c r="B17" s="122"/>
+      <c r="E17" s="123"/>
+      <c r="H17" s="123"/>
+    </row>
+    <row r="18" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="122"/>
+      <c r="B18" s="122"/>
+      <c r="E18" s="123"/>
+      <c r="H18" s="123"/>
+    </row>
+    <row r="19" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="122"/>
+      <c r="B19" s="122"/>
+      <c r="E19" s="123"/>
+      <c r="H19" s="123"/>
+    </row>
+    <row r="20" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="122"/>
+      <c r="B20" s="122"/>
+      <c r="E20" s="123"/>
+      <c r="H20" s="123"/>
+    </row>
+    <row r="21" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="122"/>
+      <c r="B21" s="122"/>
+      <c r="E21" s="123"/>
+      <c r="H21" s="123"/>
+    </row>
+    <row r="22" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="122"/>
+      <c r="B22" s="122"/>
+      <c r="E22" s="123"/>
+      <c r="H22" s="123"/>
+    </row>
+    <row r="23" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="122"/>
+      <c r="B23" s="122"/>
+      <c r="E23" s="123"/>
+      <c r="H23" s="123"/>
+    </row>
+    <row r="24" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="122"/>
+      <c r="B24" s="122"/>
+      <c r="E24" s="123"/>
+      <c r="H24" s="123"/>
+    </row>
+    <row r="25" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="122"/>
+      <c r="B25" s="122"/>
+      <c r="F25" s="123"/>
+      <c r="H25" s="123"/>
+    </row>
+    <row r="26" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="122"/>
+      <c r="B26" s="122"/>
+      <c r="F26" s="123"/>
+      <c r="H26" s="123"/>
+    </row>
+    <row r="27" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
+      <c r="H27" s="123"/>
+    </row>
+    <row r="28" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A28" s="122"/>
+      <c r="B28" s="122"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="H28" s="123"/>
+    </row>
+    <row r="29" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A29" s="122"/>
+      <c r="B29" s="122"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="H29" s="123"/>
+    </row>
+    <row r="30" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A30" s="122"/>
+      <c r="B30" s="122"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="H30" s="123"/>
+    </row>
+    <row r="31" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A31" s="122"/>
+      <c r="B31" s="122"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="123"/>
+      <c r="H31" s="123"/>
+    </row>
+    <row r="32" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A32" s="122"/>
+      <c r="B32" s="122"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="H32" s="123"/>
+    </row>
+    <row r="33" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="122"/>
+      <c r="B33" s="122"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="123"/>
+      <c r="H33" s="123"/>
+    </row>
+    <row r="34" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A34" s="122"/>
+      <c r="B34" s="122"/>
+      <c r="H34" s="123"/>
+    </row>
+    <row r="35" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A35" s="122"/>
+      <c r="B35" s="122"/>
+      <c r="H35" s="123"/>
+    </row>
+    <row r="36" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A36" s="122"/>
+      <c r="B36" s="122"/>
+      <c r="H36" s="123"/>
+    </row>
+    <row r="37" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A37" s="122"/>
+      <c r="B37" s="122"/>
+      <c r="H37" s="123"/>
+    </row>
+    <row r="38" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="122"/>
+      <c r="B38" s="122"/>
+      <c r="H38" s="123"/>
+    </row>
+    <row r="39" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A39" s="122"/>
+      <c r="B39" s="122"/>
+      <c r="H39" s="123"/>
+    </row>
+    <row r="40" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A40" s="122"/>
+      <c r="B40" s="122"/>
+      <c r="H40" s="123"/>
+    </row>
+    <row r="41" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A41" s="122"/>
+      <c r="B41" s="122"/>
+      <c r="H41" s="123"/>
+    </row>
+    <row r="42" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A42" s="122"/>
+      <c r="B42" s="122"/>
+      <c r="E42" s="123"/>
+      <c r="F42" s="123"/>
+      <c r="H42" s="123"/>
+    </row>
+    <row r="43" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A43" s="122"/>
+      <c r="B43" s="122"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="123"/>
+      <c r="H43" s="123"/>
+    </row>
+    <row r="44" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A44" s="122"/>
+      <c r="B44" s="122"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
+      <c r="H44" s="123"/>
+    </row>
+    <row r="45" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A45" s="122"/>
+      <c r="B45" s="122"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
+      <c r="H45" s="123"/>
+    </row>
+    <row r="46" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A46" s="122"/>
+      <c r="B46" s="122"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="123"/>
+      <c r="H46" s="123"/>
+    </row>
+    <row r="47" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A47" s="122"/>
+      <c r="B47" s="122"/>
+      <c r="E47" s="123"/>
+      <c r="F47" s="123"/>
+      <c r="H47" s="123"/>
+    </row>
+    <row r="48" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A48" s="122"/>
+      <c r="B48" s="122"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
+      <c r="H48" s="123"/>
+    </row>
+    <row r="49" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A49" s="122"/>
+      <c r="B49" s="122"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
+      <c r="H49" s="123"/>
+    </row>
+    <row r="50" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A50" s="122"/>
+      <c r="B50" s="122"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="123"/>
+      <c r="H50" s="123"/>
+    </row>
+    <row r="51" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A51" s="122"/>
+      <c r="B51" s="122"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="H51" s="123"/>
+    </row>
+    <row r="52" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A52" s="122"/>
+      <c r="B52" s="122"/>
+      <c r="E52" s="123"/>
+      <c r="F52" s="123"/>
+      <c r="H52" s="123"/>
+    </row>
+    <row r="53" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="122"/>
+      <c r="B53" s="122"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
+      <c r="H53" s="123"/>
+    </row>
+    <row r="54" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="122"/>
+      <c r="B54" s="122"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
+      <c r="H54" s="123"/>
+    </row>
+    <row r="55" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A55" s="122"/>
+      <c r="B55" s="122"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="123"/>
+      <c r="H55" s="123"/>
+    </row>
+    <row r="56" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A56" s="122"/>
+      <c r="B56" s="122"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="123"/>
+      <c r="H56" s="123"/>
+    </row>
+    <row r="57" spans="1:8" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A57" s="122"/>
+      <c r="B57" s="122"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="123"/>
+      <c r="H57" s="123"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E213E05-C678-DD41-9D11-284BE15D402F}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12875,13 +13822,13 @@
       </c>
       <c r="B4" s="122"/>
       <c r="C4" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="123" t="s">
         <v>331</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="E4" s="123" t="s">
         <v>332</v>
-      </c>
-      <c r="E4" s="123" t="s">
-        <v>333</v>
       </c>
       <c r="F4" s="123" t="s">
         <v>182</v>
@@ -12893,28 +13840,28 @@
         <v>182</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K4" s="124">
         <v>1</v>
       </c>
       <c r="L4" s="123" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M4" s="123" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N4" s="124" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O4" s="124" t="s">
         <v>182</v>
       </c>
       <c r="P4" s="124" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -12923,13 +13870,13 @@
       </c>
       <c r="B5" s="122"/>
       <c r="C5" s="123" t="s">
-        <v>331</v>
+        <v>25</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E5" s="123" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F5" s="123" t="s">
         <v>182</v>
@@ -12941,16 +13888,16 @@
         <v>182</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J5" s="124" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K5" s="124">
         <v>2</v>
       </c>
       <c r="L5" s="124" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M5" s="123"/>
       <c r="N5" s="124"/>
@@ -14999,6 +15946,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -15080,6 +16030,9 @@
     <hyperlink ref="E4" r:id="rId1" xr:uid="{DD8FB635-29D9-CB45-A5A6-A674B24C110A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -15088,7 +16041,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16268,6 +17221,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -16343,6 +17299,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -16354,7 +17313,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17968,6 +18927,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -19278,6 +20240,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -19285,8 +20250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19772,13 +20737,13 @@
       <c r="C20" t="s">
         <v>125</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="66" t="s">
         <v>123</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="66" t="s">
         <v>124</v>
       </c>
       <c r="L20" t="s">
@@ -20778,6 +21743,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -22010,6 +22978,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -22026,4 +22997,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{4af293e6-3850-4258-b2c7-0aa0e3bfa7d9}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="3" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
GA-133 Add new Tab AccessType and AccessTypeRole in the DefinitionStore to replace the AccessTypeRoles Tab
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenbird/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenbird/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0942AC-1B5F-2E41-8EAB-850DD3548EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C063BAC1-9E11-AB4B-9867-4C9E1D4BA040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
GA-133 amended test spreadsheet
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenbird/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0942AC-1B5F-2E41-8EAB-850DD3548EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89414EA2-65A2-5E4E-BAA0-2D6CE8D8CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -37,11 +37,12 @@
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId22"/>
     <sheet name="SearchAlias" sheetId="20" r:id="rId23"/>
     <sheet name="RoleToAccessProfiles" sheetId="26" r:id="rId24"/>
-    <sheet name="AccessTypeRoles" sheetId="25" r:id="rId25"/>
+    <sheet name="AccessType" sheetId="25" r:id="rId25"/>
+    <sheet name="AccessTypeRole" sheetId="27" r:id="rId26"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
+    <externalReference r:id="rId28"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="354">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1006,13 +1007,6 @@
 MaxLength: 200</t>
   </si>
   <si>
-    <t>This can be a CCD base type (see confluence) or a OrganisationProfile ID).  
-MaxLength: 200</t>
-  </si>
-  <si>
-    <t>Access type is mandatory for the given organisation type. (YesOrNo field Optional)</t>
-  </si>
-  <si>
     <t>Field that indicates whether this access is applied by default for the given organisation type.
 If no specific configuration has been provided for a user (either to explicitly enable or disable the accesstype), this determines whether the user receives the access type by default.
 (YesOrNo field Optional)</t>
@@ -1022,33 +1016,10 @@
 (YesOrNo field Optional)</t>
   </si>
   <si>
-    <t>The long description to decribe the access type.
-MaxLength: 200</t>
-  </si>
-  <si>
-    <t>The hint text that is present for this access type
-MaxLength: 300</t>
-  </si>
-  <si>
-    <t>The Order access types are displayed in UI</t>
-  </si>
-  <si>
     <t>The role name that is used to create organisation role assignments for this record.
 MaxLength: 70</t>
   </si>
   <si>
-    <t>The role name that is used to create access role assignments for this record.
-MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Identifies the organisation policy field through which an organisation gets group access.
-MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Indicates whether this record is active for group access.
-(YesOrNo field Optional)</t>
-  </si>
-  <si>
     <t>A text template used to generate the case access group identifier for role assignments and case data.
 MaxLength: 200</t>
   </si>
@@ -1141,6 +1112,45 @@
   </si>
   <si>
     <t>AccessProfile1</t>
+  </si>
+  <si>
+    <t>AccessType</t>
+  </si>
+  <si>
+    <t>The identifier which defines the organisation profile to which this access type applies.
+MaxLength: 200</t>
+  </si>
+  <si>
+    <t>Indicates that this access type is mandatory for the given organisation type. (YesOrNo field Optional)</t>
+  </si>
+  <si>
+    <t>The description rendered in the UI for this access type.
+MaxLength: 200</t>
+  </si>
+  <si>
+    <t>A longer description used in the UI as a hint.
+MaxLength: 300</t>
+  </si>
+  <si>
+    <t>An integer indicating the order in which the AccessTypes are displayed in the UI</t>
+  </si>
+  <si>
+    <t>FT_MasterCaseType</t>
+  </si>
+  <si>
+    <t>The role name that is used to create the group access role assignments for this record.
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This field uniquely identifies the OrganisationPolicy.
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Indicates whether this record is active for Group Access.
+(YesOrNo field Optional)</t>
+  </si>
+  <si>
+    <t>DD/01/YYYY</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1163,7 @@
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
   </numFmts>
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1525,8 +1535,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1551,8 +1580,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor rgb="FF0432FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFDCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1685,6 +1726,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1694,7 +1765,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1921,6 +1992,52 @@
     <xf numFmtId="14" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="56" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="57" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="34" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1930,117 +2047,7 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="86">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="95">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2290,6 +2297,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2327,13 +2341,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2367,6 +2374,158 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0432FF"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0432FF"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3465,33 +3624,51 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="5" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleDefinitionsTab" pivot="0" count="7" xr9:uid="{5DF7EA3F-64CE-4247-925E-FA6B786D4D35}">
-      <tableStyleElement type="wholeTable" dxfId="85"/>
-      <tableStyleElement type="headerRow" dxfId="84"/>
-      <tableStyleElement type="totalRow" dxfId="83"/>
-      <tableStyleElement type="firstColumn" dxfId="82"/>
-      <tableStyleElement type="lastColumn" dxfId="81"/>
-      <tableStyleElement type="firstRowStripe" dxfId="80"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="79"/>
+      <tableStyleElement type="wholeTable" dxfId="94"/>
+      <tableStyleElement type="headerRow" dxfId="93"/>
+      <tableStyleElement type="totalRow" dxfId="92"/>
+      <tableStyleElement type="firstColumn" dxfId="91"/>
+      <tableStyleElement type="lastColumn" dxfId="90"/>
+      <tableStyleElement type="firstRowStripe" dxfId="89"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="88"/>
     </tableStyle>
     <tableStyle name="TableStyleDefinitionsTab 2" pivot="0" count="7" xr9:uid="{07DBC3E2-672D-304E-8827-44CA02ACC044}">
-      <tableStyleElement type="wholeTable" dxfId="78"/>
-      <tableStyleElement type="headerRow" dxfId="77"/>
-      <tableStyleElement type="totalRow" dxfId="76"/>
-      <tableStyleElement type="firstColumn" dxfId="75"/>
-      <tableStyleElement type="lastColumn" dxfId="74"/>
-      <tableStyleElement type="firstRowStripe" dxfId="73"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="72"/>
+      <tableStyleElement type="wholeTable" dxfId="87"/>
+      <tableStyleElement type="headerRow" dxfId="86"/>
+      <tableStyleElement type="totalRow" dxfId="85"/>
+      <tableStyleElement type="firstColumn" dxfId="84"/>
+      <tableStyleElement type="lastColumn" dxfId="83"/>
+      <tableStyleElement type="firstRowStripe" dxfId="82"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="81"/>
+    </tableStyle>
+    <tableStyle name="TableStyleDefinitionsTab 3" pivot="0" count="7" xr9:uid="{514ABE8E-A2FC-7040-A314-26005F4E04FE}">
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="firstColumn" dxfId="26"/>
+      <tableStyleElement type="lastColumn" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="23"/>
+    </tableStyle>
+    <tableStyle name="TableStyleDefinitionsTab 4" pivot="0" count="7" xr9:uid="{60638E0F-CA40-DC45-A674-F5F7DCBEB02B}">
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumn" dxfId="19"/>
+      <tableStyleElement type="lastColumn" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
-      <tableStyleElement type="wholeTable" dxfId="71"/>
-      <tableStyleElement type="headerRow" dxfId="70"/>
-      <tableStyleElement type="totalRow" dxfId="69"/>
-      <tableStyleElement type="firstColumn" dxfId="68"/>
-      <tableStyleElement type="lastColumn" dxfId="67"/>
-      <tableStyleElement type="firstRowStripe" dxfId="66"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="65"/>
+      <tableStyleElement type="wholeTable" dxfId="80"/>
+      <tableStyleElement type="headerRow" dxfId="79"/>
+      <tableStyleElement type="totalRow" dxfId="78"/>
+      <tableStyleElement type="firstColumn" dxfId="77"/>
+      <tableStyleElement type="lastColumn" dxfId="76"/>
+      <tableStyleElement type="firstRowStripe" dxfId="75"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="74"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3643,18 +3820,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="57" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="66" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="65">
   <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3674,7 +3851,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="64">
   <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3696,7 +3873,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
   <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3707,20 +3884,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="52" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="51" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="50" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="49" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="48" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="47" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="46" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="61" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="60" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="59" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="58" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="57" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="56" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="55" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3742,58 +3919,53 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
   <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="40" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="39" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="38" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="37" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="36" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="35" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="49" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="48" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="47" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="46" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="45" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="44" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}" name="Table2214" displayName="Table2214" ref="A3:I57" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}" name="Table2214" displayName="Table2214" ref="A3:I57" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A3:I57" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{33AF10A0-FD17-A947-9CAA-77E9D3542027}" name="LiveFrom" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{E7E5D7A6-3126-B949-A296-371E77432DF6}" name="LiveTo" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{1FFE52D3-59DC-5F48-8695-25CA9FA2F50C}" name="RoleName" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{EF4600F5-0195-3240-930C-17499C4A0874}" name="Authorisation" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{48CA193A-9E00-BD47-A75E-FF4789D4202D}" name="CaseTypeID" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{45A53A60-CAD6-4F42-A6E3-8EF7193F4F4E}" name="AccessProfiles" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{B51B665F-933C-0B41-9EB0-3A10D78D250E}" name="ReadOnly" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{C959F86F-34F5-3540-91F1-44591632390E}" name="Disabled" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{F4A1B44D-5922-8542-A473-3D3610C6383D}" name="CaseAccessCategories" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{33AF10A0-FD17-A947-9CAA-77E9D3542027}" name="LiveFrom" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{E7E5D7A6-3126-B949-A296-371E77432DF6}" name="LiveTo" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{1FFE52D3-59DC-5F48-8695-25CA9FA2F50C}" name="RoleName" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{EF4600F5-0195-3240-930C-17499C4A0874}" name="Authorisation" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{48CA193A-9E00-BD47-A75E-FF4789D4202D}" name="CaseTypeID" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{45A53A60-CAD6-4F42-A6E3-8EF7193F4F4E}" name="AccessProfiles" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{B51B665F-933C-0B41-9EB0-3A10D78D250E}" name="ReadOnly" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{C959F86F-34F5-3540-91F1-44591632390E}" name="Disabled" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{F4A1B44D-5922-8542-A473-3D3610C6383D}" name="CaseAccessCategories" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}" name="Table230" displayName="Table230" ref="A3:P128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A3:P128" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{8C3C6264-6488-4B46-844F-78CC8AF0EDBF}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{95AB0CD9-F14A-EA40-B121-07641BAA248A}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{18A561CE-791A-3A43-B06A-B27A02FAAFDB}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6A586A4E-EA35-4E4B-BC60-732047B49C80}" name="AccessTypeID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{1475CF15-4AE2-D547-A87F-CCA3AF2C780B}" name="OrganisationProfileID" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{930AF5C9-9016-7246-995A-DF6FB6AAC8DC}" name="AccessMandatory" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{769BF7CA-E071-0A47-AA62-48684CBE997A}" name="AccessDefault" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{5EDA7EBC-00F3-204D-B4FD-A9A0115A6E14}" name="Display" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{F76B90E0-19CB-144F-B0C5-C959BA87ABE7}" name="Description" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{0E637EFA-4DDB-AB45-9C96-596ACB0AC71C}" name="HintText" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{97A904CD-4B78-4F41-B725-D733390E4F60}" name="DisplayOrder" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{1658B47E-5FBB-D340-BE0B-BDC42B9F01FF}" name="OrganisationalRoleName" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{3140418B-F23F-CD40-AD19-B8DD152035B9}" name="GroupRoleName" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{62607777-04A9-FB40-B101-1CD50AC850DF}" name="CaseAssignedRoleField" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{3FC77184-E5A9-1240-98B2-ABD9520779C3}" name="GroupAccessEnabled" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{8DEA16FB-7E2A-E74C-9CAF-EC6D2776B5D6}" name="CaseAccessGroupIDTemplate" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34824A92-561B-D44E-8BBB-DDC8CFAD9858}" name="Table23031" displayName="Table23031" ref="A3:K128" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A3:K128" xr:uid="{34824A92-561B-D44E-8BBB-DDC8CFAD9858}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{C211E3DA-F14B-0D45-B648-5A02FBC237F4}" name="LiveFrom" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{9C76A7F0-8919-8A41-8581-0D9A18199764}" name="LiveTo" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{25328C6F-AB22-B34F-95A5-C57832B21DA8}" name="CaseTypeID" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A8C1540B-9781-8645-BFBD-AD146D4A4749}" name="AccessTypeID" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{630137AD-3995-9249-9BB5-3A269900D964}" name="OrganisationProfileID" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{43759662-50A8-3042-B4B8-DDBFB2319DC8}" name="AccessMandatory" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9A638417-7AB6-344E-9D83-63BE6802DE2C}" name="AccessDefault" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{77E4638F-45B8-4441-A64A-A4449DA766AD}" name="Display" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EF674114-0D73-6E4A-8BD2-47FC835B4419}" name="Description" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{02742F77-B39A-5E4A-A7E4-4DCFA58F7A7E}" name="HintText" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{38F0C388-84F3-ED4A-A068-CD2487C5C904}" name="DisplayOrder" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12485,7 +12657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -13234,7 +13406,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="111" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="112"/>
@@ -13252,23 +13424,23 @@
         <v>306</v>
       </c>
       <c r="C2" s="117" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D2" s="117"/>
       <c r="E2" s="117" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F2" s="117" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="G2" s="117" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="H2" s="117" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I2" s="132" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="121" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13279,25 +13451,25 @@
         <v>8</v>
       </c>
       <c r="C3" s="119" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E3" s="119" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="119" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="G3" s="119" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="H3" s="119" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="I3" s="119" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13306,22 +13478,22 @@
       </c>
       <c r="B4" s="122"/>
       <c r="C4" s="124" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D4" s="124" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E4" s="123" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="124" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="G4" s="124" t="s">
         <v>293</v>
       </c>
       <c r="H4" s="123" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13681,10 +13853,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E213E05-C678-DD41-9D11-284BE15D402F}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13699,16 +13871,11 @@
     <col min="8" max="8" width="11.1640625" customWidth="1"/>
     <col min="9" max="10" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" customWidth="1"/>
-    <col min="14" max="14" width="28.83203125" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="111" t="s">
-        <v>304</v>
+        <v>343</v>
       </c>
       <c r="B1" s="112"/>
       <c r="C1" s="113"/>
@@ -13716,7 +13883,7 @@
       <c r="I1" s="115"/>
       <c r="K1" s="116"/>
     </row>
-    <row r="2" spans="1:16" ht="168" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="168" x14ac:dyDescent="0.15">
       <c r="A2" s="117" t="s">
         <v>305</v>
       </c>
@@ -13730,43 +13897,28 @@
         <v>308</v>
       </c>
       <c r="E2" s="117" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="117" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="117" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="H2" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="G2" s="117" t="s">
-        <v>311</v>
-      </c>
-      <c r="H2" s="91" t="s">
-        <v>312</v>
-      </c>
       <c r="I2" s="117" t="s">
-        <v>313</v>
+        <v>346</v>
       </c>
       <c r="J2" s="117" t="s">
-        <v>314</v>
+        <v>347</v>
       </c>
       <c r="K2" s="118" t="s">
-        <v>315</v>
-      </c>
-      <c r="L2" s="118" t="s">
-        <v>316</v>
-      </c>
-      <c r="M2" s="118" t="s">
-        <v>317</v>
-      </c>
-      <c r="N2" s="117" t="s">
-        <v>318</v>
-      </c>
-      <c r="O2" s="91" t="s">
-        <v>319</v>
-      </c>
-      <c r="P2" s="91" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="119" t="s">
         <v>7</v>
       </c>
@@ -13777,19 +13929,19 @@
         <v>37</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E3" s="119" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F3" s="119" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="G3" s="119" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="H3" s="119" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="I3" s="119" t="s">
         <v>11</v>
@@ -13800,35 +13952,20 @@
       <c r="K3" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="121" t="s">
-        <v>326</v>
-      </c>
-      <c r="M3" s="119" t="s">
-        <v>327</v>
-      </c>
-      <c r="N3" s="119" t="s">
-        <v>328</v>
-      </c>
-      <c r="O3" s="119" t="s">
-        <v>329</v>
-      </c>
-      <c r="P3" s="119" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="122">
         <v>44927</v>
       </c>
       <c r="B4" s="122"/>
       <c r="C4" s="123" t="s">
-        <v>25</v>
+        <v>349</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E4" s="123" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="F4" s="123" t="s">
         <v>182</v>
@@ -13840,43 +13977,28 @@
         <v>182</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="K4" s="124">
         <v>1</v>
       </c>
-      <c r="L4" s="123" t="s">
-        <v>334</v>
-      </c>
-      <c r="M4" s="123" t="s">
-        <v>334</v>
-      </c>
-      <c r="N4" s="124" t="s">
-        <v>334</v>
-      </c>
-      <c r="O4" s="124" t="s">
-        <v>182</v>
-      </c>
-      <c r="P4" s="124" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="122">
         <v>44927</v>
       </c>
       <c r="B5" s="122"/>
       <c r="C5" s="123" t="s">
-        <v>25</v>
+        <v>349</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E5" s="123" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="F5" s="123" t="s">
         <v>182</v>
@@ -13888,23 +14010,16 @@
         <v>182</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="J5" s="124" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="K5" s="124">
         <v>2</v>
       </c>
-      <c r="L5" s="124" t="s">
-        <v>334</v>
-      </c>
-      <c r="M5" s="123"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="122"/>
       <c r="B6" s="122"/>
       <c r="C6" s="123"/>
@@ -13916,13 +14031,8 @@
       <c r="I6" s="123"/>
       <c r="J6" s="124"/>
       <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="122"/>
       <c r="B7" s="122"/>
       <c r="C7" s="123"/>
@@ -13934,13 +14044,8 @@
       <c r="I7" s="123"/>
       <c r="J7" s="124"/>
       <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="122"/>
       <c r="B8" s="122"/>
       <c r="C8" s="123"/>
@@ -13952,13 +14057,8 @@
       <c r="I8" s="123"/>
       <c r="J8" s="124"/>
       <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="122"/>
       <c r="B9" s="122"/>
       <c r="C9" s="123"/>
@@ -13970,13 +14070,8 @@
       <c r="I9" s="123"/>
       <c r="J9" s="124"/>
       <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="122"/>
       <c r="B10" s="122"/>
       <c r="C10" s="123"/>
@@ -13988,13 +14083,8 @@
       <c r="I10" s="123"/>
       <c r="J10" s="124"/>
       <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="124"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="122"/>
       <c r="B11" s="122"/>
       <c r="C11" s="123"/>
@@ -14006,13 +14096,8 @@
       <c r="I11" s="123"/>
       <c r="J11" s="124"/>
       <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="122"/>
       <c r="B12" s="122"/>
       <c r="C12" s="123"/>
@@ -14024,13 +14109,8 @@
       <c r="I12" s="123"/>
       <c r="J12" s="124"/>
       <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="122"/>
       <c r="B13" s="122"/>
       <c r="C13" s="123"/>
@@ -14042,13 +14122,8 @@
       <c r="I13" s="123"/>
       <c r="J13" s="124"/>
       <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="122"/>
       <c r="B14" s="122"/>
       <c r="C14" s="123"/>
@@ -14060,13 +14135,8 @@
       <c r="I14" s="123"/>
       <c r="J14" s="124"/>
       <c r="K14" s="125"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="122"/>
       <c r="B15" s="122"/>
       <c r="C15" s="123"/>
@@ -14078,13 +14148,8 @@
       <c r="I15" s="123"/>
       <c r="J15" s="124"/>
       <c r="K15" s="125"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="122"/>
       <c r="B16" s="122"/>
       <c r="C16" s="123"/>
@@ -14096,13 +14161,8 @@
       <c r="I16" s="124"/>
       <c r="J16" s="124"/>
       <c r="K16" s="125"/>
-      <c r="L16" s="124"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="124"/>
-      <c r="O16" s="124"/>
-      <c r="P16" s="124"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="122"/>
       <c r="B17" s="122"/>
       <c r="C17" s="123"/>
@@ -14114,13 +14174,8 @@
       <c r="I17" s="124"/>
       <c r="J17" s="124"/>
       <c r="K17" s="125"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="122"/>
       <c r="B18" s="122"/>
       <c r="C18" s="123"/>
@@ -14132,13 +14187,8 @@
       <c r="I18" s="124"/>
       <c r="J18" s="124"/>
       <c r="K18" s="125"/>
-      <c r="L18" s="124"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="124"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="122"/>
       <c r="B19" s="122"/>
       <c r="C19" s="123"/>
@@ -14150,13 +14200,8 @@
       <c r="I19" s="124"/>
       <c r="J19" s="124"/>
       <c r="K19" s="125"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="124"/>
-      <c r="O19" s="124"/>
-      <c r="P19" s="124"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="122"/>
       <c r="B20" s="122"/>
       <c r="C20" s="123"/>
@@ -14168,13 +14213,8 @@
       <c r="I20" s="124"/>
       <c r="J20" s="124"/>
       <c r="K20" s="125"/>
-      <c r="L20" s="124"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="124"/>
-      <c r="P20" s="124"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="122"/>
       <c r="B21" s="122"/>
       <c r="C21" s="123"/>
@@ -14186,13 +14226,8 @@
       <c r="I21" s="124"/>
       <c r="J21" s="124"/>
       <c r="K21" s="124"/>
-      <c r="L21" s="124"/>
-      <c r="M21" s="123"/>
-      <c r="N21" s="124"/>
-      <c r="O21" s="124"/>
-      <c r="P21" s="124"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="122"/>
       <c r="B22" s="122"/>
       <c r="C22" s="123"/>
@@ -14203,13 +14238,8 @@
       <c r="H22" s="123"/>
       <c r="I22" s="124"/>
       <c r="J22" s="124"/>
-      <c r="L22" s="124"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="124"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="122"/>
       <c r="B23" s="122"/>
       <c r="C23" s="123"/>
@@ -14220,13 +14250,8 @@
       <c r="H23" s="123"/>
       <c r="I23" s="124"/>
       <c r="J23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="124"/>
-      <c r="O23" s="124"/>
-      <c r="P23" s="124"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="122"/>
       <c r="B24" s="122"/>
       <c r="C24" s="123"/>
@@ -14237,13 +14262,8 @@
       <c r="H24" s="123"/>
       <c r="I24" s="124"/>
       <c r="J24" s="124"/>
-      <c r="L24" s="124"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="124"/>
-      <c r="O24" s="124"/>
-      <c r="P24" s="124"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="122"/>
       <c r="B25" s="122"/>
       <c r="C25" s="123"/>
@@ -14254,13 +14274,8 @@
       <c r="H25" s="123"/>
       <c r="I25" s="124"/>
       <c r="J25" s="124"/>
-      <c r="L25" s="124"/>
-      <c r="M25" s="123"/>
-      <c r="N25" s="124"/>
-      <c r="O25" s="124"/>
-      <c r="P25" s="124"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="122"/>
       <c r="B26" s="122"/>
       <c r="C26" s="123"/>
@@ -14271,13 +14286,8 @@
       <c r="H26" s="123"/>
       <c r="I26" s="124"/>
       <c r="J26" s="124"/>
-      <c r="L26" s="124"/>
-      <c r="M26" s="123"/>
-      <c r="N26" s="124"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="122"/>
       <c r="B27" s="122"/>
       <c r="C27" s="123"/>
@@ -14288,13 +14298,8 @@
       <c r="H27" s="123"/>
       <c r="I27" s="124"/>
       <c r="J27" s="124"/>
-      <c r="L27" s="124"/>
-      <c r="M27" s="123"/>
-      <c r="N27" s="124"/>
-      <c r="O27" s="124"/>
-      <c r="P27" s="124"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="122"/>
       <c r="B28" s="122"/>
       <c r="C28" s="123"/>
@@ -14305,13 +14310,8 @@
       <c r="H28" s="123"/>
       <c r="I28" s="124"/>
       <c r="J28" s="124"/>
-      <c r="L28" s="124"/>
-      <c r="M28" s="123"/>
-      <c r="N28" s="124"/>
-      <c r="O28" s="124"/>
-      <c r="P28" s="124"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="122"/>
       <c r="B29" s="122"/>
       <c r="C29" s="123"/>
@@ -14322,13 +14322,8 @@
       <c r="H29" s="123"/>
       <c r="I29" s="124"/>
       <c r="J29" s="124"/>
-      <c r="L29" s="124"/>
-      <c r="M29" s="123"/>
-      <c r="N29" s="124"/>
-      <c r="O29" s="124"/>
-      <c r="P29" s="124"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="122"/>
       <c r="B30" s="122"/>
       <c r="C30" s="123"/>
@@ -14339,13 +14334,8 @@
       <c r="H30" s="123"/>
       <c r="I30" s="124"/>
       <c r="J30" s="124"/>
-      <c r="L30" s="124"/>
-      <c r="M30" s="123"/>
-      <c r="N30" s="124"/>
-      <c r="O30" s="124"/>
-      <c r="P30" s="124"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="122"/>
       <c r="B31" s="122"/>
       <c r="C31" s="123"/>
@@ -14356,13 +14346,8 @@
       <c r="H31" s="123"/>
       <c r="I31" s="124"/>
       <c r="J31" s="124"/>
-      <c r="L31" s="124"/>
-      <c r="M31" s="123"/>
-      <c r="N31" s="124"/>
-      <c r="O31" s="124"/>
-      <c r="P31" s="124"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="122"/>
       <c r="B32" s="122"/>
       <c r="C32" s="123"/>
@@ -14373,13 +14358,8 @@
       <c r="H32" s="123"/>
       <c r="I32" s="124"/>
       <c r="J32" s="124"/>
-      <c r="L32" s="124"/>
-      <c r="M32" s="123"/>
-      <c r="N32" s="124"/>
-      <c r="O32" s="124"/>
-      <c r="P32" s="124"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="122"/>
       <c r="B33" s="122"/>
       <c r="C33" s="123"/>
@@ -14390,13 +14370,8 @@
       <c r="H33" s="123"/>
       <c r="I33" s="124"/>
       <c r="J33" s="124"/>
-      <c r="L33" s="124"/>
-      <c r="M33" s="123"/>
-      <c r="N33" s="124"/>
-      <c r="O33" s="124"/>
-      <c r="P33" s="124"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="122"/>
       <c r="B34" s="122"/>
       <c r="C34" s="123"/>
@@ -14407,13 +14382,8 @@
       <c r="H34" s="123"/>
       <c r="I34" s="124"/>
       <c r="J34" s="124"/>
-      <c r="L34" s="124"/>
-      <c r="M34" s="123"/>
-      <c r="N34" s="124"/>
-      <c r="O34" s="124"/>
-      <c r="P34" s="124"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="122"/>
       <c r="B35" s="122"/>
       <c r="C35" s="123"/>
@@ -14424,13 +14394,8 @@
       <c r="H35" s="123"/>
       <c r="I35" s="124"/>
       <c r="J35" s="124"/>
-      <c r="L35" s="124"/>
-      <c r="M35" s="123"/>
-      <c r="N35" s="124"/>
-      <c r="O35" s="124"/>
-      <c r="P35" s="124"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="122"/>
       <c r="B36" s="122"/>
       <c r="C36" s="123"/>
@@ -14441,13 +14406,8 @@
       <c r="H36" s="123"/>
       <c r="I36" s="126"/>
       <c r="J36" s="124"/>
-      <c r="L36" s="124"/>
-      <c r="M36" s="123"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="124"/>
-      <c r="P36" s="124"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="122"/>
       <c r="B37" s="122"/>
       <c r="C37" s="123"/>
@@ -14458,13 +14418,8 @@
       <c r="H37" s="123"/>
       <c r="I37" s="126"/>
       <c r="J37" s="124"/>
-      <c r="L37" s="124"/>
-      <c r="M37" s="123"/>
-      <c r="N37" s="124"/>
-      <c r="O37" s="124"/>
-      <c r="P37" s="124"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="122"/>
       <c r="B38" s="122"/>
       <c r="C38" s="123"/>
@@ -14475,13 +14430,8 @@
       <c r="H38" s="123"/>
       <c r="I38" s="126"/>
       <c r="J38" s="124"/>
-      <c r="L38" s="124"/>
-      <c r="M38" s="123"/>
-      <c r="N38" s="124"/>
-      <c r="O38" s="124"/>
-      <c r="P38" s="124"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="122"/>
       <c r="B39" s="122"/>
       <c r="C39" s="123"/>
@@ -14492,13 +14442,8 @@
       <c r="H39" s="123"/>
       <c r="I39" s="126"/>
       <c r="J39" s="124"/>
-      <c r="L39" s="124"/>
-      <c r="M39" s="123"/>
-      <c r="N39" s="124"/>
-      <c r="O39" s="124"/>
-      <c r="P39" s="124"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="122"/>
       <c r="B40" s="122"/>
       <c r="C40" s="123"/>
@@ -14509,13 +14454,8 @@
       <c r="H40" s="123"/>
       <c r="I40" s="127"/>
       <c r="J40" s="124"/>
-      <c r="L40" s="124"/>
-      <c r="M40" s="123"/>
-      <c r="N40" s="124"/>
-      <c r="O40" s="124"/>
-      <c r="P40" s="124"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="122"/>
       <c r="B41" s="122"/>
       <c r="C41" s="123"/>
@@ -14526,13 +14466,8 @@
       <c r="H41" s="123"/>
       <c r="I41" s="127"/>
       <c r="J41" s="124"/>
-      <c r="L41" s="124"/>
-      <c r="M41" s="123"/>
-      <c r="N41" s="124"/>
-      <c r="O41" s="124"/>
-      <c r="P41" s="124"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="122"/>
       <c r="B42" s="122"/>
       <c r="C42" s="124"/>
@@ -14543,13 +14478,8 @@
       <c r="H42" s="123"/>
       <c r="I42" s="127"/>
       <c r="J42" s="124"/>
-      <c r="L42" s="124"/>
-      <c r="M42" s="123"/>
-      <c r="N42" s="124"/>
-      <c r="O42" s="124"/>
-      <c r="P42" s="124"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="122"/>
       <c r="B43" s="122"/>
       <c r="C43" s="124"/>
@@ -14560,13 +14490,8 @@
       <c r="H43" s="123"/>
       <c r="I43" s="127"/>
       <c r="J43" s="124"/>
-      <c r="L43" s="124"/>
-      <c r="M43" s="123"/>
-      <c r="N43" s="124"/>
-      <c r="O43" s="124"/>
-      <c r="P43" s="124"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="122"/>
       <c r="B44" s="122"/>
       <c r="C44" s="124"/>
@@ -14577,13 +14502,8 @@
       <c r="H44" s="123"/>
       <c r="I44" s="127"/>
       <c r="J44" s="124"/>
-      <c r="L44" s="124"/>
-      <c r="M44" s="123"/>
-      <c r="N44" s="124"/>
-      <c r="O44" s="124"/>
-      <c r="P44" s="124"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="122"/>
       <c r="B45" s="122"/>
       <c r="C45" s="124"/>
@@ -14594,13 +14514,8 @@
       <c r="H45" s="123"/>
       <c r="I45" s="127"/>
       <c r="J45" s="124"/>
-      <c r="L45" s="124"/>
-      <c r="M45" s="123"/>
-      <c r="N45" s="124"/>
-      <c r="O45" s="124"/>
-      <c r="P45" s="124"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="122"/>
       <c r="B46" s="122"/>
       <c r="C46" s="123"/>
@@ -14611,13 +14526,8 @@
       <c r="H46" s="123"/>
       <c r="I46" s="126"/>
       <c r="J46" s="124"/>
-      <c r="L46" s="124"/>
-      <c r="M46" s="123"/>
-      <c r="N46" s="124"/>
-      <c r="O46" s="124"/>
-      <c r="P46" s="124"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="122"/>
       <c r="B47" s="122"/>
       <c r="C47" s="123"/>
@@ -14628,13 +14538,8 @@
       <c r="H47" s="123"/>
       <c r="I47" s="124"/>
       <c r="J47" s="124"/>
-      <c r="L47" s="124"/>
-      <c r="M47" s="123"/>
-      <c r="N47" s="124"/>
-      <c r="O47" s="124"/>
-      <c r="P47" s="124"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="122"/>
       <c r="B48" s="122"/>
       <c r="C48" s="123"/>
@@ -14645,13 +14550,8 @@
       <c r="H48" s="123"/>
       <c r="I48" s="124"/>
       <c r="J48" s="124"/>
-      <c r="L48" s="124"/>
-      <c r="M48" s="123"/>
-      <c r="N48" s="124"/>
-      <c r="O48" s="124"/>
-      <c r="P48" s="124"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="122"/>
       <c r="B49" s="122"/>
       <c r="C49" s="124"/>
@@ -14662,13 +14562,8 @@
       <c r="H49" s="123"/>
       <c r="I49" s="124"/>
       <c r="J49" s="124"/>
-      <c r="L49" s="124"/>
-      <c r="M49" s="123"/>
-      <c r="N49" s="124"/>
-      <c r="O49" s="124"/>
-      <c r="P49" s="124"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="122"/>
       <c r="B50" s="122"/>
       <c r="C50" s="123"/>
@@ -14679,13 +14574,8 @@
       <c r="H50" s="123"/>
       <c r="I50" s="124"/>
       <c r="J50" s="124"/>
-      <c r="L50" s="124"/>
-      <c r="M50" s="123"/>
-      <c r="N50" s="124"/>
-      <c r="O50" s="124"/>
-      <c r="P50" s="124"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="122"/>
       <c r="B51" s="122"/>
       <c r="C51" s="123"/>
@@ -14696,13 +14586,8 @@
       <c r="H51" s="123"/>
       <c r="I51" s="124"/>
       <c r="J51" s="122"/>
-      <c r="L51" s="124"/>
-      <c r="M51" s="123"/>
-      <c r="N51" s="124"/>
-      <c r="O51" s="124"/>
-      <c r="P51" s="124"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="122"/>
       <c r="B52" s="122"/>
       <c r="C52" s="123"/>
@@ -14713,13 +14598,8 @@
       <c r="H52" s="123"/>
       <c r="I52" s="124"/>
       <c r="J52" s="122"/>
-      <c r="L52" s="124"/>
-      <c r="M52" s="123"/>
-      <c r="N52" s="124"/>
-      <c r="O52" s="124"/>
-      <c r="P52" s="124"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="122"/>
       <c r="B53" s="122"/>
       <c r="C53" s="122"/>
@@ -14730,13 +14610,8 @@
       <c r="H53" s="123"/>
       <c r="I53" s="124"/>
       <c r="J53" s="122"/>
-      <c r="L53" s="124"/>
-      <c r="M53" s="122"/>
-      <c r="N53" s="122"/>
-      <c r="O53" s="122"/>
-      <c r="P53" s="122"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="122"/>
       <c r="B54" s="122"/>
       <c r="C54" s="122"/>
@@ -14747,13 +14622,8 @@
       <c r="H54" s="123"/>
       <c r="I54" s="124"/>
       <c r="J54" s="122"/>
-      <c r="L54" s="124"/>
-      <c r="M54" s="122"/>
-      <c r="N54" s="122"/>
-      <c r="O54" s="122"/>
-      <c r="P54" s="122"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="122"/>
       <c r="B55" s="122"/>
       <c r="C55" s="122"/>
@@ -14764,13 +14634,8 @@
       <c r="H55" s="123"/>
       <c r="I55" s="124"/>
       <c r="J55" s="122"/>
-      <c r="L55" s="124"/>
-      <c r="M55" s="122"/>
-      <c r="N55" s="124"/>
-      <c r="O55" s="124"/>
-      <c r="P55" s="124"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="122"/>
       <c r="B56" s="122"/>
       <c r="C56" s="123"/>
@@ -14781,13 +14646,8 @@
       <c r="H56" s="123"/>
       <c r="I56" s="124"/>
       <c r="J56" s="124"/>
-      <c r="L56" s="124"/>
-      <c r="M56" s="123"/>
-      <c r="N56" s="124"/>
-      <c r="O56" s="124"/>
-      <c r="P56" s="124"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="122"/>
       <c r="B57" s="122"/>
       <c r="C57" s="123"/>
@@ -14798,13 +14658,8 @@
       <c r="H57" s="123"/>
       <c r="I57" s="124"/>
       <c r="J57" s="124"/>
-      <c r="L57" s="124"/>
-      <c r="M57" s="123"/>
-      <c r="N57" s="124"/>
-      <c r="O57" s="124"/>
-      <c r="P57" s="124"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="122"/>
       <c r="B58" s="122"/>
       <c r="C58" s="123"/>
@@ -14815,13 +14670,8 @@
       <c r="H58" s="123"/>
       <c r="I58" s="124"/>
       <c r="J58" s="124"/>
-      <c r="L58" s="124"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="124"/>
-      <c r="O58" s="124"/>
-      <c r="P58" s="124"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="122"/>
       <c r="B59" s="122"/>
       <c r="C59" s="123"/>
@@ -14832,13 +14682,8 @@
       <c r="H59" s="123"/>
       <c r="I59" s="124"/>
       <c r="J59" s="124"/>
-      <c r="L59" s="124"/>
-      <c r="M59" s="123"/>
-      <c r="N59" s="124"/>
-      <c r="O59" s="124"/>
-      <c r="P59" s="124"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="122"/>
       <c r="B60" s="122"/>
       <c r="C60" s="123"/>
@@ -14849,13 +14694,8 @@
       <c r="H60" s="123"/>
       <c r="I60" s="124"/>
       <c r="J60" s="124"/>
-      <c r="L60" s="124"/>
-      <c r="M60" s="123"/>
-      <c r="N60" s="124"/>
-      <c r="O60" s="124"/>
-      <c r="P60" s="124"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="122"/>
       <c r="B61" s="122"/>
       <c r="C61" s="123"/>
@@ -14866,13 +14706,8 @@
       <c r="H61" s="123"/>
       <c r="I61" s="124"/>
       <c r="J61" s="124"/>
-      <c r="L61" s="124"/>
-      <c r="M61" s="123"/>
-      <c r="N61" s="124"/>
-      <c r="O61" s="124"/>
-      <c r="P61" s="124"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A62" s="122"/>
       <c r="B62" s="122"/>
       <c r="C62" s="123"/>
@@ -14882,13 +14717,8 @@
       <c r="G62" s="123"/>
       <c r="H62" s="123"/>
       <c r="J62" s="124"/>
-      <c r="L62" s="124"/>
-      <c r="M62" s="123"/>
-      <c r="N62" s="124"/>
-      <c r="O62" s="124"/>
-      <c r="P62" s="124"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="122"/>
       <c r="B63" s="122"/>
       <c r="C63" s="123"/>
@@ -14898,13 +14728,8 @@
       <c r="G63" s="124"/>
       <c r="H63" s="123"/>
       <c r="J63" s="124"/>
-      <c r="L63" s="124"/>
-      <c r="M63" s="123"/>
-      <c r="N63" s="124"/>
-      <c r="O63" s="124"/>
-      <c r="P63" s="124"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="122"/>
       <c r="B64" s="122"/>
       <c r="C64" s="123"/>
@@ -14914,13 +14739,8 @@
       <c r="G64" s="124"/>
       <c r="H64" s="123"/>
       <c r="J64" s="124"/>
-      <c r="L64" s="124"/>
-      <c r="M64" s="123"/>
-      <c r="N64" s="124"/>
-      <c r="O64" s="124"/>
-      <c r="P64" s="124"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="122"/>
       <c r="B65" s="122"/>
       <c r="C65" s="123"/>
@@ -14930,13 +14750,8 @@
       <c r="G65" s="124"/>
       <c r="H65" s="123"/>
       <c r="J65" s="124"/>
-      <c r="L65" s="124"/>
-      <c r="M65" s="123"/>
-      <c r="N65" s="124"/>
-      <c r="O65" s="124"/>
-      <c r="P65" s="124"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="122"/>
       <c r="B66" s="122"/>
       <c r="C66" s="123"/>
@@ -14946,13 +14761,8 @@
       <c r="G66" s="124"/>
       <c r="H66" s="123"/>
       <c r="J66" s="124"/>
-      <c r="L66" s="124"/>
-      <c r="M66" s="123"/>
-      <c r="N66" s="124"/>
-      <c r="O66" s="124"/>
-      <c r="P66" s="124"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="122"/>
       <c r="B67" s="122"/>
       <c r="C67" s="124"/>
@@ -14962,13 +14772,8 @@
       <c r="G67" s="124"/>
       <c r="H67" s="123"/>
       <c r="J67" s="124"/>
-      <c r="L67" s="124"/>
-      <c r="M67" s="124"/>
-      <c r="N67" s="124"/>
-      <c r="O67" s="124"/>
-      <c r="P67" s="124"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A68" s="122"/>
       <c r="B68" s="122"/>
       <c r="C68" s="124"/>
@@ -14978,13 +14783,8 @@
       <c r="G68" s="124"/>
       <c r="H68" s="123"/>
       <c r="J68" s="124"/>
-      <c r="L68" s="124"/>
-      <c r="M68" s="124"/>
-      <c r="N68" s="124"/>
-      <c r="O68" s="124"/>
-      <c r="P68" s="124"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="122"/>
       <c r="B69" s="122"/>
       <c r="C69" s="124"/>
@@ -14994,13 +14794,8 @@
       <c r="G69" s="124"/>
       <c r="H69" s="123"/>
       <c r="J69" s="124"/>
-      <c r="L69" s="124"/>
-      <c r="M69" s="124"/>
-      <c r="N69" s="124"/>
-      <c r="O69" s="124"/>
-      <c r="P69" s="124"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="122"/>
       <c r="B70" s="122"/>
       <c r="C70" s="124"/>
@@ -15010,13 +14805,8 @@
       <c r="G70" s="124"/>
       <c r="H70" s="123"/>
       <c r="J70" s="124"/>
-      <c r="L70" s="124"/>
-      <c r="M70" s="124"/>
-      <c r="N70" s="124"/>
-      <c r="O70" s="124"/>
-      <c r="P70" s="124"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="122"/>
       <c r="B71" s="122"/>
       <c r="C71" s="123"/>
@@ -15026,13 +14816,8 @@
       <c r="G71" s="124"/>
       <c r="H71" s="123"/>
       <c r="J71" s="124"/>
-      <c r="L71" s="124"/>
-      <c r="M71" s="124"/>
-      <c r="N71" s="124"/>
-      <c r="O71" s="124"/>
-      <c r="P71" s="124"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="122"/>
       <c r="B72" s="122"/>
       <c r="C72" s="123"/>
@@ -15042,13 +14827,8 @@
       <c r="G72" s="124"/>
       <c r="H72" s="123"/>
       <c r="J72" s="124"/>
-      <c r="L72" s="124"/>
-      <c r="M72" s="124"/>
-      <c r="N72" s="124"/>
-      <c r="O72" s="124"/>
-      <c r="P72" s="124"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="122"/>
       <c r="B73" s="122"/>
       <c r="C73" s="123"/>
@@ -15058,13 +14838,8 @@
       <c r="G73" s="124"/>
       <c r="H73" s="123"/>
       <c r="J73" s="124"/>
-      <c r="L73" s="124"/>
-      <c r="M73" s="124"/>
-      <c r="N73" s="124"/>
-      <c r="O73" s="124"/>
-      <c r="P73" s="124"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="122"/>
       <c r="B74" s="122"/>
       <c r="C74" s="123"/>
@@ -15074,13 +14849,8 @@
       <c r="G74" s="124"/>
       <c r="H74" s="123"/>
       <c r="J74" s="124"/>
-      <c r="L74" s="124"/>
-      <c r="M74" s="124"/>
-      <c r="N74" s="124"/>
-      <c r="O74" s="124"/>
-      <c r="P74" s="124"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" s="122"/>
       <c r="B75" s="122"/>
       <c r="C75" s="123"/>
@@ -15090,13 +14860,8 @@
       <c r="G75" s="124"/>
       <c r="H75" s="123"/>
       <c r="J75" s="124"/>
-      <c r="L75" s="124"/>
-      <c r="M75" s="124"/>
-      <c r="N75" s="124"/>
-      <c r="O75" s="124"/>
-      <c r="P75" s="124"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="122"/>
       <c r="B76" s="122"/>
       <c r="C76" s="123"/>
@@ -15106,13 +14871,8 @@
       <c r="G76" s="124"/>
       <c r="H76" s="123"/>
       <c r="J76" s="124"/>
-      <c r="L76" s="124"/>
-      <c r="M76" s="124"/>
-      <c r="N76" s="124"/>
-      <c r="O76" s="124"/>
-      <c r="P76" s="124"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A77" s="122"/>
       <c r="B77" s="122"/>
       <c r="C77" s="123"/>
@@ -15122,13 +14882,8 @@
       <c r="G77" s="124"/>
       <c r="H77" s="123"/>
       <c r="J77" s="124"/>
-      <c r="L77" s="124"/>
-      <c r="M77" s="123"/>
-      <c r="N77" s="124"/>
-      <c r="O77" s="123"/>
-      <c r="P77" s="123"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="122"/>
       <c r="B78" s="122"/>
       <c r="C78" s="123"/>
@@ -15138,13 +14893,8 @@
       <c r="G78" s="124"/>
       <c r="H78" s="123"/>
       <c r="J78" s="124"/>
-      <c r="L78" s="124"/>
-      <c r="M78" s="123"/>
-      <c r="N78" s="124"/>
-      <c r="O78" s="123"/>
-      <c r="P78" s="123"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A79" s="122"/>
       <c r="B79" s="122"/>
       <c r="C79" s="123"/>
@@ -15154,13 +14904,8 @@
       <c r="G79" s="124"/>
       <c r="H79" s="123"/>
       <c r="J79" s="124"/>
-      <c r="L79" s="124"/>
-      <c r="M79" s="123"/>
-      <c r="N79" s="124"/>
-      <c r="O79" s="124"/>
-      <c r="P79" s="124"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A80" s="122"/>
       <c r="B80" s="122"/>
       <c r="C80" s="123"/>
@@ -15170,13 +14915,8 @@
       <c r="G80" s="124"/>
       <c r="H80" s="123"/>
       <c r="J80" s="124"/>
-      <c r="L80" s="124"/>
-      <c r="M80" s="123"/>
-      <c r="N80" s="124"/>
-      <c r="O80" s="124"/>
-      <c r="P80" s="124"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A81" s="122"/>
       <c r="B81" s="122"/>
       <c r="C81" s="123"/>
@@ -15186,13 +14926,8 @@
       <c r="G81" s="124"/>
       <c r="H81" s="123"/>
       <c r="J81" s="124"/>
-      <c r="L81" s="124"/>
-      <c r="M81" s="123"/>
-      <c r="N81" s="124"/>
-      <c r="O81" s="124"/>
-      <c r="P81" s="124"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A82" s="122"/>
       <c r="B82" s="122"/>
       <c r="C82" s="123"/>
@@ -15202,13 +14937,8 @@
       <c r="G82" s="124"/>
       <c r="H82" s="123"/>
       <c r="J82" s="124"/>
-      <c r="L82" s="124"/>
-      <c r="M82" s="123"/>
-      <c r="N82" s="124"/>
-      <c r="O82" s="124"/>
-      <c r="P82" s="124"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A83" s="122"/>
       <c r="B83" s="122"/>
       <c r="C83" s="123"/>
@@ -15218,13 +14948,8 @@
       <c r="G83" s="124"/>
       <c r="H83" s="123"/>
       <c r="J83" s="124"/>
-      <c r="L83" s="124"/>
-      <c r="M83" s="123"/>
-      <c r="N83" s="124"/>
-      <c r="O83" s="124"/>
-      <c r="P83" s="124"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A84" s="122"/>
       <c r="B84" s="122"/>
       <c r="C84" s="123"/>
@@ -15234,13 +14959,8 @@
       <c r="G84" s="124"/>
       <c r="H84" s="123"/>
       <c r="J84" s="124"/>
-      <c r="L84" s="124"/>
-      <c r="M84" s="123"/>
-      <c r="N84" s="124"/>
-      <c r="O84" s="124"/>
-      <c r="P84" s="124"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A85" s="122"/>
       <c r="B85" s="122"/>
       <c r="C85" s="123"/>
@@ -15250,13 +14970,8 @@
       <c r="G85" s="124"/>
       <c r="H85" s="123"/>
       <c r="J85" s="124"/>
-      <c r="L85" s="124"/>
-      <c r="M85" s="123"/>
-      <c r="N85" s="124"/>
-      <c r="O85" s="124"/>
-      <c r="P85" s="124"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A86" s="122"/>
       <c r="B86" s="122"/>
       <c r="C86" s="123"/>
@@ -15266,13 +14981,8 @@
       <c r="G86" s="124"/>
       <c r="H86" s="123"/>
       <c r="J86" s="124"/>
-      <c r="L86" s="124"/>
-      <c r="M86" s="123"/>
-      <c r="N86" s="124"/>
-      <c r="O86" s="124"/>
-      <c r="P86" s="124"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A87" s="122"/>
       <c r="B87" s="122"/>
       <c r="C87" s="123"/>
@@ -15282,13 +14992,8 @@
       <c r="G87" s="124"/>
       <c r="H87" s="123"/>
       <c r="J87" s="124"/>
-      <c r="L87" s="124"/>
-      <c r="M87" s="123"/>
-      <c r="N87" s="124"/>
-      <c r="O87" s="124"/>
-      <c r="P87" s="124"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A88" s="122"/>
       <c r="B88" s="122"/>
       <c r="C88" s="123"/>
@@ -15298,13 +15003,8 @@
       <c r="G88" s="124"/>
       <c r="H88" s="123"/>
       <c r="J88" s="124"/>
-      <c r="L88" s="124"/>
-      <c r="M88" s="123"/>
-      <c r="N88" s="124"/>
-      <c r="O88" s="124"/>
-      <c r="P88" s="124"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A89" s="122"/>
       <c r="B89" s="122"/>
       <c r="C89" s="123"/>
@@ -15314,13 +15014,8 @@
       <c r="G89" s="122"/>
       <c r="H89" s="123"/>
       <c r="J89" s="122"/>
-      <c r="L89" s="124"/>
-      <c r="M89" s="123"/>
-      <c r="N89" s="124"/>
-      <c r="O89" s="124"/>
-      <c r="P89" s="124"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A90" s="122"/>
       <c r="B90" s="122"/>
       <c r="C90" s="123"/>
@@ -15330,13 +15025,8 @@
       <c r="G90" s="122"/>
       <c r="H90" s="123"/>
       <c r="J90" s="122"/>
-      <c r="L90" s="124"/>
-      <c r="M90" s="123"/>
-      <c r="N90" s="124"/>
-      <c r="O90" s="124"/>
-      <c r="P90" s="124"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A91" s="122"/>
       <c r="B91" s="122"/>
       <c r="C91" s="123"/>
@@ -15346,13 +15036,8 @@
       <c r="G91" s="124"/>
       <c r="H91" s="123"/>
       <c r="J91" s="124"/>
-      <c r="L91" s="124"/>
-      <c r="M91" s="123"/>
-      <c r="N91" s="124"/>
-      <c r="O91" s="124"/>
-      <c r="P91" s="124"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A92" s="122"/>
       <c r="B92" s="122"/>
       <c r="C92" s="123"/>
@@ -15362,13 +15047,8 @@
       <c r="G92" s="124"/>
       <c r="H92" s="123"/>
       <c r="J92" s="124"/>
-      <c r="L92" s="124"/>
-      <c r="M92" s="123"/>
-      <c r="N92" s="124"/>
-      <c r="O92" s="124"/>
-      <c r="P92" s="124"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A93" s="122"/>
       <c r="B93" s="122"/>
       <c r="C93" s="123"/>
@@ -15378,13 +15058,8 @@
       <c r="G93" s="124"/>
       <c r="H93" s="123"/>
       <c r="J93" s="124"/>
-      <c r="L93" s="124"/>
-      <c r="M93" s="123"/>
-      <c r="N93" s="124"/>
-      <c r="O93" s="124"/>
-      <c r="P93" s="124"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A94" s="122"/>
       <c r="B94" s="122"/>
       <c r="C94" s="123"/>
@@ -15394,13 +15069,8 @@
       <c r="G94" s="124"/>
       <c r="H94" s="123"/>
       <c r="J94" s="124"/>
-      <c r="L94" s="124"/>
-      <c r="M94" s="123"/>
-      <c r="N94" s="124"/>
-      <c r="O94" s="124"/>
-      <c r="P94" s="124"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A95" s="122"/>
       <c r="B95" s="122"/>
       <c r="C95" s="123"/>
@@ -15410,13 +15080,8 @@
       <c r="G95" s="124"/>
       <c r="H95" s="123"/>
       <c r="J95" s="124"/>
-      <c r="L95" s="124"/>
-      <c r="M95" s="123"/>
-      <c r="N95" s="124"/>
-      <c r="O95" s="124"/>
-      <c r="P95" s="124"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A96" s="122"/>
       <c r="B96" s="122"/>
       <c r="C96" s="123"/>
@@ -15426,13 +15091,8 @@
       <c r="G96" s="124"/>
       <c r="H96" s="123"/>
       <c r="J96" s="124"/>
-      <c r="L96" s="124"/>
-      <c r="M96" s="123"/>
-      <c r="N96" s="124"/>
-      <c r="O96" s="124"/>
-      <c r="P96" s="124"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A97" s="122"/>
       <c r="B97" s="122"/>
       <c r="C97" s="123"/>
@@ -15442,13 +15102,8 @@
       <c r="G97" s="124"/>
       <c r="H97" s="123"/>
       <c r="J97" s="124"/>
-      <c r="L97" s="124"/>
-      <c r="M97" s="123"/>
-      <c r="N97" s="124"/>
-      <c r="O97" s="124"/>
-      <c r="P97" s="124"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A98" s="122"/>
       <c r="B98" s="122"/>
       <c r="C98" s="123"/>
@@ -15458,13 +15113,8 @@
       <c r="G98" s="124"/>
       <c r="H98" s="123"/>
       <c r="J98" s="124"/>
-      <c r="L98" s="124"/>
-      <c r="M98" s="123"/>
-      <c r="N98" s="124"/>
-      <c r="O98" s="124"/>
-      <c r="P98" s="124"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A99" s="122"/>
       <c r="B99" s="122"/>
       <c r="C99" s="123"/>
@@ -15474,13 +15124,8 @@
       <c r="G99" s="124"/>
       <c r="H99" s="123"/>
       <c r="J99" s="124"/>
-      <c r="L99" s="124"/>
-      <c r="M99" s="123"/>
-      <c r="N99" s="124"/>
-      <c r="O99" s="124"/>
-      <c r="P99" s="124"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A100" s="122"/>
       <c r="B100" s="122"/>
       <c r="C100" s="123"/>
@@ -15490,13 +15135,8 @@
       <c r="G100" s="124"/>
       <c r="H100" s="123"/>
       <c r="J100" s="124"/>
-      <c r="L100" s="124"/>
-      <c r="M100" s="123"/>
-      <c r="N100" s="124"/>
-      <c r="O100" s="124"/>
-      <c r="P100" s="124"/>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A101" s="122"/>
       <c r="B101" s="122"/>
       <c r="C101" s="123"/>
@@ -15506,13 +15146,8 @@
       <c r="G101" s="124"/>
       <c r="H101" s="123"/>
       <c r="J101" s="124"/>
-      <c r="L101" s="124"/>
-      <c r="M101" s="123"/>
-      <c r="N101" s="124"/>
-      <c r="O101" s="124"/>
-      <c r="P101" s="124"/>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="122"/>
       <c r="B102" s="122"/>
       <c r="C102" s="123"/>
@@ -15522,13 +15157,8 @@
       <c r="G102" s="124"/>
       <c r="H102" s="123"/>
       <c r="J102" s="124"/>
-      <c r="L102" s="124"/>
-      <c r="M102" s="123"/>
-      <c r="N102" s="124"/>
-      <c r="O102" s="124"/>
-      <c r="P102" s="124"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="122"/>
       <c r="B103" s="122"/>
       <c r="C103" s="123"/>
@@ -15538,13 +15168,8 @@
       <c r="G103" s="124"/>
       <c r="H103" s="123"/>
       <c r="J103" s="124"/>
-      <c r="L103" s="124"/>
-      <c r="M103" s="123"/>
-      <c r="N103" s="124"/>
-      <c r="O103" s="124"/>
-      <c r="P103" s="124"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A104" s="122"/>
       <c r="B104" s="122"/>
       <c r="C104" s="123"/>
@@ -15554,13 +15179,8 @@
       <c r="G104" s="124"/>
       <c r="H104" s="123"/>
       <c r="J104" s="124"/>
-      <c r="L104" s="124"/>
-      <c r="M104" s="123"/>
-      <c r="N104" s="124"/>
-      <c r="O104" s="124"/>
-      <c r="P104" s="124"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A105" s="122"/>
       <c r="B105" s="122"/>
       <c r="C105" s="123"/>
@@ -15570,13 +15190,8 @@
       <c r="G105" s="124"/>
       <c r="H105" s="123"/>
       <c r="J105" s="124"/>
-      <c r="L105" s="124"/>
-      <c r="M105" s="123"/>
-      <c r="N105" s="124"/>
-      <c r="O105" s="124"/>
-      <c r="P105" s="124"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="122"/>
       <c r="B106" s="122"/>
       <c r="C106" s="123"/>
@@ -15586,13 +15201,8 @@
       <c r="G106" s="124"/>
       <c r="H106" s="123"/>
       <c r="J106" s="124"/>
-      <c r="L106" s="124"/>
-      <c r="M106" s="123"/>
-      <c r="N106" s="124"/>
-      <c r="O106" s="124"/>
-      <c r="P106" s="124"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="122"/>
       <c r="B107" s="122"/>
       <c r="C107" s="123"/>
@@ -15602,13 +15212,8 @@
       <c r="G107" s="124"/>
       <c r="H107" s="123"/>
       <c r="J107" s="124"/>
-      <c r="L107" s="124"/>
-      <c r="M107" s="123"/>
-      <c r="N107" s="124"/>
-      <c r="O107" s="124"/>
-      <c r="P107" s="124"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A108" s="129"/>
       <c r="B108" s="130"/>
       <c r="C108" s="131"/>
@@ -15618,13 +15223,8 @@
       <c r="G108" s="125"/>
       <c r="H108" s="131"/>
       <c r="J108" s="125"/>
-      <c r="L108" s="124"/>
-      <c r="M108" s="131"/>
-      <c r="N108" s="125"/>
-      <c r="O108" s="125"/>
-      <c r="P108" s="124"/>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A109" s="129"/>
       <c r="B109" s="130"/>
       <c r="C109" s="131"/>
@@ -15634,13 +15234,8 @@
       <c r="G109" s="125"/>
       <c r="H109" s="131"/>
       <c r="J109" s="125"/>
-      <c r="L109" s="124"/>
-      <c r="M109" s="131"/>
-      <c r="N109" s="125"/>
-      <c r="O109" s="125"/>
-      <c r="P109" s="124"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A110" s="129"/>
       <c r="B110" s="130"/>
       <c r="C110" s="131"/>
@@ -15650,13 +15245,8 @@
       <c r="G110" s="125"/>
       <c r="H110" s="131"/>
       <c r="J110" s="125"/>
-      <c r="L110" s="124"/>
-      <c r="M110" s="131"/>
-      <c r="N110" s="125"/>
-      <c r="O110" s="125"/>
-      <c r="P110" s="124"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A111" s="129"/>
       <c r="B111" s="130"/>
       <c r="C111" s="131"/>
@@ -15666,13 +15256,8 @@
       <c r="G111" s="125"/>
       <c r="H111" s="131"/>
       <c r="J111" s="125"/>
-      <c r="L111" s="124"/>
-      <c r="M111" s="131"/>
-      <c r="N111" s="125"/>
-      <c r="O111" s="125"/>
-      <c r="P111" s="124"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A112" s="129"/>
       <c r="B112" s="130"/>
       <c r="C112" s="131"/>
@@ -15682,13 +15267,8 @@
       <c r="G112" s="125"/>
       <c r="H112" s="131"/>
       <c r="J112" s="125"/>
-      <c r="L112" s="124"/>
-      <c r="M112" s="131"/>
-      <c r="N112" s="125"/>
-      <c r="O112" s="125"/>
-      <c r="P112" s="124"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A113" s="129"/>
       <c r="B113" s="130"/>
       <c r="C113" s="131"/>
@@ -15698,13 +15278,8 @@
       <c r="G113" s="125"/>
       <c r="H113" s="131"/>
       <c r="J113" s="125"/>
-      <c r="L113" s="124"/>
-      <c r="M113" s="131"/>
-      <c r="N113" s="125"/>
-      <c r="O113" s="125"/>
-      <c r="P113" s="124"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A114" s="129"/>
       <c r="B114" s="130"/>
       <c r="C114" s="131"/>
@@ -15714,13 +15289,8 @@
       <c r="G114" s="125"/>
       <c r="H114" s="131"/>
       <c r="J114" s="125"/>
-      <c r="L114" s="124"/>
-      <c r="M114" s="131"/>
-      <c r="N114" s="125"/>
-      <c r="O114" s="125"/>
-      <c r="P114" s="124"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A115" s="129"/>
       <c r="B115" s="130"/>
       <c r="C115" s="131"/>
@@ -15730,13 +15300,8 @@
       <c r="G115" s="125"/>
       <c r="H115" s="131"/>
       <c r="J115" s="125"/>
-      <c r="L115" s="124"/>
-      <c r="M115" s="131"/>
-      <c r="N115" s="125"/>
-      <c r="O115" s="125"/>
-      <c r="P115" s="124"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="129"/>
       <c r="B116" s="130"/>
       <c r="C116" s="131"/>
@@ -15746,13 +15311,8 @@
       <c r="G116" s="125"/>
       <c r="H116" s="131"/>
       <c r="J116" s="125"/>
-      <c r="L116" s="124"/>
-      <c r="M116" s="131"/>
-      <c r="N116" s="125"/>
-      <c r="O116" s="125"/>
-      <c r="P116" s="124"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A117" s="122"/>
       <c r="B117" s="122"/>
       <c r="C117" s="123"/>
@@ -15762,13 +15322,8 @@
       <c r="G117" s="124"/>
       <c r="H117" s="123"/>
       <c r="J117" s="124"/>
-      <c r="L117" s="124"/>
-      <c r="M117" s="123"/>
-      <c r="N117" s="124"/>
-      <c r="O117" s="124"/>
-      <c r="P117" s="124"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A118" s="122"/>
       <c r="B118" s="122"/>
       <c r="C118" s="123"/>
@@ -15778,13 +15333,8 @@
       <c r="G118" s="124"/>
       <c r="H118" s="123"/>
       <c r="J118" s="124"/>
-      <c r="L118" s="124"/>
-      <c r="M118" s="123"/>
-      <c r="N118" s="124"/>
-      <c r="O118" s="124"/>
-      <c r="P118" s="124"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A119" s="122"/>
       <c r="B119" s="122"/>
       <c r="C119" s="123"/>
@@ -15794,13 +15344,8 @@
       <c r="G119" s="124"/>
       <c r="H119" s="123"/>
       <c r="J119" s="124"/>
-      <c r="L119" s="124"/>
-      <c r="M119" s="123"/>
-      <c r="N119" s="124"/>
-      <c r="O119" s="124"/>
-      <c r="P119" s="124"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A120" s="122"/>
       <c r="B120" s="122"/>
       <c r="C120" s="123"/>
@@ -15810,13 +15355,8 @@
       <c r="G120" s="124"/>
       <c r="H120" s="123"/>
       <c r="J120" s="124"/>
-      <c r="L120" s="124"/>
-      <c r="M120" s="123"/>
-      <c r="N120" s="124"/>
-      <c r="O120" s="124"/>
-      <c r="P120" s="124"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A121" s="122"/>
       <c r="B121" s="122"/>
       <c r="C121" s="123"/>
@@ -15826,13 +15366,8 @@
       <c r="G121" s="124"/>
       <c r="H121" s="123"/>
       <c r="J121" s="124"/>
-      <c r="L121" s="124"/>
-      <c r="M121" s="123"/>
-      <c r="N121" s="124"/>
-      <c r="O121" s="124"/>
-      <c r="P121" s="124"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A122" s="122"/>
       <c r="B122" s="122"/>
       <c r="C122" s="123"/>
@@ -15842,13 +15377,8 @@
       <c r="G122" s="124"/>
       <c r="H122" s="123"/>
       <c r="J122" s="124"/>
-      <c r="L122" s="124"/>
-      <c r="M122" s="123"/>
-      <c r="N122" s="124"/>
-      <c r="O122" s="124"/>
-      <c r="P122" s="124"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A123" s="122"/>
       <c r="B123" s="122"/>
       <c r="C123" s="123"/>
@@ -15858,13 +15388,8 @@
       <c r="G123" s="124"/>
       <c r="H123" s="123"/>
       <c r="J123" s="124"/>
-      <c r="L123" s="124"/>
-      <c r="M123" s="123"/>
-      <c r="N123" s="124"/>
-      <c r="O123" s="124"/>
-      <c r="P123" s="124"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A124" s="122"/>
       <c r="B124" s="122"/>
       <c r="C124" s="123"/>
@@ -15874,13 +15399,8 @@
       <c r="G124" s="124"/>
       <c r="H124" s="123"/>
       <c r="J124" s="124"/>
-      <c r="L124" s="124"/>
-      <c r="M124" s="123"/>
-      <c r="N124" s="124"/>
-      <c r="O124" s="124"/>
-      <c r="P124" s="124"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A125" s="122"/>
       <c r="B125" s="122"/>
       <c r="C125" s="123"/>
@@ -15890,13 +15410,8 @@
       <c r="G125" s="124"/>
       <c r="H125" s="123"/>
       <c r="J125" s="124"/>
-      <c r="L125" s="124"/>
-      <c r="M125" s="123"/>
-      <c r="N125" s="124"/>
-      <c r="O125" s="124"/>
-      <c r="P125" s="124"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A126" s="122"/>
       <c r="B126" s="122"/>
       <c r="C126" s="123"/>
@@ -15906,13 +15421,8 @@
       <c r="G126" s="124"/>
       <c r="H126" s="123"/>
       <c r="J126" s="124"/>
-      <c r="L126" s="124"/>
-      <c r="M126" s="123"/>
-      <c r="N126" s="124"/>
-      <c r="O126" s="124"/>
-      <c r="P126" s="124"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A127" s="122"/>
       <c r="B127" s="122"/>
       <c r="C127" s="123"/>
@@ -15922,13 +15432,8 @@
       <c r="G127" s="124"/>
       <c r="H127" s="123"/>
       <c r="J127" s="124"/>
-      <c r="L127" s="124"/>
-      <c r="M127" s="123"/>
-      <c r="N127" s="124"/>
-      <c r="O127" s="124"/>
-      <c r="P127" s="124"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="122"/>
       <c r="B128" s="122"/>
       <c r="C128" s="123"/>
@@ -15938,11 +15443,6 @@
       <c r="G128" s="124"/>
       <c r="H128" s="123"/>
       <c r="J128" s="124"/>
-      <c r="L128" s="124"/>
-      <c r="M128" s="123"/>
-      <c r="N128" s="124"/>
-      <c r="O128" s="124"/>
-      <c r="P128" s="124"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15952,6 +15452,1638 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC0AB9D-7434-8140-878B-BA2062BCF21F}">
+  <dimension ref="A1:J128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="134" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="135"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+    </row>
+    <row r="2" spans="1:10" ht="98" x14ac:dyDescent="0.15">
+      <c r="A2" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="117" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="117" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="117" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" s="117" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="118" t="s">
+        <v>311</v>
+      </c>
+      <c r="G2" s="118" t="s">
+        <v>350</v>
+      </c>
+      <c r="H2" s="117" t="s">
+        <v>351</v>
+      </c>
+      <c r="I2" s="91" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2" s="91" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="138" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="138" t="s">
+        <v>313</v>
+      </c>
+      <c r="E3" s="138" t="s">
+        <v>314</v>
+      </c>
+      <c r="F3" s="139" t="s">
+        <v>318</v>
+      </c>
+      <c r="G3" s="138" t="s">
+        <v>319</v>
+      </c>
+      <c r="H3" s="138" t="s">
+        <v>320</v>
+      </c>
+      <c r="I3" s="138" t="s">
+        <v>321</v>
+      </c>
+      <c r="J3" s="138" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="140" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141" t="s">
+        <v>349</v>
+      </c>
+      <c r="D4" s="141" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="141" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" s="141" t="s">
+        <v>326</v>
+      </c>
+      <c r="G4" s="141" t="s">
+        <v>326</v>
+      </c>
+      <c r="H4" s="142" t="s">
+        <v>326</v>
+      </c>
+      <c r="I4" s="142" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" s="142" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="143" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="143"/>
+      <c r="C5" s="144" t="s">
+        <v>349</v>
+      </c>
+      <c r="D5" s="144" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="144" t="s">
+        <v>324</v>
+      </c>
+      <c r="F5" s="145" t="s">
+        <v>326</v>
+      </c>
+      <c r="G5" s="144"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="140"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="141"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
+      <c r="J6" s="142"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="143"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="140"/>
+      <c r="B8" s="140"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="142"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="143"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="144"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="140"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="141"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="141"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="143"/>
+      <c r="B11" s="143"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="144"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="140"/>
+      <c r="B12" s="140"/>
+      <c r="C12" s="141"/>
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="142"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="142"/>
+      <c r="I12" s="142"/>
+      <c r="J12" s="142"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="143"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="145"/>
+      <c r="I13" s="145"/>
+      <c r="J13" s="145"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="140"/>
+      <c r="B14" s="140"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="142"/>
+      <c r="I14" s="142"/>
+      <c r="J14" s="142"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="143"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="140"/>
+      <c r="B16" s="140"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="142"/>
+      <c r="I16" s="142"/>
+      <c r="J16" s="142"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="143"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="140"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="142"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A19" s="143"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="144"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="145"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" s="140"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="142"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="142"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="142"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="143"/>
+      <c r="B21" s="143"/>
+      <c r="C21" s="144"/>
+      <c r="D21" s="144"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="145"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="145"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="145"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="140"/>
+      <c r="B22" s="140"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="142"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="142"/>
+      <c r="I22" s="142"/>
+      <c r="J22" s="142"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="143"/>
+      <c r="B23" s="143"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="145"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="140"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="141"/>
+      <c r="E24" s="141"/>
+      <c r="F24" s="142"/>
+      <c r="G24" s="141"/>
+      <c r="H24" s="142"/>
+      <c r="I24" s="142"/>
+      <c r="J24" s="142"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="143"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="140"/>
+      <c r="B26" s="140"/>
+      <c r="C26" s="141"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="142"/>
+      <c r="I26" s="142"/>
+      <c r="J26" s="142"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="143"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="144"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="144"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="144"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" s="140"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="142"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" s="143"/>
+      <c r="B29" s="143"/>
+      <c r="C29" s="144"/>
+      <c r="D29" s="144"/>
+      <c r="E29" s="144"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" s="140"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="141"/>
+      <c r="F30" s="142"/>
+      <c r="G30" s="141"/>
+      <c r="H30" s="142"/>
+      <c r="I30" s="142"/>
+      <c r="J30" s="142"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A31" s="143"/>
+      <c r="B31" s="143"/>
+      <c r="C31" s="144"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="145"/>
+      <c r="G31" s="144"/>
+      <c r="H31" s="145"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="140"/>
+      <c r="B32" s="140"/>
+      <c r="C32" s="141"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="141"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="142"/>
+      <c r="I32" s="142"/>
+      <c r="J32" s="142"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="143"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="144"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="140"/>
+      <c r="B34" s="140"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="141"/>
+      <c r="H34" s="142"/>
+      <c r="I34" s="142"/>
+      <c r="J34" s="142"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="143"/>
+      <c r="B35" s="143"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="144"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="140"/>
+      <c r="B36" s="140"/>
+      <c r="C36" s="141"/>
+      <c r="D36" s="141"/>
+      <c r="E36" s="141"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="141"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="142"/>
+      <c r="J36" s="142"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A37" s="143"/>
+      <c r="B37" s="143"/>
+      <c r="C37" s="144"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="145"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="145"/>
+      <c r="I37" s="145"/>
+      <c r="J37" s="145"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="140"/>
+      <c r="B38" s="140"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="142"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="142"/>
+      <c r="I38" s="142"/>
+      <c r="J38" s="142"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A39" s="143"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="144"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="144"/>
+      <c r="F39" s="145"/>
+      <c r="G39" s="144"/>
+      <c r="H39" s="145"/>
+      <c r="I39" s="145"/>
+      <c r="J39" s="145"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A40" s="140"/>
+      <c r="B40" s="140"/>
+      <c r="C40" s="141"/>
+      <c r="D40" s="141"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="142"/>
+      <c r="G40" s="141"/>
+      <c r="H40" s="142"/>
+      <c r="I40" s="142"/>
+      <c r="J40" s="142"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A41" s="143"/>
+      <c r="B41" s="143"/>
+      <c r="C41" s="144"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="144"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="144"/>
+      <c r="H41" s="145"/>
+      <c r="I41" s="145"/>
+      <c r="J41" s="145"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A42" s="140"/>
+      <c r="B42" s="140"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="142"/>
+      <c r="G42" s="141"/>
+      <c r="H42" s="142"/>
+      <c r="I42" s="142"/>
+      <c r="J42" s="142"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A43" s="143"/>
+      <c r="B43" s="143"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="144"/>
+      <c r="E43" s="144"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="144"/>
+      <c r="H43" s="145"/>
+      <c r="I43" s="145"/>
+      <c r="J43" s="145"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A44" s="140"/>
+      <c r="B44" s="140"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141"/>
+      <c r="F44" s="142"/>
+      <c r="G44" s="141"/>
+      <c r="H44" s="142"/>
+      <c r="I44" s="142"/>
+      <c r="J44" s="142"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A45" s="143"/>
+      <c r="B45" s="143"/>
+      <c r="C45" s="145"/>
+      <c r="D45" s="144"/>
+      <c r="E45" s="145"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="144"/>
+      <c r="H45" s="145"/>
+      <c r="I45" s="145"/>
+      <c r="J45" s="145"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A46" s="140"/>
+      <c r="B46" s="140"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="141"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="142"/>
+      <c r="G46" s="141"/>
+      <c r="H46" s="142"/>
+      <c r="I46" s="142"/>
+      <c r="J46" s="142"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A47" s="143"/>
+      <c r="B47" s="143"/>
+      <c r="C47" s="144"/>
+      <c r="D47" s="144"/>
+      <c r="E47" s="144"/>
+      <c r="F47" s="145"/>
+      <c r="G47" s="144"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145"/>
+      <c r="J47" s="145"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A48" s="140"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="141"/>
+      <c r="E48" s="141"/>
+      <c r="F48" s="142"/>
+      <c r="G48" s="141"/>
+      <c r="H48" s="142"/>
+      <c r="I48" s="142"/>
+      <c r="J48" s="142"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A49" s="143"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="144"/>
+      <c r="E49" s="144"/>
+      <c r="F49" s="145"/>
+      <c r="G49" s="144"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="145"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A50" s="140"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="141"/>
+      <c r="D50" s="141"/>
+      <c r="E50" s="142"/>
+      <c r="F50" s="142"/>
+      <c r="G50" s="141"/>
+      <c r="H50" s="142"/>
+      <c r="I50" s="142"/>
+      <c r="J50" s="142"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A51" s="143"/>
+      <c r="B51" s="143"/>
+      <c r="C51" s="144"/>
+      <c r="D51" s="143"/>
+      <c r="E51" s="143"/>
+      <c r="F51" s="145"/>
+      <c r="G51" s="144"/>
+      <c r="H51" s="145"/>
+      <c r="I51" s="145"/>
+      <c r="J51" s="145"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A52" s="140"/>
+      <c r="B52" s="140"/>
+      <c r="C52" s="141"/>
+      <c r="D52" s="140"/>
+      <c r="E52" s="140"/>
+      <c r="F52" s="142"/>
+      <c r="G52" s="141"/>
+      <c r="H52" s="142"/>
+      <c r="I52" s="142"/>
+      <c r="J52" s="142"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A53" s="143"/>
+      <c r="B53" s="143"/>
+      <c r="C53" s="143"/>
+      <c r="D53" s="143"/>
+      <c r="E53" s="143"/>
+      <c r="F53" s="145"/>
+      <c r="G53" s="143"/>
+      <c r="H53" s="143"/>
+      <c r="I53" s="143"/>
+      <c r="J53" s="143"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A54" s="140"/>
+      <c r="B54" s="140"/>
+      <c r="C54" s="140"/>
+      <c r="D54" s="140"/>
+      <c r="E54" s="141"/>
+      <c r="F54" s="142"/>
+      <c r="G54" s="140"/>
+      <c r="H54" s="140"/>
+      <c r="I54" s="140"/>
+      <c r="J54" s="140"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A55" s="143"/>
+      <c r="B55" s="143"/>
+      <c r="C55" s="143"/>
+      <c r="D55" s="143"/>
+      <c r="E55" s="144"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="143"/>
+      <c r="H55" s="145"/>
+      <c r="I55" s="145"/>
+      <c r="J55" s="145"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A56" s="140"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="141"/>
+      <c r="D56" s="141"/>
+      <c r="E56" s="141"/>
+      <c r="F56" s="142"/>
+      <c r="G56" s="141"/>
+      <c r="H56" s="142"/>
+      <c r="I56" s="142"/>
+      <c r="J56" s="142"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A57" s="143"/>
+      <c r="B57" s="143"/>
+      <c r="C57" s="144"/>
+      <c r="D57" s="144"/>
+      <c r="E57" s="144"/>
+      <c r="F57" s="145"/>
+      <c r="G57" s="144"/>
+      <c r="H57" s="145"/>
+      <c r="I57" s="145"/>
+      <c r="J57" s="145"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A58" s="140"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="141"/>
+      <c r="D58" s="141"/>
+      <c r="E58" s="141"/>
+      <c r="F58" s="142"/>
+      <c r="G58" s="141"/>
+      <c r="H58" s="142"/>
+      <c r="I58" s="142"/>
+      <c r="J58" s="142"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A59" s="143"/>
+      <c r="B59" s="143"/>
+      <c r="C59" s="144"/>
+      <c r="D59" s="144"/>
+      <c r="E59" s="144"/>
+      <c r="F59" s="145"/>
+      <c r="G59" s="144"/>
+      <c r="H59" s="145"/>
+      <c r="I59" s="145"/>
+      <c r="J59" s="145"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A60" s="140"/>
+      <c r="B60" s="140"/>
+      <c r="C60" s="141"/>
+      <c r="D60" s="141"/>
+      <c r="E60" s="141"/>
+      <c r="F60" s="142"/>
+      <c r="G60" s="141"/>
+      <c r="H60" s="142"/>
+      <c r="I60" s="142"/>
+      <c r="J60" s="142"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A61" s="143"/>
+      <c r="B61" s="143"/>
+      <c r="C61" s="144"/>
+      <c r="D61" s="144"/>
+      <c r="E61" s="144"/>
+      <c r="F61" s="145"/>
+      <c r="G61" s="144"/>
+      <c r="H61" s="145"/>
+      <c r="I61" s="145"/>
+      <c r="J61" s="145"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A62" s="140"/>
+      <c r="B62" s="140"/>
+      <c r="C62" s="141"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="141"/>
+      <c r="F62" s="142"/>
+      <c r="G62" s="141"/>
+      <c r="H62" s="142"/>
+      <c r="I62" s="142"/>
+      <c r="J62" s="142"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A63" s="143"/>
+      <c r="B63" s="143"/>
+      <c r="C63" s="144"/>
+      <c r="D63" s="144"/>
+      <c r="E63" s="144"/>
+      <c r="F63" s="145"/>
+      <c r="G63" s="144"/>
+      <c r="H63" s="145"/>
+      <c r="I63" s="145"/>
+      <c r="J63" s="145"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A64" s="140"/>
+      <c r="B64" s="140"/>
+      <c r="C64" s="141"/>
+      <c r="D64" s="141"/>
+      <c r="E64" s="141"/>
+      <c r="F64" s="142"/>
+      <c r="G64" s="141"/>
+      <c r="H64" s="142"/>
+      <c r="I64" s="142"/>
+      <c r="J64" s="142"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A65" s="143"/>
+      <c r="B65" s="143"/>
+      <c r="C65" s="144"/>
+      <c r="D65" s="144"/>
+      <c r="E65" s="144"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="144"/>
+      <c r="H65" s="145"/>
+      <c r="I65" s="145"/>
+      <c r="J65" s="145"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A66" s="140"/>
+      <c r="B66" s="140"/>
+      <c r="C66" s="141"/>
+      <c r="D66" s="142"/>
+      <c r="E66" s="141"/>
+      <c r="F66" s="142"/>
+      <c r="G66" s="141"/>
+      <c r="H66" s="142"/>
+      <c r="I66" s="142"/>
+      <c r="J66" s="142"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A67" s="143"/>
+      <c r="B67" s="143"/>
+      <c r="C67" s="145"/>
+      <c r="D67" s="145"/>
+      <c r="E67" s="144"/>
+      <c r="F67" s="145"/>
+      <c r="G67" s="145"/>
+      <c r="H67" s="145"/>
+      <c r="I67" s="145"/>
+      <c r="J67" s="145"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A68" s="140"/>
+      <c r="B68" s="140"/>
+      <c r="C68" s="142"/>
+      <c r="D68" s="142"/>
+      <c r="E68" s="141"/>
+      <c r="F68" s="142"/>
+      <c r="G68" s="142"/>
+      <c r="H68" s="142"/>
+      <c r="I68" s="142"/>
+      <c r="J68" s="142"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A69" s="143"/>
+      <c r="B69" s="143"/>
+      <c r="C69" s="145"/>
+      <c r="D69" s="145"/>
+      <c r="E69" s="144"/>
+      <c r="F69" s="145"/>
+      <c r="G69" s="145"/>
+      <c r="H69" s="145"/>
+      <c r="I69" s="145"/>
+      <c r="J69" s="145"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A70" s="140"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="142"/>
+      <c r="D70" s="142"/>
+      <c r="E70" s="141"/>
+      <c r="F70" s="142"/>
+      <c r="G70" s="142"/>
+      <c r="H70" s="142"/>
+      <c r="I70" s="142"/>
+      <c r="J70" s="142"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A71" s="143"/>
+      <c r="B71" s="143"/>
+      <c r="C71" s="144"/>
+      <c r="D71" s="145"/>
+      <c r="E71" s="144"/>
+      <c r="F71" s="145"/>
+      <c r="G71" s="145"/>
+      <c r="H71" s="145"/>
+      <c r="I71" s="145"/>
+      <c r="J71" s="145"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A72" s="140"/>
+      <c r="B72" s="140"/>
+      <c r="C72" s="141"/>
+      <c r="D72" s="142"/>
+      <c r="E72" s="141"/>
+      <c r="F72" s="142"/>
+      <c r="G72" s="142"/>
+      <c r="H72" s="142"/>
+      <c r="I72" s="142"/>
+      <c r="J72" s="142"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A73" s="143"/>
+      <c r="B73" s="143"/>
+      <c r="C73" s="144"/>
+      <c r="D73" s="145"/>
+      <c r="E73" s="144"/>
+      <c r="F73" s="145"/>
+      <c r="G73" s="145"/>
+      <c r="H73" s="145"/>
+      <c r="I73" s="145"/>
+      <c r="J73" s="145"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A74" s="140"/>
+      <c r="B74" s="140"/>
+      <c r="C74" s="141"/>
+      <c r="D74" s="142"/>
+      <c r="E74" s="141"/>
+      <c r="F74" s="142"/>
+      <c r="G74" s="142"/>
+      <c r="H74" s="142"/>
+      <c r="I74" s="142"/>
+      <c r="J74" s="142"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A75" s="143"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="144"/>
+      <c r="D75" s="145"/>
+      <c r="E75" s="144"/>
+      <c r="F75" s="145"/>
+      <c r="G75" s="145"/>
+      <c r="H75" s="145"/>
+      <c r="I75" s="145"/>
+      <c r="J75" s="145"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A76" s="140"/>
+      <c r="B76" s="140"/>
+      <c r="C76" s="141"/>
+      <c r="D76" s="142"/>
+      <c r="E76" s="142"/>
+      <c r="F76" s="142"/>
+      <c r="G76" s="142"/>
+      <c r="H76" s="142"/>
+      <c r="I76" s="142"/>
+      <c r="J76" s="142"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A77" s="143"/>
+      <c r="B77" s="143"/>
+      <c r="C77" s="144"/>
+      <c r="D77" s="144"/>
+      <c r="E77" s="144"/>
+      <c r="F77" s="145"/>
+      <c r="G77" s="144"/>
+      <c r="H77" s="145"/>
+      <c r="I77" s="144"/>
+      <c r="J77" s="144"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A78" s="140"/>
+      <c r="B78" s="140"/>
+      <c r="C78" s="141"/>
+      <c r="D78" s="141"/>
+      <c r="E78" s="141"/>
+      <c r="F78" s="142"/>
+      <c r="G78" s="141"/>
+      <c r="H78" s="142"/>
+      <c r="I78" s="141"/>
+      <c r="J78" s="141"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A79" s="143"/>
+      <c r="B79" s="143"/>
+      <c r="C79" s="144"/>
+      <c r="D79" s="144"/>
+      <c r="E79" s="144"/>
+      <c r="F79" s="145"/>
+      <c r="G79" s="144"/>
+      <c r="H79" s="145"/>
+      <c r="I79" s="145"/>
+      <c r="J79" s="145"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A80" s="140"/>
+      <c r="B80" s="140"/>
+      <c r="C80" s="141"/>
+      <c r="D80" s="141"/>
+      <c r="E80" s="141"/>
+      <c r="F80" s="142"/>
+      <c r="G80" s="141"/>
+      <c r="H80" s="142"/>
+      <c r="I80" s="142"/>
+      <c r="J80" s="142"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A81" s="143"/>
+      <c r="B81" s="143"/>
+      <c r="C81" s="144"/>
+      <c r="D81" s="144"/>
+      <c r="E81" s="144"/>
+      <c r="F81" s="145"/>
+      <c r="G81" s="144"/>
+      <c r="H81" s="145"/>
+      <c r="I81" s="145"/>
+      <c r="J81" s="145"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A82" s="140"/>
+      <c r="B82" s="140"/>
+      <c r="C82" s="141"/>
+      <c r="D82" s="141"/>
+      <c r="E82" s="141"/>
+      <c r="F82" s="142"/>
+      <c r="G82" s="141"/>
+      <c r="H82" s="142"/>
+      <c r="I82" s="142"/>
+      <c r="J82" s="142"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A83" s="143"/>
+      <c r="B83" s="143"/>
+      <c r="C83" s="144"/>
+      <c r="D83" s="144"/>
+      <c r="E83" s="144"/>
+      <c r="F83" s="145"/>
+      <c r="G83" s="144"/>
+      <c r="H83" s="145"/>
+      <c r="I83" s="145"/>
+      <c r="J83" s="145"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A84" s="140"/>
+      <c r="B84" s="140"/>
+      <c r="C84" s="141"/>
+      <c r="D84" s="141"/>
+      <c r="E84" s="141"/>
+      <c r="F84" s="142"/>
+      <c r="G84" s="141"/>
+      <c r="H84" s="142"/>
+      <c r="I84" s="142"/>
+      <c r="J84" s="142"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A85" s="143"/>
+      <c r="B85" s="143"/>
+      <c r="C85" s="144"/>
+      <c r="D85" s="144"/>
+      <c r="E85" s="144"/>
+      <c r="F85" s="145"/>
+      <c r="G85" s="144"/>
+      <c r="H85" s="145"/>
+      <c r="I85" s="145"/>
+      <c r="J85" s="145"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A86" s="140"/>
+      <c r="B86" s="140"/>
+      <c r="C86" s="141"/>
+      <c r="D86" s="141"/>
+      <c r="E86" s="141"/>
+      <c r="F86" s="142"/>
+      <c r="G86" s="141"/>
+      <c r="H86" s="142"/>
+      <c r="I86" s="142"/>
+      <c r="J86" s="142"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A87" s="143"/>
+      <c r="B87" s="143"/>
+      <c r="C87" s="144"/>
+      <c r="D87" s="144"/>
+      <c r="E87" s="144"/>
+      <c r="F87" s="145"/>
+      <c r="G87" s="144"/>
+      <c r="H87" s="145"/>
+      <c r="I87" s="145"/>
+      <c r="J87" s="145"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A88" s="140"/>
+      <c r="B88" s="140"/>
+      <c r="C88" s="141"/>
+      <c r="D88" s="141"/>
+      <c r="E88" s="141"/>
+      <c r="F88" s="142"/>
+      <c r="G88" s="141"/>
+      <c r="H88" s="142"/>
+      <c r="I88" s="142"/>
+      <c r="J88" s="142"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A89" s="143"/>
+      <c r="B89" s="143"/>
+      <c r="C89" s="144"/>
+      <c r="D89" s="144"/>
+      <c r="E89" s="144"/>
+      <c r="F89" s="145"/>
+      <c r="G89" s="144"/>
+      <c r="H89" s="145"/>
+      <c r="I89" s="145"/>
+      <c r="J89" s="145"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A90" s="140"/>
+      <c r="B90" s="140"/>
+      <c r="C90" s="141"/>
+      <c r="D90" s="141"/>
+      <c r="E90" s="141"/>
+      <c r="F90" s="142"/>
+      <c r="G90" s="141"/>
+      <c r="H90" s="142"/>
+      <c r="I90" s="142"/>
+      <c r="J90" s="142"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A91" s="143"/>
+      <c r="B91" s="143"/>
+      <c r="C91" s="144"/>
+      <c r="D91" s="144"/>
+      <c r="E91" s="144"/>
+      <c r="F91" s="145"/>
+      <c r="G91" s="144"/>
+      <c r="H91" s="145"/>
+      <c r="I91" s="145"/>
+      <c r="J91" s="145"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A92" s="140"/>
+      <c r="B92" s="140"/>
+      <c r="C92" s="141"/>
+      <c r="D92" s="141"/>
+      <c r="E92" s="141"/>
+      <c r="F92" s="142"/>
+      <c r="G92" s="141"/>
+      <c r="H92" s="142"/>
+      <c r="I92" s="142"/>
+      <c r="J92" s="142"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A93" s="143"/>
+      <c r="B93" s="143"/>
+      <c r="C93" s="144"/>
+      <c r="D93" s="144"/>
+      <c r="E93" s="144"/>
+      <c r="F93" s="145"/>
+      <c r="G93" s="144"/>
+      <c r="H93" s="145"/>
+      <c r="I93" s="145"/>
+      <c r="J93" s="145"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A94" s="140"/>
+      <c r="B94" s="140"/>
+      <c r="C94" s="141"/>
+      <c r="D94" s="141"/>
+      <c r="E94" s="141"/>
+      <c r="F94" s="142"/>
+      <c r="G94" s="141"/>
+      <c r="H94" s="142"/>
+      <c r="I94" s="142"/>
+      <c r="J94" s="142"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A95" s="143"/>
+      <c r="B95" s="143"/>
+      <c r="C95" s="144"/>
+      <c r="D95" s="144"/>
+      <c r="E95" s="146"/>
+      <c r="F95" s="145"/>
+      <c r="G95" s="144"/>
+      <c r="H95" s="145"/>
+      <c r="I95" s="145"/>
+      <c r="J95" s="145"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A96" s="140"/>
+      <c r="B96" s="140"/>
+      <c r="C96" s="141"/>
+      <c r="D96" s="141"/>
+      <c r="E96" s="141"/>
+      <c r="F96" s="142"/>
+      <c r="G96" s="141"/>
+      <c r="H96" s="142"/>
+      <c r="I96" s="142"/>
+      <c r="J96" s="142"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A97" s="143"/>
+      <c r="B97" s="143"/>
+      <c r="C97" s="144"/>
+      <c r="D97" s="144"/>
+      <c r="E97" s="146"/>
+      <c r="F97" s="145"/>
+      <c r="G97" s="144"/>
+      <c r="H97" s="145"/>
+      <c r="I97" s="145"/>
+      <c r="J97" s="145"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A98" s="140"/>
+      <c r="B98" s="140"/>
+      <c r="C98" s="141"/>
+      <c r="D98" s="141"/>
+      <c r="E98" s="141"/>
+      <c r="F98" s="142"/>
+      <c r="G98" s="141"/>
+      <c r="H98" s="142"/>
+      <c r="I98" s="142"/>
+      <c r="J98" s="142"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A99" s="143"/>
+      <c r="B99" s="143"/>
+      <c r="C99" s="144"/>
+      <c r="D99" s="144"/>
+      <c r="E99" s="144"/>
+      <c r="F99" s="145"/>
+      <c r="G99" s="144"/>
+      <c r="H99" s="145"/>
+      <c r="I99" s="145"/>
+      <c r="J99" s="145"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A100" s="140"/>
+      <c r="B100" s="140"/>
+      <c r="C100" s="141"/>
+      <c r="D100" s="141"/>
+      <c r="E100" s="141"/>
+      <c r="F100" s="142"/>
+      <c r="G100" s="141"/>
+      <c r="H100" s="142"/>
+      <c r="I100" s="142"/>
+      <c r="J100" s="142"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A101" s="143"/>
+      <c r="B101" s="143"/>
+      <c r="C101" s="144"/>
+      <c r="D101" s="144"/>
+      <c r="E101" s="144"/>
+      <c r="F101" s="145"/>
+      <c r="G101" s="144"/>
+      <c r="H101" s="145"/>
+      <c r="I101" s="145"/>
+      <c r="J101" s="145"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A102" s="140"/>
+      <c r="B102" s="140"/>
+      <c r="C102" s="141"/>
+      <c r="D102" s="141"/>
+      <c r="E102" s="141"/>
+      <c r="F102" s="142"/>
+      <c r="G102" s="141"/>
+      <c r="H102" s="142"/>
+      <c r="I102" s="142"/>
+      <c r="J102" s="142"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A103" s="143"/>
+      <c r="B103" s="143"/>
+      <c r="C103" s="144"/>
+      <c r="D103" s="144"/>
+      <c r="E103" s="144"/>
+      <c r="F103" s="145"/>
+      <c r="G103" s="144"/>
+      <c r="H103" s="145"/>
+      <c r="I103" s="145"/>
+      <c r="J103" s="145"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A104" s="140"/>
+      <c r="B104" s="140"/>
+      <c r="C104" s="141"/>
+      <c r="D104" s="141"/>
+      <c r="E104" s="141"/>
+      <c r="F104" s="142"/>
+      <c r="G104" s="141"/>
+      <c r="H104" s="142"/>
+      <c r="I104" s="142"/>
+      <c r="J104" s="142"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A105" s="143"/>
+      <c r="B105" s="143"/>
+      <c r="C105" s="144"/>
+      <c r="D105" s="144"/>
+      <c r="E105" s="144"/>
+      <c r="F105" s="145"/>
+      <c r="G105" s="144"/>
+      <c r="H105" s="145"/>
+      <c r="I105" s="145"/>
+      <c r="J105" s="145"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A106" s="140"/>
+      <c r="B106" s="140"/>
+      <c r="C106" s="141"/>
+      <c r="D106" s="141"/>
+      <c r="E106" s="141"/>
+      <c r="F106" s="142"/>
+      <c r="G106" s="141"/>
+      <c r="H106" s="142"/>
+      <c r="I106" s="142"/>
+      <c r="J106" s="142"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A107" s="143"/>
+      <c r="B107" s="143"/>
+      <c r="C107" s="144"/>
+      <c r="D107" s="144"/>
+      <c r="E107" s="144"/>
+      <c r="F107" s="145"/>
+      <c r="G107" s="144"/>
+      <c r="H107" s="145"/>
+      <c r="I107" s="145"/>
+      <c r="J107" s="145"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A108" s="147"/>
+      <c r="B108" s="148"/>
+      <c r="C108" s="149"/>
+      <c r="D108" s="149"/>
+      <c r="E108" s="149"/>
+      <c r="F108" s="142"/>
+      <c r="G108" s="149"/>
+      <c r="H108" s="150"/>
+      <c r="I108" s="150"/>
+      <c r="J108" s="142"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A109" s="151"/>
+      <c r="B109" s="130"/>
+      <c r="C109" s="131"/>
+      <c r="D109" s="131"/>
+      <c r="E109" s="131"/>
+      <c r="F109" s="145"/>
+      <c r="G109" s="131"/>
+      <c r="H109" s="125"/>
+      <c r="I109" s="125"/>
+      <c r="J109" s="145"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A110" s="147"/>
+      <c r="B110" s="148"/>
+      <c r="C110" s="149"/>
+      <c r="D110" s="149"/>
+      <c r="E110" s="149"/>
+      <c r="F110" s="142"/>
+      <c r="G110" s="149"/>
+      <c r="H110" s="150"/>
+      <c r="I110" s="150"/>
+      <c r="J110" s="142"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A111" s="151"/>
+      <c r="B111" s="130"/>
+      <c r="C111" s="131"/>
+      <c r="D111" s="131"/>
+      <c r="E111" s="131"/>
+      <c r="F111" s="145"/>
+      <c r="G111" s="131"/>
+      <c r="H111" s="125"/>
+      <c r="I111" s="125"/>
+      <c r="J111" s="145"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A112" s="147"/>
+      <c r="B112" s="148"/>
+      <c r="C112" s="149"/>
+      <c r="D112" s="149"/>
+      <c r="E112" s="149"/>
+      <c r="F112" s="142"/>
+      <c r="G112" s="149"/>
+      <c r="H112" s="150"/>
+      <c r="I112" s="150"/>
+      <c r="J112" s="142"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A113" s="151"/>
+      <c r="B113" s="130"/>
+      <c r="C113" s="131"/>
+      <c r="D113" s="131"/>
+      <c r="E113" s="131"/>
+      <c r="F113" s="145"/>
+      <c r="G113" s="131"/>
+      <c r="H113" s="125"/>
+      <c r="I113" s="125"/>
+      <c r="J113" s="145"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A114" s="147"/>
+      <c r="B114" s="148"/>
+      <c r="C114" s="149"/>
+      <c r="D114" s="149"/>
+      <c r="E114" s="149"/>
+      <c r="F114" s="142"/>
+      <c r="G114" s="149"/>
+      <c r="H114" s="150"/>
+      <c r="I114" s="150"/>
+      <c r="J114" s="142"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A115" s="151"/>
+      <c r="B115" s="130"/>
+      <c r="C115" s="131"/>
+      <c r="D115" s="131"/>
+      <c r="E115" s="131"/>
+      <c r="F115" s="145"/>
+      <c r="G115" s="131"/>
+      <c r="H115" s="125"/>
+      <c r="I115" s="125"/>
+      <c r="J115" s="145"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A116" s="147"/>
+      <c r="B116" s="148"/>
+      <c r="C116" s="149"/>
+      <c r="D116" s="149"/>
+      <c r="E116" s="149"/>
+      <c r="F116" s="142"/>
+      <c r="G116" s="149"/>
+      <c r="H116" s="150"/>
+      <c r="I116" s="150"/>
+      <c r="J116" s="142"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A117" s="143"/>
+      <c r="B117" s="143"/>
+      <c r="C117" s="144"/>
+      <c r="D117" s="144"/>
+      <c r="E117" s="144"/>
+      <c r="F117" s="145"/>
+      <c r="G117" s="144"/>
+      <c r="H117" s="145"/>
+      <c r="I117" s="145"/>
+      <c r="J117" s="145"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A118" s="140"/>
+      <c r="B118" s="140"/>
+      <c r="C118" s="141"/>
+      <c r="D118" s="141"/>
+      <c r="E118" s="141"/>
+      <c r="F118" s="142"/>
+      <c r="G118" s="141"/>
+      <c r="H118" s="142"/>
+      <c r="I118" s="142"/>
+      <c r="J118" s="142"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A119" s="143"/>
+      <c r="B119" s="143"/>
+      <c r="C119" s="144"/>
+      <c r="D119" s="144"/>
+      <c r="E119" s="144"/>
+      <c r="F119" s="145"/>
+      <c r="G119" s="144"/>
+      <c r="H119" s="145"/>
+      <c r="I119" s="145"/>
+      <c r="J119" s="145"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A120" s="140"/>
+      <c r="B120" s="140"/>
+      <c r="C120" s="141"/>
+      <c r="D120" s="141"/>
+      <c r="E120" s="141"/>
+      <c r="F120" s="142"/>
+      <c r="G120" s="141"/>
+      <c r="H120" s="142"/>
+      <c r="I120" s="142"/>
+      <c r="J120" s="142"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A121" s="143"/>
+      <c r="B121" s="143"/>
+      <c r="C121" s="144"/>
+      <c r="D121" s="144"/>
+      <c r="E121" s="144"/>
+      <c r="F121" s="145"/>
+      <c r="G121" s="144"/>
+      <c r="H121" s="145"/>
+      <c r="I121" s="145"/>
+      <c r="J121" s="145"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A122" s="140"/>
+      <c r="B122" s="140"/>
+      <c r="C122" s="141"/>
+      <c r="D122" s="141"/>
+      <c r="E122" s="141"/>
+      <c r="F122" s="142"/>
+      <c r="G122" s="141"/>
+      <c r="H122" s="142"/>
+      <c r="I122" s="142"/>
+      <c r="J122" s="142"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A123" s="143"/>
+      <c r="B123" s="143"/>
+      <c r="C123" s="144"/>
+      <c r="D123" s="144"/>
+      <c r="E123" s="144"/>
+      <c r="F123" s="145"/>
+      <c r="G123" s="144"/>
+      <c r="H123" s="145"/>
+      <c r="I123" s="145"/>
+      <c r="J123" s="145"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A124" s="140"/>
+      <c r="B124" s="140"/>
+      <c r="C124" s="141"/>
+      <c r="D124" s="141"/>
+      <c r="E124" s="141"/>
+      <c r="F124" s="142"/>
+      <c r="G124" s="141"/>
+      <c r="H124" s="142"/>
+      <c r="I124" s="142"/>
+      <c r="J124" s="142"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A125" s="143"/>
+      <c r="B125" s="143"/>
+      <c r="C125" s="144"/>
+      <c r="D125" s="144"/>
+      <c r="E125" s="144"/>
+      <c r="F125" s="145"/>
+      <c r="G125" s="144"/>
+      <c r="H125" s="145"/>
+      <c r="I125" s="145"/>
+      <c r="J125" s="145"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A126" s="140"/>
+      <c r="B126" s="140"/>
+      <c r="C126" s="141"/>
+      <c r="D126" s="141"/>
+      <c r="E126" s="141"/>
+      <c r="F126" s="142"/>
+      <c r="G126" s="141"/>
+      <c r="H126" s="142"/>
+      <c r="I126" s="142"/>
+      <c r="J126" s="142"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A127" s="143"/>
+      <c r="B127" s="143"/>
+      <c r="C127" s="144"/>
+      <c r="D127" s="144"/>
+      <c r="E127" s="144"/>
+      <c r="F127" s="145"/>
+      <c r="G127" s="144"/>
+      <c r="H127" s="145"/>
+      <c r="I127" s="145"/>
+      <c r="J127" s="145"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A128" s="140"/>
+      <c r="B128" s="140"/>
+      <c r="C128" s="141"/>
+      <c r="D128" s="141"/>
+      <c r="E128" s="141"/>
+      <c r="F128" s="142"/>
+      <c r="G128" s="141"/>
+      <c r="H128" s="142"/>
+      <c r="I128" s="142"/>
+      <c r="J128" s="142"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GA-133 Add a new Tab AccessType and AccessTypeRole in the DefinitionStore to replace AccessTypeRoles Tab
</commit_message>
<xml_diff>
--- a/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
+++ b/excel-importer/src/test/resources/CCD_TestDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenbird/IdeaProjects/ccd-definition-store-api/excel-importer/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0942AC-1B5F-2E41-8EAB-850DD3548EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8667E80-8639-6A4C-96C8-769713EC17C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" tabRatio="757" firstSheet="14" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchCasesResultFields" sheetId="23" r:id="rId1"/>
@@ -37,11 +37,12 @@
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId22"/>
     <sheet name="SearchAlias" sheetId="20" r:id="rId23"/>
     <sheet name="RoleToAccessProfiles" sheetId="26" r:id="rId24"/>
-    <sheet name="AccessTypeRoles" sheetId="25" r:id="rId25"/>
+    <sheet name="AccessType" sheetId="25" r:id="rId25"/>
+    <sheet name="AccessTypeRole" sheetId="27" r:id="rId26"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
+    <externalReference r:id="rId28"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="352">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -989,9 +990,6 @@
     <t>CaseLink</t>
   </si>
   <si>
-    <t>AccessTypeRoles</t>
-  </si>
-  <si>
     <t>Start date from which the data will be valid</t>
   </si>
   <si>
@@ -1141,6 +1139,12 @@
   </si>
   <si>
     <t>AccessProfile1</t>
+  </si>
+  <si>
+    <t>AccessTypeRole</t>
+  </si>
+  <si>
+    <t>AccessType</t>
   </si>
 </sst>
 </file>
@@ -1930,7 +1934,7 @@
     <cellStyle name="Normal 2 3" xfId="2" xr:uid="{D1C84B9E-CD33-7D48-9D04-3B5C7C49583F}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{301FA0D7-E476-6D4A-B119-3BD4843C1730}"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="96">
     <dxf>
       <font>
         <b val="0"/>
@@ -2040,6 +2044,204 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3467,31 +3669,31 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleDefinitionsTab" pivot="0" count="7" xr9:uid="{5DF7EA3F-64CE-4247-925E-FA6B786D4D35}">
-      <tableStyleElement type="wholeTable" dxfId="85"/>
-      <tableStyleElement type="headerRow" dxfId="84"/>
-      <tableStyleElement type="totalRow" dxfId="83"/>
-      <tableStyleElement type="firstColumn" dxfId="82"/>
-      <tableStyleElement type="lastColumn" dxfId="81"/>
-      <tableStyleElement type="firstRowStripe" dxfId="80"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="79"/>
+      <tableStyleElement type="wholeTable" dxfId="95"/>
+      <tableStyleElement type="headerRow" dxfId="94"/>
+      <tableStyleElement type="totalRow" dxfId="93"/>
+      <tableStyleElement type="firstColumn" dxfId="92"/>
+      <tableStyleElement type="lastColumn" dxfId="91"/>
+      <tableStyleElement type="firstRowStripe" dxfId="90"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="89"/>
     </tableStyle>
     <tableStyle name="TableStyleDefinitionsTab 2" pivot="0" count="7" xr9:uid="{07DBC3E2-672D-304E-8827-44CA02ACC044}">
-      <tableStyleElement type="wholeTable" dxfId="78"/>
-      <tableStyleElement type="headerRow" dxfId="77"/>
-      <tableStyleElement type="totalRow" dxfId="76"/>
-      <tableStyleElement type="firstColumn" dxfId="75"/>
-      <tableStyleElement type="lastColumn" dxfId="74"/>
-      <tableStyleElement type="firstRowStripe" dxfId="73"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="72"/>
+      <tableStyleElement type="wholeTable" dxfId="88"/>
+      <tableStyleElement type="headerRow" dxfId="87"/>
+      <tableStyleElement type="totalRow" dxfId="86"/>
+      <tableStyleElement type="firstColumn" dxfId="85"/>
+      <tableStyleElement type="lastColumn" dxfId="84"/>
+      <tableStyleElement type="firstRowStripe" dxfId="83"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="82"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium2 2" pivot="0" count="7" xr9:uid="{543C597F-AAF7-404B-9D6B-0A2AC729EF9C}">
-      <tableStyleElement type="wholeTable" dxfId="71"/>
-      <tableStyleElement type="headerRow" dxfId="70"/>
-      <tableStyleElement type="totalRow" dxfId="69"/>
-      <tableStyleElement type="firstColumn" dxfId="68"/>
-      <tableStyleElement type="lastColumn" dxfId="67"/>
-      <tableStyleElement type="firstRowStripe" dxfId="66"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="65"/>
+      <tableStyleElement type="wholeTable" dxfId="81"/>
+      <tableStyleElement type="headerRow" dxfId="80"/>
+      <tableStyleElement type="totalRow" dxfId="79"/>
+      <tableStyleElement type="firstColumn" dxfId="78"/>
+      <tableStyleElement type="lastColumn" dxfId="77"/>
+      <tableStyleElement type="firstRowStripe" dxfId="76"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="75"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3643,18 +3845,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF26FF77-A3A9-9F49-B1EF-D3593AA4B6AF}" name="Table414" displayName="Table414" ref="A3:C7" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71" totalsRowBorderDxfId="70">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="57" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{373611EC-55C4-6B4C-8279-394008E573A5}" name="CaseTypeId" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{F42A048B-C9B0-5B4B-A950-F9B5B2BD620C}" name="ReasonRequired" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{B876B77C-B39B-F648-9659-AA6FF35B4C38}" name="NoCActionInterpretationRequired" dataDxfId="67" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A4737304-04AC-DC4D-9A7C-9F05E89BAD62}" name="AuthorisationCaseType" displayName="AuthorisationCaseType" ref="A3:E8" totalsRowShown="0" headerRowDxfId="66">
   <autoFilter ref="A3:E8" xr:uid="{DE67A763-332B-BD46-B7C3-EBA8F690E3DF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3674,7 +3876,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5442497-6E1B-1E42-A125-378A92982492}" name="AuthorisationCaseField" displayName="AuthorisationCaseField" ref="A3:F14" totalsRowShown="0" headerRowDxfId="65">
   <autoFilter ref="A3:F14" xr:uid="{D162FCBC-6067-E044-9D69-AF2CA3143CB7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3696,7 +3898,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{66DD1FE9-104F-A143-812D-C7C128638CDD}" name="AuthorisationComplexType" displayName="AuthorisationComplexType" ref="A3:G12" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" headerRowCellStyle="Normal 2 3" dataCellStyle="Normal 2">
   <autoFilter ref="A3:G12" xr:uid="{129E9FE3-9375-CC4E-B0C6-969D294192AA}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3707,20 +3909,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="52" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="51" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="50" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="49" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="48" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="47" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="46" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{8B870200-14AC-3246-BF3F-42EEC57A17B3}" name="LiveFrom" dataDxfId="62" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{9043D652-8144-2546-9732-594ADF8722FB}" name="LiveTo" dataDxfId="61" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{571802B9-6698-D347-859E-7C78BC49BDBA}" name="CaseTypeID" dataDxfId="60" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{24B866B4-D013-8F4A-8217-1BE32B10B817}" name="CaseFieldID" dataDxfId="59" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{B609DA43-C9D4-8842-82EF-5CD10CBCB4AC}" name="ListElementCode" dataDxfId="58" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{669913E0-FECF-4E41-9EEF-BDA9C5836A88}" name="AccessProfile" dataDxfId="57" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{46609C57-4B8B-474F-B135-226F423F962D}" name="CRUD" dataDxfId="56" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A61AB85F-5920-1440-9981-7E2F8C405A0B}" name="AuthorisationCaseEvent" displayName="AuthorisationCaseEvent" ref="A3:F10" totalsRowShown="0" headerRowDxfId="55">
   <autoFilter ref="A3:F10" xr:uid="{1C201DC6-4AD3-A34B-B4C5-7AF4C58C06C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3742,67 +3944,81 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{184EB418-E715-7D4A-988A-3653238A9317}" name="AuthorisationCaseState" displayName="AuthorisationCaseState" ref="A3:F12" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" headerRowCellStyle="Explanatory Text" dataCellStyle="Explanatory Text">
   <autoFilter ref="A3:F12" xr:uid="{BCDC8342-0F03-CD45-AA5C-0DCDDCDE336E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="40" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="39" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="38" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="37" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="36" dataCellStyle="Explanatory Text"/>
-    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="35" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="1" xr3:uid="{1AB5F1E1-AAF8-8841-A613-4424173F09FC}" name="LiveFrom" dataDxfId="50" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="2" xr3:uid="{2B2187EF-5A1E-9642-B9A9-329D973BDF62}" name="LiveTo" dataDxfId="49" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="3" xr3:uid="{4F821A62-8EF3-324E-8A17-8AA1E290DBB0}" name="CaseTypeID" dataDxfId="48" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="4" xr3:uid="{E7967E7C-9176-2844-8CE1-DB30CC0717A2}" name="CaseStateID" dataDxfId="47" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="5" xr3:uid="{13C303D8-F192-F343-A45F-12B4A4D90AC5}" name="AccessProfile" dataDxfId="46" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="6" xr3:uid="{18C819AE-242D-5A4B-8DA0-20122A3E6582}" name="CRUD" dataDxfId="45" dataCellStyle="Explanatory Text"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}" name="Table2214" displayName="Table2214" ref="A3:I57" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}" name="Table2214" displayName="Table2214" ref="A3:I57" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A3:I57" xr:uid="{63D54104-57AA-E54C-8594-E56646A46483}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{33AF10A0-FD17-A947-9CAA-77E9D3542027}" name="LiveFrom" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{E7E5D7A6-3126-B949-A296-371E77432DF6}" name="LiveTo" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{1FFE52D3-59DC-5F48-8695-25CA9FA2F50C}" name="RoleName" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{EF4600F5-0195-3240-930C-17499C4A0874}" name="Authorisation" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{48CA193A-9E00-BD47-A75E-FF4789D4202D}" name="CaseTypeID" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{45A53A60-CAD6-4F42-A6E3-8EF7193F4F4E}" name="AccessProfiles" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{B51B665F-933C-0B41-9EB0-3A10D78D250E}" name="ReadOnly" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{C959F86F-34F5-3540-91F1-44591632390E}" name="Disabled" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{F4A1B44D-5922-8542-A473-3D3610C6383D}" name="CaseAccessCategories" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{33AF10A0-FD17-A947-9CAA-77E9D3542027}" name="LiveFrom" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{E7E5D7A6-3126-B949-A296-371E77432DF6}" name="LiveTo" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1FFE52D3-59DC-5F48-8695-25CA9FA2F50C}" name="RoleName" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{EF4600F5-0195-3240-930C-17499C4A0874}" name="Authorisation" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{48CA193A-9E00-BD47-A75E-FF4789D4202D}" name="CaseTypeID" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{45A53A60-CAD6-4F42-A6E3-8EF7193F4F4E}" name="AccessProfiles" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{B51B665F-933C-0B41-9EB0-3A10D78D250E}" name="ReadOnly" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{C959F86F-34F5-3540-91F1-44591632390E}" name="Disabled" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{F4A1B44D-5922-8542-A473-3D3610C6383D}" name="CaseAccessCategories" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}" name="Table230" displayName="Table230" ref="A3:P128" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A3:P128" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{8C3C6264-6488-4B46-844F-78CC8AF0EDBF}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{95AB0CD9-F14A-EA40-B121-07641BAA248A}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{18A561CE-791A-3A43-B06A-B27A02FAAFDB}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6A586A4E-EA35-4E4B-BC60-732047B49C80}" name="AccessTypeID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{1475CF15-4AE2-D547-A87F-CCA3AF2C780B}" name="OrganisationProfileID" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{930AF5C9-9016-7246-995A-DF6FB6AAC8DC}" name="AccessMandatory" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{769BF7CA-E071-0A47-AA62-48684CBE997A}" name="AccessDefault" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{5EDA7EBC-00F3-204D-B4FD-A9A0115A6E14}" name="Display" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{F76B90E0-19CB-144F-B0C5-C959BA87ABE7}" name="Description" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{0E637EFA-4DDB-AB45-9C96-596ACB0AC71C}" name="HintText" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{97A904CD-4B78-4F41-B725-D733390E4F60}" name="DisplayOrder" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{1658B47E-5FBB-D340-BE0B-BDC42B9F01FF}" name="OrganisationalRoleName" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{3140418B-F23F-CD40-AD19-B8DD152035B9}" name="GroupRoleName" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{62607777-04A9-FB40-B101-1CD50AC850DF}" name="CaseAssignedRoleField" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{3FC77184-E5A9-1240-98B2-ABD9520779C3}" name="GroupAccessEnabled" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{8DEA16FB-7E2A-E74C-9CAF-EC6D2776B5D6}" name="CaseAccessGroupIDTemplate" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}" name="Table230" displayName="Table230" ref="A3:K128" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A3:K128" xr:uid="{503A127D-6DCA-7745-9024-E497C480B962}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{8C3C6264-6488-4B46-844F-78CC8AF0EDBF}" name="LiveFrom" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{95AB0CD9-F14A-EA40-B121-07641BAA248A}" name="LiveTo" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{18A561CE-791A-3A43-B06A-B27A02FAAFDB}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{6A586A4E-EA35-4E4B-BC60-732047B49C80}" name="AccessTypeID" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1475CF15-4AE2-D547-A87F-CCA3AF2C780B}" name="OrganisationProfileID" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{930AF5C9-9016-7246-995A-DF6FB6AAC8DC}" name="AccessMandatory" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{769BF7CA-E071-0A47-AA62-48684CBE997A}" name="AccessDefault" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{5EDA7EBC-00F3-204D-B4FD-A9A0115A6E14}" name="Display" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{F76B90E0-19CB-144F-B0C5-C959BA87ABE7}" name="Description" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{0E637EFA-4DDB-AB45-9C96-596ACB0AC71C}" name="HintText" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{97A904CD-4B78-4F41-B725-D733390E4F60}" name="DisplayOrder" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D4063364-7874-FD48-8D11-FE8ACF8BF090}" name="Table23010" displayName="Table23010" ref="A3:J128" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="A3:J128" xr:uid="{D4063364-7874-FD48-8D11-FE8ACF8BF090}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{ABCEF5AD-CF08-A140-85C3-145C235FE11E}" name="LiveFrom" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{569D7904-E500-524E-A058-193C2316A5FB}" name="LiveTo" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{1C39441F-1631-B44E-BC2D-569C092FA92C}" name="CaseTypeID" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{712886BA-5734-3446-8793-DA2B3B7C0B5D}" name="AccessTypeID" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{839073D9-99DF-0449-ADEB-717416AF951A}" name="OrganisationProfileID" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{4E4623EE-593E-414E-A739-6080D45CB5D8}" name="OrganisationalRoleName" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{4FB61EAD-1FB6-574D-B155-600EEA5B85D1}" name="GroupRoleName" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{51CCD360-5207-2348-A64C-2E77DAEEEF3D}" name="CaseAssignedRoleField" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{F5FB1908-7008-5440-B8BD-56F68FB0CBA6}" name="GroupAccessEnabled" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{503BD6E0-110E-024F-A79D-19EEAAB3DB39}" name="CaseAccessGroupIDTemplate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDefinitionsTab" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3840,7 +4056,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3946,7 +4162,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4088,7 +4304,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12485,7 +12701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E6EA2-C6B0-264E-B434-2DA704ABBD0D}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -13234,7 +13450,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="111" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="112"/>
@@ -13246,29 +13462,29 @@
     </row>
     <row r="2" spans="1:9" s="132" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="117" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="117" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="117" t="s">
-        <v>306</v>
-      </c>
       <c r="C2" s="117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D2" s="117"/>
       <c r="E2" s="117" t="s">
+        <v>338</v>
+      </c>
+      <c r="F2" s="117" t="s">
         <v>339</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="G2" s="117" t="s">
         <v>340</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="H2" s="117" t="s">
         <v>341</v>
       </c>
-      <c r="H2" s="117" t="s">
+      <c r="I2" s="132" t="s">
         <v>342</v>
-      </c>
-      <c r="I2" s="132" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="121" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13279,25 +13495,25 @@
         <v>8</v>
       </c>
       <c r="C3" s="119" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" s="119" t="s">
         <v>344</v>
-      </c>
-      <c r="D3" s="119" t="s">
-        <v>345</v>
       </c>
       <c r="E3" s="119" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="G3" s="119" t="s">
         <v>346</v>
       </c>
-      <c r="G3" s="119" t="s">
-        <v>347</v>
-      </c>
       <c r="H3" s="119" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="119" t="s">
         <v>342</v>
-      </c>
-      <c r="I3" s="119" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13306,22 +13522,22 @@
       </c>
       <c r="B4" s="122"/>
       <c r="C4" s="124" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D4" s="124" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E4" s="123" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="124" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G4" s="124" t="s">
         <v>293</v>
       </c>
       <c r="H4" s="123" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="124" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -13681,10 +13897,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E213E05-C678-DD41-9D11-284BE15D402F}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13699,16 +13915,11 @@
     <col min="8" max="8" width="11.1640625" customWidth="1"/>
     <col min="9" max="10" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" customWidth="1"/>
-    <col min="14" max="14" width="28.83203125" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="111" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
       <c r="B1" s="112"/>
       <c r="C1" s="113"/>
@@ -13716,57 +13927,42 @@
       <c r="I1" s="115"/>
       <c r="K1" s="116"/>
     </row>
-    <row r="2" spans="1:16" ht="168" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="168" x14ac:dyDescent="0.15">
       <c r="A2" s="117" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="117" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="C2" s="117" t="s">
         <v>306</v>
       </c>
-      <c r="C2" s="117" t="s">
+      <c r="D2" s="117" t="s">
         <v>307</v>
       </c>
-      <c r="D2" s="117" t="s">
+      <c r="E2" s="117" t="s">
         <v>308</v>
       </c>
-      <c r="E2" s="117" t="s">
+      <c r="F2" s="117" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="117" t="s">
+      <c r="G2" s="117" t="s">
         <v>310</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="H2" s="91" t="s">
         <v>311</v>
       </c>
-      <c r="H2" s="91" t="s">
+      <c r="I2" s="117" t="s">
         <v>312</v>
       </c>
-      <c r="I2" s="117" t="s">
+      <c r="J2" s="117" t="s">
         <v>313</v>
       </c>
-      <c r="J2" s="117" t="s">
+      <c r="K2" s="118" t="s">
         <v>314</v>
       </c>
-      <c r="K2" s="118" t="s">
-        <v>315</v>
-      </c>
-      <c r="L2" s="118" t="s">
-        <v>316</v>
-      </c>
-      <c r="M2" s="118" t="s">
-        <v>317</v>
-      </c>
-      <c r="N2" s="117" t="s">
-        <v>318</v>
-      </c>
-      <c r="O2" s="91" t="s">
-        <v>319</v>
-      </c>
-      <c r="P2" s="91" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="119" t="s">
         <v>7</v>
       </c>
@@ -13777,19 +13973,19 @@
         <v>37</v>
       </c>
       <c r="D3" s="119" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="119" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="F3" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="G3" s="119" t="s">
         <v>323</v>
       </c>
-      <c r="G3" s="119" t="s">
+      <c r="H3" s="119" t="s">
         <v>324</v>
-      </c>
-      <c r="H3" s="119" t="s">
-        <v>325</v>
       </c>
       <c r="I3" s="119" t="s">
         <v>11</v>
@@ -13800,23 +13996,8 @@
       <c r="K3" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="121" t="s">
-        <v>326</v>
-      </c>
-      <c r="M3" s="119" t="s">
-        <v>327</v>
-      </c>
-      <c r="N3" s="119" t="s">
-        <v>328</v>
-      </c>
-      <c r="O3" s="119" t="s">
-        <v>329</v>
-      </c>
-      <c r="P3" s="119" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="122">
         <v>44927</v>
       </c>
@@ -13825,10 +14006,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="123" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="123" t="s">
         <v>331</v>
-      </c>
-      <c r="E4" s="123" t="s">
-        <v>332</v>
       </c>
       <c r="F4" s="123" t="s">
         <v>182</v>
@@ -13840,31 +14021,16 @@
         <v>182</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K4" s="124">
         <v>1</v>
       </c>
-      <c r="L4" s="123" t="s">
-        <v>334</v>
-      </c>
-      <c r="M4" s="123" t="s">
-        <v>334</v>
-      </c>
-      <c r="N4" s="124" t="s">
-        <v>334</v>
-      </c>
-      <c r="O4" s="124" t="s">
-        <v>182</v>
-      </c>
-      <c r="P4" s="124" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="122">
         <v>44927</v>
       </c>
@@ -13873,10 +14039,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E5" s="123" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F5" s="123" t="s">
         <v>182</v>
@@ -13888,23 +14054,16 @@
         <v>182</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J5" s="124" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K5" s="124">
         <v>2</v>
       </c>
-      <c r="L5" s="124" t="s">
-        <v>334</v>
-      </c>
-      <c r="M5" s="123"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="122"/>
       <c r="B6" s="122"/>
       <c r="C6" s="123"/>
@@ -13916,13 +14075,8 @@
       <c r="I6" s="123"/>
       <c r="J6" s="124"/>
       <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="122"/>
       <c r="B7" s="122"/>
       <c r="C7" s="123"/>
@@ -13934,13 +14088,8 @@
       <c r="I7" s="123"/>
       <c r="J7" s="124"/>
       <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="122"/>
       <c r="B8" s="122"/>
       <c r="C8" s="123"/>
@@ -13952,13 +14101,8 @@
       <c r="I8" s="123"/>
       <c r="J8" s="124"/>
       <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="122"/>
       <c r="B9" s="122"/>
       <c r="C9" s="123"/>
@@ -13970,13 +14114,8 @@
       <c r="I9" s="123"/>
       <c r="J9" s="124"/>
       <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="122"/>
       <c r="B10" s="122"/>
       <c r="C10" s="123"/>
@@ -13988,13 +14127,8 @@
       <c r="I10" s="123"/>
       <c r="J10" s="124"/>
       <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="124"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="122"/>
       <c r="B11" s="122"/>
       <c r="C11" s="123"/>
@@ -14006,13 +14140,8 @@
       <c r="I11" s="123"/>
       <c r="J11" s="124"/>
       <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="122"/>
       <c r="B12" s="122"/>
       <c r="C12" s="123"/>
@@ -14024,13 +14153,8 @@
       <c r="I12" s="123"/>
       <c r="J12" s="124"/>
       <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="122"/>
       <c r="B13" s="122"/>
       <c r="C13" s="123"/>
@@ -14042,13 +14166,8 @@
       <c r="I13" s="123"/>
       <c r="J13" s="124"/>
       <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="122"/>
       <c r="B14" s="122"/>
       <c r="C14" s="123"/>
@@ -14060,13 +14179,8 @@
       <c r="I14" s="123"/>
       <c r="J14" s="124"/>
       <c r="K14" s="125"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="122"/>
       <c r="B15" s="122"/>
       <c r="C15" s="123"/>
@@ -14078,13 +14192,8 @@
       <c r="I15" s="123"/>
       <c r="J15" s="124"/>
       <c r="K15" s="125"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="122"/>
       <c r="B16" s="122"/>
       <c r="C16" s="123"/>
@@ -14096,13 +14205,8 @@
       <c r="I16" s="124"/>
       <c r="J16" s="124"/>
       <c r="K16" s="125"/>
-      <c r="L16" s="124"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="124"/>
-      <c r="O16" s="124"/>
-      <c r="P16" s="124"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="122"/>
       <c r="B17" s="122"/>
       <c r="C17" s="123"/>
@@ -14114,13 +14218,8 @@
       <c r="I17" s="124"/>
       <c r="J17" s="124"/>
       <c r="K17" s="125"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="122"/>
       <c r="B18" s="122"/>
       <c r="C18" s="123"/>
@@ -14132,13 +14231,8 @@
       <c r="I18" s="124"/>
       <c r="J18" s="124"/>
       <c r="K18" s="125"/>
-      <c r="L18" s="124"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="124"/>
-      <c r="O18" s="124"/>
-      <c r="P18" s="124"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="122"/>
       <c r="B19" s="122"/>
       <c r="C19" s="123"/>
@@ -14150,13 +14244,8 @@
       <c r="I19" s="124"/>
       <c r="J19" s="124"/>
       <c r="K19" s="125"/>
-      <c r="L19" s="124"/>
-      <c r="M19" s="123"/>
-      <c r="N19" s="124"/>
-      <c r="O19" s="124"/>
-      <c r="P19" s="124"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="122"/>
       <c r="B20" s="122"/>
       <c r="C20" s="123"/>
@@ -14168,13 +14257,8 @@
       <c r="I20" s="124"/>
       <c r="J20" s="124"/>
       <c r="K20" s="125"/>
-      <c r="L20" s="124"/>
-      <c r="M20" s="123"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="124"/>
-      <c r="P20" s="124"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="122"/>
       <c r="B21" s="122"/>
       <c r="C21" s="123"/>
@@ -14186,13 +14270,8 @@
       <c r="I21" s="124"/>
       <c r="J21" s="124"/>
       <c r="K21" s="124"/>
-      <c r="L21" s="124"/>
-      <c r="M21" s="123"/>
-      <c r="N21" s="124"/>
-      <c r="O21" s="124"/>
-      <c r="P21" s="124"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="122"/>
       <c r="B22" s="122"/>
       <c r="C22" s="123"/>
@@ -14203,13 +14282,8 @@
       <c r="H22" s="123"/>
       <c r="I22" s="124"/>
       <c r="J22" s="124"/>
-      <c r="L22" s="124"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="124"/>
-      <c r="P22" s="124"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="122"/>
       <c r="B23" s="122"/>
       <c r="C23" s="123"/>
@@ -14220,13 +14294,8 @@
       <c r="H23" s="123"/>
       <c r="I23" s="124"/>
       <c r="J23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="124"/>
-      <c r="O23" s="124"/>
-      <c r="P23" s="124"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="122"/>
       <c r="B24" s="122"/>
       <c r="C24" s="123"/>
@@ -14237,13 +14306,8 @@
       <c r="H24" s="123"/>
       <c r="I24" s="124"/>
       <c r="J24" s="124"/>
-      <c r="L24" s="124"/>
-      <c r="M24" s="123"/>
-      <c r="N24" s="124"/>
-      <c r="O24" s="124"/>
-      <c r="P24" s="124"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="122"/>
       <c r="B25" s="122"/>
       <c r="C25" s="123"/>
@@ -14254,13 +14318,8 @@
       <c r="H25" s="123"/>
       <c r="I25" s="124"/>
       <c r="J25" s="124"/>
-      <c r="L25" s="124"/>
-      <c r="M25" s="123"/>
-      <c r="N25" s="124"/>
-      <c r="O25" s="124"/>
-      <c r="P25" s="124"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="122"/>
       <c r="B26" s="122"/>
       <c r="C26" s="123"/>
@@ -14271,13 +14330,8 @@
       <c r="H26" s="123"/>
       <c r="I26" s="124"/>
       <c r="J26" s="124"/>
-      <c r="L26" s="124"/>
-      <c r="M26" s="123"/>
-      <c r="N26" s="124"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="122"/>
       <c r="B27" s="122"/>
       <c r="C27" s="123"/>
@@ -14288,13 +14342,8 @@
       <c r="H27" s="123"/>
       <c r="I27" s="124"/>
       <c r="J27" s="124"/>
-      <c r="L27" s="124"/>
-      <c r="M27" s="123"/>
-      <c r="N27" s="124"/>
-      <c r="O27" s="124"/>
-      <c r="P27" s="124"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="122"/>
       <c r="B28" s="122"/>
       <c r="C28" s="123"/>
@@ -14305,13 +14354,8 @@
       <c r="H28" s="123"/>
       <c r="I28" s="124"/>
       <c r="J28" s="124"/>
-      <c r="L28" s="124"/>
-      <c r="M28" s="123"/>
-      <c r="N28" s="124"/>
-      <c r="O28" s="124"/>
-      <c r="P28" s="124"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="122"/>
       <c r="B29" s="122"/>
       <c r="C29" s="123"/>
@@ -14322,13 +14366,8 @@
       <c r="H29" s="123"/>
       <c r="I29" s="124"/>
       <c r="J29" s="124"/>
-      <c r="L29" s="124"/>
-      <c r="M29" s="123"/>
-      <c r="N29" s="124"/>
-      <c r="O29" s="124"/>
-      <c r="P29" s="124"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="122"/>
       <c r="B30" s="122"/>
       <c r="C30" s="123"/>
@@ -14339,13 +14378,8 @@
       <c r="H30" s="123"/>
       <c r="I30" s="124"/>
       <c r="J30" s="124"/>
-      <c r="L30" s="124"/>
-      <c r="M30" s="123"/>
-      <c r="N30" s="124"/>
-      <c r="O30" s="124"/>
-      <c r="P30" s="124"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="122"/>
       <c r="B31" s="122"/>
       <c r="C31" s="123"/>
@@ -14356,13 +14390,8 @@
       <c r="H31" s="123"/>
       <c r="I31" s="124"/>
       <c r="J31" s="124"/>
-      <c r="L31" s="124"/>
-      <c r="M31" s="123"/>
-      <c r="N31" s="124"/>
-      <c r="O31" s="124"/>
-      <c r="P31" s="124"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="122"/>
       <c r="B32" s="122"/>
       <c r="C32" s="123"/>
@@ -14373,13 +14402,8 @@
       <c r="H32" s="123"/>
       <c r="I32" s="124"/>
       <c r="J32" s="124"/>
-      <c r="L32" s="124"/>
-      <c r="M32" s="123"/>
-      <c r="N32" s="124"/>
-      <c r="O32" s="124"/>
-      <c r="P32" s="124"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="122"/>
       <c r="B33" s="122"/>
       <c r="C33" s="123"/>
@@ -14390,13 +14414,8 @@
       <c r="H33" s="123"/>
       <c r="I33" s="124"/>
       <c r="J33" s="124"/>
-      <c r="L33" s="124"/>
-      <c r="M33" s="123"/>
-      <c r="N33" s="124"/>
-      <c r="O33" s="124"/>
-      <c r="P33" s="124"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="122"/>
       <c r="B34" s="122"/>
       <c r="C34" s="123"/>
@@ -14407,13 +14426,8 @@
       <c r="H34" s="123"/>
       <c r="I34" s="124"/>
       <c r="J34" s="124"/>
-      <c r="L34" s="124"/>
-      <c r="M34" s="123"/>
-      <c r="N34" s="124"/>
-      <c r="O34" s="124"/>
-      <c r="P34" s="124"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="122"/>
       <c r="B35" s="122"/>
       <c r="C35" s="123"/>
@@ -14424,13 +14438,8 @@
       <c r="H35" s="123"/>
       <c r="I35" s="124"/>
       <c r="J35" s="124"/>
-      <c r="L35" s="124"/>
-      <c r="M35" s="123"/>
-      <c r="N35" s="124"/>
-      <c r="O35" s="124"/>
-      <c r="P35" s="124"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="122"/>
       <c r="B36" s="122"/>
       <c r="C36" s="123"/>
@@ -14441,13 +14450,8 @@
       <c r="H36" s="123"/>
       <c r="I36" s="126"/>
       <c r="J36" s="124"/>
-      <c r="L36" s="124"/>
-      <c r="M36" s="123"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="124"/>
-      <c r="P36" s="124"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="122"/>
       <c r="B37" s="122"/>
       <c r="C37" s="123"/>
@@ -14458,13 +14462,8 @@
       <c r="H37" s="123"/>
       <c r="I37" s="126"/>
       <c r="J37" s="124"/>
-      <c r="L37" s="124"/>
-      <c r="M37" s="123"/>
-      <c r="N37" s="124"/>
-      <c r="O37" s="124"/>
-      <c r="P37" s="124"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="122"/>
       <c r="B38" s="122"/>
       <c r="C38" s="123"/>
@@ -14475,13 +14474,8 @@
       <c r="H38" s="123"/>
       <c r="I38" s="126"/>
       <c r="J38" s="124"/>
-      <c r="L38" s="124"/>
-      <c r="M38" s="123"/>
-      <c r="N38" s="124"/>
-      <c r="O38" s="124"/>
-      <c r="P38" s="124"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="122"/>
       <c r="B39" s="122"/>
       <c r="C39" s="123"/>
@@ -14492,13 +14486,8 @@
       <c r="H39" s="123"/>
       <c r="I39" s="126"/>
       <c r="J39" s="124"/>
-      <c r="L39" s="124"/>
-      <c r="M39" s="123"/>
-      <c r="N39" s="124"/>
-      <c r="O39" s="124"/>
-      <c r="P39" s="124"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="122"/>
       <c r="B40" s="122"/>
       <c r="C40" s="123"/>
@@ -14509,13 +14498,8 @@
       <c r="H40" s="123"/>
       <c r="I40" s="127"/>
       <c r="J40" s="124"/>
-      <c r="L40" s="124"/>
-      <c r="M40" s="123"/>
-      <c r="N40" s="124"/>
-      <c r="O40" s="124"/>
-      <c r="P40" s="124"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="122"/>
       <c r="B41" s="122"/>
       <c r="C41" s="123"/>
@@ -14526,13 +14510,8 @@
       <c r="H41" s="123"/>
       <c r="I41" s="127"/>
       <c r="J41" s="124"/>
-      <c r="L41" s="124"/>
-      <c r="M41" s="123"/>
-      <c r="N41" s="124"/>
-      <c r="O41" s="124"/>
-      <c r="P41" s="124"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="122"/>
       <c r="B42" s="122"/>
       <c r="C42" s="124"/>
@@ -14543,13 +14522,8 @@
       <c r="H42" s="123"/>
       <c r="I42" s="127"/>
       <c r="J42" s="124"/>
-      <c r="L42" s="124"/>
-      <c r="M42" s="123"/>
-      <c r="N42" s="124"/>
-      <c r="O42" s="124"/>
-      <c r="P42" s="124"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="122"/>
       <c r="B43" s="122"/>
       <c r="C43" s="124"/>
@@ -14560,13 +14534,8 @@
       <c r="H43" s="123"/>
       <c r="I43" s="127"/>
       <c r="J43" s="124"/>
-      <c r="L43" s="124"/>
-      <c r="M43" s="123"/>
-      <c r="N43" s="124"/>
-      <c r="O43" s="124"/>
-      <c r="P43" s="124"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="122"/>
       <c r="B44" s="122"/>
       <c r="C44" s="124"/>
@@ -14577,13 +14546,8 @@
       <c r="H44" s="123"/>
       <c r="I44" s="127"/>
       <c r="J44" s="124"/>
-      <c r="L44" s="124"/>
-      <c r="M44" s="123"/>
-      <c r="N44" s="124"/>
-      <c r="O44" s="124"/>
-      <c r="P44" s="124"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="122"/>
       <c r="B45" s="122"/>
       <c r="C45" s="124"/>
@@ -14594,13 +14558,8 @@
       <c r="H45" s="123"/>
       <c r="I45" s="127"/>
       <c r="J45" s="124"/>
-      <c r="L45" s="124"/>
-      <c r="M45" s="123"/>
-      <c r="N45" s="124"/>
-      <c r="O45" s="124"/>
-      <c r="P45" s="124"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="122"/>
       <c r="B46" s="122"/>
       <c r="C46" s="123"/>
@@ -14611,13 +14570,8 @@
       <c r="H46" s="123"/>
       <c r="I46" s="126"/>
       <c r="J46" s="124"/>
-      <c r="L46" s="124"/>
-      <c r="M46" s="123"/>
-      <c r="N46" s="124"/>
-      <c r="O46" s="124"/>
-      <c r="P46" s="124"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="122"/>
       <c r="B47" s="122"/>
       <c r="C47" s="123"/>
@@ -14628,13 +14582,8 @@
       <c r="H47" s="123"/>
       <c r="I47" s="124"/>
       <c r="J47" s="124"/>
-      <c r="L47" s="124"/>
-      <c r="M47" s="123"/>
-      <c r="N47" s="124"/>
-      <c r="O47" s="124"/>
-      <c r="P47" s="124"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="122"/>
       <c r="B48" s="122"/>
       <c r="C48" s="123"/>
@@ -14645,13 +14594,8 @@
       <c r="H48" s="123"/>
       <c r="I48" s="124"/>
       <c r="J48" s="124"/>
-      <c r="L48" s="124"/>
-      <c r="M48" s="123"/>
-      <c r="N48" s="124"/>
-      <c r="O48" s="124"/>
-      <c r="P48" s="124"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="122"/>
       <c r="B49" s="122"/>
       <c r="C49" s="124"/>
@@ -14662,13 +14606,8 @@
       <c r="H49" s="123"/>
       <c r="I49" s="124"/>
       <c r="J49" s="124"/>
-      <c r="L49" s="124"/>
-      <c r="M49" s="123"/>
-      <c r="N49" s="124"/>
-      <c r="O49" s="124"/>
-      <c r="P49" s="124"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="122"/>
       <c r="B50" s="122"/>
       <c r="C50" s="123"/>
@@ -14679,13 +14618,8 @@
       <c r="H50" s="123"/>
       <c r="I50" s="124"/>
       <c r="J50" s="124"/>
-      <c r="L50" s="124"/>
-      <c r="M50" s="123"/>
-      <c r="N50" s="124"/>
-      <c r="O50" s="124"/>
-      <c r="P50" s="124"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="122"/>
       <c r="B51" s="122"/>
       <c r="C51" s="123"/>
@@ -14696,13 +14630,8 @@
       <c r="H51" s="123"/>
       <c r="I51" s="124"/>
       <c r="J51" s="122"/>
-      <c r="L51" s="124"/>
-      <c r="M51" s="123"/>
-      <c r="N51" s="124"/>
-      <c r="O51" s="124"/>
-      <c r="P51" s="124"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="122"/>
       <c r="B52" s="122"/>
       <c r="C52" s="123"/>
@@ -14713,13 +14642,8 @@
       <c r="H52" s="123"/>
       <c r="I52" s="124"/>
       <c r="J52" s="122"/>
-      <c r="L52" s="124"/>
-      <c r="M52" s="123"/>
-      <c r="N52" s="124"/>
-      <c r="O52" s="124"/>
-      <c r="P52" s="124"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="122"/>
       <c r="B53" s="122"/>
       <c r="C53" s="122"/>
@@ -14730,13 +14654,8 @@
       <c r="H53" s="123"/>
       <c r="I53" s="124"/>
       <c r="J53" s="122"/>
-      <c r="L53" s="124"/>
-      <c r="M53" s="122"/>
-      <c r="N53" s="122"/>
-      <c r="O53" s="122"/>
-      <c r="P53" s="122"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="122"/>
       <c r="B54" s="122"/>
       <c r="C54" s="122"/>
@@ -14747,13 +14666,8 @@
       <c r="H54" s="123"/>
       <c r="I54" s="124"/>
       <c r="J54" s="122"/>
-      <c r="L54" s="124"/>
-      <c r="M54" s="122"/>
-      <c r="N54" s="122"/>
-      <c r="O54" s="122"/>
-      <c r="P54" s="122"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="122"/>
       <c r="B55" s="122"/>
       <c r="C55" s="122"/>
@@ -14764,13 +14678,8 @@
       <c r="H55" s="123"/>
       <c r="I55" s="124"/>
       <c r="J55" s="122"/>
-      <c r="L55" s="124"/>
-      <c r="M55" s="122"/>
-      <c r="N55" s="124"/>
-      <c r="O55" s="124"/>
-      <c r="P55" s="124"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="122"/>
       <c r="B56" s="122"/>
       <c r="C56" s="123"/>
@@ -14781,13 +14690,8 @@
       <c r="H56" s="123"/>
       <c r="I56" s="124"/>
       <c r="J56" s="124"/>
-      <c r="L56" s="124"/>
-      <c r="M56" s="123"/>
-      <c r="N56" s="124"/>
-      <c r="O56" s="124"/>
-      <c r="P56" s="124"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="122"/>
       <c r="B57" s="122"/>
       <c r="C57" s="123"/>
@@ -14798,13 +14702,8 @@
       <c r="H57" s="123"/>
       <c r="I57" s="124"/>
       <c r="J57" s="124"/>
-      <c r="L57" s="124"/>
-      <c r="M57" s="123"/>
-      <c r="N57" s="124"/>
-      <c r="O57" s="124"/>
-      <c r="P57" s="124"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="122"/>
       <c r="B58" s="122"/>
       <c r="C58" s="123"/>
@@ -14815,13 +14714,8 @@
       <c r="H58" s="123"/>
       <c r="I58" s="124"/>
       <c r="J58" s="124"/>
-      <c r="L58" s="124"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="124"/>
-      <c r="O58" s="124"/>
-      <c r="P58" s="124"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="122"/>
       <c r="B59" s="122"/>
       <c r="C59" s="123"/>
@@ -14832,13 +14726,8 @@
       <c r="H59" s="123"/>
       <c r="I59" s="124"/>
       <c r="J59" s="124"/>
-      <c r="L59" s="124"/>
-      <c r="M59" s="123"/>
-      <c r="N59" s="124"/>
-      <c r="O59" s="124"/>
-      <c r="P59" s="124"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="122"/>
       <c r="B60" s="122"/>
       <c r="C60" s="123"/>
@@ -14849,13 +14738,8 @@
       <c r="H60" s="123"/>
       <c r="I60" s="124"/>
       <c r="J60" s="124"/>
-      <c r="L60" s="124"/>
-      <c r="M60" s="123"/>
-      <c r="N60" s="124"/>
-      <c r="O60" s="124"/>
-      <c r="P60" s="124"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="122"/>
       <c r="B61" s="122"/>
       <c r="C61" s="123"/>
@@ -14866,13 +14750,8 @@
       <c r="H61" s="123"/>
       <c r="I61" s="124"/>
       <c r="J61" s="124"/>
-      <c r="L61" s="124"/>
-      <c r="M61" s="123"/>
-      <c r="N61" s="124"/>
-      <c r="O61" s="124"/>
-      <c r="P61" s="124"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A62" s="122"/>
       <c r="B62" s="122"/>
       <c r="C62" s="123"/>
@@ -14882,13 +14761,8 @@
       <c r="G62" s="123"/>
       <c r="H62" s="123"/>
       <c r="J62" s="124"/>
-      <c r="L62" s="124"/>
-      <c r="M62" s="123"/>
-      <c r="N62" s="124"/>
-      <c r="O62" s="124"/>
-      <c r="P62" s="124"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="122"/>
       <c r="B63" s="122"/>
       <c r="C63" s="123"/>
@@ -14898,13 +14772,8 @@
       <c r="G63" s="124"/>
       <c r="H63" s="123"/>
       <c r="J63" s="124"/>
-      <c r="L63" s="124"/>
-      <c r="M63" s="123"/>
-      <c r="N63" s="124"/>
-      <c r="O63" s="124"/>
-      <c r="P63" s="124"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="122"/>
       <c r="B64" s="122"/>
       <c r="C64" s="123"/>
@@ -14914,13 +14783,8 @@
       <c r="G64" s="124"/>
       <c r="H64" s="123"/>
       <c r="J64" s="124"/>
-      <c r="L64" s="124"/>
-      <c r="M64" s="123"/>
-      <c r="N64" s="124"/>
-      <c r="O64" s="124"/>
-      <c r="P64" s="124"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="122"/>
       <c r="B65" s="122"/>
       <c r="C65" s="123"/>
@@ -14930,13 +14794,8 @@
       <c r="G65" s="124"/>
       <c r="H65" s="123"/>
       <c r="J65" s="124"/>
-      <c r="L65" s="124"/>
-      <c r="M65" s="123"/>
-      <c r="N65" s="124"/>
-      <c r="O65" s="124"/>
-      <c r="P65" s="124"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="122"/>
       <c r="B66" s="122"/>
       <c r="C66" s="123"/>
@@ -14946,13 +14805,8 @@
       <c r="G66" s="124"/>
       <c r="H66" s="123"/>
       <c r="J66" s="124"/>
-      <c r="L66" s="124"/>
-      <c r="M66" s="123"/>
-      <c r="N66" s="124"/>
-      <c r="O66" s="124"/>
-      <c r="P66" s="124"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="122"/>
       <c r="B67" s="122"/>
       <c r="C67" s="124"/>
@@ -14962,13 +14816,8 @@
       <c r="G67" s="124"/>
       <c r="H67" s="123"/>
       <c r="J67" s="124"/>
-      <c r="L67" s="124"/>
-      <c r="M67" s="124"/>
-      <c r="N67" s="124"/>
-      <c r="O67" s="124"/>
-      <c r="P67" s="124"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A68" s="122"/>
       <c r="B68" s="122"/>
       <c r="C68" s="124"/>
@@ -14978,13 +14827,8 @@
       <c r="G68" s="124"/>
       <c r="H68" s="123"/>
       <c r="J68" s="124"/>
-      <c r="L68" s="124"/>
-      <c r="M68" s="124"/>
-      <c r="N68" s="124"/>
-      <c r="O68" s="124"/>
-      <c r="P68" s="124"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="122"/>
       <c r="B69" s="122"/>
       <c r="C69" s="124"/>
@@ -14994,13 +14838,8 @@
       <c r="G69" s="124"/>
       <c r="H69" s="123"/>
       <c r="J69" s="124"/>
-      <c r="L69" s="124"/>
-      <c r="M69" s="124"/>
-      <c r="N69" s="124"/>
-      <c r="O69" s="124"/>
-      <c r="P69" s="124"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="122"/>
       <c r="B70" s="122"/>
       <c r="C70" s="124"/>
@@ -15010,13 +14849,8 @@
       <c r="G70" s="124"/>
       <c r="H70" s="123"/>
       <c r="J70" s="124"/>
-      <c r="L70" s="124"/>
-      <c r="M70" s="124"/>
-      <c r="N70" s="124"/>
-      <c r="O70" s="124"/>
-      <c r="P70" s="124"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="122"/>
       <c r="B71" s="122"/>
       <c r="C71" s="123"/>
@@ -15026,13 +14860,8 @@
       <c r="G71" s="124"/>
       <c r="H71" s="123"/>
       <c r="J71" s="124"/>
-      <c r="L71" s="124"/>
-      <c r="M71" s="124"/>
-      <c r="N71" s="124"/>
-      <c r="O71" s="124"/>
-      <c r="P71" s="124"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="122"/>
       <c r="B72" s="122"/>
       <c r="C72" s="123"/>
@@ -15042,13 +14871,8 @@
       <c r="G72" s="124"/>
       <c r="H72" s="123"/>
       <c r="J72" s="124"/>
-      <c r="L72" s="124"/>
-      <c r="M72" s="124"/>
-      <c r="N72" s="124"/>
-      <c r="O72" s="124"/>
-      <c r="P72" s="124"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="122"/>
       <c r="B73" s="122"/>
       <c r="C73" s="123"/>
@@ -15058,13 +14882,8 @@
       <c r="G73" s="124"/>
       <c r="H73" s="123"/>
       <c r="J73" s="124"/>
-      <c r="L73" s="124"/>
-      <c r="M73" s="124"/>
-      <c r="N73" s="124"/>
-      <c r="O73" s="124"/>
-      <c r="P73" s="124"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="122"/>
       <c r="B74" s="122"/>
       <c r="C74" s="123"/>
@@ -15074,13 +14893,8 @@
       <c r="G74" s="124"/>
       <c r="H74" s="123"/>
       <c r="J74" s="124"/>
-      <c r="L74" s="124"/>
-      <c r="M74" s="124"/>
-      <c r="N74" s="124"/>
-      <c r="O74" s="124"/>
-      <c r="P74" s="124"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" s="122"/>
       <c r="B75" s="122"/>
       <c r="C75" s="123"/>
@@ -15090,13 +14904,8 @@
       <c r="G75" s="124"/>
       <c r="H75" s="123"/>
       <c r="J75" s="124"/>
-      <c r="L75" s="124"/>
-      <c r="M75" s="124"/>
-      <c r="N75" s="124"/>
-      <c r="O75" s="124"/>
-      <c r="P75" s="124"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="122"/>
       <c r="B76" s="122"/>
       <c r="C76" s="123"/>
@@ -15106,13 +14915,8 @@
       <c r="G76" s="124"/>
       <c r="H76" s="123"/>
       <c r="J76" s="124"/>
-      <c r="L76" s="124"/>
-      <c r="M76" s="124"/>
-      <c r="N76" s="124"/>
-      <c r="O76" s="124"/>
-      <c r="P76" s="124"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A77" s="122"/>
       <c r="B77" s="122"/>
       <c r="C77" s="123"/>
@@ -15122,13 +14926,8 @@
       <c r="G77" s="124"/>
       <c r="H77" s="123"/>
       <c r="J77" s="124"/>
-      <c r="L77" s="124"/>
-      <c r="M77" s="123"/>
-      <c r="N77" s="124"/>
-      <c r="O77" s="123"/>
-      <c r="P77" s="123"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="122"/>
       <c r="B78" s="122"/>
       <c r="C78" s="123"/>
@@ -15138,13 +14937,8 @@
       <c r="G78" s="124"/>
       <c r="H78" s="123"/>
       <c r="J78" s="124"/>
-      <c r="L78" s="124"/>
-      <c r="M78" s="123"/>
-      <c r="N78" s="124"/>
-      <c r="O78" s="123"/>
-      <c r="P78" s="123"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A79" s="122"/>
       <c r="B79" s="122"/>
       <c r="C79" s="123"/>
@@ -15154,13 +14948,8 @@
       <c r="G79" s="124"/>
       <c r="H79" s="123"/>
       <c r="J79" s="124"/>
-      <c r="L79" s="124"/>
-      <c r="M79" s="123"/>
-      <c r="N79" s="124"/>
-      <c r="O79" s="124"/>
-      <c r="P79" s="124"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A80" s="122"/>
       <c r="B80" s="122"/>
       <c r="C80" s="123"/>
@@ -15170,13 +14959,8 @@
       <c r="G80" s="124"/>
       <c r="H80" s="123"/>
       <c r="J80" s="124"/>
-      <c r="L80" s="124"/>
-      <c r="M80" s="123"/>
-      <c r="N80" s="124"/>
-      <c r="O80" s="124"/>
-      <c r="P80" s="124"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A81" s="122"/>
       <c r="B81" s="122"/>
       <c r="C81" s="123"/>
@@ -15186,13 +14970,8 @@
       <c r="G81" s="124"/>
       <c r="H81" s="123"/>
       <c r="J81" s="124"/>
-      <c r="L81" s="124"/>
-      <c r="M81" s="123"/>
-      <c r="N81" s="124"/>
-      <c r="O81" s="124"/>
-      <c r="P81" s="124"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A82" s="122"/>
       <c r="B82" s="122"/>
       <c r="C82" s="123"/>
@@ -15202,13 +14981,8 @@
       <c r="G82" s="124"/>
       <c r="H82" s="123"/>
       <c r="J82" s="124"/>
-      <c r="L82" s="124"/>
-      <c r="M82" s="123"/>
-      <c r="N82" s="124"/>
-      <c r="O82" s="124"/>
-      <c r="P82" s="124"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A83" s="122"/>
       <c r="B83" s="122"/>
       <c r="C83" s="123"/>
@@ -15218,13 +14992,8 @@
       <c r="G83" s="124"/>
       <c r="H83" s="123"/>
       <c r="J83" s="124"/>
-      <c r="L83" s="124"/>
-      <c r="M83" s="123"/>
-      <c r="N83" s="124"/>
-      <c r="O83" s="124"/>
-      <c r="P83" s="124"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A84" s="122"/>
       <c r="B84" s="122"/>
       <c r="C84" s="123"/>
@@ -15234,13 +15003,8 @@
       <c r="G84" s="124"/>
       <c r="H84" s="123"/>
       <c r="J84" s="124"/>
-      <c r="L84" s="124"/>
-      <c r="M84" s="123"/>
-      <c r="N84" s="124"/>
-      <c r="O84" s="124"/>
-      <c r="P84" s="124"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A85" s="122"/>
       <c r="B85" s="122"/>
       <c r="C85" s="123"/>
@@ -15250,13 +15014,8 @@
       <c r="G85" s="124"/>
       <c r="H85" s="123"/>
       <c r="J85" s="124"/>
-      <c r="L85" s="124"/>
-      <c r="M85" s="123"/>
-      <c r="N85" s="124"/>
-      <c r="O85" s="124"/>
-      <c r="P85" s="124"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A86" s="122"/>
       <c r="B86" s="122"/>
       <c r="C86" s="123"/>
@@ -15266,13 +15025,8 @@
       <c r="G86" s="124"/>
       <c r="H86" s="123"/>
       <c r="J86" s="124"/>
-      <c r="L86" s="124"/>
-      <c r="M86" s="123"/>
-      <c r="N86" s="124"/>
-      <c r="O86" s="124"/>
-      <c r="P86" s="124"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A87" s="122"/>
       <c r="B87" s="122"/>
       <c r="C87" s="123"/>
@@ -15282,13 +15036,8 @@
       <c r="G87" s="124"/>
       <c r="H87" s="123"/>
       <c r="J87" s="124"/>
-      <c r="L87" s="124"/>
-      <c r="M87" s="123"/>
-      <c r="N87" s="124"/>
-      <c r="O87" s="124"/>
-      <c r="P87" s="124"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A88" s="122"/>
       <c r="B88" s="122"/>
       <c r="C88" s="123"/>
@@ -15298,13 +15047,8 @@
       <c r="G88" s="124"/>
       <c r="H88" s="123"/>
       <c r="J88" s="124"/>
-      <c r="L88" s="124"/>
-      <c r="M88" s="123"/>
-      <c r="N88" s="124"/>
-      <c r="O88" s="124"/>
-      <c r="P88" s="124"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A89" s="122"/>
       <c r="B89" s="122"/>
       <c r="C89" s="123"/>
@@ -15314,13 +15058,8 @@
       <c r="G89" s="122"/>
       <c r="H89" s="123"/>
       <c r="J89" s="122"/>
-      <c r="L89" s="124"/>
-      <c r="M89" s="123"/>
-      <c r="N89" s="124"/>
-      <c r="O89" s="124"/>
-      <c r="P89" s="124"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A90" s="122"/>
       <c r="B90" s="122"/>
       <c r="C90" s="123"/>
@@ -15330,13 +15069,8 @@
       <c r="G90" s="122"/>
       <c r="H90" s="123"/>
       <c r="J90" s="122"/>
-      <c r="L90" s="124"/>
-      <c r="M90" s="123"/>
-      <c r="N90" s="124"/>
-      <c r="O90" s="124"/>
-      <c r="P90" s="124"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A91" s="122"/>
       <c r="B91" s="122"/>
       <c r="C91" s="123"/>
@@ -15346,13 +15080,8 @@
       <c r="G91" s="124"/>
       <c r="H91" s="123"/>
       <c r="J91" s="124"/>
-      <c r="L91" s="124"/>
-      <c r="M91" s="123"/>
-      <c r="N91" s="124"/>
-      <c r="O91" s="124"/>
-      <c r="P91" s="124"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A92" s="122"/>
       <c r="B92" s="122"/>
       <c r="C92" s="123"/>
@@ -15362,13 +15091,8 @@
       <c r="G92" s="124"/>
       <c r="H92" s="123"/>
       <c r="J92" s="124"/>
-      <c r="L92" s="124"/>
-      <c r="M92" s="123"/>
-      <c r="N92" s="124"/>
-      <c r="O92" s="124"/>
-      <c r="P92" s="124"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A93" s="122"/>
       <c r="B93" s="122"/>
       <c r="C93" s="123"/>
@@ -15378,13 +15102,8 @@
       <c r="G93" s="124"/>
       <c r="H93" s="123"/>
       <c r="J93" s="124"/>
-      <c r="L93" s="124"/>
-      <c r="M93" s="123"/>
-      <c r="N93" s="124"/>
-      <c r="O93" s="124"/>
-      <c r="P93" s="124"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A94" s="122"/>
       <c r="B94" s="122"/>
       <c r="C94" s="123"/>
@@ -15394,13 +15113,8 @@
       <c r="G94" s="124"/>
       <c r="H94" s="123"/>
       <c r="J94" s="124"/>
-      <c r="L94" s="124"/>
-      <c r="M94" s="123"/>
-      <c r="N94" s="124"/>
-      <c r="O94" s="124"/>
-      <c r="P94" s="124"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A95" s="122"/>
       <c r="B95" s="122"/>
       <c r="C95" s="123"/>
@@ -15410,13 +15124,8 @@
       <c r="G95" s="124"/>
       <c r="H95" s="123"/>
       <c r="J95" s="124"/>
-      <c r="L95" s="124"/>
-      <c r="M95" s="123"/>
-      <c r="N95" s="124"/>
-      <c r="O95" s="124"/>
-      <c r="P95" s="124"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A96" s="122"/>
       <c r="B96" s="122"/>
       <c r="C96" s="123"/>
@@ -15426,13 +15135,8 @@
       <c r="G96" s="124"/>
       <c r="H96" s="123"/>
       <c r="J96" s="124"/>
-      <c r="L96" s="124"/>
-      <c r="M96" s="123"/>
-      <c r="N96" s="124"/>
-      <c r="O96" s="124"/>
-      <c r="P96" s="124"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A97" s="122"/>
       <c r="B97" s="122"/>
       <c r="C97" s="123"/>
@@ -15442,13 +15146,8 @@
       <c r="G97" s="124"/>
       <c r="H97" s="123"/>
       <c r="J97" s="124"/>
-      <c r="L97" s="124"/>
-      <c r="M97" s="123"/>
-      <c r="N97" s="124"/>
-      <c r="O97" s="124"/>
-      <c r="P97" s="124"/>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A98" s="122"/>
       <c r="B98" s="122"/>
       <c r="C98" s="123"/>
@@ -15458,13 +15157,8 @@
       <c r="G98" s="124"/>
       <c r="H98" s="123"/>
       <c r="J98" s="124"/>
-      <c r="L98" s="124"/>
-      <c r="M98" s="123"/>
-      <c r="N98" s="124"/>
-      <c r="O98" s="124"/>
-      <c r="P98" s="124"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A99" s="122"/>
       <c r="B99" s="122"/>
       <c r="C99" s="123"/>
@@ -15474,13 +15168,8 @@
       <c r="G99" s="124"/>
       <c r="H99" s="123"/>
       <c r="J99" s="124"/>
-      <c r="L99" s="124"/>
-      <c r="M99" s="123"/>
-      <c r="N99" s="124"/>
-      <c r="O99" s="124"/>
-      <c r="P99" s="124"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A100" s="122"/>
       <c r="B100" s="122"/>
       <c r="C100" s="123"/>
@@ -15490,13 +15179,8 @@
       <c r="G100" s="124"/>
       <c r="H100" s="123"/>
       <c r="J100" s="124"/>
-      <c r="L100" s="124"/>
-      <c r="M100" s="123"/>
-      <c r="N100" s="124"/>
-      <c r="O100" s="124"/>
-      <c r="P100" s="124"/>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A101" s="122"/>
       <c r="B101" s="122"/>
       <c r="C101" s="123"/>
@@ -15506,13 +15190,8 @@
       <c r="G101" s="124"/>
       <c r="H101" s="123"/>
       <c r="J101" s="124"/>
-      <c r="L101" s="124"/>
-      <c r="M101" s="123"/>
-      <c r="N101" s="124"/>
-      <c r="O101" s="124"/>
-      <c r="P101" s="124"/>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="122"/>
       <c r="B102" s="122"/>
       <c r="C102" s="123"/>
@@ -15522,13 +15201,8 @@
       <c r="G102" s="124"/>
       <c r="H102" s="123"/>
       <c r="J102" s="124"/>
-      <c r="L102" s="124"/>
-      <c r="M102" s="123"/>
-      <c r="N102" s="124"/>
-      <c r="O102" s="124"/>
-      <c r="P102" s="124"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="122"/>
       <c r="B103" s="122"/>
       <c r="C103" s="123"/>
@@ -15538,13 +15212,8 @@
       <c r="G103" s="124"/>
       <c r="H103" s="123"/>
       <c r="J103" s="124"/>
-      <c r="L103" s="124"/>
-      <c r="M103" s="123"/>
-      <c r="N103" s="124"/>
-      <c r="O103" s="124"/>
-      <c r="P103" s="124"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A104" s="122"/>
       <c r="B104" s="122"/>
       <c r="C104" s="123"/>
@@ -15554,13 +15223,8 @@
       <c r="G104" s="124"/>
       <c r="H104" s="123"/>
       <c r="J104" s="124"/>
-      <c r="L104" s="124"/>
-      <c r="M104" s="123"/>
-      <c r="N104" s="124"/>
-      <c r="O104" s="124"/>
-      <c r="P104" s="124"/>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A105" s="122"/>
       <c r="B105" s="122"/>
       <c r="C105" s="123"/>
@@ -15570,13 +15234,8 @@
       <c r="G105" s="124"/>
       <c r="H105" s="123"/>
       <c r="J105" s="124"/>
-      <c r="L105" s="124"/>
-      <c r="M105" s="123"/>
-      <c r="N105" s="124"/>
-      <c r="O105" s="124"/>
-      <c r="P105" s="124"/>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="122"/>
       <c r="B106" s="122"/>
       <c r="C106" s="123"/>
@@ -15586,13 +15245,8 @@
       <c r="G106" s="124"/>
       <c r="H106" s="123"/>
       <c r="J106" s="124"/>
-      <c r="L106" s="124"/>
-      <c r="M106" s="123"/>
-      <c r="N106" s="124"/>
-      <c r="O106" s="124"/>
-      <c r="P106" s="124"/>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="122"/>
       <c r="B107" s="122"/>
       <c r="C107" s="123"/>
@@ -15602,13 +15256,8 @@
       <c r="G107" s="124"/>
       <c r="H107" s="123"/>
       <c r="J107" s="124"/>
-      <c r="L107" s="124"/>
-      <c r="M107" s="123"/>
-      <c r="N107" s="124"/>
-      <c r="O107" s="124"/>
-      <c r="P107" s="124"/>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A108" s="129"/>
       <c r="B108" s="130"/>
       <c r="C108" s="131"/>
@@ -15618,13 +15267,8 @@
       <c r="G108" s="125"/>
       <c r="H108" s="131"/>
       <c r="J108" s="125"/>
-      <c r="L108" s="124"/>
-      <c r="M108" s="131"/>
-      <c r="N108" s="125"/>
-      <c r="O108" s="125"/>
-      <c r="P108" s="124"/>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A109" s="129"/>
       <c r="B109" s="130"/>
       <c r="C109" s="131"/>
@@ -15634,13 +15278,8 @@
       <c r="G109" s="125"/>
       <c r="H109" s="131"/>
       <c r="J109" s="125"/>
-      <c r="L109" s="124"/>
-      <c r="M109" s="131"/>
-      <c r="N109" s="125"/>
-      <c r="O109" s="125"/>
-      <c r="P109" s="124"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A110" s="129"/>
       <c r="B110" s="130"/>
       <c r="C110" s="131"/>
@@ -15650,13 +15289,8 @@
       <c r="G110" s="125"/>
       <c r="H110" s="131"/>
       <c r="J110" s="125"/>
-      <c r="L110" s="124"/>
-      <c r="M110" s="131"/>
-      <c r="N110" s="125"/>
-      <c r="O110" s="125"/>
-      <c r="P110" s="124"/>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A111" s="129"/>
       <c r="B111" s="130"/>
       <c r="C111" s="131"/>
@@ -15666,13 +15300,8 @@
       <c r="G111" s="125"/>
       <c r="H111" s="131"/>
       <c r="J111" s="125"/>
-      <c r="L111" s="124"/>
-      <c r="M111" s="131"/>
-      <c r="N111" s="125"/>
-      <c r="O111" s="125"/>
-      <c r="P111" s="124"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A112" s="129"/>
       <c r="B112" s="130"/>
       <c r="C112" s="131"/>
@@ -15682,13 +15311,8 @@
       <c r="G112" s="125"/>
       <c r="H112" s="131"/>
       <c r="J112" s="125"/>
-      <c r="L112" s="124"/>
-      <c r="M112" s="131"/>
-      <c r="N112" s="125"/>
-      <c r="O112" s="125"/>
-      <c r="P112" s="124"/>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A113" s="129"/>
       <c r="B113" s="130"/>
       <c r="C113" s="131"/>
@@ -15698,13 +15322,8 @@
       <c r="G113" s="125"/>
       <c r="H113" s="131"/>
       <c r="J113" s="125"/>
-      <c r="L113" s="124"/>
-      <c r="M113" s="131"/>
-      <c r="N113" s="125"/>
-      <c r="O113" s="125"/>
-      <c r="P113" s="124"/>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A114" s="129"/>
       <c r="B114" s="130"/>
       <c r="C114" s="131"/>
@@ -15714,13 +15333,8 @@
       <c r="G114" s="125"/>
       <c r="H114" s="131"/>
       <c r="J114" s="125"/>
-      <c r="L114" s="124"/>
-      <c r="M114" s="131"/>
-      <c r="N114" s="125"/>
-      <c r="O114" s="125"/>
-      <c r="P114" s="124"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A115" s="129"/>
       <c r="B115" s="130"/>
       <c r="C115" s="131"/>
@@ -15730,13 +15344,8 @@
       <c r="G115" s="125"/>
       <c r="H115" s="131"/>
       <c r="J115" s="125"/>
-      <c r="L115" s="124"/>
-      <c r="M115" s="131"/>
-      <c r="N115" s="125"/>
-      <c r="O115" s="125"/>
-      <c r="P115" s="124"/>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="129"/>
       <c r="B116" s="130"/>
       <c r="C116" s="131"/>
@@ -15746,13 +15355,8 @@
       <c r="G116" s="125"/>
       <c r="H116" s="131"/>
       <c r="J116" s="125"/>
-      <c r="L116" s="124"/>
-      <c r="M116" s="131"/>
-      <c r="N116" s="125"/>
-      <c r="O116" s="125"/>
-      <c r="P116" s="124"/>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A117" s="122"/>
       <c r="B117" s="122"/>
       <c r="C117" s="123"/>
@@ -15762,13 +15366,8 @@
       <c r="G117" s="124"/>
       <c r="H117" s="123"/>
       <c r="J117" s="124"/>
-      <c r="L117" s="124"/>
-      <c r="M117" s="123"/>
-      <c r="N117" s="124"/>
-      <c r="O117" s="124"/>
-      <c r="P117" s="124"/>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A118" s="122"/>
       <c r="B118" s="122"/>
       <c r="C118" s="123"/>
@@ -15778,13 +15377,8 @@
       <c r="G118" s="124"/>
       <c r="H118" s="123"/>
       <c r="J118" s="124"/>
-      <c r="L118" s="124"/>
-      <c r="M118" s="123"/>
-      <c r="N118" s="124"/>
-      <c r="O118" s="124"/>
-      <c r="P118" s="124"/>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A119" s="122"/>
       <c r="B119" s="122"/>
       <c r="C119" s="123"/>
@@ -15794,13 +15388,8 @@
       <c r="G119" s="124"/>
       <c r="H119" s="123"/>
       <c r="J119" s="124"/>
-      <c r="L119" s="124"/>
-      <c r="M119" s="123"/>
-      <c r="N119" s="124"/>
-      <c r="O119" s="124"/>
-      <c r="P119" s="124"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A120" s="122"/>
       <c r="B120" s="122"/>
       <c r="C120" s="123"/>
@@ -15810,13 +15399,8 @@
       <c r="G120" s="124"/>
       <c r="H120" s="123"/>
       <c r="J120" s="124"/>
-      <c r="L120" s="124"/>
-      <c r="M120" s="123"/>
-      <c r="N120" s="124"/>
-      <c r="O120" s="124"/>
-      <c r="P120" s="124"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A121" s="122"/>
       <c r="B121" s="122"/>
       <c r="C121" s="123"/>
@@ -15826,13 +15410,8 @@
       <c r="G121" s="124"/>
       <c r="H121" s="123"/>
       <c r="J121" s="124"/>
-      <c r="L121" s="124"/>
-      <c r="M121" s="123"/>
-      <c r="N121" s="124"/>
-      <c r="O121" s="124"/>
-      <c r="P121" s="124"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A122" s="122"/>
       <c r="B122" s="122"/>
       <c r="C122" s="123"/>
@@ -15842,13 +15421,8 @@
       <c r="G122" s="124"/>
       <c r="H122" s="123"/>
       <c r="J122" s="124"/>
-      <c r="L122" s="124"/>
-      <c r="M122" s="123"/>
-      <c r="N122" s="124"/>
-      <c r="O122" s="124"/>
-      <c r="P122" s="124"/>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A123" s="122"/>
       <c r="B123" s="122"/>
       <c r="C123" s="123"/>
@@ -15858,13 +15432,8 @@
       <c r="G123" s="124"/>
       <c r="H123" s="123"/>
       <c r="J123" s="124"/>
-      <c r="L123" s="124"/>
-      <c r="M123" s="123"/>
-      <c r="N123" s="124"/>
-      <c r="O123" s="124"/>
-      <c r="P123" s="124"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A124" s="122"/>
       <c r="B124" s="122"/>
       <c r="C124" s="123"/>
@@ -15874,13 +15443,8 @@
       <c r="G124" s="124"/>
       <c r="H124" s="123"/>
       <c r="J124" s="124"/>
-      <c r="L124" s="124"/>
-      <c r="M124" s="123"/>
-      <c r="N124" s="124"/>
-      <c r="O124" s="124"/>
-      <c r="P124" s="124"/>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A125" s="122"/>
       <c r="B125" s="122"/>
       <c r="C125" s="123"/>
@@ -15890,13 +15454,8 @@
       <c r="G125" s="124"/>
       <c r="H125" s="123"/>
       <c r="J125" s="124"/>
-      <c r="L125" s="124"/>
-      <c r="M125" s="123"/>
-      <c r="N125" s="124"/>
-      <c r="O125" s="124"/>
-      <c r="P125" s="124"/>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A126" s="122"/>
       <c r="B126" s="122"/>
       <c r="C126" s="123"/>
@@ -15906,13 +15465,8 @@
       <c r="G126" s="124"/>
       <c r="H126" s="123"/>
       <c r="J126" s="124"/>
-      <c r="L126" s="124"/>
-      <c r="M126" s="123"/>
-      <c r="N126" s="124"/>
-      <c r="O126" s="124"/>
-      <c r="P126" s="124"/>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A127" s="122"/>
       <c r="B127" s="122"/>
       <c r="C127" s="123"/>
@@ -15922,13 +15476,8 @@
       <c r="G127" s="124"/>
       <c r="H127" s="123"/>
       <c r="J127" s="124"/>
-      <c r="L127" s="124"/>
-      <c r="M127" s="123"/>
-      <c r="N127" s="124"/>
-      <c r="O127" s="124"/>
-      <c r="P127" s="124"/>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="122"/>
       <c r="B128" s="122"/>
       <c r="C128" s="123"/>
@@ -15938,17 +15487,1642 @@
       <c r="G128" s="124"/>
       <c r="H128" s="123"/>
       <c r="J128" s="124"/>
-      <c r="L128" s="124"/>
-      <c r="M128" s="123"/>
-      <c r="N128" s="124"/>
-      <c r="O128" s="124"/>
-      <c r="P128" s="124"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;9&amp;K000000 Internal</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87D2317-D0EB-AE41-B4E0-FA5F5010AE48}">
+  <dimension ref="A1:J128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="111" t="s">
+        <v>350</v>
+      </c>
+      <c r="B1" s="112"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="114"/>
+    </row>
+    <row r="2" spans="1:10" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="117" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="117" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="117" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="117" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" s="117" t="s">
+        <v>308</v>
+      </c>
+      <c r="F2" s="118" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" s="118" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="117" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" s="91" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" s="91" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="119" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="119" t="s">
+        <v>321</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>325</v>
+      </c>
+      <c r="G3" s="119" t="s">
+        <v>326</v>
+      </c>
+      <c r="H3" s="119" t="s">
+        <v>327</v>
+      </c>
+      <c r="I3" s="119" t="s">
+        <v>328</v>
+      </c>
+      <c r="J3" s="119" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="122">
+        <v>44927</v>
+      </c>
+      <c r="B4" s="122"/>
+      <c r="C4" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="123" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="123" t="s">
+        <v>331</v>
+      </c>
+      <c r="F4" s="123" t="s">
+        <v>333</v>
+      </c>
+      <c r="G4" s="123" t="s">
+        <v>333</v>
+      </c>
+      <c r="H4" s="124" t="s">
+        <v>333</v>
+      </c>
+      <c r="I4" s="124" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" s="124" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="122">
+        <v>44927</v>
+      </c>
+      <c r="B5" s="122"/>
+      <c r="C5" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="123" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="123" t="s">
+        <v>331</v>
+      </c>
+      <c r="F5" s="124" t="s">
+        <v>333</v>
+      </c>
+      <c r="G5" s="123"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="122"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="122"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="122"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="122"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="122"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="122"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="122"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="124"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="122"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="122"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="122"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="122"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="122"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="124"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="122"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="124"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A19" s="122"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="123"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" s="122"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
+      <c r="J20" s="124"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="122"/>
+      <c r="B21" s="122"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="124"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="122"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="124"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="122"/>
+      <c r="B23" s="122"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="124"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="124"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="122"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
+      <c r="J24" s="124"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="122"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="123"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="124"/>
+      <c r="J25" s="124"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="122"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="124"/>
+      <c r="G26" s="123"/>
+      <c r="H26" s="124"/>
+      <c r="I26" s="124"/>
+      <c r="J26" s="124"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="124"/>
+      <c r="G27" s="123"/>
+      <c r="H27" s="124"/>
+      <c r="I27" s="124"/>
+      <c r="J27" s="124"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" s="122"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="124"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="124"/>
+      <c r="I28" s="124"/>
+      <c r="J28" s="124"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" s="122"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="123"/>
+      <c r="H29" s="124"/>
+      <c r="I29" s="124"/>
+      <c r="J29" s="124"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" s="122"/>
+      <c r="B30" s="122"/>
+      <c r="C30" s="123"/>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="123"/>
+      <c r="H30" s="124"/>
+      <c r="I30" s="124"/>
+      <c r="J30" s="124"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A31" s="122"/>
+      <c r="B31" s="122"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="123"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="124"/>
+      <c r="I31" s="124"/>
+      <c r="J31" s="124"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="122"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="124"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="124"/>
+      <c r="J32" s="124"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="122"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="124"/>
+      <c r="I33" s="124"/>
+      <c r="J33" s="124"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="122"/>
+      <c r="B34" s="122"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="123"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="123"/>
+      <c r="H34" s="124"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="124"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="122"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="124"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="122"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="123"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="124"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A37" s="122"/>
+      <c r="B37" s="122"/>
+      <c r="C37" s="123"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="124"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="124"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="122"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="123"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="124"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="124"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A39" s="122"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="123"/>
+      <c r="D39" s="123"/>
+      <c r="E39" s="123"/>
+      <c r="F39" s="124"/>
+      <c r="G39" s="123"/>
+      <c r="H39" s="124"/>
+      <c r="I39" s="124"/>
+      <c r="J39" s="124"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A40" s="122"/>
+      <c r="B40" s="122"/>
+      <c r="C40" s="123"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="124"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="124"/>
+      <c r="I40" s="124"/>
+      <c r="J40" s="124"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A41" s="122"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="123"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="124"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="124"/>
+      <c r="I41" s="124"/>
+      <c r="J41" s="124"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A42" s="122"/>
+      <c r="B42" s="122"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="123"/>
+      <c r="E42" s="123"/>
+      <c r="F42" s="124"/>
+      <c r="G42" s="123"/>
+      <c r="H42" s="124"/>
+      <c r="I42" s="124"/>
+      <c r="J42" s="124"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A43" s="122"/>
+      <c r="B43" s="122"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="123"/>
+      <c r="H43" s="124"/>
+      <c r="I43" s="124"/>
+      <c r="J43" s="124"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A44" s="122"/>
+      <c r="B44" s="122"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="123"/>
+      <c r="H44" s="124"/>
+      <c r="I44" s="124"/>
+      <c r="J44" s="124"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A45" s="122"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="124"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="123"/>
+      <c r="H45" s="124"/>
+      <c r="I45" s="124"/>
+      <c r="J45" s="124"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A46" s="122"/>
+      <c r="B46" s="122"/>
+      <c r="C46" s="123"/>
+      <c r="D46" s="123"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="124"/>
+      <c r="G46" s="123"/>
+      <c r="H46" s="124"/>
+      <c r="I46" s="124"/>
+      <c r="J46" s="124"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A47" s="122"/>
+      <c r="B47" s="122"/>
+      <c r="C47" s="123"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="123"/>
+      <c r="F47" s="124"/>
+      <c r="G47" s="123"/>
+      <c r="H47" s="124"/>
+      <c r="I47" s="124"/>
+      <c r="J47" s="124"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A48" s="122"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="123"/>
+      <c r="D48" s="123"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="124"/>
+      <c r="G48" s="123"/>
+      <c r="H48" s="124"/>
+      <c r="I48" s="124"/>
+      <c r="J48" s="124"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A49" s="122"/>
+      <c r="B49" s="122"/>
+      <c r="C49" s="124"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="124"/>
+      <c r="G49" s="123"/>
+      <c r="H49" s="124"/>
+      <c r="I49" s="124"/>
+      <c r="J49" s="124"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A50" s="122"/>
+      <c r="B50" s="122"/>
+      <c r="C50" s="123"/>
+      <c r="D50" s="123"/>
+      <c r="E50" s="124"/>
+      <c r="F50" s="124"/>
+      <c r="G50" s="123"/>
+      <c r="H50" s="124"/>
+      <c r="I50" s="124"/>
+      <c r="J50" s="124"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A51" s="122"/>
+      <c r="B51" s="122"/>
+      <c r="C51" s="123"/>
+      <c r="D51" s="122"/>
+      <c r="E51" s="122"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="124"/>
+      <c r="I51" s="124"/>
+      <c r="J51" s="124"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A52" s="122"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="123"/>
+      <c r="D52" s="122"/>
+      <c r="E52" s="122"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="123"/>
+      <c r="H52" s="124"/>
+      <c r="I52" s="124"/>
+      <c r="J52" s="124"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A53" s="122"/>
+      <c r="B53" s="122"/>
+      <c r="C53" s="122"/>
+      <c r="D53" s="122"/>
+      <c r="E53" s="122"/>
+      <c r="F53" s="124"/>
+      <c r="G53" s="122"/>
+      <c r="H53" s="122"/>
+      <c r="I53" s="122"/>
+      <c r="J53" s="122"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A54" s="122"/>
+      <c r="B54" s="122"/>
+      <c r="C54" s="122"/>
+      <c r="D54" s="122"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="124"/>
+      <c r="G54" s="122"/>
+      <c r="H54" s="122"/>
+      <c r="I54" s="122"/>
+      <c r="J54" s="122"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A55" s="122"/>
+      <c r="B55" s="122"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="122"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="124"/>
+      <c r="J55" s="124"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A56" s="122"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="123"/>
+      <c r="D56" s="123"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="124"/>
+      <c r="G56" s="123"/>
+      <c r="H56" s="124"/>
+      <c r="I56" s="124"/>
+      <c r="J56" s="124"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A57" s="122"/>
+      <c r="B57" s="122"/>
+      <c r="C57" s="123"/>
+      <c r="D57" s="123"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="124"/>
+      <c r="G57" s="123"/>
+      <c r="H57" s="124"/>
+      <c r="I57" s="124"/>
+      <c r="J57" s="124"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A58" s="122"/>
+      <c r="B58" s="122"/>
+      <c r="C58" s="123"/>
+      <c r="D58" s="123"/>
+      <c r="E58" s="123"/>
+      <c r="F58" s="124"/>
+      <c r="G58" s="123"/>
+      <c r="H58" s="124"/>
+      <c r="I58" s="124"/>
+      <c r="J58" s="124"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A59" s="122"/>
+      <c r="B59" s="122"/>
+      <c r="C59" s="123"/>
+      <c r="D59" s="123"/>
+      <c r="E59" s="123"/>
+      <c r="F59" s="124"/>
+      <c r="G59" s="123"/>
+      <c r="H59" s="124"/>
+      <c r="I59" s="124"/>
+      <c r="J59" s="124"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A60" s="122"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="123"/>
+      <c r="D60" s="123"/>
+      <c r="E60" s="123"/>
+      <c r="F60" s="124"/>
+      <c r="G60" s="123"/>
+      <c r="H60" s="124"/>
+      <c r="I60" s="124"/>
+      <c r="J60" s="124"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A61" s="122"/>
+      <c r="B61" s="122"/>
+      <c r="C61" s="123"/>
+      <c r="D61" s="123"/>
+      <c r="E61" s="123"/>
+      <c r="F61" s="124"/>
+      <c r="G61" s="123"/>
+      <c r="H61" s="124"/>
+      <c r="I61" s="124"/>
+      <c r="J61" s="124"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A62" s="122"/>
+      <c r="B62" s="122"/>
+      <c r="C62" s="123"/>
+      <c r="D62" s="123"/>
+      <c r="E62" s="123"/>
+      <c r="F62" s="124"/>
+      <c r="G62" s="123"/>
+      <c r="H62" s="124"/>
+      <c r="I62" s="124"/>
+      <c r="J62" s="124"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A63" s="122"/>
+      <c r="B63" s="122"/>
+      <c r="C63" s="123"/>
+      <c r="D63" s="123"/>
+      <c r="E63" s="123"/>
+      <c r="F63" s="124"/>
+      <c r="G63" s="123"/>
+      <c r="H63" s="124"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="124"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A64" s="122"/>
+      <c r="B64" s="122"/>
+      <c r="C64" s="123"/>
+      <c r="D64" s="123"/>
+      <c r="E64" s="123"/>
+      <c r="F64" s="124"/>
+      <c r="G64" s="123"/>
+      <c r="H64" s="124"/>
+      <c r="I64" s="124"/>
+      <c r="J64" s="124"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A65" s="122"/>
+      <c r="B65" s="122"/>
+      <c r="C65" s="123"/>
+      <c r="D65" s="123"/>
+      <c r="E65" s="123"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="123"/>
+      <c r="H65" s="124"/>
+      <c r="I65" s="124"/>
+      <c r="J65" s="124"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A66" s="122"/>
+      <c r="B66" s="122"/>
+      <c r="C66" s="123"/>
+      <c r="D66" s="124"/>
+      <c r="E66" s="123"/>
+      <c r="F66" s="124"/>
+      <c r="G66" s="123"/>
+      <c r="H66" s="124"/>
+      <c r="I66" s="124"/>
+      <c r="J66" s="124"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A67" s="122"/>
+      <c r="B67" s="122"/>
+      <c r="C67" s="124"/>
+      <c r="D67" s="124"/>
+      <c r="E67" s="123"/>
+      <c r="F67" s="124"/>
+      <c r="G67" s="124"/>
+      <c r="H67" s="124"/>
+      <c r="I67" s="124"/>
+      <c r="J67" s="124"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A68" s="122"/>
+      <c r="B68" s="122"/>
+      <c r="C68" s="124"/>
+      <c r="D68" s="124"/>
+      <c r="E68" s="123"/>
+      <c r="F68" s="124"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="124"/>
+      <c r="I68" s="124"/>
+      <c r="J68" s="124"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A69" s="122"/>
+      <c r="B69" s="122"/>
+      <c r="C69" s="124"/>
+      <c r="D69" s="124"/>
+      <c r="E69" s="123"/>
+      <c r="F69" s="124"/>
+      <c r="G69" s="124"/>
+      <c r="H69" s="124"/>
+      <c r="I69" s="124"/>
+      <c r="J69" s="124"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A70" s="122"/>
+      <c r="B70" s="122"/>
+      <c r="C70" s="124"/>
+      <c r="D70" s="124"/>
+      <c r="E70" s="123"/>
+      <c r="F70" s="124"/>
+      <c r="G70" s="124"/>
+      <c r="H70" s="124"/>
+      <c r="I70" s="124"/>
+      <c r="J70" s="124"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A71" s="122"/>
+      <c r="B71" s="122"/>
+      <c r="C71" s="123"/>
+      <c r="D71" s="124"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="124"/>
+      <c r="I71" s="124"/>
+      <c r="J71" s="124"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A72" s="122"/>
+      <c r="B72" s="122"/>
+      <c r="C72" s="123"/>
+      <c r="D72" s="124"/>
+      <c r="E72" s="123"/>
+      <c r="F72" s="124"/>
+      <c r="G72" s="124"/>
+      <c r="H72" s="124"/>
+      <c r="I72" s="124"/>
+      <c r="J72" s="124"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A73" s="122"/>
+      <c r="B73" s="122"/>
+      <c r="C73" s="123"/>
+      <c r="D73" s="124"/>
+      <c r="E73" s="123"/>
+      <c r="F73" s="124"/>
+      <c r="G73" s="124"/>
+      <c r="H73" s="124"/>
+      <c r="I73" s="124"/>
+      <c r="J73" s="124"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A74" s="122"/>
+      <c r="B74" s="122"/>
+      <c r="C74" s="123"/>
+      <c r="D74" s="124"/>
+      <c r="E74" s="123"/>
+      <c r="F74" s="124"/>
+      <c r="G74" s="124"/>
+      <c r="H74" s="124"/>
+      <c r="I74" s="124"/>
+      <c r="J74" s="124"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A75" s="122"/>
+      <c r="B75" s="122"/>
+      <c r="C75" s="123"/>
+      <c r="D75" s="124"/>
+      <c r="E75" s="123"/>
+      <c r="F75" s="124"/>
+      <c r="G75" s="124"/>
+      <c r="H75" s="124"/>
+      <c r="I75" s="124"/>
+      <c r="J75" s="124"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A76" s="122"/>
+      <c r="B76" s="122"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="124"/>
+      <c r="E76" s="124"/>
+      <c r="F76" s="124"/>
+      <c r="G76" s="124"/>
+      <c r="H76" s="124"/>
+      <c r="I76" s="124"/>
+      <c r="J76" s="124"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A77" s="122"/>
+      <c r="B77" s="122"/>
+      <c r="C77" s="123"/>
+      <c r="D77" s="123"/>
+      <c r="E77" s="123"/>
+      <c r="F77" s="124"/>
+      <c r="G77" s="123"/>
+      <c r="H77" s="124"/>
+      <c r="I77" s="123"/>
+      <c r="J77" s="123"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A78" s="122"/>
+      <c r="B78" s="122"/>
+      <c r="C78" s="123"/>
+      <c r="D78" s="123"/>
+      <c r="E78" s="123"/>
+      <c r="F78" s="124"/>
+      <c r="G78" s="123"/>
+      <c r="H78" s="124"/>
+      <c r="I78" s="123"/>
+      <c r="J78" s="123"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A79" s="122"/>
+      <c r="B79" s="122"/>
+      <c r="C79" s="123"/>
+      <c r="D79" s="123"/>
+      <c r="E79" s="123"/>
+      <c r="F79" s="124"/>
+      <c r="G79" s="123"/>
+      <c r="H79" s="124"/>
+      <c r="I79" s="124"/>
+      <c r="J79" s="124"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A80" s="122"/>
+      <c r="B80" s="122"/>
+      <c r="C80" s="123"/>
+      <c r="D80" s="123"/>
+      <c r="E80" s="123"/>
+      <c r="F80" s="124"/>
+      <c r="G80" s="123"/>
+      <c r="H80" s="124"/>
+      <c r="I80" s="124"/>
+      <c r="J80" s="124"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A81" s="122"/>
+      <c r="B81" s="122"/>
+      <c r="C81" s="123"/>
+      <c r="D81" s="123"/>
+      <c r="E81" s="123"/>
+      <c r="F81" s="124"/>
+      <c r="G81" s="123"/>
+      <c r="H81" s="124"/>
+      <c r="I81" s="124"/>
+      <c r="J81" s="124"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A82" s="122"/>
+      <c r="B82" s="122"/>
+      <c r="C82" s="123"/>
+      <c r="D82" s="123"/>
+      <c r="E82" s="123"/>
+      <c r="F82" s="124"/>
+      <c r="G82" s="123"/>
+      <c r="H82" s="124"/>
+      <c r="I82" s="124"/>
+      <c r="J82" s="124"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A83" s="122"/>
+      <c r="B83" s="122"/>
+      <c r="C83" s="123"/>
+      <c r="D83" s="123"/>
+      <c r="E83" s="123"/>
+      <c r="F83" s="124"/>
+      <c r="G83" s="123"/>
+      <c r="H83" s="124"/>
+      <c r="I83" s="124"/>
+      <c r="J83" s="124"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A84" s="122"/>
+      <c r="B84" s="122"/>
+      <c r="C84" s="123"/>
+      <c r="D84" s="123"/>
+      <c r="E84" s="123"/>
+      <c r="F84" s="124"/>
+      <c r="G84" s="123"/>
+      <c r="H84" s="124"/>
+      <c r="I84" s="124"/>
+      <c r="J84" s="124"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A85" s="122"/>
+      <c r="B85" s="122"/>
+      <c r="C85" s="123"/>
+      <c r="D85" s="123"/>
+      <c r="E85" s="123"/>
+      <c r="F85" s="124"/>
+      <c r="G85" s="123"/>
+      <c r="H85" s="124"/>
+      <c r="I85" s="124"/>
+      <c r="J85" s="124"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A86" s="122"/>
+      <c r="B86" s="122"/>
+      <c r="C86" s="123"/>
+      <c r="D86" s="123"/>
+      <c r="E86" s="123"/>
+      <c r="F86" s="124"/>
+      <c r="G86" s="123"/>
+      <c r="H86" s="124"/>
+      <c r="I86" s="124"/>
+      <c r="J86" s="124"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A87" s="122"/>
+      <c r="B87" s="122"/>
+      <c r="C87" s="123"/>
+      <c r="D87" s="123"/>
+      <c r="E87" s="123"/>
+      <c r="F87" s="124"/>
+      <c r="G87" s="123"/>
+      <c r="H87" s="124"/>
+      <c r="I87" s="124"/>
+      <c r="J87" s="124"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A88" s="122"/>
+      <c r="B88" s="122"/>
+      <c r="C88" s="123"/>
+      <c r="D88" s="123"/>
+      <c r="E88" s="123"/>
+      <c r="F88" s="124"/>
+      <c r="G88" s="123"/>
+      <c r="H88" s="124"/>
+      <c r="I88" s="124"/>
+      <c r="J88" s="124"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A89" s="122"/>
+      <c r="B89" s="122"/>
+      <c r="C89" s="123"/>
+      <c r="D89" s="123"/>
+      <c r="E89" s="123"/>
+      <c r="F89" s="124"/>
+      <c r="G89" s="123"/>
+      <c r="H89" s="124"/>
+      <c r="I89" s="124"/>
+      <c r="J89" s="124"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A90" s="122"/>
+      <c r="B90" s="122"/>
+      <c r="C90" s="123"/>
+      <c r="D90" s="123"/>
+      <c r="E90" s="123"/>
+      <c r="F90" s="124"/>
+      <c r="G90" s="123"/>
+      <c r="H90" s="124"/>
+      <c r="I90" s="124"/>
+      <c r="J90" s="124"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A91" s="122"/>
+      <c r="B91" s="122"/>
+      <c r="C91" s="123"/>
+      <c r="D91" s="123"/>
+      <c r="E91" s="123"/>
+      <c r="F91" s="124"/>
+      <c r="G91" s="123"/>
+      <c r="H91" s="124"/>
+      <c r="I91" s="124"/>
+      <c r="J91" s="124"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A92" s="122"/>
+      <c r="B92" s="122"/>
+      <c r="C92" s="123"/>
+      <c r="D92" s="123"/>
+      <c r="E92" s="123"/>
+      <c r="F92" s="124"/>
+      <c r="G92" s="123"/>
+      <c r="H92" s="124"/>
+      <c r="I92" s="124"/>
+      <c r="J92" s="124"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A93" s="122"/>
+      <c r="B93" s="122"/>
+      <c r="C93" s="123"/>
+      <c r="D93" s="123"/>
+      <c r="E93" s="123"/>
+      <c r="F93" s="124"/>
+      <c r="G93" s="123"/>
+      <c r="H93" s="124"/>
+      <c r="I93" s="124"/>
+      <c r="J93" s="124"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A94" s="122"/>
+      <c r="B94" s="122"/>
+      <c r="C94" s="123"/>
+      <c r="D94" s="123"/>
+      <c r="E94" s="123"/>
+      <c r="F94" s="124"/>
+      <c r="G94" s="123"/>
+      <c r="H94" s="124"/>
+      <c r="I94" s="124"/>
+      <c r="J94" s="124"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A95" s="122"/>
+      <c r="B95" s="122"/>
+      <c r="C95" s="123"/>
+      <c r="D95" s="123"/>
+      <c r="E95" s="128"/>
+      <c r="F95" s="124"/>
+      <c r="G95" s="123"/>
+      <c r="H95" s="124"/>
+      <c r="I95" s="124"/>
+      <c r="J95" s="124"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A96" s="122"/>
+      <c r="B96" s="122"/>
+      <c r="C96" s="123"/>
+      <c r="D96" s="123"/>
+      <c r="E96" s="123"/>
+      <c r="F96" s="124"/>
+      <c r="G96" s="123"/>
+      <c r="H96" s="124"/>
+      <c r="I96" s="124"/>
+      <c r="J96" s="124"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A97" s="122"/>
+      <c r="B97" s="122"/>
+      <c r="C97" s="123"/>
+      <c r="D97" s="123"/>
+      <c r="E97" s="128"/>
+      <c r="F97" s="124"/>
+      <c r="G97" s="123"/>
+      <c r="H97" s="124"/>
+      <c r="I97" s="124"/>
+      <c r="J97" s="124"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A98" s="122"/>
+      <c r="B98" s="122"/>
+      <c r="C98" s="123"/>
+      <c r="D98" s="123"/>
+      <c r="E98" s="123"/>
+      <c r="F98" s="124"/>
+      <c r="G98" s="123"/>
+      <c r="H98" s="124"/>
+      <c r="I98" s="124"/>
+      <c r="J98" s="124"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A99" s="122"/>
+      <c r="B99" s="122"/>
+      <c r="C99" s="123"/>
+      <c r="D99" s="123"/>
+      <c r="E99" s="123"/>
+      <c r="F99" s="124"/>
+      <c r="G99" s="123"/>
+      <c r="H99" s="124"/>
+      <c r="I99" s="124"/>
+      <c r="J99" s="124"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A100" s="122"/>
+      <c r="B100" s="122"/>
+      <c r="C100" s="123"/>
+      <c r="D100" s="123"/>
+      <c r="E100" s="123"/>
+      <c r="F100" s="124"/>
+      <c r="G100" s="123"/>
+      <c r="H100" s="124"/>
+      <c r="I100" s="124"/>
+      <c r="J100" s="124"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A101" s="122"/>
+      <c r="B101" s="122"/>
+      <c r="C101" s="123"/>
+      <c r="D101" s="123"/>
+      <c r="E101" s="123"/>
+      <c r="F101" s="124"/>
+      <c r="G101" s="123"/>
+      <c r="H101" s="124"/>
+      <c r="I101" s="124"/>
+      <c r="J101" s="124"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A102" s="122"/>
+      <c r="B102" s="122"/>
+      <c r="C102" s="123"/>
+      <c r="D102" s="123"/>
+      <c r="E102" s="123"/>
+      <c r="F102" s="124"/>
+      <c r="G102" s="123"/>
+      <c r="H102" s="124"/>
+      <c r="I102" s="124"/>
+      <c r="J102" s="124"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A103" s="122"/>
+      <c r="B103" s="122"/>
+      <c r="C103" s="123"/>
+      <c r="D103" s="123"/>
+      <c r="E103" s="123"/>
+      <c r="F103" s="124"/>
+      <c r="G103" s="123"/>
+      <c r="H103" s="124"/>
+      <c r="I103" s="124"/>
+      <c r="J103" s="124"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A104" s="122"/>
+      <c r="B104" s="122"/>
+      <c r="C104" s="123"/>
+      <c r="D104" s="123"/>
+      <c r="E104" s="123"/>
+      <c r="F104" s="124"/>
+      <c r="G104" s="123"/>
+      <c r="H104" s="124"/>
+      <c r="I104" s="124"/>
+      <c r="J104" s="124"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A105" s="122"/>
+      <c r="B105" s="122"/>
+      <c r="C105" s="123"/>
+      <c r="D105" s="123"/>
+      <c r="E105" s="123"/>
+      <c r="F105" s="124"/>
+      <c r="G105" s="123"/>
+      <c r="H105" s="124"/>
+      <c r="I105" s="124"/>
+      <c r="J105" s="124"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A106" s="122"/>
+      <c r="B106" s="122"/>
+      <c r="C106" s="123"/>
+      <c r="D106" s="123"/>
+      <c r="E106" s="123"/>
+      <c r="F106" s="124"/>
+      <c r="G106" s="123"/>
+      <c r="H106" s="124"/>
+      <c r="I106" s="124"/>
+      <c r="J106" s="124"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A107" s="122"/>
+      <c r="B107" s="122"/>
+      <c r="C107" s="123"/>
+      <c r="D107" s="123"/>
+      <c r="E107" s="123"/>
+      <c r="F107" s="124"/>
+      <c r="G107" s="123"/>
+      <c r="H107" s="124"/>
+      <c r="I107" s="124"/>
+      <c r="J107" s="124"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A108" s="129"/>
+      <c r="B108" s="130"/>
+      <c r="C108" s="131"/>
+      <c r="D108" s="131"/>
+      <c r="E108" s="131"/>
+      <c r="F108" s="124"/>
+      <c r="G108" s="131"/>
+      <c r="H108" s="125"/>
+      <c r="I108" s="125"/>
+      <c r="J108" s="124"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A109" s="129"/>
+      <c r="B109" s="130"/>
+      <c r="C109" s="131"/>
+      <c r="D109" s="131"/>
+      <c r="E109" s="131"/>
+      <c r="F109" s="124"/>
+      <c r="G109" s="131"/>
+      <c r="H109" s="125"/>
+      <c r="I109" s="125"/>
+      <c r="J109" s="124"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A110" s="129"/>
+      <c r="B110" s="130"/>
+      <c r="C110" s="131"/>
+      <c r="D110" s="131"/>
+      <c r="E110" s="131"/>
+      <c r="F110" s="124"/>
+      <c r="G110" s="131"/>
+      <c r="H110" s="125"/>
+      <c r="I110" s="125"/>
+      <c r="J110" s="124"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A111" s="129"/>
+      <c r="B111" s="130"/>
+      <c r="C111" s="131"/>
+      <c r="D111" s="131"/>
+      <c r="E111" s="131"/>
+      <c r="F111" s="124"/>
+      <c r="G111" s="131"/>
+      <c r="H111" s="125"/>
+      <c r="I111" s="125"/>
+      <c r="J111" s="124"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A112" s="129"/>
+      <c r="B112" s="130"/>
+      <c r="C112" s="131"/>
+      <c r="D112" s="131"/>
+      <c r="E112" s="131"/>
+      <c r="F112" s="124"/>
+      <c r="G112" s="131"/>
+      <c r="H112" s="125"/>
+      <c r="I112" s="125"/>
+      <c r="J112" s="124"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A113" s="129"/>
+      <c r="B113" s="130"/>
+      <c r="C113" s="131"/>
+      <c r="D113" s="131"/>
+      <c r="E113" s="131"/>
+      <c r="F113" s="124"/>
+      <c r="G113" s="131"/>
+      <c r="H113" s="125"/>
+      <c r="I113" s="125"/>
+      <c r="J113" s="124"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A114" s="129"/>
+      <c r="B114" s="130"/>
+      <c r="C114" s="131"/>
+      <c r="D114" s="131"/>
+      <c r="E114" s="131"/>
+      <c r="F114" s="124"/>
+      <c r="G114" s="131"/>
+      <c r="H114" s="125"/>
+      <c r="I114" s="125"/>
+      <c r="J114" s="124"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A115" s="129"/>
+      <c r="B115" s="130"/>
+      <c r="C115" s="131"/>
+      <c r="D115" s="131"/>
+      <c r="E115" s="131"/>
+      <c r="F115" s="124"/>
+      <c r="G115" s="131"/>
+      <c r="H115" s="125"/>
+      <c r="I115" s="125"/>
+      <c r="J115" s="124"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A116" s="129"/>
+      <c r="B116" s="130"/>
+      <c r="C116" s="131"/>
+      <c r="D116" s="131"/>
+      <c r="E116" s="131"/>
+      <c r="F116" s="124"/>
+      <c r="G116" s="131"/>
+      <c r="H116" s="125"/>
+      <c r="I116" s="125"/>
+      <c r="J116" s="124"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A117" s="122"/>
+      <c r="B117" s="122"/>
+      <c r="C117" s="123"/>
+      <c r="D117" s="123"/>
+      <c r="E117" s="123"/>
+      <c r="F117" s="124"/>
+      <c r="G117" s="123"/>
+      <c r="H117" s="124"/>
+      <c r="I117" s="124"/>
+      <c r="J117" s="124"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A118" s="122"/>
+      <c r="B118" s="122"/>
+      <c r="C118" s="123"/>
+      <c r="D118" s="123"/>
+      <c r="E118" s="123"/>
+      <c r="F118" s="124"/>
+      <c r="G118" s="123"/>
+      <c r="H118" s="124"/>
+      <c r="I118" s="124"/>
+      <c r="J118" s="124"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A119" s="122"/>
+      <c r="B119" s="122"/>
+      <c r="C119" s="123"/>
+      <c r="D119" s="123"/>
+      <c r="E119" s="123"/>
+      <c r="F119" s="124"/>
+      <c r="G119" s="123"/>
+      <c r="H119" s="124"/>
+      <c r="I119" s="124"/>
+      <c r="J119" s="124"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A120" s="122"/>
+      <c r="B120" s="122"/>
+      <c r="C120" s="123"/>
+      <c r="D120" s="123"/>
+      <c r="E120" s="123"/>
+      <c r="F120" s="124"/>
+      <c r="G120" s="123"/>
+      <c r="H120" s="124"/>
+      <c r="I120" s="124"/>
+      <c r="J120" s="124"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A121" s="122"/>
+      <c r="B121" s="122"/>
+      <c r="C121" s="123"/>
+      <c r="D121" s="123"/>
+      <c r="E121" s="123"/>
+      <c r="F121" s="124"/>
+      <c r="G121" s="123"/>
+      <c r="H121" s="124"/>
+      <c r="I121" s="124"/>
+      <c r="J121" s="124"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A122" s="122"/>
+      <c r="B122" s="122"/>
+      <c r="C122" s="123"/>
+      <c r="D122" s="123"/>
+      <c r="E122" s="123"/>
+      <c r="F122" s="124"/>
+      <c r="G122" s="123"/>
+      <c r="H122" s="124"/>
+      <c r="I122" s="124"/>
+      <c r="J122" s="124"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A123" s="122"/>
+      <c r="B123" s="122"/>
+      <c r="C123" s="123"/>
+      <c r="D123" s="123"/>
+      <c r="E123" s="123"/>
+      <c r="F123" s="124"/>
+      <c r="G123" s="123"/>
+      <c r="H123" s="124"/>
+      <c r="I123" s="124"/>
+      <c r="J123" s="124"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A124" s="122"/>
+      <c r="B124" s="122"/>
+      <c r="C124" s="123"/>
+      <c r="D124" s="123"/>
+      <c r="E124" s="123"/>
+      <c r="F124" s="124"/>
+      <c r="G124" s="123"/>
+      <c r="H124" s="124"/>
+      <c r="I124" s="124"/>
+      <c r="J124" s="124"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A125" s="122"/>
+      <c r="B125" s="122"/>
+      <c r="C125" s="123"/>
+      <c r="D125" s="123"/>
+      <c r="E125" s="123"/>
+      <c r="F125" s="124"/>
+      <c r="G125" s="123"/>
+      <c r="H125" s="124"/>
+      <c r="I125" s="124"/>
+      <c r="J125" s="124"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A126" s="122"/>
+      <c r="B126" s="122"/>
+      <c r="C126" s="123"/>
+      <c r="D126" s="123"/>
+      <c r="E126" s="123"/>
+      <c r="F126" s="124"/>
+      <c r="G126" s="123"/>
+      <c r="H126" s="124"/>
+      <c r="I126" s="124"/>
+      <c r="J126" s="124"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A127" s="122"/>
+      <c r="B127" s="122"/>
+      <c r="C127" s="123"/>
+      <c r="D127" s="123"/>
+      <c r="E127" s="123"/>
+      <c r="F127" s="124"/>
+      <c r="G127" s="123"/>
+      <c r="H127" s="124"/>
+      <c r="I127" s="124"/>
+      <c r="J127" s="124"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A128" s="122"/>
+      <c r="B128" s="122"/>
+      <c r="C128" s="123"/>
+      <c r="D128" s="123"/>
+      <c r="E128" s="123"/>
+      <c r="F128" s="124"/>
+      <c r="G128" s="123"/>
+      <c r="H128" s="124"/>
+      <c r="I128" s="124"/>
+      <c r="J128" s="124"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>